<commit_message>
Increase sprite limit, meteor storm mode begins
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819B5FFB-06A0-4012-9EFB-DBE9EEC13210}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB729B1-FE4A-4526-A9ED-189E53408D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -1001,8 +1001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="A1:P58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1675,7 +1675,7 @@
         <v>72</v>
       </c>
       <c r="F19" s="9">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="27"/>
@@ -1930,7 +1930,7 @@
       </c>
       <c r="G26" s="8">
         <f>F19*F26</f>
-        <v>32</v>
+        <v>128</v>
       </c>
       <c r="H26" s="12"/>
       <c r="I26" s="28"/>
@@ -1966,6 +1966,7 @@
         <v>73</v>
       </c>
       <c r="F27" s="8">
+        <f>F19*F26</f>
         <v>128</v>
       </c>
       <c r="H27" s="12"/>

</xml_diff>

<commit_message>
Fix starfield direction and add speed modifier
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB729B1-FE4A-4526-A9ED-189E53408D90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DBB97C-A0C3-475B-98F8-C063525E7804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="124">
   <si>
     <t>Per sprite</t>
   </si>
@@ -182,9 +182,6 @@
   </si>
   <si>
     <t>0x00FF</t>
-  </si>
-  <si>
-    <t>0x06EF</t>
   </si>
   <si>
     <t>Area</t>
@@ -400,6 +397,21 @@
   </si>
   <si>
     <t>0x8000</t>
+  </si>
+  <si>
+    <t>0x8A00</t>
+  </si>
+  <si>
+    <t>0x00EF</t>
+  </si>
+  <si>
+    <t>Starfield</t>
+  </si>
+  <si>
+    <t>0x0010</t>
+  </si>
+  <si>
+    <t>0x05F0</t>
   </si>
 </sst>
 </file>
@@ -617,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -673,16 +685,28 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -999,10 +1023,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
-  <dimension ref="A1:P58"/>
+  <dimension ref="A1:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,7 +1056,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>34</v>
@@ -1049,16 +1073,16 @@
         <v>2</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F2" s="9">
         <v>1</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J2" s="5" t="s">
         <v>41</v>
@@ -1093,16 +1117,16 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F3">
         <v>16</v>
       </c>
       <c r="G3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I3" s="14" t="s">
         <v>12</v>
@@ -1111,7 +1135,7 @@
         <v>10</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="L3" s="3" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(O3))</f>
@@ -1135,17 +1159,17 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F4">
         <v>16</v>
       </c>
       <c r="H4" s="12"/>
-      <c r="I4" s="27" t="s">
-        <v>50</v>
+      <c r="I4" s="29" t="s">
+        <v>49</v>
       </c>
       <c r="J4" s="3" t="str">
-        <f t="shared" ref="J4:J35" si="1">L3</f>
+        <f t="shared" ref="J4:J37" si="1">L3</f>
         <v>0x8000</v>
       </c>
       <c r="K4" s="3" t="s">
@@ -1173,14 +1197,14 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E5" s="8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F5" s="8">
         <f>F3*F4</f>
         <v>256</v>
       </c>
       <c r="H5" s="12"/>
-      <c r="I5" s="27"/>
+      <c r="I5" s="30"/>
       <c r="J5" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8001</v>
@@ -1210,14 +1234,14 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F6">
         <f>F5/8</f>
         <v>32</v>
       </c>
       <c r="H6" s="12"/>
-      <c r="I6" s="27"/>
+      <c r="I6" s="30"/>
       <c r="J6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8100</v>
@@ -1251,14 +1275,14 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F7" s="8">
         <f>F6</f>
         <v>32</v>
       </c>
       <c r="H7" s="12"/>
-      <c r="I7" s="27"/>
+      <c r="I7" s="30"/>
       <c r="J7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x81C0</v>
@@ -1288,7 +1312,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H8" s="12"/>
-      <c r="I8" s="27"/>
+      <c r="I8" s="30"/>
       <c r="J8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8200</v>
@@ -1318,10 +1342,10 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H9" s="12"/>
-      <c r="I9" s="27"/>
+      <c r="I9" s="30"/>
       <c r="J9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8260</v>
@@ -1351,13 +1375,13 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E10" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" s="9">
         <v>16</v>
       </c>
       <c r="H10" s="12"/>
-      <c r="I10" s="27"/>
+      <c r="I10" s="30"/>
       <c r="J10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8300</v>
@@ -1387,13 +1411,13 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F11">
         <v>16</v>
       </c>
       <c r="H11" s="12"/>
-      <c r="I11" s="27"/>
+      <c r="I11" s="30"/>
       <c r="J11" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8360</v>
@@ -1423,13 +1447,13 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E12" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F12">
         <v>16</v>
       </c>
       <c r="H12" s="12"/>
-      <c r="I12" s="27"/>
+      <c r="I12" s="30"/>
       <c r="J12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8400</v>
@@ -1459,16 +1483,16 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F13">
         <v>4</v>
       </c>
       <c r="G13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H13" s="12"/>
-      <c r="I13" s="27"/>
+      <c r="I13" s="30"/>
       <c r="J13" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8430</v>
@@ -1498,14 +1522,14 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E14" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F14" s="8">
         <f>F11*F12*F13</f>
         <v>1024</v>
       </c>
       <c r="H14" s="12"/>
-      <c r="I14" s="27"/>
+      <c r="I14" s="30"/>
       <c r="J14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8500</v>
@@ -1535,14 +1559,14 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F15">
         <f>F14/8</f>
         <v>128</v>
       </c>
       <c r="H15" s="12"/>
-      <c r="I15" s="27"/>
+      <c r="I15" s="30"/>
       <c r="J15" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8560</v>
@@ -1572,14 +1596,14 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E16" s="8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F16" s="8">
         <f>F10*F15</f>
         <v>2048</v>
       </c>
       <c r="H16" s="12"/>
-      <c r="I16" s="27"/>
+      <c r="I16" s="30"/>
       <c r="J16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8600</v>
@@ -1609,7 +1633,7 @@
     </row>
     <row r="17" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H17" s="12"/>
-      <c r="I17" s="27"/>
+      <c r="I17" s="30"/>
       <c r="J17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x860C</v>
@@ -1639,10 +1663,10 @@
     </row>
     <row r="18" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="H18" s="12"/>
-      <c r="I18" s="27"/>
+      <c r="I18" s="30"/>
       <c r="J18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8700</v>
@@ -1672,13 +1696,13 @@
     </row>
     <row r="19" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E19" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F19" s="9">
         <v>32</v>
       </c>
       <c r="H19" s="12"/>
-      <c r="I19" s="27"/>
+      <c r="I19" s="30"/>
       <c r="J19" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8730</v>
@@ -1708,13 +1732,13 @@
     </row>
     <row r="20" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E20" s="10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="H20" s="12"/>
-      <c r="I20" s="27"/>
+      <c r="I20" s="30"/>
       <c r="J20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8800</v>
@@ -1727,7 +1751,7 @@
         <v>0x8821</v>
       </c>
       <c r="M20" s="3">
-        <f t="shared" ref="M20:N22" si="25">HEX2DEC(MID(J20, 3, LEN(J20)-2))</f>
+        <f t="shared" ref="M20:N23" si="25">HEX2DEC(MID(J20, 3, LEN(J20)-2))</f>
         <v>34816</v>
       </c>
       <c r="N20" s="3">
@@ -1744,13 +1768,13 @@
     </row>
     <row r="21" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E21" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F21">
         <v>15</v>
       </c>
       <c r="H21" s="12"/>
-      <c r="I21" s="27"/>
+      <c r="I21" s="30"/>
       <c r="J21" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8821</v>
@@ -1780,13 +1804,13 @@
     </row>
     <row r="22" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E22" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F22">
         <v>4</v>
       </c>
       <c r="H22" s="12"/>
-      <c r="I22" s="27"/>
+      <c r="I22" s="30"/>
       <c r="J22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8900</v>
@@ -1816,35 +1840,35 @@
     </row>
     <row r="23" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E23" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F23">
         <v>12</v>
       </c>
       <c r="H23" s="12"/>
-      <c r="I23" s="27"/>
+      <c r="I23" s="30"/>
       <c r="J23" s="4" t="str">
-        <f t="shared" si="1"/>
+        <f>L22</f>
         <v>0x8911</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="L23" s="4" t="str">
         <f t="shared" ref="L23" si="27">_xlfn.CONCAT("0x",DEC2HEX(O23))</f>
-        <v>0x9000</v>
+        <v>0x8A00</v>
       </c>
       <c r="M23" s="4">
-        <f t="shared" ref="M23" si="28">HEX2DEC(MID(J23, 3, LEN(J23)-2))</f>
+        <f t="shared" si="25"/>
         <v>35089</v>
       </c>
       <c r="N23" s="4">
-        <f t="shared" ref="N23" si="29">HEX2DEC(MID(K23, 3, LEN(K23)-2))</f>
-        <v>1775</v>
+        <f t="shared" si="25"/>
+        <v>239</v>
       </c>
       <c r="O23" s="4">
-        <f t="shared" ref="O23" si="30">M23+N23</f>
-        <v>36864</v>
+        <f t="shared" ref="O23" si="28">M23+N23</f>
+        <v>35328</v>
       </c>
       <c r="P23" s="4" t="s">
         <v>35</v>
@@ -1853,34 +1877,31 @@
     <row r="24" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E24" s="10"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="J24" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x9000</v>
+      <c r="I24" s="30"/>
+      <c r="J24" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>13</v>
+        <v>122</v>
       </c>
       <c r="L24" s="3" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(O24))</f>
-        <v>0x9800</v>
+        <v>0x8A10</v>
       </c>
       <c r="M24" s="3">
-        <f>HEX2DEC(MID(J24, 3, LEN(J24)-2))</f>
-        <v>36864</v>
+        <f t="shared" ref="M24" si="29">HEX2DEC(MID(J24, 3, LEN(J24)-2))</f>
+        <v>35328</v>
       </c>
       <c r="N24" s="3">
-        <f>HEX2DEC(MID(K24, 3, LEN(K24)-2))</f>
-        <v>2048</v>
+        <f t="shared" ref="N24" si="30">HEX2DEC(MID(K24, 3, LEN(K24)-2))</f>
+        <v>16</v>
       </c>
       <c r="O24" s="3">
         <f>M24+N24</f>
-        <v>38912</v>
+        <v>35344</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>14</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="5:16" x14ac:dyDescent="0.25">
@@ -1892,32 +1913,32 @@
         <v>32</v>
       </c>
       <c r="H25" s="12"/>
-      <c r="I25" s="28"/>
-      <c r="J25" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x9800</v>
-      </c>
-      <c r="K25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L25" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(O25))</f>
-        <v>0xA000</v>
-      </c>
-      <c r="M25" s="3">
-        <f>HEX2DEC(MID(J25, 3, LEN(J25)-2))</f>
-        <v>38912</v>
-      </c>
-      <c r="N25" s="3">
-        <f>HEX2DEC(MID(K25, 3, LEN(K25)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="O25" s="3">
-        <f>M25+N25</f>
-        <v>40960</v>
-      </c>
-      <c r="P25" s="3" t="s">
-        <v>52</v>
+      <c r="I25" s="31"/>
+      <c r="J25" s="4" t="str">
+        <f>L24</f>
+        <v>0x8A10</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="L25" s="4" t="str">
+        <f t="shared" ref="L25" si="31">_xlfn.CONCAT("0x",DEC2HEX(O25))</f>
+        <v>0x9000</v>
+      </c>
+      <c r="M25" s="4">
+        <f t="shared" ref="M25" si="32">HEX2DEC(MID(J25, 3, LEN(J25)-2))</f>
+        <v>35344</v>
+      </c>
+      <c r="N25" s="4">
+        <f t="shared" ref="N25" si="33">HEX2DEC(MID(K25, 3, LEN(K25)-2))</f>
+        <v>1520</v>
+      </c>
+      <c r="O25" s="4">
+        <f t="shared" ref="O25" si="34">M25+N25</f>
+        <v>36864</v>
+      </c>
+      <c r="P25" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="5:16" x14ac:dyDescent="0.25">
@@ -1933,135 +1954,134 @@
         <v>128</v>
       </c>
       <c r="H26" s="12"/>
-      <c r="I26" s="28"/>
+      <c r="I26" s="32" t="s">
+        <v>53</v>
+      </c>
       <c r="J26" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0xA000</v>
+        <v>0x9000</v>
       </c>
       <c r="K26" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L26" s="3" t="str">
-        <f t="shared" ref="L26" si="31">_xlfn.CONCAT("0x",DEC2HEX(O26))</f>
-        <v>0xA800</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(O26))</f>
+        <v>0x9800</v>
       </c>
       <c r="M26" s="3">
-        <f t="shared" ref="M26" si="32">HEX2DEC(MID(J26, 3, LEN(J26)-2))</f>
-        <v>40960</v>
+        <f>HEX2DEC(MID(J26, 3, LEN(J26)-2))</f>
+        <v>36864</v>
       </c>
       <c r="N26" s="3">
-        <f t="shared" ref="N26" si="33">HEX2DEC(MID(K26, 3, LEN(K26)-2))</f>
+        <f>HEX2DEC(MID(K26, 3, LEN(K26)-2))</f>
         <v>2048</v>
       </c>
       <c r="O26" s="3">
-        <f t="shared" ref="O26" si="34">M26+N26</f>
-        <v>43008</v>
+        <f>M26+N26</f>
+        <v>38912</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>51</v>
+        <v>14</v>
       </c>
     </row>
     <row r="27" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E27" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F27" s="8">
         <f>F19*F26</f>
         <v>128</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="28"/>
+      <c r="I27" s="33"/>
       <c r="J27" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0xA800</v>
+        <v>0x9800</v>
       </c>
       <c r="K27" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L27" s="3" t="str">
-        <f t="shared" ref="L27" si="35">_xlfn.CONCAT("0x",DEC2HEX(O27))</f>
-        <v>0xB000</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(O27))</f>
+        <v>0xA000</v>
       </c>
       <c r="M27" s="3">
-        <f t="shared" ref="M27" si="36">HEX2DEC(MID(J27, 3, LEN(J27)-2))</f>
-        <v>43008</v>
+        <f>HEX2DEC(MID(J27, 3, LEN(J27)-2))</f>
+        <v>38912</v>
       </c>
       <c r="N27" s="3">
-        <f t="shared" ref="N27" si="37">HEX2DEC(MID(K27, 3, LEN(K27)-2))</f>
+        <f>HEX2DEC(MID(K27, 3, LEN(K27)-2))</f>
         <v>2048</v>
       </c>
       <c r="O27" s="3">
-        <f t="shared" ref="O27" si="38">M27+N27</f>
-        <v>45056</v>
+        <f>M27+N27</f>
+        <v>40960</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H28" s="12"/>
-      <c r="I28" s="24" t="s">
-        <v>65</v>
-      </c>
+      <c r="I28" s="33"/>
       <c r="J28" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0xB000</v>
-      </c>
-      <c r="K28" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(F27))</f>
-        <v>0x80</v>
+        <v>0xA000</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="L28" s="3" t="str">
-        <f t="shared" ref="L28:L30" si="39">_xlfn.CONCAT("0x",DEC2HEX(O28))</f>
-        <v>0xB080</v>
+        <f t="shared" ref="L28" si="35">_xlfn.CONCAT("0x",DEC2HEX(O28))</f>
+        <v>0xA800</v>
       </c>
       <c r="M28" s="3">
-        <f t="shared" ref="M28:M30" si="40">HEX2DEC(MID(J28, 3, LEN(J28)-2))</f>
-        <v>45056</v>
+        <f t="shared" ref="M28" si="36">HEX2DEC(MID(J28, 3, LEN(J28)-2))</f>
+        <v>40960</v>
       </c>
       <c r="N28" s="3">
-        <f t="shared" ref="N28:N30" si="41">HEX2DEC(MID(K28, 3, LEN(K28)-2))</f>
-        <v>128</v>
+        <f t="shared" ref="N28" si="37">HEX2DEC(MID(K28, 3, LEN(K28)-2))</f>
+        <v>2048</v>
       </c>
       <c r="O28" s="3">
-        <f t="shared" ref="O28:O30" si="42">M28+N28</f>
-        <v>45184</v>
+        <f t="shared" ref="O28" si="38">M28+N28</f>
+        <v>43008</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E29" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H29" s="12"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="4" t="str">
+      <c r="I29" s="34"/>
+      <c r="J29" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0xB080</v>
-      </c>
-      <c r="K29" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L29" s="4" t="str">
-        <f t="shared" si="39"/>
-        <v>0xB800</v>
-      </c>
-      <c r="M29" s="4">
-        <f t="shared" si="40"/>
-        <v>45184</v>
-      </c>
-      <c r="N29" s="4">
-        <f t="shared" si="41"/>
-        <v>1920</v>
-      </c>
-      <c r="O29" s="4">
-        <f t="shared" si="42"/>
-        <v>47104</v>
-      </c>
-      <c r="P29" s="4" t="s">
-        <v>35</v>
+        <v>0xA800</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L29" s="3" t="str">
+        <f t="shared" ref="L29" si="39">_xlfn.CONCAT("0x",DEC2HEX(O29))</f>
+        <v>0xB000</v>
+      </c>
+      <c r="M29" s="3">
+        <f t="shared" ref="M29" si="40">HEX2DEC(MID(J29, 3, LEN(J29)-2))</f>
+        <v>43008</v>
+      </c>
+      <c r="N29" s="3">
+        <f t="shared" ref="N29" si="41">HEX2DEC(MID(K29, 3, LEN(K29)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="O29" s="3">
+        <f t="shared" ref="O29" si="42">M29+N29</f>
+        <v>45056</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="5:16" x14ac:dyDescent="0.25">
@@ -2076,33 +2096,35 @@
         <v>352</v>
       </c>
       <c r="H30" s="12"/>
-      <c r="I30" s="25"/>
+      <c r="I30" s="24" t="s">
+        <v>64</v>
+      </c>
       <c r="J30" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0xB800</v>
+        <v>0xB000</v>
       </c>
       <c r="K30" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(F38))</f>
-        <v>0x800</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(F27))</f>
+        <v>0x80</v>
       </c>
       <c r="L30" s="3" t="str">
-        <f t="shared" si="39"/>
-        <v>0xC000</v>
+        <f t="shared" ref="L30:L32" si="43">_xlfn.CONCAT("0x",DEC2HEX(O30))</f>
+        <v>0xB080</v>
       </c>
       <c r="M30" s="3">
-        <f t="shared" si="40"/>
-        <v>47104</v>
+        <f t="shared" ref="M30:M32" si="44">HEX2DEC(MID(J30, 3, LEN(J30)-2))</f>
+        <v>45056</v>
       </c>
       <c r="N30" s="3">
-        <f t="shared" si="41"/>
-        <v>2048</v>
+        <f t="shared" ref="N30:N32" si="45">HEX2DEC(MID(K30, 3, LEN(K30)-2))</f>
+        <v>128</v>
       </c>
       <c r="O30" s="3">
-        <f t="shared" si="42"/>
-        <v>49152</v>
+        <f t="shared" ref="O30:O32" si="46">M30+N30</f>
+        <v>45184</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>92</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="5:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2117,14 +2139,33 @@
         <v>272</v>
       </c>
       <c r="H31" s="12"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-      <c r="M31" s="4"/>
-      <c r="N31" s="4"/>
-      <c r="O31" s="4"/>
-      <c r="P31" s="4"/>
+      <c r="I31" s="25"/>
+      <c r="J31" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB080</v>
+      </c>
+      <c r="K31" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L31" s="4" t="str">
+        <f t="shared" si="43"/>
+        <v>0xB800</v>
+      </c>
+      <c r="M31" s="4">
+        <f t="shared" si="44"/>
+        <v>45184</v>
+      </c>
+      <c r="N31" s="4">
+        <f t="shared" si="45"/>
+        <v>1920</v>
+      </c>
+      <c r="O31" s="4">
+        <f t="shared" si="46"/>
+        <v>47104</v>
+      </c>
+      <c r="P31" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="32" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
@@ -2133,156 +2174,162 @@
       <c r="F32">
         <v>240</v>
       </c>
-      <c r="H32" s="13"/>
-      <c r="I32" s="15" t="s">
-        <v>55</v>
-      </c>
+      <c r="H32" s="12"/>
+      <c r="I32" s="25"/>
       <c r="J32" s="3" t="str">
-        <f>L30</f>
+        <f t="shared" si="1"/>
+        <v>0xB800</v>
+      </c>
+      <c r="K32" s="3" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(F38))</f>
+        <v>0x800</v>
+      </c>
+      <c r="L32" s="3" t="str">
+        <f t="shared" si="43"/>
         <v>0xC000</v>
       </c>
-      <c r="K32" s="3" t="s">
+      <c r="M32" s="3">
+        <f t="shared" si="44"/>
+        <v>47104</v>
+      </c>
+      <c r="N32" s="3">
+        <f t="shared" si="45"/>
+        <v>2048</v>
+      </c>
+      <c r="O32" s="3">
+        <f t="shared" si="46"/>
+        <v>49152</v>
+      </c>
+      <c r="P32" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H33" s="12"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H34" s="13"/>
+      <c r="I34" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J34" s="3" t="str">
+        <f>L32</f>
+        <v>0xC000</v>
+      </c>
+      <c r="K34" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="L32" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(O32))</f>
+      <c r="L34" s="3" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(O34))</f>
         <v>0x10000</v>
       </c>
-      <c r="M32" s="3">
-        <f>HEX2DEC(MID(J32, 3, LEN(J32)-2))</f>
+      <c r="M34" s="3">
+        <f>HEX2DEC(MID(J34, 3, LEN(J34)-2))</f>
         <v>49152</v>
       </c>
-      <c r="N32" s="3">
-        <f>HEX2DEC(MID(K32, 3, LEN(K32)-2))</f>
+      <c r="N34" s="3">
+        <f>HEX2DEC(MID(K34, 3, LEN(K34)-2))</f>
         <v>16384</v>
       </c>
-      <c r="O32" s="3">
-        <f>M32+N32</f>
+      <c r="O34" s="3">
+        <f>M34+N34</f>
         <v>65536</v>
       </c>
-      <c r="P32" s="3" t="s">
+      <c r="P34" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="30" x14ac:dyDescent="0.25">
-      <c r="H33" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="I33" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="J33" s="3" t="str">
+    <row r="35" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I35" s="27" t="s">
+        <v>63</v>
+      </c>
+      <c r="J35" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x10000</v>
       </c>
-      <c r="K33" s="3" t="str">
+      <c r="K35" s="3" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(F6))</f>
         <v>0x20</v>
       </c>
-      <c r="L33" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(O33))</f>
+      <c r="L35" s="3" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(O35))</f>
         <v>0x10020</v>
       </c>
-      <c r="M33" s="3">
-        <f>HEX2DEC(MID(J33, 3, LEN(J33)-2))</f>
+      <c r="M35" s="3">
+        <f>HEX2DEC(MID(J35, 3, LEN(J35)-2))</f>
         <v>65536</v>
       </c>
-      <c r="N33" s="3">
-        <f>HEX2DEC(MID(K33, 3, LEN(K33)-2))</f>
+      <c r="N35" s="3">
+        <f>HEX2DEC(MID(K35, 3, LEN(K35)-2))</f>
         <v>32</v>
       </c>
-      <c r="O33" s="3">
-        <f>M33+N33</f>
+      <c r="O35" s="3">
+        <f>M35+N35</f>
         <v>65568</v>
       </c>
-      <c r="P33" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E34" s="1" t="s">
+      <c r="P35" s="3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
         <v>87</v>
       </c>
-      <c r="H34" s="7"/>
-      <c r="I34" s="30"/>
-      <c r="J34" s="4" t="str">
+      <c r="F36">
+        <v>512</v>
+      </c>
+      <c r="H36" s="7"/>
+      <c r="I36" s="28"/>
+      <c r="J36" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x10020</v>
       </c>
-      <c r="K34" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="L34" s="4" t="str">
-        <f t="shared" ref="L34" si="43">_xlfn.CONCAT("0x",DEC2HEX(O34))</f>
+      <c r="K36" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L36" s="4" t="str">
+        <f t="shared" ref="L36" si="47">_xlfn.CONCAT("0x",DEC2HEX(O36))</f>
         <v>0x11000</v>
       </c>
-      <c r="M34" s="4">
-        <f t="shared" ref="M34" si="44">HEX2DEC(MID(J34, 3, LEN(J34)-2))</f>
+      <c r="M36" s="4">
+        <f t="shared" ref="M36" si="48">HEX2DEC(MID(J36, 3, LEN(J36)-2))</f>
         <v>65568</v>
       </c>
-      <c r="N34" s="4">
-        <f t="shared" ref="N34" si="45">HEX2DEC(MID(K34, 3, LEN(K34)-2))</f>
+      <c r="N36" s="4">
+        <f t="shared" ref="N36" si="49">HEX2DEC(MID(K36, 3, LEN(K36)-2))</f>
         <v>4064</v>
       </c>
-      <c r="O34" s="4">
-        <f t="shared" ref="O34" si="46">M34+N34</f>
+      <c r="O36" s="4">
+        <f t="shared" ref="O36" si="50">M36+N36</f>
         <v>69632</v>
       </c>
-      <c r="P34" s="4" t="s">
+      <c r="P36" s="4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E35" t="s">
-        <v>115</v>
-      </c>
-      <c r="F35">
-        <v>2</v>
-      </c>
-      <c r="H35" s="7"/>
-      <c r="I35" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="J35" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x11000</v>
-      </c>
-      <c r="K35" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(F16))</f>
-        <v>0x800</v>
-      </c>
-      <c r="L35" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(O35))</f>
-        <v>0x11800</v>
-      </c>
-      <c r="M35" s="3">
-        <f>HEX2DEC(MID(J35, 3, LEN(J35)-2))</f>
-        <v>69632</v>
-      </c>
-      <c r="N35" s="3">
-        <f>HEX2DEC(MID(K35, 3, LEN(K35)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="O35" s="3">
-        <f>M35+N35</f>
-        <v>71680</v>
-      </c>
-      <c r="P35" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="E36" t="s">
-        <v>88</v>
-      </c>
-      <c r="F36">
-        <v>512</v>
-      </c>
-      <c r="H36" s="7"/>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F37">
         <v>16</v>
@@ -2292,10 +2339,40 @@
         <v>2</v>
       </c>
       <c r="H37" s="7"/>
+      <c r="I37" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J37" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x11000</v>
+      </c>
+      <c r="K37" s="3" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(F16))</f>
+        <v>0x800</v>
+      </c>
+      <c r="L37" s="3" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(O37))</f>
+        <v>0x11800</v>
+      </c>
+      <c r="M37" s="3">
+        <f>HEX2DEC(MID(J37, 3, LEN(J37)-2))</f>
+        <v>69632</v>
+      </c>
+      <c r="N37" s="3">
+        <f>HEX2DEC(MID(K37, 3, LEN(K37)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="O37" s="3">
+        <f>M37+N37</f>
+        <v>71680</v>
+      </c>
+      <c r="P37" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E38" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F38" s="19">
         <f>F35*F36*F37/8</f>
@@ -2305,7 +2382,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E39" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F39">
         <v>256</v>
@@ -2337,7 +2414,7 @@
         <v>640</v>
       </c>
       <c r="C43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H43" s="7"/>
     </row>
@@ -2346,31 +2423,31 @@
         <v>791</v>
       </c>
       <c r="C44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H44" s="7"/>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D45" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="H45" s="7"/>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E46" s="9" t="s">
         <v>95</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E46" s="9" t="s">
-        <v>96</v>
       </c>
       <c r="F46" s="9">
         <v>1</v>
@@ -2382,10 +2459,10 @@
         <v>0</v>
       </c>
       <c r="D47" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E47" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F47" s="19">
         <v>1</v>
@@ -2394,10 +2471,10 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="D48" s="19" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E48" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F48" s="19">
         <v>1</v>
@@ -2406,17 +2483,17 @@
     </row>
     <row r="49" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H49" s="7"/>
     </row>
     <row r="50" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D50" s="9"/>
       <c r="E50" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F50" s="9">
         <v>1</v>
@@ -2425,10 +2502,10 @@
     </row>
     <row r="51" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D51" s="19" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E51" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F51" s="21">
         <v>1</v>
@@ -2437,10 +2514,10 @@
     </row>
     <row r="52" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D52" s="9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F52" s="9">
         <v>1</v>
@@ -2449,10 +2526,10 @@
     </row>
     <row r="53" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D53" s="8" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E53" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F53" s="8">
         <v>1</v>
@@ -2471,7 +2548,7 @@
     <row r="56" spans="4:8" x14ac:dyDescent="0.25">
       <c r="D56" s="9"/>
       <c r="E56" s="9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F56" s="9">
         <v>1</v>
@@ -2482,14 +2559,17 @@
       <c r="H57" s="7"/>
     </row>
     <row r="58" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="H58" s="20"/>
+      <c r="H58" s="7"/>
+    </row>
+    <row r="59" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H59" s="7"/>
+    </row>
+    <row r="60" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H60" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="I4:I23"/>
-    <mergeCell ref="I24:I27"/>
-    <mergeCell ref="I33:I34"/>
+  <mergeCells count="1">
+    <mergeCell ref="I35:I36"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Add more starfield layers
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DBB97C-A0C3-475B-98F8-C063525E7804}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD6A1C2-0C60-4EAE-8DDA-7462C749090B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="126">
   <si>
     <t>Per sprite</t>
   </si>
@@ -405,13 +405,19 @@
     <t>0x00EF</t>
   </si>
   <si>
-    <t>Starfield</t>
-  </si>
-  <si>
     <t>0x0010</t>
   </si>
   <si>
-    <t>0x05F0</t>
+    <t>Starfield 2</t>
+  </si>
+  <si>
+    <t>Starfield 3</t>
+  </si>
+  <si>
+    <t>Starfield 1</t>
+  </si>
+  <si>
+    <t>0x05E8</t>
   </si>
 </sst>
 </file>
@@ -629,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -685,12 +691,6 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -707,6 +707,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1023,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
-  <dimension ref="A1:P60"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="F10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1165,11 +1174,11 @@
         <v>16</v>
       </c>
       <c r="H4" s="12"/>
-      <c r="I4" s="29" t="s">
+      <c r="I4" s="27" t="s">
         <v>49</v>
       </c>
       <c r="J4" s="3" t="str">
-        <f t="shared" ref="J4:J37" si="1">L3</f>
+        <f t="shared" ref="J4:J39" si="1">L3</f>
         <v>0x8000</v>
       </c>
       <c r="K4" s="3" t="s">
@@ -1204,7 +1213,7 @@
         <v>256</v>
       </c>
       <c r="H5" s="12"/>
-      <c r="I5" s="30"/>
+      <c r="I5" s="28"/>
       <c r="J5" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8001</v>
@@ -1241,7 +1250,7 @@
         <v>32</v>
       </c>
       <c r="H6" s="12"/>
-      <c r="I6" s="30"/>
+      <c r="I6" s="28"/>
       <c r="J6" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8100</v>
@@ -1282,7 +1291,7 @@
         <v>32</v>
       </c>
       <c r="H7" s="12"/>
-      <c r="I7" s="30"/>
+      <c r="I7" s="28"/>
       <c r="J7" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x81C0</v>
@@ -1312,7 +1321,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H8" s="12"/>
-      <c r="I8" s="30"/>
+      <c r="I8" s="28"/>
       <c r="J8" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8200</v>
@@ -1345,7 +1354,7 @@
         <v>68</v>
       </c>
       <c r="H9" s="12"/>
-      <c r="I9" s="30"/>
+      <c r="I9" s="28"/>
       <c r="J9" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8260</v>
@@ -1381,7 +1390,7 @@
         <v>16</v>
       </c>
       <c r="H10" s="12"/>
-      <c r="I10" s="30"/>
+      <c r="I10" s="28"/>
       <c r="J10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8300</v>
@@ -1417,7 +1426,7 @@
         <v>16</v>
       </c>
       <c r="H11" s="12"/>
-      <c r="I11" s="30"/>
+      <c r="I11" s="28"/>
       <c r="J11" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8360</v>
@@ -1453,7 +1462,7 @@
         <v>16</v>
       </c>
       <c r="H12" s="12"/>
-      <c r="I12" s="30"/>
+      <c r="I12" s="28"/>
       <c r="J12" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8400</v>
@@ -1492,7 +1501,7 @@
         <v>67</v>
       </c>
       <c r="H13" s="12"/>
-      <c r="I13" s="30"/>
+      <c r="I13" s="28"/>
       <c r="J13" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8430</v>
@@ -1529,7 +1538,7 @@
         <v>1024</v>
       </c>
       <c r="H14" s="12"/>
-      <c r="I14" s="30"/>
+      <c r="I14" s="28"/>
       <c r="J14" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8500</v>
@@ -1566,7 +1575,7 @@
         <v>128</v>
       </c>
       <c r="H15" s="12"/>
-      <c r="I15" s="30"/>
+      <c r="I15" s="28"/>
       <c r="J15" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8560</v>
@@ -1603,7 +1612,7 @@
         <v>2048</v>
       </c>
       <c r="H16" s="12"/>
-      <c r="I16" s="30"/>
+      <c r="I16" s="28"/>
       <c r="J16" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8600</v>
@@ -1633,7 +1642,7 @@
     </row>
     <row r="17" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H17" s="12"/>
-      <c r="I17" s="30"/>
+      <c r="I17" s="28"/>
       <c r="J17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x860C</v>
@@ -1666,7 +1675,7 @@
         <v>69</v>
       </c>
       <c r="H18" s="12"/>
-      <c r="I18" s="30"/>
+      <c r="I18" s="28"/>
       <c r="J18" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8700</v>
@@ -1702,7 +1711,7 @@
         <v>32</v>
       </c>
       <c r="H19" s="12"/>
-      <c r="I19" s="30"/>
+      <c r="I19" s="28"/>
       <c r="J19" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8730</v>
@@ -1738,7 +1747,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="12"/>
-      <c r="I20" s="30"/>
+      <c r="I20" s="28"/>
       <c r="J20" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8800</v>
@@ -1751,7 +1760,7 @@
         <v>0x8821</v>
       </c>
       <c r="M20" s="3">
-        <f t="shared" ref="M20:N23" si="25">HEX2DEC(MID(J20, 3, LEN(J20)-2))</f>
+        <f t="shared" ref="M20:N25" si="25">HEX2DEC(MID(J20, 3, LEN(J20)-2))</f>
         <v>34816</v>
       </c>
       <c r="N20" s="3">
@@ -1774,7 +1783,7 @@
         <v>15</v>
       </c>
       <c r="H21" s="12"/>
-      <c r="I21" s="30"/>
+      <c r="I21" s="28"/>
       <c r="J21" s="4" t="str">
         <f t="shared" si="1"/>
         <v>0x8821</v>
@@ -1810,7 +1819,7 @@
         <v>4</v>
       </c>
       <c r="H22" s="12"/>
-      <c r="I22" s="30"/>
+      <c r="I22" s="28"/>
       <c r="J22" s="3" t="str">
         <f t="shared" si="1"/>
         <v>0x8900</v>
@@ -1846,7 +1855,7 @@
         <v>12</v>
       </c>
       <c r="H23" s="12"/>
-      <c r="I23" s="30"/>
+      <c r="I23" s="28"/>
       <c r="J23" s="4" t="str">
         <f>L22</f>
         <v>0x8911</v>
@@ -1877,31 +1886,30 @@
     <row r="24" spans="5:16" x14ac:dyDescent="0.25">
       <c r="E24" s="10"/>
       <c r="H24" s="12"/>
-      <c r="I24" s="30"/>
+      <c r="I24" s="28"/>
       <c r="J24" s="3" t="s">
         <v>119</v>
       </c>
       <c r="K24" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="L24" s="3" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(O24))</f>
-        <v>0x8A10</v>
+        <v>0x8A08</v>
       </c>
       <c r="M24" s="3">
-        <f t="shared" ref="M24" si="29">HEX2DEC(MID(J24, 3, LEN(J24)-2))</f>
+        <f t="shared" si="25"/>
         <v>35328</v>
       </c>
       <c r="N24" s="3">
-        <f t="shared" ref="N24" si="30">HEX2DEC(MID(K24, 3, LEN(K24)-2))</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="O24" s="3">
         <f>M24+N24</f>
-        <v>35344</v>
+        <v>35336</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
     </row>
     <row r="25" spans="5:16" x14ac:dyDescent="0.25">
@@ -1913,32 +1921,31 @@
         <v>32</v>
       </c>
       <c r="H25" s="12"/>
-      <c r="I25" s="31"/>
-      <c r="J25" s="4" t="str">
+      <c r="I25" s="35"/>
+      <c r="J25" s="3" t="str">
         <f>L24</f>
+        <v>0x8A08</v>
+      </c>
+      <c r="K25" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="L25" s="3" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(O25))</f>
         <v>0x8A10</v>
       </c>
-      <c r="K25" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="L25" s="4" t="str">
-        <f t="shared" ref="L25" si="31">_xlfn.CONCAT("0x",DEC2HEX(O25))</f>
-        <v>0x9000</v>
-      </c>
-      <c r="M25" s="4">
-        <f t="shared" ref="M25" si="32">HEX2DEC(MID(J25, 3, LEN(J25)-2))</f>
+      <c r="M25" s="3">
+        <f t="shared" ref="M25:M26" si="29">HEX2DEC(MID(J25, 3, LEN(J25)-2))</f>
+        <v>35336</v>
+      </c>
+      <c r="N25" s="3">
+        <v>8</v>
+      </c>
+      <c r="O25" s="3">
+        <f>M25+N25</f>
         <v>35344</v>
       </c>
-      <c r="N25" s="4">
-        <f t="shared" ref="N25" si="33">HEX2DEC(MID(K25, 3, LEN(K25)-2))</f>
-        <v>1520</v>
-      </c>
-      <c r="O25" s="4">
-        <f t="shared" ref="O25" si="34">M25+N25</f>
-        <v>36864</v>
-      </c>
-      <c r="P25" s="4" t="s">
-        <v>35</v>
+      <c r="P25" s="3" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="5:16" x14ac:dyDescent="0.25">
@@ -1954,34 +1961,31 @@
         <v>128</v>
       </c>
       <c r="H26" s="12"/>
-      <c r="I26" s="32" t="s">
-        <v>53</v>
-      </c>
+      <c r="I26" s="35"/>
       <c r="J26" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x9000</v>
+        <f>L25</f>
+        <v>0x8A10</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>13</v>
+        <v>121</v>
       </c>
       <c r="L26" s="3" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(O26))</f>
-        <v>0x9800</v>
+        <v>0x8A18</v>
       </c>
       <c r="M26" s="3">
-        <f>HEX2DEC(MID(J26, 3, LEN(J26)-2))</f>
-        <v>36864</v>
+        <f t="shared" si="29"/>
+        <v>35344</v>
       </c>
       <c r="N26" s="3">
-        <f>HEX2DEC(MID(K26, 3, LEN(K26)-2))</f>
-        <v>2048</v>
+        <v>8</v>
       </c>
       <c r="O26" s="3">
         <f>M26+N26</f>
-        <v>38912</v>
+        <v>35352</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>14</v>
+        <v>123</v>
       </c>
     </row>
     <row r="27" spans="5:16" x14ac:dyDescent="0.25">
@@ -1993,62 +1997,64 @@
         <v>128</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x9800</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="L27" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(O27))</f>
-        <v>0xA000</v>
-      </c>
-      <c r="M27" s="3">
-        <f>HEX2DEC(MID(J27, 3, LEN(J27)-2))</f>
-        <v>38912</v>
-      </c>
-      <c r="N27" s="3">
-        <f>HEX2DEC(MID(K27, 3, LEN(K27)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="O27" s="3">
-        <f>M27+N27</f>
-        <v>40960</v>
-      </c>
-      <c r="P27" s="3" t="s">
-        <v>51</v>
+      <c r="I27" s="29"/>
+      <c r="J27" s="4" t="str">
+        <f>L26</f>
+        <v>0x8A18</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="L27" s="4" t="str">
+        <f t="shared" ref="L27" si="30">_xlfn.CONCAT("0x",DEC2HEX(O27))</f>
+        <v>0x9000</v>
+      </c>
+      <c r="M27" s="4">
+        <f t="shared" ref="M27" si="31">HEX2DEC(MID(J27, 3, LEN(J27)-2))</f>
+        <v>35352</v>
+      </c>
+      <c r="N27" s="4">
+        <f t="shared" ref="N27" si="32">HEX2DEC(MID(K27, 3, LEN(K27)-2))</f>
+        <v>1512</v>
+      </c>
+      <c r="O27" s="4">
+        <f t="shared" ref="O27" si="33">M27+N27</f>
+        <v>36864</v>
+      </c>
+      <c r="P27" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="5:16" x14ac:dyDescent="0.25">
       <c r="H28" s="12"/>
-      <c r="I28" s="33"/>
+      <c r="I28" s="30" t="s">
+        <v>53</v>
+      </c>
       <c r="J28" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0xA000</v>
+        <v>0x9000</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L28" s="3" t="str">
-        <f t="shared" ref="L28" si="35">_xlfn.CONCAT("0x",DEC2HEX(O28))</f>
-        <v>0xA800</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(O28))</f>
+        <v>0x9800</v>
       </c>
       <c r="M28" s="3">
-        <f t="shared" ref="M28" si="36">HEX2DEC(MID(J28, 3, LEN(J28)-2))</f>
-        <v>40960</v>
+        <f>HEX2DEC(MID(J28, 3, LEN(J28)-2))</f>
+        <v>36864</v>
       </c>
       <c r="N28" s="3">
-        <f t="shared" ref="N28" si="37">HEX2DEC(MID(K28, 3, LEN(K28)-2))</f>
+        <f>HEX2DEC(MID(K28, 3, LEN(K28)-2))</f>
         <v>2048</v>
       </c>
       <c r="O28" s="3">
-        <f t="shared" ref="O28" si="38">M28+N28</f>
-        <v>43008</v>
+        <f>M28+N28</f>
+        <v>38912</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="5:16" x14ac:dyDescent="0.25">
@@ -2056,32 +2062,32 @@
         <v>70</v>
       </c>
       <c r="H29" s="12"/>
-      <c r="I29" s="34"/>
+      <c r="I29" s="31"/>
       <c r="J29" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0xA800</v>
+        <v>0x9800</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>13</v>
       </c>
       <c r="L29" s="3" t="str">
-        <f t="shared" ref="L29" si="39">_xlfn.CONCAT("0x",DEC2HEX(O29))</f>
-        <v>0xB000</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(O29))</f>
+        <v>0xA000</v>
       </c>
       <c r="M29" s="3">
-        <f t="shared" ref="M29" si="40">HEX2DEC(MID(J29, 3, LEN(J29)-2))</f>
-        <v>43008</v>
+        <f>HEX2DEC(MID(J29, 3, LEN(J29)-2))</f>
+        <v>38912</v>
       </c>
       <c r="N29" s="3">
-        <f t="shared" ref="N29" si="41">HEX2DEC(MID(K29, 3, LEN(K29)-2))</f>
+        <f>HEX2DEC(MID(K29, 3, LEN(K29)-2))</f>
         <v>2048</v>
       </c>
       <c r="O29" s="3">
-        <f t="shared" ref="O29" si="42">M29+N29</f>
-        <v>45056</v>
+        <f>M29+N29</f>
+        <v>40960</v>
       </c>
       <c r="P29" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="5:16" x14ac:dyDescent="0.25">
@@ -2096,35 +2102,32 @@
         <v>352</v>
       </c>
       <c r="H30" s="12"/>
-      <c r="I30" s="24" t="s">
-        <v>64</v>
-      </c>
+      <c r="I30" s="31"/>
       <c r="J30" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0xB000</v>
-      </c>
-      <c r="K30" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(F27))</f>
-        <v>0x80</v>
+        <v>0xA000</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="L30" s="3" t="str">
-        <f t="shared" ref="L30:L32" si="43">_xlfn.CONCAT("0x",DEC2HEX(O30))</f>
-        <v>0xB080</v>
+        <f t="shared" ref="L30" si="34">_xlfn.CONCAT("0x",DEC2HEX(O30))</f>
+        <v>0xA800</v>
       </c>
       <c r="M30" s="3">
-        <f t="shared" ref="M30:M32" si="44">HEX2DEC(MID(J30, 3, LEN(J30)-2))</f>
-        <v>45056</v>
+        <f t="shared" ref="M30" si="35">HEX2DEC(MID(J30, 3, LEN(J30)-2))</f>
+        <v>40960</v>
       </c>
       <c r="N30" s="3">
-        <f t="shared" ref="N30:N32" si="45">HEX2DEC(MID(K30, 3, LEN(K30)-2))</f>
-        <v>128</v>
+        <f t="shared" ref="N30" si="36">HEX2DEC(MID(K30, 3, LEN(K30)-2))</f>
+        <v>2048</v>
       </c>
       <c r="O30" s="3">
-        <f t="shared" ref="O30:O32" si="46">M30+N30</f>
-        <v>45184</v>
+        <f t="shared" ref="O30" si="37">M30+N30</f>
+        <v>43008</v>
       </c>
       <c r="P30" s="3" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="31" spans="5:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2139,32 +2142,32 @@
         <v>272</v>
       </c>
       <c r="H31" s="12"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="4" t="str">
+      <c r="I31" s="32"/>
+      <c r="J31" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0xB080</v>
-      </c>
-      <c r="K31" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="L31" s="4" t="str">
-        <f t="shared" si="43"/>
-        <v>0xB800</v>
-      </c>
-      <c r="M31" s="4">
-        <f t="shared" si="44"/>
-        <v>45184</v>
-      </c>
-      <c r="N31" s="4">
-        <f t="shared" si="45"/>
-        <v>1920</v>
-      </c>
-      <c r="O31" s="4">
-        <f t="shared" si="46"/>
-        <v>47104</v>
-      </c>
-      <c r="P31" s="4" t="s">
-        <v>35</v>
+        <v>0xA800</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L31" s="3" t="str">
+        <f t="shared" ref="L31" si="38">_xlfn.CONCAT("0x",DEC2HEX(O31))</f>
+        <v>0xB000</v>
+      </c>
+      <c r="M31" s="3">
+        <f t="shared" ref="M31" si="39">HEX2DEC(MID(J31, 3, LEN(J31)-2))</f>
+        <v>43008</v>
+      </c>
+      <c r="N31" s="3">
+        <f t="shared" ref="N31" si="40">HEX2DEC(MID(K31, 3, LEN(K31)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="O31" s="3">
+        <f t="shared" ref="O31" si="41">M31+N31</f>
+        <v>45056</v>
+      </c>
+      <c r="P31" s="3" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="32" spans="5:16" x14ac:dyDescent="0.25">
@@ -2175,121 +2178,117 @@
         <v>240</v>
       </c>
       <c r="H32" s="12"/>
-      <c r="I32" s="25"/>
+      <c r="I32" s="24" t="s">
+        <v>64</v>
+      </c>
       <c r="J32" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0xB800</v>
+        <v>0xB000</v>
       </c>
       <c r="K32" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(F38))</f>
-        <v>0x800</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(F27))</f>
+        <v>0x80</v>
       </c>
       <c r="L32" s="3" t="str">
-        <f t="shared" si="43"/>
-        <v>0xC000</v>
+        <f t="shared" ref="L32:L34" si="42">_xlfn.CONCAT("0x",DEC2HEX(O32))</f>
+        <v>0xB080</v>
       </c>
       <c r="M32" s="3">
-        <f t="shared" si="44"/>
-        <v>47104</v>
+        <f t="shared" ref="M32:M34" si="43">HEX2DEC(MID(J32, 3, LEN(J32)-2))</f>
+        <v>45056</v>
       </c>
       <c r="N32" s="3">
-        <f t="shared" si="45"/>
-        <v>2048</v>
+        <f t="shared" ref="N32:N34" si="44">HEX2DEC(MID(K32, 3, LEN(K32)-2))</f>
+        <v>128</v>
       </c>
       <c r="O32" s="3">
-        <f t="shared" si="46"/>
-        <v>49152</v>
+        <f t="shared" ref="O32:O34" si="45">M32+N32</f>
+        <v>45184</v>
       </c>
       <c r="P32" s="3" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H33" s="12"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4"/>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4"/>
+      <c r="I33" s="25"/>
+      <c r="J33" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB080</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="L33" s="4" t="str">
+        <f t="shared" si="42"/>
+        <v>0xB800</v>
+      </c>
+      <c r="M33" s="4">
+        <f t="shared" si="43"/>
+        <v>45184</v>
+      </c>
+      <c r="N33" s="4">
+        <f t="shared" si="44"/>
+        <v>1920</v>
+      </c>
+      <c r="O33" s="4">
+        <f t="shared" si="45"/>
+        <v>47104</v>
+      </c>
+      <c r="P33" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E34" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H34" s="13"/>
-      <c r="I34" s="15" t="s">
-        <v>54</v>
-      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="25"/>
       <c r="J34" s="3" t="str">
-        <f>L32</f>
+        <f t="shared" si="1"/>
+        <v>0xB800</v>
+      </c>
+      <c r="K34" s="3" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(F38))</f>
+        <v>0x800</v>
+      </c>
+      <c r="L34" s="3" t="str">
+        <f t="shared" si="42"/>
         <v>0xC000</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="L34" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(O34))</f>
-        <v>0x10000</v>
-      </c>
       <c r="M34" s="3">
-        <f>HEX2DEC(MID(J34, 3, LEN(J34)-2))</f>
+        <f t="shared" si="43"/>
+        <v>47104</v>
+      </c>
+      <c r="N34" s="3">
+        <f t="shared" si="44"/>
+        <v>2048</v>
+      </c>
+      <c r="O34" s="3">
+        <f t="shared" si="45"/>
         <v>49152</v>
       </c>
-      <c r="N34" s="3">
-        <f>HEX2DEC(MID(K34, 3, LEN(K34)-2))</f>
-        <v>16384</v>
-      </c>
-      <c r="O34" s="3">
-        <f>M34+N34</f>
-        <v>65536</v>
-      </c>
       <c r="P34" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>114</v>
       </c>
       <c r="F35">
         <v>2</v>
       </c>
-      <c r="H35" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="I35" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="J35" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>0x10000</v>
-      </c>
-      <c r="K35" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(F6))</f>
-        <v>0x20</v>
-      </c>
-      <c r="L35" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(O35))</f>
-        <v>0x10020</v>
-      </c>
-      <c r="M35" s="3">
-        <f>HEX2DEC(MID(J35, 3, LEN(J35)-2))</f>
-        <v>65536</v>
-      </c>
-      <c r="N35" s="3">
-        <f>HEX2DEC(MID(K35, 3, LEN(K35)-2))</f>
-        <v>32</v>
-      </c>
-      <c r="O35" s="3">
-        <f>M35+N35</f>
-        <v>65568</v>
-      </c>
-      <c r="P35" s="3" t="s">
-        <v>62</v>
-      </c>
+      <c r="H35" s="12"/>
+      <c r="I35" s="26"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="O35" s="4"/>
+      <c r="P35" s="4"/>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
@@ -2298,36 +2297,38 @@
       <c r="F36">
         <v>512</v>
       </c>
-      <c r="H36" s="7"/>
-      <c r="I36" s="28"/>
-      <c r="J36" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>0x10020</v>
-      </c>
-      <c r="K36" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="L36" s="4" t="str">
-        <f t="shared" ref="L36" si="47">_xlfn.CONCAT("0x",DEC2HEX(O36))</f>
-        <v>0x11000</v>
-      </c>
-      <c r="M36" s="4">
-        <f t="shared" ref="M36" si="48">HEX2DEC(MID(J36, 3, LEN(J36)-2))</f>
-        <v>65568</v>
-      </c>
-      <c r="N36" s="4">
-        <f t="shared" ref="N36" si="49">HEX2DEC(MID(K36, 3, LEN(K36)-2))</f>
-        <v>4064</v>
-      </c>
-      <c r="O36" s="4">
-        <f t="shared" ref="O36" si="50">M36+N36</f>
-        <v>69632</v>
-      </c>
-      <c r="P36" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H36" s="13"/>
+      <c r="I36" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J36" s="3" t="str">
+        <f>L34</f>
+        <v>0xC000</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" s="3" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(O36))</f>
+        <v>0x10000</v>
+      </c>
+      <c r="M36" s="3">
+        <f>HEX2DEC(MID(J36, 3, LEN(J36)-2))</f>
+        <v>49152</v>
+      </c>
+      <c r="N36" s="3">
+        <f>HEX2DEC(MID(K36, 3, LEN(K36)-2))</f>
+        <v>16384</v>
+      </c>
+      <c r="O36" s="3">
+        <f>M36+N36</f>
+        <v>65536</v>
+      </c>
+      <c r="P36" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="E37" t="s">
         <v>88</v>
       </c>
@@ -2338,36 +2339,38 @@
         <f>F37/8</f>
         <v>2</v>
       </c>
-      <c r="H37" s="7"/>
-      <c r="I37" s="16" t="s">
-        <v>64</v>
+      <c r="H37" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="I37" s="33" t="s">
+        <v>63</v>
       </c>
       <c r="J37" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>0x11000</v>
+        <v>0x10000</v>
       </c>
       <c r="K37" s="3" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(F16))</f>
-        <v>0x800</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(F6))</f>
+        <v>0x20</v>
       </c>
       <c r="L37" s="3" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(O37))</f>
-        <v>0x11800</v>
+        <v>0x10020</v>
       </c>
       <c r="M37" s="3">
         <f>HEX2DEC(MID(J37, 3, LEN(J37)-2))</f>
-        <v>69632</v>
+        <v>65536</v>
       </c>
       <c r="N37" s="3">
         <f>HEX2DEC(MID(K37, 3, LEN(K37)-2))</f>
-        <v>2048</v>
+        <v>32</v>
       </c>
       <c r="O37" s="3">
         <f>M37+N37</f>
-        <v>71680</v>
+        <v>65568</v>
       </c>
       <c r="P37" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
@@ -2379,6 +2382,33 @@
         <v>2048</v>
       </c>
       <c r="H38" s="7"/>
+      <c r="I38" s="34"/>
+      <c r="J38" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>0x10020</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="L38" s="4" t="str">
+        <f t="shared" ref="L38" si="46">_xlfn.CONCAT("0x",DEC2HEX(O38))</f>
+        <v>0x11000</v>
+      </c>
+      <c r="M38" s="4">
+        <f t="shared" ref="M38" si="47">HEX2DEC(MID(J38, 3, LEN(J38)-2))</f>
+        <v>65568</v>
+      </c>
+      <c r="N38" s="4">
+        <f t="shared" ref="N38" si="48">HEX2DEC(MID(K38, 3, LEN(K38)-2))</f>
+        <v>4064</v>
+      </c>
+      <c r="O38" s="4">
+        <f t="shared" ref="O38" si="49">M38+N38</f>
+        <v>69632</v>
+      </c>
+      <c r="P38" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E39" s="8" t="s">
@@ -2388,6 +2418,36 @@
         <v>256</v>
       </c>
       <c r="H39" s="7"/>
+      <c r="I39" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="J39" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>0x11000</v>
+      </c>
+      <c r="K39" s="3" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(F16))</f>
+        <v>0x800</v>
+      </c>
+      <c r="L39" s="3" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(O39))</f>
+        <v>0x11800</v>
+      </c>
+      <c r="M39" s="3">
+        <f>HEX2DEC(MID(J39, 3, LEN(J39)-2))</f>
+        <v>69632</v>
+      </c>
+      <c r="N39" s="3">
+        <f>HEX2DEC(MID(K39, 3, LEN(K39)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="O39" s="3">
+        <f>M39+N39</f>
+        <v>71680</v>
+      </c>
+      <c r="P39" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="H40" s="7"/>
@@ -2565,11 +2625,18 @@
       <c r="H59" s="7"/>
     </row>
     <row r="60" spans="4:8" x14ac:dyDescent="0.25">
-      <c r="H60" s="20"/>
+      <c r="H60" s="7"/>
+    </row>
+    <row r="61" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H61" s="7"/>
+    </row>
+    <row r="62" spans="4:8" x14ac:dyDescent="0.25">
+      <c r="H62" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="I35:I36"/>
+  <mergeCells count="2">
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="I25:I26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Audio fixes, refactoring etc
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC0827D-2A91-4E74-9E9E-749A06C9F454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D03C7CB-F510-41D6-AE13-24BC896F5B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="163">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -311,15 +311,6 @@
   </si>
   <si>
     <t>Starfield 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ???(Sound)</t>
-  </si>
-  <si>
-    <t>Sound RAM</t>
-  </si>
-  <si>
-    <t>0x05D0</t>
   </si>
   <si>
     <t>Sprite Collision RAM</t>
@@ -581,6 +572,21 @@
   </si>
   <si>
     <t>0x600</t>
+  </si>
+  <si>
+    <t>Deikun (Sound system)</t>
+  </si>
+  <si>
+    <t>Sound RAM (YM2419)</t>
+  </si>
+  <si>
+    <t>0x04E0</t>
+  </si>
+  <si>
+    <t>Music RAM (YM Player)</t>
+  </si>
+  <si>
+    <t>0x10000</t>
   </si>
 </sst>
 </file>
@@ -816,7 +822,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -917,20 +923,23 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1246,10 +1255,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
-  <dimension ref="B1:P63"/>
+  <dimension ref="B1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1310,7 +1319,7 @@
     </row>
     <row r="3" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>7</v>
@@ -1353,13 +1362,13 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>44</v>
       </c>
       <c r="D4" s="24" t="str">
-        <f t="shared" ref="D4:D42" si="1">F3</f>
+        <f t="shared" ref="D4:D43" si="1">F3</f>
         <v>0x8000</v>
       </c>
       <c r="E4" s="24" t="s">
@@ -1709,7 +1718,7 @@
         <v>30</v>
       </c>
       <c r="L13" s="30" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="M13" s="30">
         <f>M12</f>
@@ -1779,7 +1788,7 @@
         <v>59</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
@@ -1941,7 +1950,7 @@
         <v>0x8821</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" ref="G20:H30" si="25">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
+        <f t="shared" ref="G20:H31" si="25">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
         <v>34816</v>
       </c>
       <c r="H20" s="24">
@@ -2030,7 +2039,7 @@
         <v>20</v>
       </c>
       <c r="L22" s="30" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="M22" s="30">
         <f>M16*M21</f>
@@ -2101,7 +2110,7 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="25"/>
-      <c r="C25" s="31"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="24" t="str">
         <f>F24</f>
         <v>0x8A10</v>
@@ -2137,7 +2146,7 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="25"/>
-      <c r="C26" s="31"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="24" t="str">
         <f>F25</f>
         <v>0x8A20</v>
@@ -2210,7 +2219,7 @@
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="25"/>
       <c r="C28" s="26" t="s">
-        <v>91</v>
+        <v>158</v>
       </c>
       <c r="D28" s="24" t="str">
         <f>F27</f>
@@ -2236,7 +2245,7 @@
         <v>35600</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>92</v>
+        <v>159</v>
       </c>
       <c r="L28" s="32" t="s">
         <v>81</v>
@@ -2247,32 +2256,32 @@
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="25"/>
-      <c r="C29" s="33"/>
-      <c r="D29" s="28" t="str">
-        <f>F26</f>
-        <v>0x8A30</v>
-      </c>
-      <c r="E29" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="F29" s="28" t="str">
-        <f t="shared" ref="F29" si="34">_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
-        <v>0x9000</v>
-      </c>
-      <c r="G29" s="28">
-        <f t="shared" ref="G29" si="35">HEX2DEC(MID(D29, 3, LEN(D29)-2))</f>
-        <v>35376</v>
-      </c>
-      <c r="H29" s="28">
-        <f t="shared" ref="H29" si="36">HEX2DEC(MID(E29, 3, LEN(E29)-2))</f>
-        <v>1488</v>
-      </c>
-      <c r="I29" s="28">
-        <f t="shared" ref="I29" si="37">G29+H29</f>
-        <v>36864</v>
-      </c>
-      <c r="J29" s="28" t="s">
-        <v>30</v>
+      <c r="C29" s="31"/>
+      <c r="D29" s="24" t="str">
+        <f>F28</f>
+        <v>0x8B10</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="F29" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
+        <v>0x8B20</v>
+      </c>
+      <c r="G29" s="24">
+        <f t="shared" ref="G29" si="34">HEX2DEC(MID(D29, 3, LEN(D29)-2))</f>
+        <v>35600</v>
+      </c>
+      <c r="H29" s="24">
+        <f t="shared" ref="H29" si="35">HEX2DEC(MID(E29, 3, LEN(E29)-2))</f>
+        <v>16</v>
+      </c>
+      <c r="I29" s="24">
+        <f>G29+H29</f>
+        <v>35616</v>
+      </c>
+      <c r="J29" s="24" t="s">
+        <v>161</v>
       </c>
       <c r="L29" s="32" t="s">
         <v>71</v>
@@ -2283,34 +2292,32 @@
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="25"/>
-      <c r="C30" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="24" t="str">
-        <f t="shared" si="1"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="28" t="str">
+        <f>F29</f>
+        <v>0x8B20</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="F30" s="28" t="str">
+        <f t="shared" ref="F30" si="36">_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
         <v>0x9000</v>
       </c>
-      <c r="E30" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
-        <v>0x9800</v>
-      </c>
-      <c r="G30" s="24">
-        <f>HEX2DEC(MID(D30, 3, LEN(D30)-2))</f>
+      <c r="G30" s="28">
+        <f t="shared" ref="G30" si="37">HEX2DEC(MID(D30, 3, LEN(D30)-2))</f>
+        <v>35616</v>
+      </c>
+      <c r="H30" s="28">
+        <f t="shared" ref="H30" si="38">HEX2DEC(MID(E30, 3, LEN(E30)-2))</f>
+        <v>1248</v>
+      </c>
+      <c r="I30" s="28">
+        <f t="shared" ref="I30" si="39">G30+H30</f>
         <v>36864</v>
       </c>
-      <c r="H30" s="24">
-        <f t="shared" si="25"/>
-        <v>2048</v>
-      </c>
-      <c r="I30" s="24">
-        <f>G30+H30</f>
-        <v>38912</v>
-      </c>
-      <c r="J30" s="24" t="s">
-        <v>9</v>
+      <c r="J30" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L30" s="30" t="s">
         <v>4</v>
@@ -2323,32 +2330,34 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" s="25"/>
-      <c r="C31" s="36"/>
+      <c r="C31" s="34" t="s">
+        <v>48</v>
+      </c>
       <c r="D31" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0x9800</v>
+        <v>0x9000</v>
       </c>
       <c r="E31" s="24" t="s">
         <v>8</v>
       </c>
       <c r="F31" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I31))</f>
-        <v>0xA000</v>
+        <v>0x9800</v>
       </c>
       <c r="G31" s="24">
         <f>HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
-        <v>38912</v>
+        <v>36864</v>
       </c>
       <c r="H31" s="24">
-        <f>HEX2DEC(MID(E31, 3, LEN(E31)-2))</f>
+        <f t="shared" si="25"/>
         <v>2048</v>
       </c>
       <c r="I31" s="24">
         <f>G31+H31</f>
-        <v>40960</v>
+        <v>38912</v>
       </c>
       <c r="J31" s="24" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="L31" s="19" t="s">
         <v>3</v>
@@ -2363,32 +2372,32 @@
       <c r="C32" s="36"/>
       <c r="D32" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0xA000</v>
+        <v>0x9800</v>
       </c>
       <c r="E32" s="24" t="s">
         <v>8</v>
       </c>
       <c r="F32" s="24" t="str">
-        <f t="shared" ref="F32" si="38">_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
-        <v>0xA800</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
+        <v>0xA000</v>
       </c>
       <c r="G32" s="24">
-        <f t="shared" ref="G32" si="39">HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
+        <f>HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
+        <v>38912</v>
+      </c>
+      <c r="H32" s="24">
+        <f>HEX2DEC(MID(E32, 3, LEN(E32)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I32" s="24">
+        <f>G32+H32</f>
         <v>40960</v>
       </c>
-      <c r="H32" s="24">
-        <f t="shared" ref="H32" si="40">HEX2DEC(MID(E32, 3, LEN(E32)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I32" s="24">
-        <f t="shared" ref="I32" si="41">G32+H32</f>
-        <v>43008</v>
-      </c>
       <c r="J32" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L32" s="30" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="M32" s="30">
         <f>M25*M31</f>
@@ -2397,101 +2406,101 @@
     </row>
     <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="25"/>
-      <c r="C33" s="37"/>
+      <c r="C33" s="36"/>
       <c r="D33" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0xA800</v>
+        <v>0xA000</v>
       </c>
       <c r="E33" s="24" t="s">
         <v>8</v>
       </c>
       <c r="F33" s="24" t="str">
-        <f t="shared" ref="F33" si="42">_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
-        <v>0xB000</v>
+        <f t="shared" ref="F33" si="40">_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
+        <v>0xA800</v>
       </c>
       <c r="G33" s="24">
-        <f t="shared" ref="G33" si="43">HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
+        <f t="shared" ref="G33" si="41">HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
+        <v>40960</v>
+      </c>
+      <c r="H33" s="24">
+        <f t="shared" ref="H33" si="42">HEX2DEC(MID(E33, 3, LEN(E33)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I33" s="24">
+        <f t="shared" ref="I33" si="43">G33+H33</f>
         <v>43008</v>
       </c>
-      <c r="H33" s="24">
-        <f t="shared" ref="H33" si="44">HEX2DEC(MID(E33, 3, LEN(E33)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I33" s="24">
-        <f t="shared" ref="I33" si="45">G33+H33</f>
-        <v>45056</v>
-      </c>
       <c r="J33" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B34" s="25"/>
-      <c r="C34" s="38" t="s">
-        <v>56</v>
-      </c>
+      <c r="C34" s="37"/>
       <c r="D34" s="24" t="str">
         <f t="shared" si="1"/>
+        <v>0xA800</v>
+      </c>
+      <c r="E34" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="24" t="str">
+        <f t="shared" ref="F34" si="44">_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
         <v>0xB000</v>
       </c>
-      <c r="E34" s="24" t="str">
+      <c r="G34" s="24">
+        <f t="shared" ref="G34" si="45">HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
+        <v>43008</v>
+      </c>
+      <c r="H34" s="24">
+        <f t="shared" ref="H34" si="46">HEX2DEC(MID(E34, 3, LEN(E34)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I34" s="24">
+        <f t="shared" ref="I34" si="47">G34+H34</f>
+        <v>45056</v>
+      </c>
+      <c r="J34" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="L34" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="M34" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B35" s="25"/>
+      <c r="C35" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB000</v>
+      </c>
+      <c r="E35" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M32))</f>
         <v>0x80</v>
       </c>
-      <c r="F34" s="24" t="str">
-        <f t="shared" ref="F34:F35" si="46">_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
+      <c r="F35" s="24" t="str">
+        <f t="shared" ref="F35:F36" si="48">_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
         <v>0xB080</v>
       </c>
-      <c r="G34" s="24">
-        <f t="shared" ref="G34:G35" si="47">HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
+      <c r="G35" s="24">
+        <f t="shared" ref="G35:G36" si="49">HEX2DEC(MID(D35, 3, LEN(D35)-2))</f>
         <v>45056</v>
       </c>
-      <c r="H34" s="24">
-        <f t="shared" ref="H34:H35" si="48">HEX2DEC(MID(E34, 3, LEN(E34)-2))</f>
+      <c r="H35" s="24">
+        <f t="shared" ref="H35:H36" si="50">HEX2DEC(MID(E35, 3, LEN(E35)-2))</f>
         <v>128</v>
       </c>
-      <c r="I34" s="24">
-        <f t="shared" ref="I34:I35" si="49">G34+H34</f>
+      <c r="I35" s="24">
+        <f t="shared" ref="I35:I36" si="51">G35+H35</f>
         <v>45184</v>
       </c>
-      <c r="J34" s="24" t="s">
+      <c r="J35" s="24" t="s">
         <v>57</v>
-      </c>
-      <c r="L34" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="M34" s="19" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B35" s="25"/>
-      <c r="C35" s="39"/>
-      <c r="D35" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v>0xB080</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="F35" s="28" t="str">
-        <f t="shared" si="46"/>
-        <v>0xB400</v>
-      </c>
-      <c r="G35" s="28">
-        <f t="shared" si="47"/>
-        <v>45184</v>
-      </c>
-      <c r="H35" s="28">
-        <f t="shared" si="48"/>
-        <v>896</v>
-      </c>
-      <c r="I35" s="28">
-        <f t="shared" si="49"/>
-        <v>46080</v>
-      </c>
-      <c r="J35" s="28" t="s">
-        <v>30</v>
       </c>
       <c r="L35" s="19" t="s">
         <v>80</v>
@@ -2503,32 +2512,31 @@
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="25"/>
       <c r="C36" s="39"/>
-      <c r="D36" s="24" t="str">
-        <f t="shared" ref="D36:D37" si="50">F35</f>
+      <c r="D36" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB080</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="F36" s="28" t="str">
+        <f t="shared" si="48"/>
         <v>0xB400</v>
       </c>
-      <c r="E36" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M45))</f>
-        <v>0x4</v>
-      </c>
-      <c r="F36" s="24" t="str">
-        <f t="shared" ref="F36:F37" si="51">_xlfn.CONCAT("0x",DEC2HEX(I36))</f>
-        <v>0xB404</v>
-      </c>
-      <c r="G36" s="24">
-        <f t="shared" ref="G36:G37" si="52">HEX2DEC(MID(D36, 3, LEN(D36)-2))</f>
+      <c r="G36" s="28">
+        <f t="shared" si="49"/>
+        <v>45184</v>
+      </c>
+      <c r="H36" s="28">
+        <f t="shared" si="50"/>
+        <v>896</v>
+      </c>
+      <c r="I36" s="28">
+        <f t="shared" si="51"/>
         <v>46080</v>
       </c>
-      <c r="H36" s="24">
-        <f t="shared" ref="H36:H37" si="53">HEX2DEC(MID(E36, 3, LEN(E36)-2))</f>
-        <v>4</v>
-      </c>
-      <c r="I36" s="24">
-        <f t="shared" ref="I36:I37" si="54">G36+H36</f>
-        <v>46084</v>
-      </c>
-      <c r="J36" s="24" t="s">
-        <v>94</v>
+      <c r="J36" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L36" s="19" t="s">
         <v>74</v>
@@ -2540,31 +2548,32 @@
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" s="25"/>
       <c r="C37" s="39"/>
-      <c r="D37" s="28" t="str">
-        <f t="shared" si="50"/>
+      <c r="D37" s="24" t="str">
+        <f t="shared" ref="D37:D38" si="52">F36</f>
+        <v>0xB400</v>
+      </c>
+      <c r="E37" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M45))</f>
+        <v>0x4</v>
+      </c>
+      <c r="F37" s="24" t="str">
+        <f t="shared" ref="F37:F38" si="53">_xlfn.CONCAT("0x",DEC2HEX(I37))</f>
         <v>0xB404</v>
       </c>
-      <c r="E37" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="F37" s="28" t="str">
-        <f t="shared" si="51"/>
-        <v>0xB800</v>
-      </c>
-      <c r="G37" s="28">
-        <f t="shared" si="52"/>
+      <c r="G37" s="24">
+        <f t="shared" ref="G37:G38" si="54">HEX2DEC(MID(D37, 3, LEN(D37)-2))</f>
+        <v>46080</v>
+      </c>
+      <c r="H37" s="24">
+        <f t="shared" ref="H37:H38" si="55">HEX2DEC(MID(E37, 3, LEN(E37)-2))</f>
+        <v>4</v>
+      </c>
+      <c r="I37" s="24">
+        <f t="shared" ref="I37:I38" si="56">G37+H37</f>
         <v>46084</v>
       </c>
-      <c r="H37" s="28">
-        <f t="shared" si="53"/>
-        <v>1020</v>
-      </c>
-      <c r="I37" s="28">
-        <f t="shared" si="54"/>
-        <v>47104</v>
-      </c>
-      <c r="J37" s="28" t="s">
-        <v>30</v>
+      <c r="J37" s="24" t="s">
+        <v>91</v>
       </c>
       <c r="L37" s="29" t="s">
         <v>75</v>
@@ -2575,36 +2584,35 @@
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B38" s="25"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="24" t="str">
-        <f>F37</f>
+      <c r="C38" s="39"/>
+      <c r="D38" s="28" t="str">
+        <f t="shared" si="52"/>
+        <v>0xB404</v>
+      </c>
+      <c r="E38" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="F38" s="28" t="str">
+        <f t="shared" si="53"/>
         <v>0xB800</v>
       </c>
-      <c r="E38" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M39))</f>
-        <v>0x800</v>
-      </c>
-      <c r="F38" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I38))</f>
-        <v>0xC000</v>
-      </c>
-      <c r="G38" s="24">
-        <f t="shared" ref="G38:H43" si="55">HEX2DEC(MID(D38, 3, LEN(D38)-2))</f>
+      <c r="G38" s="28">
+        <f t="shared" si="54"/>
+        <v>46084</v>
+      </c>
+      <c r="H38" s="28">
+        <f t="shared" si="55"/>
+        <v>1020</v>
+      </c>
+      <c r="I38" s="28">
+        <f t="shared" si="56"/>
         <v>47104</v>
       </c>
-      <c r="H38" s="24">
-        <f t="shared" si="55"/>
-        <v>2048</v>
-      </c>
-      <c r="I38" s="24">
-        <f>G38+H38</f>
-        <v>49152</v>
-      </c>
-      <c r="J38" s="24" t="s">
-        <v>76</v>
+      <c r="J38" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L38" s="19" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="M38" s="19">
         <f>M35*M36*M37</f>
@@ -2612,38 +2620,37 @@
       </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B39" s="41"/>
-      <c r="C39" s="42" t="s">
-        <v>49</v>
-      </c>
+      <c r="B39" s="25"/>
+      <c r="C39" s="40"/>
       <c r="D39" s="24" t="str">
         <f>F38</f>
-        <v>0xC000</v>
-      </c>
-      <c r="E39" s="24" t="s">
-        <v>6</v>
+        <v>0xB800</v>
+      </c>
+      <c r="E39" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M39))</f>
+        <v>0x800</v>
       </c>
       <c r="F39" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I39))</f>
-        <v>0x10000</v>
+        <v>0xC000</v>
       </c>
       <c r="G39" s="24">
-        <f t="shared" si="55"/>
-        <v>49152</v>
+        <f t="shared" ref="G39:H44" si="57">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
+        <v>47104</v>
       </c>
       <c r="H39" s="24">
-        <f t="shared" si="55"/>
-        <v>16384</v>
+        <f t="shared" si="57"/>
+        <v>2048</v>
       </c>
       <c r="I39" s="24">
         <f>G39+H39</f>
-        <v>65536</v>
+        <v>49152</v>
       </c>
       <c r="J39" s="24" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="L39" s="19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="M39" s="19">
         <f>M38/8</f>
@@ -2651,145 +2658,147 @@
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B40" s="43" t="s">
-        <v>147</v>
-      </c>
-      <c r="C40" s="44" t="s">
+      <c r="B40" s="41"/>
+      <c r="C40" s="42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D40" s="24" t="str">
+        <f>F39</f>
+        <v>0xC000</v>
+      </c>
+      <c r="E40" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
+        <v>0x10000</v>
+      </c>
+      <c r="G40" s="24">
+        <f t="shared" si="57"/>
+        <v>49152</v>
+      </c>
+      <c r="H40" s="24">
+        <f t="shared" si="57"/>
+        <v>16384</v>
+      </c>
+      <c r="I40" s="24">
+        <f>G40+H40</f>
+        <v>65536</v>
+      </c>
+      <c r="J40" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B41" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="C41" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="24" t="str">
+      <c r="D41" s="24" t="str">
         <f t="shared" si="1"/>
         <v>0x10000</v>
       </c>
-      <c r="E40" s="24" t="str">
+      <c r="E41" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M12))</f>
         <v>0x40</v>
       </c>
-      <c r="F40" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
+      <c r="F41" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I41))</f>
         <v>0x10040</v>
       </c>
-      <c r="G40" s="24">
-        <f t="shared" si="55"/>
+      <c r="G41" s="24">
+        <f t="shared" si="57"/>
         <v>65536</v>
       </c>
-      <c r="H40" s="24">
-        <f t="shared" si="55"/>
+      <c r="H41" s="24">
+        <f t="shared" si="57"/>
         <v>64</v>
       </c>
-      <c r="I40" s="24">
-        <f>G40+H40</f>
+      <c r="I41" s="24">
+        <f>G41+H41</f>
         <v>65600</v>
       </c>
-      <c r="J40" s="24" t="s">
+      <c r="J41" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B41" s="45" t="s">
-        <v>146</v>
-      </c>
-      <c r="C41" s="46"/>
-      <c r="D41" s="28" t="str">
+      <c r="L41" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="M41" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B42" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" s="48"/>
+      <c r="D42" s="28" t="str">
         <f t="shared" si="1"/>
         <v>0x10040</v>
       </c>
-      <c r="E41" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="F41" s="28" t="str">
-        <f t="shared" ref="F41" si="56">_xlfn.CONCAT("0x",DEC2HEX(I41))</f>
+      <c r="E42" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="F42" s="28" t="str">
+        <f t="shared" ref="F42" si="58">_xlfn.CONCAT("0x",DEC2HEX(I42))</f>
         <v>0x11000</v>
       </c>
-      <c r="G41" s="28">
-        <f t="shared" ref="G41" si="57">HEX2DEC(MID(D41, 3, LEN(D41)-2))</f>
+      <c r="G42" s="28">
+        <f t="shared" ref="G42" si="59">HEX2DEC(MID(D42, 3, LEN(D42)-2))</f>
         <v>65600</v>
       </c>
-      <c r="H41" s="28">
-        <f t="shared" ref="H41" si="58">HEX2DEC(MID(E41, 3, LEN(E41)-2))</f>
+      <c r="H42" s="28">
+        <f t="shared" ref="H42" si="60">HEX2DEC(MID(E42, 3, LEN(E42)-2))</f>
         <v>4032</v>
       </c>
-      <c r="I41" s="28">
-        <f t="shared" ref="I41" si="59">G41+H41</f>
+      <c r="I42" s="28">
+        <f t="shared" ref="I42" si="61">G42+H42</f>
         <v>69632</v>
       </c>
-      <c r="J41" s="28" t="s">
+      <c r="J42" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L41" s="21" t="s">
-        <v>96</v>
-      </c>
-      <c r="M41" s="19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B42" s="45"/>
-      <c r="C42" s="47" t="s">
+      <c r="L42" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="M42" s="19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B43" s="44"/>
+      <c r="C43" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="D42" s="24" t="str">
+      <c r="D43" s="24" t="str">
         <f t="shared" si="1"/>
         <v>0x11000</v>
       </c>
-      <c r="E42" s="24" t="str">
+      <c r="E43" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
         <v>0xA00</v>
       </c>
-      <c r="F42" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I42))</f>
+      <c r="F43" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I43))</f>
         <v>0x11A00</v>
       </c>
-      <c r="G42" s="24">
-        <f>HEX2DEC(MID(D42, 3, LEN(D42)-2))</f>
+      <c r="G43" s="24">
+        <f>HEX2DEC(MID(D43, 3, LEN(D43)-2))</f>
         <v>69632</v>
       </c>
-      <c r="H42" s="24">
-        <f t="shared" si="55"/>
+      <c r="H43" s="24">
+        <f t="shared" si="57"/>
         <v>2560</v>
       </c>
-      <c r="I42" s="24">
-        <f>G42+H42</f>
+      <c r="I43" s="24">
+        <f>G43+H43</f>
         <v>72192</v>
       </c>
-      <c r="J42" s="24" t="s">
+      <c r="J43" s="24" t="s">
         <v>51</v>
-      </c>
-      <c r="L42" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="M42" s="19">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="43" spans="2:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="45"/>
-      <c r="C43"/>
-      <c r="D43" s="28" t="str">
-        <f t="shared" ref="D43" si="60">F42</f>
-        <v>0x11A00</v>
-      </c>
-      <c r="E43" s="28" t="s">
-        <v>160</v>
-      </c>
-      <c r="F43" s="28" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I43))</f>
-        <v>0x12000</v>
-      </c>
-      <c r="G43" s="28">
-        <f>HEX2DEC(MID(D43, 3, LEN(D43)-2))</f>
-        <v>72192</v>
-      </c>
-      <c r="H43" s="28">
-        <f t="shared" si="55"/>
-        <v>1536</v>
-      </c>
-      <c r="I43" s="28">
-        <f>G43+H43</f>
-        <v>73728</v>
-      </c>
-      <c r="J43" s="28" t="s">
-        <v>30</v>
       </c>
       <c r="L43" s="29" t="s">
         <v>4</v>
@@ -2798,39 +2807,37 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B44" s="45"/>
-      <c r="C44" s="47" t="s">
-        <v>159</v>
-      </c>
-      <c r="D44" s="24" t="str">
-        <f t="shared" ref="D44" si="61">F43</f>
+    <row r="44" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="B44" s="44"/>
+      <c r="C44"/>
+      <c r="D44" s="28" t="str">
+        <f t="shared" ref="D44" si="62">F43</f>
+        <v>0x11A00</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="F44" s="28" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I44))</f>
         <v>0x12000</v>
       </c>
-      <c r="E44" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="F44" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I44))</f>
-        <v>0x1A000</v>
-      </c>
-      <c r="G44" s="24">
+      <c r="G44" s="28">
         <f>HEX2DEC(MID(D44, 3, LEN(D44)-2))</f>
+        <v>72192</v>
+      </c>
+      <c r="H44" s="28">
+        <f t="shared" si="57"/>
+        <v>1536</v>
+      </c>
+      <c r="I44" s="28">
+        <f>G44+H44</f>
         <v>73728</v>
       </c>
-      <c r="H44" s="24">
-        <f t="shared" ref="H44" si="62">HEX2DEC(MID(E44, 3, LEN(E44)-2))</f>
-        <v>32768</v>
-      </c>
-      <c r="I44" s="24">
-        <f>G44+H44</f>
-        <v>106496</v>
-      </c>
-      <c r="J44" s="24" t="s">
-        <v>51</v>
+      <c r="J44" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L44" s="19" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="M44" s="19">
         <f>M42*M43</f>
@@ -2838,9 +2845,38 @@
       </c>
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B45" s="45"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="24" t="str">
+        <f t="shared" ref="D45" si="63">F44</f>
+        <v>0x12000</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="F45" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I45))</f>
+        <v>0x22000</v>
+      </c>
+      <c r="G45" s="24">
+        <f>HEX2DEC(MID(D45, 3, LEN(D45)-2))</f>
+        <v>73728</v>
+      </c>
+      <c r="H45" s="24">
+        <f t="shared" ref="H45" si="64">HEX2DEC(MID(E45, 3, LEN(E45)-2))</f>
+        <v>65536</v>
+      </c>
+      <c r="I45" s="24">
+        <f>G45+H45</f>
+        <v>139264</v>
+      </c>
+      <c r="J45" s="24" t="s">
+        <v>156</v>
+      </c>
       <c r="L45" s="19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="M45" s="19">
         <f>M44/8</f>
@@ -2848,45 +2884,45 @@
       </c>
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B46" s="45"/>
+      <c r="B46" s="44"/>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B47" s="45"/>
+      <c r="B47" s="44"/>
       <c r="L47" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="M47" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="M47" s="19" t="s">
-        <v>140</v>
-      </c>
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B48" s="45"/>
+      <c r="B48" s="44"/>
       <c r="L48" s="19" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="M48" s="19">
         <v>512</v>
       </c>
       <c r="N48" s="19" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B49" s="45"/>
+      <c r="B49" s="44"/>
       <c r="L49" s="19" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="M49" s="29">
         <v>32</v>
       </c>
       <c r="N49" s="19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B50" s="45"/>
+      <c r="B50" s="44"/>
       <c r="L50" s="30" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="M50" s="19">
         <f>M48*M49</f>
@@ -2894,9 +2930,9 @@
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B51" s="45"/>
+      <c r="B51" s="44"/>
       <c r="L51" s="19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="M51" s="19">
         <f>M50/8</f>
@@ -2907,48 +2943,51 @@
         <v>768</v>
       </c>
       <c r="P51" s="19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B52" s="45"/>
+      <c r="B52" s="44"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B53" s="45"/>
+      <c r="B53" s="44"/>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B54" s="45"/>
+      <c r="B54" s="44"/>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B55" s="45"/>
+      <c r="B55" s="44"/>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B56" s="45"/>
+      <c r="B56" s="44"/>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B57" s="45"/>
+      <c r="B57" s="44"/>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B58" s="45"/>
+      <c r="B58" s="44"/>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B59" s="45"/>
+      <c r="B59" s="44"/>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B60" s="45"/>
+      <c r="B60" s="44"/>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B61" s="45"/>
+      <c r="B61" s="44"/>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B62" s="45"/>
+      <c r="B62" s="44"/>
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B63" s="48"/>
+      <c r="B63" s="44"/>
+    </row>
+    <row r="64" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B64" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C41:C42"/>
     <mergeCell ref="C25:C26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2976,10 +3015,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
@@ -2988,10 +3027,10 @@
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F3" s="16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -3013,141 +3052,141 @@
         <v>83</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sprite collision working (for the first 8)
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D03C7CB-F510-41D6-AE13-24BC896F5B02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE349ED3-4CB4-4C98-80B6-FB19345BBBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="167">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -571,9 +571,6 @@
     <t>Music ROM</t>
   </si>
   <si>
-    <t>0x600</t>
-  </si>
-  <si>
     <t>Deikun (Sound system)</t>
   </si>
   <si>
@@ -586,7 +583,22 @@
     <t>Music RAM (YM Player)</t>
   </si>
   <si>
-    <t>0x10000</t>
+    <t>0x20000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Pixel is about to be written to sprite line buffer</t>
+  </si>
+  <si>
+    <t>Send to collision system</t>
+  </si>
+  <si>
+    <t>----</t>
+  </si>
+  <si>
+    <t>Is there a pixel already in master collision buffer at this location?  Set flag if so</t>
   </si>
 </sst>
 </file>
@@ -822,7 +834,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -941,6 +953,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1257,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="B1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2112,7 +2125,7 @@
       <c r="B25" s="25"/>
       <c r="C25" s="49"/>
       <c r="D25" s="24" t="str">
-        <f>F24</f>
+        <f t="shared" ref="D25:D30" si="29">F24</f>
         <v>0x8A10</v>
       </c>
       <c r="E25" s="24" t="s">
@@ -2123,7 +2136,7 @@
         <v>0x8A20</v>
       </c>
       <c r="G25" s="24">
-        <f t="shared" ref="G25:G27" si="29">HEX2DEC(MID(D25, 3, LEN(D25)-2))</f>
+        <f t="shared" ref="G25:G27" si="30">HEX2DEC(MID(D25, 3, LEN(D25)-2))</f>
         <v>35344</v>
       </c>
       <c r="H25" s="24">
@@ -2148,7 +2161,7 @@
       <c r="B26" s="25"/>
       <c r="C26" s="49"/>
       <c r="D26" s="24" t="str">
-        <f>F25</f>
+        <f t="shared" si="29"/>
         <v>0x8A20</v>
       </c>
       <c r="E26" s="24" t="s">
@@ -2159,7 +2172,7 @@
         <v>0x8A30</v>
       </c>
       <c r="G26" s="24">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>35360</v>
       </c>
       <c r="H26" s="24">
@@ -2184,26 +2197,26 @@
       <c r="B27" s="25"/>
       <c r="C27" s="27"/>
       <c r="D27" s="28" t="str">
-        <f>F26</f>
+        <f t="shared" si="29"/>
         <v>0x8A30</v>
       </c>
       <c r="E27" s="28" t="s">
         <v>39</v>
       </c>
       <c r="F27" s="28" t="str">
-        <f t="shared" ref="F27" si="30">_xlfn.CONCAT("0x",DEC2HEX(I27))</f>
+        <f t="shared" ref="F27" si="31">_xlfn.CONCAT("0x",DEC2HEX(I27))</f>
         <v>0x8B00</v>
       </c>
       <c r="G27" s="28">
-        <f t="shared" si="29"/>
+        <f t="shared" si="30"/>
         <v>35376</v>
       </c>
       <c r="H27" s="28">
-        <f t="shared" ref="H27" si="31">HEX2DEC(MID(E27, 3, LEN(E27)-2))</f>
+        <f t="shared" ref="H27" si="32">HEX2DEC(MID(E27, 3, LEN(E27)-2))</f>
         <v>208</v>
       </c>
       <c r="I27" s="28">
-        <f t="shared" ref="I27" si="32">G27+H27</f>
+        <f t="shared" ref="I27" si="33">G27+H27</f>
         <v>35584</v>
       </c>
       <c r="J27" s="28" t="s">
@@ -2219,10 +2232,10 @@
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="25"/>
       <c r="C28" s="26" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D28" s="24" t="str">
-        <f>F27</f>
+        <f t="shared" si="29"/>
         <v>0x8B00</v>
       </c>
       <c r="E28" s="24" t="s">
@@ -2233,7 +2246,7 @@
         <v>0x8B10</v>
       </c>
       <c r="G28" s="24">
-        <f t="shared" ref="G28" si="33">HEX2DEC(MID(D28, 3, LEN(D28)-2))</f>
+        <f t="shared" ref="G28" si="34">HEX2DEC(MID(D28, 3, LEN(D28)-2))</f>
         <v>35584</v>
       </c>
       <c r="H28" s="24">
@@ -2245,7 +2258,7 @@
         <v>35600</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="L28" s="32" t="s">
         <v>81</v>
@@ -2258,7 +2271,7 @@
       <c r="B29" s="25"/>
       <c r="C29" s="31"/>
       <c r="D29" s="24" t="str">
-        <f>F28</f>
+        <f t="shared" si="29"/>
         <v>0x8B10</v>
       </c>
       <c r="E29" s="24" t="s">
@@ -2269,11 +2282,11 @@
         <v>0x8B20</v>
       </c>
       <c r="G29" s="24">
-        <f t="shared" ref="G29" si="34">HEX2DEC(MID(D29, 3, LEN(D29)-2))</f>
+        <f t="shared" ref="G29" si="35">HEX2DEC(MID(D29, 3, LEN(D29)-2))</f>
         <v>35600</v>
       </c>
       <c r="H29" s="24">
-        <f t="shared" ref="H29" si="35">HEX2DEC(MID(E29, 3, LEN(E29)-2))</f>
+        <f t="shared" ref="H29" si="36">HEX2DEC(MID(E29, 3, LEN(E29)-2))</f>
         <v>16</v>
       </c>
       <c r="I29" s="24">
@@ -2281,7 +2294,7 @@
         <v>35616</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L29" s="32" t="s">
         <v>71</v>
@@ -2294,26 +2307,26 @@
       <c r="B30" s="25"/>
       <c r="C30" s="33"/>
       <c r="D30" s="28" t="str">
-        <f>F29</f>
+        <f t="shared" si="29"/>
         <v>0x8B20</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F30" s="28" t="str">
-        <f t="shared" ref="F30" si="36">_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
+        <f t="shared" ref="F30" si="37">_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
         <v>0x9000</v>
       </c>
       <c r="G30" s="28">
-        <f t="shared" ref="G30" si="37">HEX2DEC(MID(D30, 3, LEN(D30)-2))</f>
+        <f t="shared" ref="G30" si="38">HEX2DEC(MID(D30, 3, LEN(D30)-2))</f>
         <v>35616</v>
       </c>
       <c r="H30" s="28">
-        <f t="shared" ref="H30" si="38">HEX2DEC(MID(E30, 3, LEN(E30)-2))</f>
+        <f t="shared" ref="H30" si="39">HEX2DEC(MID(E30, 3, LEN(E30)-2))</f>
         <v>1248</v>
       </c>
       <c r="I30" s="28">
-        <f t="shared" ref="I30" si="39">G30+H30</f>
+        <f t="shared" ref="I30" si="40">G30+H30</f>
         <v>36864</v>
       </c>
       <c r="J30" s="28" t="s">
@@ -2415,19 +2428,19 @@
         <v>8</v>
       </c>
       <c r="F33" s="24" t="str">
-        <f t="shared" ref="F33" si="40">_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
+        <f t="shared" ref="F33" si="41">_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
         <v>0xA800</v>
       </c>
       <c r="G33" s="24">
-        <f t="shared" ref="G33" si="41">HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
+        <f t="shared" ref="G33" si="42">HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
         <v>40960</v>
       </c>
       <c r="H33" s="24">
-        <f t="shared" ref="H33" si="42">HEX2DEC(MID(E33, 3, LEN(E33)-2))</f>
+        <f t="shared" ref="H33" si="43">HEX2DEC(MID(E33, 3, LEN(E33)-2))</f>
         <v>2048</v>
       </c>
       <c r="I33" s="24">
-        <f t="shared" ref="I33" si="43">G33+H33</f>
+        <f t="shared" ref="I33" si="44">G33+H33</f>
         <v>43008</v>
       </c>
       <c r="J33" s="24" t="s">
@@ -2445,19 +2458,19 @@
         <v>8</v>
       </c>
       <c r="F34" s="24" t="str">
-        <f t="shared" ref="F34" si="44">_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
+        <f t="shared" ref="F34" si="45">_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
         <v>0xB000</v>
       </c>
       <c r="G34" s="24">
-        <f t="shared" ref="G34" si="45">HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
+        <f t="shared" ref="G34" si="46">HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
         <v>43008</v>
       </c>
       <c r="H34" s="24">
-        <f t="shared" ref="H34" si="46">HEX2DEC(MID(E34, 3, LEN(E34)-2))</f>
+        <f t="shared" ref="H34" si="47">HEX2DEC(MID(E34, 3, LEN(E34)-2))</f>
         <v>2048</v>
       </c>
       <c r="I34" s="24">
-        <f t="shared" ref="I34" si="47">G34+H34</f>
+        <f t="shared" ref="I34" si="48">G34+H34</f>
         <v>45056</v>
       </c>
       <c r="J34" s="24" t="s">
@@ -2484,19 +2497,19 @@
         <v>0x80</v>
       </c>
       <c r="F35" s="24" t="str">
-        <f t="shared" ref="F35:F36" si="48">_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
+        <f t="shared" ref="F35:F36" si="49">_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
         <v>0xB080</v>
       </c>
       <c r="G35" s="24">
-        <f t="shared" ref="G35:G36" si="49">HEX2DEC(MID(D35, 3, LEN(D35)-2))</f>
+        <f t="shared" ref="G35:G36" si="50">HEX2DEC(MID(D35, 3, LEN(D35)-2))</f>
         <v>45056</v>
       </c>
       <c r="H35" s="24">
-        <f t="shared" ref="H35:H36" si="50">HEX2DEC(MID(E35, 3, LEN(E35)-2))</f>
+        <f t="shared" ref="H35:H36" si="51">HEX2DEC(MID(E35, 3, LEN(E35)-2))</f>
         <v>128</v>
       </c>
       <c r="I35" s="24">
-        <f t="shared" ref="I35:I36" si="51">G35+H35</f>
+        <f t="shared" ref="I35:I36" si="52">G35+H35</f>
         <v>45184</v>
       </c>
       <c r="J35" s="24" t="s">
@@ -2520,19 +2533,19 @@
         <v>92</v>
       </c>
       <c r="F36" s="28" t="str">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>0xB400</v>
       </c>
       <c r="G36" s="28">
-        <f t="shared" si="49"/>
+        <f t="shared" si="50"/>
         <v>45184</v>
       </c>
       <c r="H36" s="28">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>896</v>
       </c>
       <c r="I36" s="28">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>46080</v>
       </c>
       <c r="J36" s="28" t="s">
@@ -2549,7 +2562,7 @@
       <c r="B37" s="25"/>
       <c r="C37" s="39"/>
       <c r="D37" s="24" t="str">
-        <f t="shared" ref="D37:D38" si="52">F36</f>
+        <f t="shared" ref="D37:D38" si="53">F36</f>
         <v>0xB400</v>
       </c>
       <c r="E37" s="24" t="str">
@@ -2557,19 +2570,19 @@
         <v>0x4</v>
       </c>
       <c r="F37" s="24" t="str">
-        <f t="shared" ref="F37:F38" si="53">_xlfn.CONCAT("0x",DEC2HEX(I37))</f>
+        <f t="shared" ref="F37:F38" si="54">_xlfn.CONCAT("0x",DEC2HEX(I37))</f>
         <v>0xB404</v>
       </c>
       <c r="G37" s="24">
-        <f t="shared" ref="G37:G38" si="54">HEX2DEC(MID(D37, 3, LEN(D37)-2))</f>
+        <f t="shared" ref="G37:G38" si="55">HEX2DEC(MID(D37, 3, LEN(D37)-2))</f>
         <v>46080</v>
       </c>
       <c r="H37" s="24">
-        <f t="shared" ref="H37:H38" si="55">HEX2DEC(MID(E37, 3, LEN(E37)-2))</f>
+        <f t="shared" ref="H37:H38" si="56">HEX2DEC(MID(E37, 3, LEN(E37)-2))</f>
         <v>4</v>
       </c>
       <c r="I37" s="24">
-        <f t="shared" ref="I37:I38" si="56">G37+H37</f>
+        <f t="shared" ref="I37:I38" si="57">G37+H37</f>
         <v>46084</v>
       </c>
       <c r="J37" s="24" t="s">
@@ -2586,26 +2599,26 @@
       <c r="B38" s="25"/>
       <c r="C38" s="39"/>
       <c r="D38" s="28" t="str">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>0xB404</v>
       </c>
       <c r="E38" s="28" t="s">
         <v>132</v>
       </c>
       <c r="F38" s="28" t="str">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>0xB800</v>
       </c>
       <c r="G38" s="28">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v>46084</v>
       </c>
       <c r="H38" s="28">
-        <f t="shared" si="55"/>
+        <f t="shared" si="56"/>
         <v>1020</v>
       </c>
       <c r="I38" s="28">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v>47104</v>
       </c>
       <c r="J38" s="28" t="s">
@@ -2635,11 +2648,11 @@
         <v>0xC000</v>
       </c>
       <c r="G39" s="24">
-        <f t="shared" ref="G39:H44" si="57">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
+        <f t="shared" ref="G39:H44" si="58">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
         <v>47104</v>
       </c>
       <c r="H39" s="24">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>2048</v>
       </c>
       <c r="I39" s="24">
@@ -2674,11 +2687,11 @@
         <v>0x10000</v>
       </c>
       <c r="G40" s="24">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>49152</v>
       </c>
       <c r="H40" s="24">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>16384</v>
       </c>
       <c r="I40" s="24">
@@ -2709,11 +2722,11 @@
         <v>0x10040</v>
       </c>
       <c r="G41" s="24">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>65536</v>
       </c>
       <c r="H41" s="24">
-        <f t="shared" si="57"/>
+        <f t="shared" si="58"/>
         <v>64</v>
       </c>
       <c r="I41" s="24">
@@ -2743,19 +2756,19 @@
         <v>154</v>
       </c>
       <c r="F42" s="28" t="str">
-        <f t="shared" ref="F42" si="58">_xlfn.CONCAT("0x",DEC2HEX(I42))</f>
+        <f t="shared" ref="F42" si="59">_xlfn.CONCAT("0x",DEC2HEX(I42))</f>
         <v>0x11000</v>
       </c>
       <c r="G42" s="28">
-        <f t="shared" ref="G42" si="59">HEX2DEC(MID(D42, 3, LEN(D42)-2))</f>
+        <f t="shared" ref="G42" si="60">HEX2DEC(MID(D42, 3, LEN(D42)-2))</f>
         <v>65600</v>
       </c>
       <c r="H42" s="28">
-        <f t="shared" ref="H42" si="60">HEX2DEC(MID(E42, 3, LEN(E42)-2))</f>
+        <f t="shared" ref="H42" si="61">HEX2DEC(MID(E42, 3, LEN(E42)-2))</f>
         <v>4032</v>
       </c>
       <c r="I42" s="28">
-        <f t="shared" ref="I42" si="61">G42+H42</f>
+        <f t="shared" ref="I42" si="62">G42+H42</f>
         <v>69632</v>
       </c>
       <c r="J42" s="28" t="s">
@@ -2770,36 +2783,6 @@
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B43" s="44"/>
-      <c r="C43" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="D43" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v>0x11000</v>
-      </c>
-      <c r="E43" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
-        <v>0xA00</v>
-      </c>
-      <c r="F43" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I43))</f>
-        <v>0x11A00</v>
-      </c>
-      <c r="G43" s="24">
-        <f>HEX2DEC(MID(D43, 3, LEN(D43)-2))</f>
-        <v>69632</v>
-      </c>
-      <c r="H43" s="24">
-        <f t="shared" si="57"/>
-        <v>2560</v>
-      </c>
-      <c r="I43" s="24">
-        <f>G43+H43</f>
-        <v>72192</v>
-      </c>
-      <c r="J43" s="24" t="s">
-        <v>51</v>
-      </c>
       <c r="L43" s="29" t="s">
         <v>4</v>
       </c>
@@ -2810,32 +2793,13 @@
     <row r="44" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B44" s="44"/>
       <c r="C44"/>
-      <c r="D44" s="28" t="str">
-        <f t="shared" ref="D44" si="62">F43</f>
-        <v>0x11A00</v>
-      </c>
-      <c r="E44" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="F44" s="28" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I44))</f>
-        <v>0x12000</v>
-      </c>
-      <c r="G44" s="28">
-        <f>HEX2DEC(MID(D44, 3, LEN(D44)-2))</f>
-        <v>72192</v>
-      </c>
-      <c r="H44" s="28">
-        <f t="shared" si="57"/>
-        <v>1536</v>
-      </c>
-      <c r="I44" s="28">
-        <f>G44+H44</f>
-        <v>73728</v>
-      </c>
-      <c r="J44" s="28" t="s">
-        <v>30</v>
-      </c>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
       <c r="L44" s="19" t="s">
         <v>140</v>
       </c>
@@ -2846,34 +2810,23 @@
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B45" s="44"/>
-      <c r="C45" s="45" t="s">
-        <v>156</v>
-      </c>
-      <c r="D45" s="24" t="str">
-        <f t="shared" ref="D45" si="63">F44</f>
-        <v>0x12000</v>
-      </c>
-      <c r="E45" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="F45" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I45))</f>
-        <v>0x22000</v>
-      </c>
-      <c r="G45" s="24">
-        <f>HEX2DEC(MID(D45, 3, LEN(D45)-2))</f>
-        <v>73728</v>
-      </c>
+      <c r="C45" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="24"/>
+      <c r="E45" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
+        <v>0xA00</v>
+      </c>
+      <c r="F45" s="24"/>
+      <c r="G45" s="24"/>
       <c r="H45" s="24">
-        <f t="shared" ref="H45" si="64">HEX2DEC(MID(E45, 3, LEN(E45)-2))</f>
-        <v>65536</v>
-      </c>
-      <c r="I45" s="24">
-        <f>G45+H45</f>
-        <v>139264</v>
-      </c>
+        <f>HEX2DEC(MID(E45, 3, LEN(E45)-2))</f>
+        <v>2560</v>
+      </c>
+      <c r="I45" s="24"/>
       <c r="J45" s="24" t="s">
-        <v>156</v>
+        <v>51</v>
       </c>
       <c r="L45" s="19" t="s">
         <v>139</v>
@@ -2885,6 +2838,24 @@
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B46" s="44"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M51))</f>
+        <v>0x800</v>
+      </c>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24">
+        <f>HEX2DEC(MID(E46, 3, LEN(E46)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I46" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="J46" s="24" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B47" s="44"/>
@@ -2909,6 +2880,23 @@
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B49" s="44"/>
+      <c r="C49" s="45" t="s">
+        <v>156</v>
+      </c>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24">
+        <f t="shared" ref="H49" si="63">HEX2DEC(MID(E49, 3, LEN(E49)-2))</f>
+        <v>131072</v>
+      </c>
+      <c r="I49" s="24"/>
+      <c r="J49" s="24" t="s">
+        <v>156</v>
+      </c>
       <c r="L49" s="19" t="s">
         <v>149</v>
       </c>
@@ -2998,10 +2986,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A3B691-5BC9-488D-96B0-3685B8BF2439}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3011,6 +2999,7 @@
     <col min="4" max="4" width="3.5703125" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
     <col min="7" max="7" width="31.42578125" customWidth="1"/>
+    <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
@@ -3157,7 +3146,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="180" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>116</v>
       </c>
@@ -3165,7 +3154,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>118</v>
       </c>
@@ -3173,7 +3162,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>120</v>
       </c>
@@ -3181,12 +3170,35 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>122</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>118</v>
+      </c>
+      <c r="I21" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="50" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I24" t="s">
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add collision flag to sprites
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE349ED3-4CB4-4C98-80B6-FB19345BBBF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85675D2-7435-4D13-B0EC-4B6C0542C185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="168">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -599,6 +599,9 @@
   </si>
   <si>
     <t>Is there a pixel already in master collision buffer at this location?  Set flag if so</t>
+  </si>
+  <si>
+    <t>SPRITE_COLLIDE</t>
   </si>
 </sst>
 </file>
@@ -944,6 +947,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -953,7 +957,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1270,8 +1273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="B1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28:M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1381,7 +1384,7 @@
         <v>44</v>
       </c>
       <c r="D4" s="24" t="str">
-        <f t="shared" ref="D4:D43" si="1">F3</f>
+        <f t="shared" ref="D4:D42" si="1">F3</f>
         <v>0x8000</v>
       </c>
       <c r="E4" s="24" t="s">
@@ -2123,7 +2126,7 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="25"/>
-      <c r="C25" s="49"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="24" t="str">
         <f t="shared" ref="D25:D30" si="29">F24</f>
         <v>0x8A10</v>
@@ -2159,7 +2162,7 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="25"/>
-      <c r="C26" s="49"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="24" t="str">
         <f t="shared" si="29"/>
         <v>0x8A20</v>
@@ -2222,11 +2225,11 @@
       <c r="J27" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L27" s="32" t="s">
-        <v>72</v>
+      <c r="L27" s="19" t="s">
+        <v>167</v>
       </c>
       <c r="M27" s="19">
-        <v>15</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
@@ -2261,10 +2264,10 @@
         <v>158</v>
       </c>
       <c r="L28" s="32" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="M28" s="19">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
@@ -2297,10 +2300,10 @@
         <v>160</v>
       </c>
       <c r="L29" s="32" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="M29" s="19">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
@@ -2332,14 +2335,12 @@
       <c r="J30" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L30" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="M30" s="30">
-        <f>SUM(M26:M29)</f>
-        <v>32</v>
-      </c>
-      <c r="N30" s="35"/>
+      <c r="L30" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="M30" s="19">
+        <v>12</v>
+      </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" s="25"/>
@@ -2372,13 +2373,14 @@
       <c r="J31" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L31" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M31" s="19">
-        <f>M30/8</f>
+      <c r="L31" s="30" t="s">
         <v>4</v>
       </c>
+      <c r="M31" s="30">
+        <f>SUM(M26:M30)</f>
+        <v>32</v>
+      </c>
+      <c r="N31" s="35"/>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B32" s="25"/>
@@ -2409,15 +2411,15 @@
       <c r="J32" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="L32" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="M32" s="30">
-        <f>M25*M31</f>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L32" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="M32" s="19">
+        <f>M31/8</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="25"/>
       <c r="C33" s="36"/>
       <c r="D33" s="24" t="str">
@@ -2446,8 +2448,15 @@
       <c r="J33" s="24" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L33" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="M33" s="30">
+        <f>M25*M32</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B34" s="25"/>
       <c r="C34" s="37"/>
       <c r="D34" s="24" t="str">
@@ -2476,14 +2485,8 @@
       <c r="J34" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="L34" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="M34" s="19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B35" s="25"/>
       <c r="C35" s="38" t="s">
         <v>56</v>
@@ -2493,7 +2496,7 @@
         <v>0xB000</v>
       </c>
       <c r="E35" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M32))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M33))</f>
         <v>0x80</v>
       </c>
       <c r="F35" s="24" t="str">
@@ -2515,14 +2518,14 @@
       <c r="J35" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="L35" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="M35" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L35" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="M35" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B36" s="25"/>
       <c r="C36" s="39"/>
       <c r="D36" s="28" t="str">
@@ -2552,13 +2555,13 @@
         <v>30</v>
       </c>
       <c r="L36" s="19" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="M36" s="19">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B37" s="25"/>
       <c r="C37" s="39"/>
       <c r="D37" s="24" t="str">
@@ -2566,7 +2569,7 @@
         <v>0xB400</v>
       </c>
       <c r="E37" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M45))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M46))</f>
         <v>0x4</v>
       </c>
       <c r="F37" s="24" t="str">
@@ -2588,14 +2591,14 @@
       <c r="J37" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="L37" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="M37" s="29">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L37" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="M37" s="19">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B38" s="25"/>
       <c r="C38" s="39"/>
       <c r="D38" s="28" t="str">
@@ -2624,15 +2627,14 @@
       <c r="J38" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L38" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="M38" s="19">
-        <f>M35*M36*M37</f>
-        <v>16384</v>
-      </c>
-    </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L38" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="M38" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B39" s="25"/>
       <c r="C39" s="40"/>
       <c r="D39" s="24" t="str">
@@ -2640,7 +2642,7 @@
         <v>0xB800</v>
       </c>
       <c r="E39" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M39))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M40))</f>
         <v>0x800</v>
       </c>
       <c r="F39" s="24" t="str">
@@ -2648,7 +2650,7 @@
         <v>0xC000</v>
       </c>
       <c r="G39" s="24">
-        <f t="shared" ref="G39:H44" si="58">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
+        <f t="shared" ref="G39:H41" si="58">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
         <v>47104</v>
       </c>
       <c r="H39" s="24">
@@ -2663,14 +2665,14 @@
         <v>76</v>
       </c>
       <c r="L39" s="19" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="M39" s="19">
-        <f>M38/8</f>
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+        <f>M36*M37*M38</f>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B40" s="41"/>
       <c r="C40" s="42" t="s">
         <v>49</v>
@@ -2701,12 +2703,19 @@
       <c r="J40" s="24" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L40" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="M40" s="19">
+        <f>M39/8</f>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B41" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="C41" s="47" t="s">
+      <c r="C41" s="48" t="s">
         <v>55</v>
       </c>
       <c r="D41" s="24" t="str">
@@ -2736,18 +2745,12 @@
       <c r="J41" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="L41" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="M41" s="19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B42" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="C42" s="48"/>
+      <c r="C42" s="49"/>
       <c r="D42" s="28" t="str">
         <f t="shared" si="1"/>
         <v>0x10040</v>
@@ -2774,23 +2777,23 @@
       <c r="J42" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L42" s="19" t="s">
+      <c r="L42" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="M42" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B43" s="44"/>
+      <c r="L43" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="M42" s="19">
+      <c r="M43" s="19">
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B43" s="44"/>
-      <c r="L43" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="M43" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:13" ht="15" x14ac:dyDescent="0.25">
       <c r="B44" s="44"/>
       <c r="C44"/>
       <c r="D44"/>
@@ -2800,15 +2803,14 @@
       <c r="H44"/>
       <c r="I44"/>
       <c r="J44"/>
-      <c r="L44" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="M44" s="19">
-        <f>M42*M43</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L44" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="M44" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B45" s="44"/>
       <c r="C45" s="38" t="s">
         <v>56</v>
@@ -2829,19 +2831,19 @@
         <v>51</v>
       </c>
       <c r="L45" s="19" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M45" s="19">
-        <f>M44/8</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
+        <f>M43*M44</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B46" s="44"/>
       <c r="C46" s="40"/>
       <c r="D46" s="24"/>
       <c r="E46" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M51))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M52))</f>
         <v>0x800</v>
       </c>
       <c r="F46" s="24"/>
@@ -2856,26 +2858,24 @@
       <c r="J46" s="24" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L46" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="M46" s="19">
+        <f>M45/8</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B47" s="44"/>
-      <c r="L47" s="21" t="s">
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B48" s="44"/>
+      <c r="L48" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="M47" s="19" t="s">
+      <c r="M48" s="19" t="s">
         <v>137</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B48" s="44"/>
-      <c r="L48" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="M48" s="19">
-        <v>512</v>
-      </c>
-      <c r="N48" s="19" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.2">
@@ -2898,44 +2898,53 @@
         <v>156</v>
       </c>
       <c r="L49" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="M49" s="29">
-        <v>32</v>
+        <v>135</v>
+      </c>
+      <c r="M49" s="19">
+        <v>512</v>
       </c>
       <c r="N49" s="19" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B50" s="44"/>
-      <c r="L50" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="M50" s="19">
-        <f>M48*M49</f>
-        <v>16384</v>
+      <c r="L50" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="M50" s="29">
+        <v>32</v>
+      </c>
+      <c r="N50" s="19" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B51" s="44"/>
-      <c r="L51" s="19" t="s">
+      <c r="L51" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="M51" s="19">
+        <f>M49*M50</f>
+        <v>16384</v>
+      </c>
+      <c r="P51" s="19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B52" s="44"/>
+      <c r="L52" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="M51" s="19">
-        <f>M50/8</f>
+      <c r="M52" s="19">
+        <f>M51/8</f>
         <v>2048</v>
       </c>
-      <c r="O51" s="19">
+      <c r="O52" s="19">
         <f>384*2</f>
         <v>768</v>
       </c>
-      <c r="P51" s="19" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B52" s="44"/>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B53" s="44"/>
@@ -3192,7 +3201,7 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I23" s="50" t="s">
+      <c r="I23" s="47" t="s">
         <v>165</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add multiple palettes, reduce sprite update time
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D85675D2-7435-4D13-B0EC-4B6C0542C185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3502A66-42A8-4476-BE82-9EC7B47F0F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="171">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -562,9 +562,6 @@
     <t>CPU addressable</t>
   </si>
   <si>
-    <t>0x0FC0</t>
-  </si>
-  <si>
     <t>5-bit index for palette colour</t>
   </si>
   <si>
@@ -602,13 +599,25 @@
   </si>
   <si>
     <t>SPRITE_COLLIDE</t>
+  </si>
+  <si>
+    <t>&lt;UNUSED&gt;</t>
+  </si>
+  <si>
+    <t>5 bit index currently used</t>
+  </si>
+  <si>
+    <t>SPRITE_PALETTE_INDEX</t>
+  </si>
+  <si>
+    <t>This really only needs 9 bits?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -675,8 +684,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -734,12 +751,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -837,7 +848,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -948,12 +959,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1273,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="B1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28:M33"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1384,7 +1390,7 @@
         <v>44</v>
       </c>
       <c r="D4" s="24" t="str">
-        <f t="shared" ref="D4:D42" si="1">F3</f>
+        <f t="shared" ref="D4:D41" si="1">F3</f>
         <v>0x8000</v>
       </c>
       <c r="E4" s="24" t="s">
@@ -1552,7 +1558,7 @@
         <v>58</v>
       </c>
       <c r="M8" s="29">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
@@ -1737,8 +1743,8 @@
         <v>145</v>
       </c>
       <c r="M13" s="30">
-        <f>M12</f>
-        <v>64</v>
+        <f>M12*M8</f>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
@@ -1804,7 +1810,7 @@
         <v>59</v>
       </c>
       <c r="N15" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
@@ -1840,7 +1846,7 @@
         <v>65</v>
       </c>
       <c r="M16" s="29">
-        <v>16</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
@@ -1948,7 +1954,10 @@
         <v>68</v>
       </c>
       <c r="M19" s="19">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="N19" s="19" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
@@ -1985,7 +1994,7 @@
       </c>
       <c r="M20" s="30">
         <f>M17*M18*M19</f>
-        <v>1280</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
@@ -2022,7 +2031,7 @@
       </c>
       <c r="M21" s="19">
         <f>M20/8</f>
-        <v>160</v>
+        <v>256</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
@@ -2059,7 +2068,7 @@
       </c>
       <c r="M22" s="30">
         <f>M16*M21</f>
-        <v>2560</v>
+        <v>16384</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
@@ -2126,7 +2135,7 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="25"/>
-      <c r="C25" s="50"/>
+      <c r="C25" s="49"/>
       <c r="D25" s="24" t="str">
         <f t="shared" ref="D25:D30" si="29">F24</f>
         <v>0x8A10</v>
@@ -2162,7 +2171,7 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="25"/>
-      <c r="C26" s="50"/>
+      <c r="C26" s="49"/>
       <c r="D26" s="24" t="str">
         <f t="shared" si="29"/>
         <v>0x8A20</v>
@@ -2226,7 +2235,7 @@
         <v>30</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="M27" s="19">
         <v>1</v>
@@ -2235,7 +2244,7 @@
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="25"/>
       <c r="C28" s="26" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D28" s="24" t="str">
         <f t="shared" si="29"/>
@@ -2261,13 +2270,13 @@
         <v>35600</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="L28" s="32" t="s">
-        <v>72</v>
+        <v>157</v>
+      </c>
+      <c r="L28" s="19" t="s">
+        <v>169</v>
       </c>
       <c r="M28" s="19">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
@@ -2297,13 +2306,13 @@
         <v>35616</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="L29" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="M29" s="19">
-        <v>4</v>
+        <v>159</v>
+      </c>
+      <c r="L29" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="M29" s="48">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
@@ -2314,7 +2323,7 @@
         <v>0x8B20</v>
       </c>
       <c r="E30" s="28" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F30" s="28" t="str">
         <f t="shared" ref="F30" si="37">_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
@@ -2336,10 +2345,13 @@
         <v>30</v>
       </c>
       <c r="L30" s="32" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="M30" s="19">
         <v>12</v>
+      </c>
+      <c r="N30" s="19" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
@@ -2373,14 +2385,12 @@
       <c r="J31" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L31" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="M31" s="30">
-        <f>SUM(M26:M30)</f>
-        <v>32</v>
-      </c>
-      <c r="N31" s="35"/>
+      <c r="L31" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="M31" s="19">
+        <v>6</v>
+      </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B32" s="25"/>
@@ -2411,15 +2421,17 @@
       <c r="J32" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="L32" s="19" t="s">
-        <v>3</v>
+      <c r="L32" s="32" t="s">
+        <v>71</v>
       </c>
       <c r="M32" s="19">
-        <f>M31/8</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="N32" s="19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="25"/>
       <c r="C33" s="36"/>
       <c r="D33" s="24" t="str">
@@ -2449,14 +2461,15 @@
         <v>45</v>
       </c>
       <c r="L33" s="30" t="s">
-        <v>139</v>
+        <v>4</v>
       </c>
       <c r="M33" s="30">
-        <f>M25*M32</f>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+        <f>SUM(M26:M32)</f>
+        <v>32</v>
+      </c>
+      <c r="N33" s="35"/>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B34" s="25"/>
       <c r="C34" s="37"/>
       <c r="D34" s="24" t="str">
@@ -2485,8 +2498,15 @@
       <c r="J34" s="24" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L34" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="M34" s="19">
+        <f>M33/8</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B35" s="25"/>
       <c r="C35" s="38" t="s">
         <v>56</v>
@@ -2496,7 +2516,7 @@
         <v>0xB000</v>
       </c>
       <c r="E35" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M33))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M35))</f>
         <v>0x80</v>
       </c>
       <c r="F35" s="24" t="str">
@@ -2518,14 +2538,15 @@
       <c r="J35" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="L35" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="M35" s="19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L35" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="M35" s="30">
+        <f>M25*M34</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="25"/>
       <c r="C36" s="39"/>
       <c r="D36" s="28" t="str">
@@ -2554,14 +2575,8 @@
       <c r="J36" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L36" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="M36" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" s="25"/>
       <c r="C37" s="39"/>
       <c r="D37" s="24" t="str">
@@ -2569,7 +2584,7 @@
         <v>0xB400</v>
       </c>
       <c r="E37" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M46))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M48))</f>
         <v>0x4</v>
       </c>
       <c r="F37" s="24" t="str">
@@ -2591,14 +2606,14 @@
       <c r="J37" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="L37" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="M37" s="19">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L37" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="M37" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B38" s="25"/>
       <c r="C38" s="39"/>
       <c r="D38" s="28" t="str">
@@ -2627,14 +2642,14 @@
       <c r="J38" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L38" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="M38" s="29">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L38" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="M38" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" s="25"/>
       <c r="C39" s="40"/>
       <c r="D39" s="24" t="str">
@@ -2642,7 +2657,7 @@
         <v>0xB800</v>
       </c>
       <c r="E39" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M40))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M42))</f>
         <v>0x800</v>
       </c>
       <c r="F39" s="24" t="str">
@@ -2665,14 +2680,13 @@
         <v>76</v>
       </c>
       <c r="L39" s="19" t="s">
-        <v>148</v>
+        <v>74</v>
       </c>
       <c r="M39" s="19">
-        <f>M36*M37*M38</f>
-        <v>16384</v>
-      </c>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B40" s="41"/>
       <c r="C40" s="42" t="s">
         <v>49</v>
@@ -2703,19 +2717,18 @@
       <c r="J40" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="L40" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="M40" s="19">
-        <f>M39/8</f>
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L40" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="M40" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B41" s="43" t="s">
         <v>144</v>
       </c>
-      <c r="C41" s="48" t="s">
+      <c r="C41" s="45" t="s">
         <v>55</v>
       </c>
       <c r="D41" s="24" t="str">
@@ -2723,12 +2736,12 @@
         <v>0x10000</v>
       </c>
       <c r="E41" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M12))</f>
-        <v>0x40</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M13))</f>
+        <v>0x100</v>
       </c>
       <c r="F41" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I41))</f>
-        <v>0x10040</v>
+        <v>0x10100</v>
       </c>
       <c r="G41" s="24">
         <f t="shared" si="58"/>
@@ -2736,222 +2749,209 @@
       </c>
       <c r="H41" s="24">
         <f t="shared" si="58"/>
-        <v>64</v>
+        <v>256</v>
       </c>
       <c r="I41" s="24">
         <f>G41+H41</f>
-        <v>65600</v>
+        <v>65792</v>
       </c>
       <c r="J41" s="24" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L41" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="M41" s="19">
+        <f>M38*M39*M40</f>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B42" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="C42" s="49"/>
-      <c r="D42" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v>0x10040</v>
-      </c>
-      <c r="E42" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="F42" s="28" t="str">
-        <f t="shared" ref="F42" si="59">_xlfn.CONCAT("0x",DEC2HEX(I42))</f>
-        <v>0x11000</v>
-      </c>
-      <c r="G42" s="28">
-        <f t="shared" ref="G42" si="60">HEX2DEC(MID(D42, 3, LEN(D42)-2))</f>
-        <v>65600</v>
-      </c>
-      <c r="H42" s="28">
-        <f t="shared" ref="H42" si="61">HEX2DEC(MID(E42, 3, LEN(E42)-2))</f>
-        <v>4032</v>
-      </c>
-      <c r="I42" s="28">
-        <f t="shared" ref="I42" si="62">G42+H42</f>
-        <v>69632</v>
-      </c>
-      <c r="J42" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L42" s="21" t="s">
+      <c r="L42" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="M42" s="19">
+        <f>M41/8</f>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="B43" s="44"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B44" s="44"/>
+      <c r="C44" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="24"/>
+      <c r="E44" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
+        <v>0x4000</v>
+      </c>
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="24">
+        <f>HEX2DEC(MID(E44, 3, LEN(E44)-2))</f>
+        <v>16384</v>
+      </c>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="L44" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="M42" s="19" t="s">
+      <c r="M44" s="19" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B43" s="44"/>
-      <c r="L43" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="M43" s="19">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="B44" s="44"/>
-      <c r="C44"/>
-      <c r="D44"/>
-      <c r="E44"/>
-      <c r="F44"/>
-      <c r="G44"/>
-      <c r="H44"/>
-      <c r="I44"/>
-      <c r="J44"/>
-      <c r="L44" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="M44" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B45" s="44"/>
-      <c r="C45" s="38" t="s">
-        <v>56</v>
-      </c>
+      <c r="C45" s="40"/>
       <c r="D45" s="24"/>
       <c r="E45" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
-        <v>0xA00</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M54))</f>
+        <v>0x800</v>
       </c>
       <c r="F45" s="24"/>
       <c r="G45" s="24"/>
       <c r="H45" s="24">
         <f>HEX2DEC(MID(E45, 3, LEN(E45)-2))</f>
-        <v>2560</v>
-      </c>
-      <c r="I45" s="24"/>
+        <v>2048</v>
+      </c>
+      <c r="I45" s="24" t="s">
+        <v>161</v>
+      </c>
       <c r="J45" s="24" t="s">
-        <v>51</v>
+        <v>134</v>
       </c>
       <c r="L45" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="M45" s="19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B46" s="44"/>
+      <c r="L46" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="M46" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B47" s="44"/>
+      <c r="L47" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="M45" s="19">
-        <f>M43*M44</f>
+      <c r="M47" s="19">
+        <f>M45*M46</f>
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B46" s="44"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M52))</f>
-        <v>0x800</v>
-      </c>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24">
-        <f>HEX2DEC(MID(E46, 3, LEN(E46)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I46" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="J46" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="L46" s="19" t="s">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B48" s="44"/>
+      <c r="C48" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24">
+        <f t="shared" ref="H48" si="59">HEX2DEC(MID(E48, 3, LEN(E48)-2))</f>
+        <v>131072</v>
+      </c>
+      <c r="I48" s="24"/>
+      <c r="J48" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="L48" s="19" t="s">
         <v>139</v>
       </c>
-      <c r="M46" s="19">
-        <f>M45/8</f>
+      <c r="M48" s="19">
+        <f>M47/8</f>
         <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B47" s="44"/>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B48" s="44"/>
-      <c r="L48" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="M48" s="19" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B49" s="44"/>
-      <c r="C49" s="45" t="s">
-        <v>156</v>
-      </c>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24">
-        <f t="shared" ref="H49" si="63">HEX2DEC(MID(E49, 3, LEN(E49)-2))</f>
-        <v>131072</v>
-      </c>
-      <c r="I49" s="24"/>
-      <c r="J49" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="L49" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="M49" s="19">
-        <v>512</v>
-      </c>
-      <c r="N49" s="19" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B50" s="44"/>
-      <c r="L50" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="M50" s="29">
-        <v>32</v>
-      </c>
-      <c r="N50" s="19" t="s">
-        <v>138</v>
+      <c r="L50" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="M50" s="19" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B51" s="44"/>
-      <c r="L51" s="30" t="s">
-        <v>142</v>
+      <c r="L51" s="19" t="s">
+        <v>135</v>
       </c>
       <c r="M51" s="19">
-        <f>M49*M50</f>
-        <v>16384</v>
-      </c>
-      <c r="P51" s="19" t="s">
-        <v>151</v>
+        <v>512</v>
+      </c>
+      <c r="N51" s="19" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B52" s="44"/>
       <c r="L52" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="M52" s="29">
+        <v>32</v>
+      </c>
+      <c r="N52" s="19" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B53" s="44"/>
+      <c r="L53" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="M53" s="19">
+        <f>M51*M52</f>
+        <v>16384</v>
+      </c>
+      <c r="P53" s="19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B54" s="44"/>
+      <c r="L54" s="19" t="s">
         <v>141</v>
       </c>
-      <c r="M52" s="19">
-        <f>M51/8</f>
+      <c r="M54" s="19">
+        <f>M53/8</f>
         <v>2048</v>
       </c>
-      <c r="O52" s="19">
+      <c r="O54" s="19">
         <f>384*2</f>
         <v>768</v>
       </c>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B53" s="44"/>
-    </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B54" s="44"/>
-    </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B55" s="44"/>
     </row>
@@ -2983,8 +2983,7 @@
       <c r="B64" s="46"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C41:C42"/>
+  <mergeCells count="1">
     <mergeCell ref="C25:C26"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3192,22 +3191,22 @@
         <v>118</v>
       </c>
       <c r="I21" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I23" s="47" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add pickups (collision broken on fpga currently)
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3502A66-42A8-4476-BE82-9EC7B47F0F8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E929F060-A0BA-45F5-B13B-029C0F899D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -1279,8 +1279,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="B1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M28" sqref="M28"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M46" sqref="M46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix collision on FPGA, improve sprite updates
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E929F060-A0BA-45F5-B13B-029C0F899D7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99866AE2-C3D5-4CBC-A6DE-D85230060CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="173">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -611,6 +611,12 @@
   </si>
   <si>
     <t>This really only needs 9 bits?</t>
+  </si>
+  <si>
+    <t>System pause trigger</t>
+  </si>
+  <si>
+    <t>0x00CF</t>
   </si>
 </sst>
 </file>
@@ -848,7 +854,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -960,6 +966,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1277,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
-  <dimension ref="B1:P64"/>
+  <dimension ref="B1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M46" sqref="M46"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1390,7 +1399,7 @@
         <v>44</v>
       </c>
       <c r="D4" s="24" t="str">
-        <f t="shared" ref="D4:D41" si="1">F3</f>
+        <f t="shared" ref="D4:D42" si="1">F3</f>
         <v>0x8000</v>
       </c>
       <c r="E4" s="24" t="s">
@@ -1975,7 +1984,7 @@
         <v>0x8821</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" ref="G20:H31" si="25">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
+        <f t="shared" ref="G20:H32" si="25">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
         <v>34816</v>
       </c>
       <c r="H20" s="24">
@@ -2135,9 +2144,9 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="25"/>
-      <c r="C25" s="49"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="24" t="str">
-        <f t="shared" ref="D25:D30" si="29">F24</f>
+        <f t="shared" ref="D25:D31" si="29">F24</f>
         <v>0x8A10</v>
       </c>
       <c r="E25" s="24" t="s">
@@ -2148,7 +2157,7 @@
         <v>0x8A20</v>
       </c>
       <c r="G25" s="24">
-        <f t="shared" ref="G25:G27" si="30">HEX2DEC(MID(D25, 3, LEN(D25)-2))</f>
+        <f t="shared" ref="G25:G26" si="30">HEX2DEC(MID(D25, 3, LEN(D25)-2))</f>
         <v>35344</v>
       </c>
       <c r="H25" s="24">
@@ -2171,7 +2180,7 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="25"/>
-      <c r="C26" s="49"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="24" t="str">
         <f t="shared" si="29"/>
         <v>0x8A20</v>
@@ -2207,32 +2216,32 @@
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="25"/>
-      <c r="C27" s="27"/>
-      <c r="D27" s="28" t="str">
-        <f t="shared" si="29"/>
+      <c r="C27" s="49"/>
+      <c r="D27" s="24" t="str">
+        <f>F26</f>
         <v>0x8A30</v>
       </c>
-      <c r="E27" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="28" t="str">
+      <c r="E27" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="24" t="str">
         <f t="shared" ref="F27" si="31">_xlfn.CONCAT("0x",DEC2HEX(I27))</f>
-        <v>0x8B00</v>
-      </c>
-      <c r="G27" s="28">
-        <f t="shared" si="30"/>
+        <v>0x8A31</v>
+      </c>
+      <c r="G27" s="24">
+        <f>HEX2DEC(MID(D27, 3, LEN(D27)-2))</f>
         <v>35376</v>
       </c>
-      <c r="H27" s="28">
+      <c r="H27" s="24">
         <f t="shared" ref="H27" si="32">HEX2DEC(MID(E27, 3, LEN(E27)-2))</f>
-        <v>208</v>
-      </c>
-      <c r="I27" s="28">
+        <v>1</v>
+      </c>
+      <c r="I27" s="24">
         <f t="shared" ref="I27" si="33">G27+H27</f>
-        <v>35584</v>
-      </c>
-      <c r="J27" s="28" t="s">
-        <v>30</v>
+        <v>35377</v>
+      </c>
+      <c r="J27" s="24" t="s">
+        <v>171</v>
       </c>
       <c r="L27" s="19" t="s">
         <v>166</v>
@@ -2243,183 +2252,183 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="25"/>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="27"/>
+      <c r="D28" s="28" t="str">
+        <f>F27</f>
+        <v>0x8A31</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="F28" s="28" t="str">
+        <f t="shared" ref="F28" si="34">_xlfn.CONCAT("0x",DEC2HEX(I28))</f>
+        <v>0x8B00</v>
+      </c>
+      <c r="G28" s="28">
+        <f>HEX2DEC(MID(D28, 3, LEN(D28)-2))</f>
+        <v>35377</v>
+      </c>
+      <c r="H28" s="28">
+        <f t="shared" ref="H28" si="35">HEX2DEC(MID(E28, 3, LEN(E28)-2))</f>
+        <v>207</v>
+      </c>
+      <c r="I28" s="28">
+        <f t="shared" ref="I28" si="36">G28+H28</f>
+        <v>35584</v>
+      </c>
+      <c r="J28" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="L28" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="M28" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B29" s="25"/>
+      <c r="C29" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="D28" s="24" t="str">
-        <f t="shared" si="29"/>
+      <c r="D29" s="24" t="str">
+        <f>F28</f>
         <v>0x8B00</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E29" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I28))</f>
+      <c r="F29" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
         <v>0x8B10</v>
       </c>
-      <c r="G28" s="24">
-        <f t="shared" ref="G28" si="34">HEX2DEC(MID(D28, 3, LEN(D28)-2))</f>
+      <c r="G29" s="24">
+        <f t="shared" ref="G29" si="37">HEX2DEC(MID(D29, 3, LEN(D29)-2))</f>
         <v>35584</v>
       </c>
-      <c r="H28" s="24">
+      <c r="H29" s="24">
         <f t="shared" si="25"/>
         <v>16</v>
       </c>
-      <c r="I28" s="24">
-        <f>G28+H28</f>
+      <c r="I29" s="24">
+        <f>G29+H29</f>
         <v>35600</v>
       </c>
-      <c r="J28" s="24" t="s">
+      <c r="J29" s="24" t="s">
         <v>157</v>
       </c>
-      <c r="L28" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="M28" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="25"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="24" t="str">
+      <c r="L29" s="48" t="s">
+        <v>167</v>
+      </c>
+      <c r="M29" s="48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B30" s="25"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="24" t="str">
         <f t="shared" si="29"/>
         <v>0x8B10</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E30" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="F29" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
+      <c r="F30" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
         <v>0x8B20</v>
       </c>
-      <c r="G29" s="24">
-        <f t="shared" ref="G29" si="35">HEX2DEC(MID(D29, 3, LEN(D29)-2))</f>
+      <c r="G30" s="24">
+        <f t="shared" ref="G30" si="38">HEX2DEC(MID(D30, 3, LEN(D30)-2))</f>
         <v>35600</v>
       </c>
-      <c r="H29" s="24">
-        <f t="shared" ref="H29" si="36">HEX2DEC(MID(E29, 3, LEN(E29)-2))</f>
+      <c r="H30" s="24">
+        <f t="shared" ref="H30" si="39">HEX2DEC(MID(E30, 3, LEN(E30)-2))</f>
         <v>16</v>
       </c>
-      <c r="I29" s="24">
-        <f>G29+H29</f>
+      <c r="I30" s="24">
+        <f>G30+H30</f>
         <v>35616</v>
       </c>
-      <c r="J29" s="24" t="s">
+      <c r="J30" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="L29" s="48" t="s">
-        <v>167</v>
-      </c>
-      <c r="M29" s="48">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B30" s="25"/>
-      <c r="C30" s="33"/>
-      <c r="D30" s="28" t="str">
+      <c r="L30" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="M30" s="19">
+        <v>12</v>
+      </c>
+      <c r="N30" s="19" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B31" s="25"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="28" t="str">
         <f t="shared" si="29"/>
         <v>0x8B20</v>
       </c>
-      <c r="E30" s="28" t="s">
+      <c r="E31" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="F30" s="28" t="str">
-        <f t="shared" ref="F30" si="37">_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
+      <c r="F31" s="28" t="str">
+        <f t="shared" ref="F31" si="40">_xlfn.CONCAT("0x",DEC2HEX(I31))</f>
         <v>0x9000</v>
       </c>
-      <c r="G30" s="28">
-        <f t="shared" ref="G30" si="38">HEX2DEC(MID(D30, 3, LEN(D30)-2))</f>
+      <c r="G31" s="28">
+        <f t="shared" ref="G31" si="41">HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
         <v>35616</v>
       </c>
-      <c r="H30" s="28">
-        <f t="shared" ref="H30" si="39">HEX2DEC(MID(E30, 3, LEN(E30)-2))</f>
+      <c r="H31" s="28">
+        <f t="shared" ref="H31" si="42">HEX2DEC(MID(E31, 3, LEN(E31)-2))</f>
         <v>1248</v>
       </c>
-      <c r="I30" s="28">
-        <f t="shared" ref="I30" si="40">G30+H30</f>
+      <c r="I31" s="28">
+        <f t="shared" ref="I31" si="43">G31+H31</f>
         <v>36864</v>
       </c>
-      <c r="J30" s="28" t="s">
+      <c r="J31" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L30" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="M30" s="19">
-        <v>12</v>
-      </c>
-      <c r="N30" s="19" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B31" s="25"/>
-      <c r="C31" s="34" t="s">
+      <c r="L31" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="M31" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B32" s="25"/>
+      <c r="C32" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="D31" s="24" t="str">
+      <c r="D32" s="24" t="str">
         <f t="shared" si="1"/>
         <v>0x9000</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E32" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="F31" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I31))</f>
+      <c r="F32" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
         <v>0x9800</v>
       </c>
-      <c r="G31" s="24">
-        <f>HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
+      <c r="G32" s="24">
+        <f>HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
         <v>36864</v>
       </c>
-      <c r="H31" s="24">
+      <c r="H32" s="24">
         <f t="shared" si="25"/>
         <v>2048</v>
       </c>
-      <c r="I31" s="24">
-        <f>G31+H31</f>
-        <v>38912</v>
-      </c>
-      <c r="J31" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="L31" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="M31" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B32" s="25"/>
-      <c r="C32" s="36"/>
-      <c r="D32" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v>0x9800</v>
-      </c>
-      <c r="E32" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
-        <v>0xA000</v>
-      </c>
-      <c r="G32" s="24">
-        <f>HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
-        <v>38912</v>
-      </c>
-      <c r="H32" s="24">
-        <f>HEX2DEC(MID(E32, 3, LEN(E32)-2))</f>
-        <v>2048</v>
-      </c>
       <c r="I32" s="24">
         <f>G32+H32</f>
-        <v>40960</v>
+        <v>38912</v>
       </c>
       <c r="J32" s="24" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="L32" s="32" t="s">
         <v>71</v>
@@ -2436,29 +2445,29 @@
       <c r="C33" s="36"/>
       <c r="D33" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0xA000</v>
+        <v>0x9800</v>
       </c>
       <c r="E33" s="24" t="s">
         <v>8</v>
       </c>
       <c r="F33" s="24" t="str">
-        <f t="shared" ref="F33" si="41">_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
-        <v>0xA800</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
+        <v>0xA000</v>
       </c>
       <c r="G33" s="24">
-        <f t="shared" ref="G33" si="42">HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
+        <f>HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
+        <v>38912</v>
+      </c>
+      <c r="H33" s="24">
+        <f>HEX2DEC(MID(E33, 3, LEN(E33)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I33" s="24">
+        <f>G33+H33</f>
         <v>40960</v>
       </c>
-      <c r="H33" s="24">
-        <f t="shared" ref="H33" si="43">HEX2DEC(MID(E33, 3, LEN(E33)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I33" s="24">
-        <f t="shared" ref="I33" si="44">G33+H33</f>
-        <v>43008</v>
-      </c>
       <c r="J33" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L33" s="30" t="s">
         <v>4</v>
@@ -2471,32 +2480,32 @@
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B34" s="25"/>
-      <c r="C34" s="37"/>
+      <c r="C34" s="36"/>
       <c r="D34" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0xA800</v>
+        <v>0xA000</v>
       </c>
       <c r="E34" s="24" t="s">
         <v>8</v>
       </c>
       <c r="F34" s="24" t="str">
-        <f t="shared" ref="F34" si="45">_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
-        <v>0xB000</v>
+        <f t="shared" ref="F34" si="44">_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
+        <v>0xA800</v>
       </c>
       <c r="G34" s="24">
-        <f t="shared" ref="G34" si="46">HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
+        <f t="shared" ref="G34" si="45">HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
+        <v>40960</v>
+      </c>
+      <c r="H34" s="24">
+        <f t="shared" ref="H34" si="46">HEX2DEC(MID(E34, 3, LEN(E34)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I34" s="24">
+        <f t="shared" ref="I34" si="47">G34+H34</f>
         <v>43008</v>
       </c>
-      <c r="H34" s="24">
-        <f t="shared" ref="H34" si="47">HEX2DEC(MID(E34, 3, LEN(E34)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I34" s="24">
-        <f t="shared" ref="I34" si="48">G34+H34</f>
-        <v>45056</v>
-      </c>
       <c r="J34" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L34" s="19" t="s">
         <v>3</v>
@@ -2508,35 +2517,32 @@
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B35" s="25"/>
-      <c r="C35" s="38" t="s">
-        <v>56</v>
-      </c>
+      <c r="C35" s="37"/>
       <c r="D35" s="24" t="str">
         <f t="shared" si="1"/>
+        <v>0xA800</v>
+      </c>
+      <c r="E35" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="24" t="str">
+        <f t="shared" ref="F35" si="48">_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
         <v>0xB000</v>
       </c>
-      <c r="E35" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M35))</f>
-        <v>0x80</v>
-      </c>
-      <c r="F35" s="24" t="str">
-        <f t="shared" ref="F35:F36" si="49">_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
-        <v>0xB080</v>
-      </c>
       <c r="G35" s="24">
-        <f t="shared" ref="G35:G36" si="50">HEX2DEC(MID(D35, 3, LEN(D35)-2))</f>
+        <f t="shared" ref="G35" si="49">HEX2DEC(MID(D35, 3, LEN(D35)-2))</f>
+        <v>43008</v>
+      </c>
+      <c r="H35" s="24">
+        <f t="shared" ref="H35" si="50">HEX2DEC(MID(E35, 3, LEN(E35)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I35" s="24">
+        <f t="shared" ref="I35" si="51">G35+H35</f>
         <v>45056</v>
       </c>
-      <c r="H35" s="24">
-        <f t="shared" ref="H35:H36" si="51">HEX2DEC(MID(E35, 3, LEN(E35)-2))</f>
-        <v>128</v>
-      </c>
-      <c r="I35" s="24">
-        <f t="shared" ref="I35:I36" si="52">G35+H35</f>
-        <v>45184</v>
-      </c>
       <c r="J35" s="24" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="L35" s="30" t="s">
         <v>139</v>
@@ -2548,63 +2554,65 @@
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="25"/>
-      <c r="C36" s="39"/>
-      <c r="D36" s="28" t="str">
+      <c r="C36" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="24" t="str">
         <f t="shared" si="1"/>
+        <v>0xB000</v>
+      </c>
+      <c r="E36" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M35))</f>
+        <v>0x80</v>
+      </c>
+      <c r="F36" s="24" t="str">
+        <f t="shared" ref="F36:F37" si="52">_xlfn.CONCAT("0x",DEC2HEX(I36))</f>
         <v>0xB080</v>
       </c>
-      <c r="E36" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="F36" s="28" t="str">
-        <f t="shared" si="49"/>
-        <v>0xB400</v>
-      </c>
-      <c r="G36" s="28">
-        <f t="shared" si="50"/>
+      <c r="G36" s="24">
+        <f t="shared" ref="G36:G37" si="53">HEX2DEC(MID(D36, 3, LEN(D36)-2))</f>
+        <v>45056</v>
+      </c>
+      <c r="H36" s="24">
+        <f t="shared" ref="H36:H37" si="54">HEX2DEC(MID(E36, 3, LEN(E36)-2))</f>
+        <v>128</v>
+      </c>
+      <c r="I36" s="24">
+        <f t="shared" ref="I36:I37" si="55">G36+H36</f>
         <v>45184</v>
       </c>
-      <c r="H36" s="28">
-        <f t="shared" si="51"/>
-        <v>896</v>
-      </c>
-      <c r="I36" s="28">
-        <f t="shared" si="52"/>
-        <v>46080</v>
-      </c>
-      <c r="J36" s="28" t="s">
-        <v>30</v>
+      <c r="J36" s="24" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" s="25"/>
       <c r="C37" s="39"/>
-      <c r="D37" s="24" t="str">
-        <f t="shared" ref="D37:D38" si="53">F36</f>
+      <c r="D37" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB080</v>
+      </c>
+      <c r="E37" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="F37" s="28" t="str">
+        <f t="shared" si="52"/>
         <v>0xB400</v>
       </c>
-      <c r="E37" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M48))</f>
-        <v>0x4</v>
-      </c>
-      <c r="F37" s="24" t="str">
-        <f t="shared" ref="F37:F38" si="54">_xlfn.CONCAT("0x",DEC2HEX(I37))</f>
-        <v>0xB404</v>
-      </c>
-      <c r="G37" s="24">
-        <f t="shared" ref="G37:G38" si="55">HEX2DEC(MID(D37, 3, LEN(D37)-2))</f>
+      <c r="G37" s="28">
+        <f t="shared" si="53"/>
+        <v>45184</v>
+      </c>
+      <c r="H37" s="28">
+        <f t="shared" si="54"/>
+        <v>896</v>
+      </c>
+      <c r="I37" s="28">
+        <f t="shared" si="55"/>
         <v>46080</v>
       </c>
-      <c r="H37" s="24">
-        <f t="shared" ref="H37:H38" si="56">HEX2DEC(MID(E37, 3, LEN(E37)-2))</f>
-        <v>4</v>
-      </c>
-      <c r="I37" s="24">
-        <f t="shared" ref="I37:I38" si="57">G37+H37</f>
-        <v>46084</v>
-      </c>
-      <c r="J37" s="24" t="s">
-        <v>91</v>
+      <c r="J37" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L37" s="21" t="s">
         <v>73</v>
@@ -2616,31 +2624,32 @@
     <row r="38" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B38" s="25"/>
       <c r="C38" s="39"/>
-      <c r="D38" s="28" t="str">
-        <f t="shared" si="53"/>
+      <c r="D38" s="24" t="str">
+        <f t="shared" ref="D38:D39" si="56">F37</f>
+        <v>0xB400</v>
+      </c>
+      <c r="E38" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M48))</f>
+        <v>0x4</v>
+      </c>
+      <c r="F38" s="24" t="str">
+        <f t="shared" ref="F38:F39" si="57">_xlfn.CONCAT("0x",DEC2HEX(I38))</f>
         <v>0xB404</v>
       </c>
-      <c r="E38" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="F38" s="28" t="str">
-        <f t="shared" si="54"/>
-        <v>0xB800</v>
-      </c>
-      <c r="G38" s="28">
-        <f t="shared" si="55"/>
+      <c r="G38" s="24">
+        <f t="shared" ref="G38:G39" si="58">HEX2DEC(MID(D38, 3, LEN(D38)-2))</f>
+        <v>46080</v>
+      </c>
+      <c r="H38" s="24">
+        <f t="shared" ref="H38:H39" si="59">HEX2DEC(MID(E38, 3, LEN(E38)-2))</f>
+        <v>4</v>
+      </c>
+      <c r="I38" s="24">
+        <f t="shared" ref="I38:I39" si="60">G38+H38</f>
         <v>46084</v>
       </c>
-      <c r="H38" s="28">
-        <f t="shared" si="56"/>
-        <v>1020</v>
-      </c>
-      <c r="I38" s="28">
-        <f t="shared" si="57"/>
-        <v>47104</v>
-      </c>
-      <c r="J38" s="28" t="s">
-        <v>30</v>
+      <c r="J38" s="24" t="s">
+        <v>91</v>
       </c>
       <c r="L38" s="19" t="s">
         <v>80</v>
@@ -2651,71 +2660,69 @@
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" s="25"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="24" t="str">
-        <f>F38</f>
+      <c r="C39" s="39"/>
+      <c r="D39" s="28" t="str">
+        <f t="shared" si="56"/>
+        <v>0xB404</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="F39" s="28" t="str">
+        <f t="shared" si="57"/>
         <v>0xB800</v>
       </c>
-      <c r="E39" s="24" t="str">
+      <c r="G39" s="28">
+        <f t="shared" si="58"/>
+        <v>46084</v>
+      </c>
+      <c r="H39" s="28">
+        <f t="shared" si="59"/>
+        <v>1020</v>
+      </c>
+      <c r="I39" s="28">
+        <f t="shared" si="60"/>
+        <v>47104</v>
+      </c>
+      <c r="J39" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="L39" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="M39" s="19">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B40" s="25"/>
+      <c r="C40" s="40"/>
+      <c r="D40" s="24" t="str">
+        <f>F39</f>
+        <v>0xB800</v>
+      </c>
+      <c r="E40" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M42))</f>
         <v>0x800</v>
       </c>
-      <c r="F39" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I39))</f>
-        <v>0xC000</v>
-      </c>
-      <c r="G39" s="24">
-        <f t="shared" ref="G39:H41" si="58">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
-        <v>47104</v>
-      </c>
-      <c r="H39" s="24">
-        <f t="shared" si="58"/>
-        <v>2048</v>
-      </c>
-      <c r="I39" s="24">
-        <f>G39+H39</f>
-        <v>49152</v>
-      </c>
-      <c r="J39" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="L39" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="M39" s="19">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B40" s="41"/>
-      <c r="C40" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="D40" s="24" t="str">
-        <f>F39</f>
-        <v>0xC000</v>
-      </c>
-      <c r="E40" s="24" t="s">
-        <v>6</v>
-      </c>
       <c r="F40" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
-        <v>0x10000</v>
+        <v>0xC000</v>
       </c>
       <c r="G40" s="24">
-        <f t="shared" si="58"/>
-        <v>49152</v>
+        <f t="shared" ref="G40:H42" si="61">HEX2DEC(MID(D40, 3, LEN(D40)-2))</f>
+        <v>47104</v>
       </c>
       <c r="H40" s="24">
-        <f t="shared" si="58"/>
-        <v>16384</v>
+        <f t="shared" si="61"/>
+        <v>2048</v>
       </c>
       <c r="I40" s="24">
         <f>G40+H40</f>
-        <v>65536</v>
+        <v>49152</v>
       </c>
       <c r="J40" s="24" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="L40" s="29" t="s">
         <v>75</v>
@@ -2725,38 +2732,35 @@
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B41" s="43" t="s">
-        <v>144</v>
-      </c>
-      <c r="C41" s="45" t="s">
-        <v>55</v>
+      <c r="B41" s="41"/>
+      <c r="C41" s="42" t="s">
+        <v>49</v>
       </c>
       <c r="D41" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v>0x10000</v>
-      </c>
-      <c r="E41" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M13))</f>
-        <v>0x100</v>
+        <f>F40</f>
+        <v>0xC000</v>
+      </c>
+      <c r="E41" s="24" t="s">
+        <v>6</v>
       </c>
       <c r="F41" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I41))</f>
-        <v>0x10100</v>
+        <v>0x10000</v>
       </c>
       <c r="G41" s="24">
-        <f t="shared" si="58"/>
-        <v>65536</v>
+        <f t="shared" si="61"/>
+        <v>49152</v>
       </c>
       <c r="H41" s="24">
-        <f t="shared" si="58"/>
-        <v>256</v>
+        <f t="shared" si="61"/>
+        <v>16384</v>
       </c>
       <c r="I41" s="24">
         <f>G41+H41</f>
-        <v>65792</v>
+        <v>65536</v>
       </c>
       <c r="J41" s="24" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="L41" s="19" t="s">
         <v>148</v>
@@ -2767,8 +2771,38 @@
       </c>
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B42" s="44" t="s">
-        <v>143</v>
+      <c r="B42" s="43" t="s">
+        <v>144</v>
+      </c>
+      <c r="C42" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>0x10000</v>
+      </c>
+      <c r="E42" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M13))</f>
+        <v>0x100</v>
+      </c>
+      <c r="F42" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I42))</f>
+        <v>0x10100</v>
+      </c>
+      <c r="G42" s="24">
+        <f t="shared" si="61"/>
+        <v>65536</v>
+      </c>
+      <c r="H42" s="24">
+        <f t="shared" si="61"/>
+        <v>256</v>
+      </c>
+      <c r="I42" s="24">
+        <f>G42+H42</f>
+        <v>65792</v>
+      </c>
+      <c r="J42" s="24" t="s">
+        <v>54</v>
       </c>
       <c r="L42" s="19" t="s">
         <v>147</v>
@@ -2778,63 +2812,47 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="43" spans="2:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="B43" s="44"/>
-      <c r="C43"/>
-      <c r="D43"/>
-      <c r="E43"/>
-      <c r="F43"/>
-      <c r="G43"/>
-      <c r="H43"/>
-      <c r="I43"/>
-      <c r="J43"/>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B43" s="44" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B44" s="44"/>
-      <c r="C44" s="38" t="s">
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="L44" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="M44" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B45" s="44"/>
+      <c r="C45" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="D44" s="24"/>
-      <c r="E44" s="24" t="str">
+      <c r="D45" s="24"/>
+      <c r="E45" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
         <v>0x4000</v>
-      </c>
-      <c r="F44" s="24"/>
-      <c r="G44" s="24"/>
-      <c r="H44" s="24">
-        <f>HEX2DEC(MID(E44, 3, LEN(E44)-2))</f>
-        <v>16384</v>
-      </c>
-      <c r="I44" s="24"/>
-      <c r="J44" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="L44" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="M44" s="19" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B45" s="44"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M54))</f>
-        <v>0x800</v>
       </c>
       <c r="F45" s="24"/>
       <c r="G45" s="24"/>
       <c r="H45" s="24">
         <f>HEX2DEC(MID(E45, 3, LEN(E45)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I45" s="24" t="s">
-        <v>161</v>
-      </c>
+        <v>16384</v>
+      </c>
+      <c r="I45" s="24"/>
       <c r="J45" s="24" t="s">
-        <v>134</v>
+        <v>51</v>
       </c>
       <c r="L45" s="19" t="s">
         <v>62</v>
@@ -2845,6 +2863,24 @@
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B46" s="44"/>
+      <c r="C46" s="40"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M54))</f>
+        <v>0x800</v>
+      </c>
+      <c r="F46" s="24"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="24">
+        <f>HEX2DEC(MID(E46, 3, LEN(E46)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I46" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="J46" s="24" t="s">
+        <v>134</v>
+      </c>
       <c r="L46" s="29" t="s">
         <v>4</v>
       </c>
@@ -2864,23 +2900,6 @@
     </row>
     <row r="48" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B48" s="44"/>
-      <c r="C48" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24">
-        <f t="shared" ref="H48" si="59">HEX2DEC(MID(E48, 3, LEN(E48)-2))</f>
-        <v>131072</v>
-      </c>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24" t="s">
-        <v>155</v>
-      </c>
       <c r="L48" s="19" t="s">
         <v>139</v>
       </c>
@@ -2891,6 +2910,23 @@
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B49" s="44"/>
+      <c r="C49" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="F49" s="24"/>
+      <c r="G49" s="24"/>
+      <c r="H49" s="24">
+        <f t="shared" ref="H49" si="62">HEX2DEC(MID(E49, 3, LEN(E49)-2))</f>
+        <v>131072</v>
+      </c>
+      <c r="I49" s="24"/>
+      <c r="J49" s="24" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B50" s="44"/>
@@ -2980,7 +3016,10 @@
       <c r="B63" s="44"/>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B64" s="46"/>
+      <c r="B64" s="44"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Working audio, better level end, various improvements
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99866AE2-C3D5-4CBC-A6DE-D85230060CE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA31142-140D-4555-81D5-7CE7CEA7C88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware" sheetId="1" r:id="rId1"/>
     <sheet name="Casval" sheetId="2" r:id="rId2"/>
+    <sheet name="Sound" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="SCREEN_BORDER_WIDTH">Hardware!$M$3</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="178">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -571,15 +572,9 @@
     <t>Deikun (Sound system)</t>
   </si>
   <si>
-    <t>Sound RAM (YM2419)</t>
-  </si>
-  <si>
     <t>0x04E0</t>
   </si>
   <si>
-    <t>Music RAM (YM Player)</t>
-  </si>
-  <si>
     <t>0x20000</t>
   </si>
   <si>
@@ -617,6 +612,27 @@
   </si>
   <si>
     <t>0x00CF</t>
+  </si>
+  <si>
+    <t>Sound ROM</t>
+  </si>
+  <si>
+    <t>0x10000</t>
+  </si>
+  <si>
+    <t>Sound RAM (OKI M5205)</t>
+  </si>
+  <si>
+    <t>Music RAM (YM2149 Player)</t>
+  </si>
+  <si>
+    <t>Target freq</t>
+  </si>
+  <si>
+    <t>Clock</t>
+  </si>
+  <si>
+    <t>Ce_6</t>
   </si>
 </sst>
 </file>
@@ -1288,8 +1304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="B1:P65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28:J28"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1966,7 +1982,7 @@
         <v>8</v>
       </c>
       <c r="N19" s="19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
@@ -2241,10 +2257,10 @@
         <v>35377</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="M27" s="19">
         <v>1</v>
@@ -2258,7 +2274,7 @@
         <v>0x8A31</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F28" s="28" t="str">
         <f t="shared" ref="F28" si="34">_xlfn.CONCAT("0x",DEC2HEX(I28))</f>
@@ -2280,7 +2296,7 @@
         <v>30</v>
       </c>
       <c r="L28" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="M28" s="19">
         <v>2</v>
@@ -2315,10 +2331,10 @@
         <v>35600</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c r="L29" s="48" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M29" s="48">
         <v>0</v>
@@ -2351,7 +2367,7 @@
         <v>35616</v>
       </c>
       <c r="J30" s="24" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="L30" s="32" t="s">
         <v>72</v>
@@ -2360,7 +2376,7 @@
         <v>12</v>
       </c>
       <c r="N30" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
@@ -2371,7 +2387,7 @@
         <v>0x8B20</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F31" s="28" t="str">
         <f t="shared" ref="F31" si="40">_xlfn.CONCAT("0x",DEC2HEX(I31))</f>
@@ -2437,7 +2453,7 @@
         <v>10</v>
       </c>
       <c r="N32" s="19" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2876,7 +2892,7 @@
         <v>2048</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="J46" s="24" t="s">
         <v>134</v>
@@ -2915,7 +2931,7 @@
       </c>
       <c r="D49" s="24"/>
       <c r="E49" s="24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F49" s="24"/>
       <c r="G49" s="24"/>
@@ -2930,6 +2946,23 @@
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B50" s="44"/>
+      <c r="C50" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24" t="s">
+        <v>172</v>
+      </c>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="24">
+        <f t="shared" ref="H50" si="63">HEX2DEC(MID(E50, 3, LEN(E50)-2))</f>
+        <v>65536</v>
+      </c>
+      <c r="I50" s="24"/>
+      <c r="J50" s="24" t="s">
+        <v>171</v>
+      </c>
       <c r="L50" s="21" t="s">
         <v>134</v>
       </c>
@@ -3230,26 +3263,72 @@
         <v>118</v>
       </c>
       <c r="I21" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I23" s="47" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F91CF3-5A37-48D2-99AF-2EE65E2968D7}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>375</v>
+      </c>
+      <c r="B2">
+        <v>24000000</v>
+      </c>
+      <c r="C2">
+        <f>B2/4</f>
+        <v>6000000</v>
+      </c>
+      <c r="D2">
+        <f>C2/A2</f>
+        <v>16000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Too much stuff I forgot to commit
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA31142-140D-4555-81D5-7CE7CEA7C88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2F3124-9AE0-4516-9281-C7970DAEFCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware" sheetId="1" r:id="rId1"/>
@@ -1304,7 +1304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="B1:P65"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
@@ -3291,8 +3291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2F91CF3-5A37-48D2-99AF-2EE65E2968D7}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Insane variable sprite size update finally complete
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA2F3124-9AE0-4516-9281-C7970DAEFCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD93B93B-2C93-467E-AD28-80B3C1AEBC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Hardware" sheetId="1" r:id="rId1"/>
     <sheet name="Casval" sheetId="2" r:id="rId2"/>
     <sheet name="Sound" sheetId="3" r:id="rId3"/>
+    <sheet name="Tilemap" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="SCREEN_BORDER_WIDTH">Hardware!$M$3</definedName>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="190">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -572,9 +573,6 @@
     <t>Deikun (Sound system)</t>
   </si>
   <si>
-    <t>0x04E0</t>
-  </si>
-  <si>
     <t>0x20000</t>
   </si>
   <si>
@@ -605,9 +603,6 @@
     <t>SPRITE_PALETTE_INDEX</t>
   </si>
   <si>
-    <t>This really only needs 9 bits?</t>
-  </si>
-  <si>
     <t>System pause trigger</t>
   </si>
   <si>
@@ -633,6 +628,48 @@
   </si>
   <si>
     <t>Ce_6</t>
+  </si>
+  <si>
+    <t>tile size x</t>
+  </si>
+  <si>
+    <t>tile size y</t>
+  </si>
+  <si>
+    <t>Char ROM Data</t>
+  </si>
+  <si>
+    <t>CHAR_ROM_COUNT</t>
+  </si>
+  <si>
+    <t>CHAR_ROM_WIDTH</t>
+  </si>
+  <si>
+    <t>CHAR_ROM_HEIGHT</t>
+  </si>
+  <si>
+    <t>CHAR_ROM_COLOUR_DEPTH</t>
+  </si>
+  <si>
+    <t>CHAR_ROM_BITS_PER</t>
+  </si>
+  <si>
+    <t>CHAR_ROM_BYTES_PER</t>
+  </si>
+  <si>
+    <t>CHAR_ROM_BYTES_TOTAL</t>
+  </si>
+  <si>
+    <t>0x00E0</t>
+  </si>
+  <si>
+    <t>0x0400</t>
+  </si>
+  <si>
+    <t>(Tile map)</t>
+  </si>
+  <si>
+    <t>SPRITE_SIZE</t>
   </si>
 </sst>
 </file>
@@ -707,6 +744,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <i/>
       <sz val="10"/>
       <color theme="1"/>
@@ -870,7 +908,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -936,13 +974,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -981,11 +1013,20 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1302,10 +1343,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
-  <dimension ref="B1:P65"/>
+  <dimension ref="B1:P67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1415,7 +1456,7 @@
         <v>44</v>
       </c>
       <c r="D4" s="24" t="str">
-        <f t="shared" ref="D4:D42" si="1">F3</f>
+        <f t="shared" ref="D4:D44" si="1">F3</f>
         <v>0x8000</v>
       </c>
       <c r="E4" s="24" t="s">
@@ -1547,7 +1588,7 @@
         <v>30</v>
       </c>
       <c r="L7" s="21" t="s">
-        <v>55</v>
+        <v>178</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
@@ -1580,10 +1621,10 @@
         <v>27</v>
       </c>
       <c r="L8" s="29" t="s">
-        <v>58</v>
+        <v>179</v>
       </c>
       <c r="M8" s="29">
-        <v>4</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
@@ -1616,13 +1657,10 @@
         <v>30</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>52</v>
+        <v>180</v>
       </c>
       <c r="M9" s="19">
-        <v>16</v>
-      </c>
-      <c r="N9" s="19" t="s">
-        <v>82</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
@@ -1655,10 +1693,10 @@
         <v>26</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>53</v>
+        <v>181</v>
       </c>
       <c r="M10" s="19">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
@@ -1690,12 +1728,11 @@
       <c r="J11" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L11" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="M11" s="30">
-        <f>M9*M10</f>
-        <v>512</v>
+      <c r="L11" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="M11" s="19">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
@@ -1727,11 +1764,11 @@
       <c r="J12" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="M12" s="19">
-        <f>M11/8</f>
+      <c r="L12" s="30" t="s">
+        <v>183</v>
+      </c>
+      <c r="M12" s="30">
+        <f>M9*M10*M11</f>
         <v>64</v>
       </c>
     </row>
@@ -1764,12 +1801,12 @@
       <c r="J13" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L13" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="M13" s="30">
-        <f>M12*M8</f>
-        <v>256</v>
+      <c r="L13" s="19" t="s">
+        <v>184</v>
+      </c>
+      <c r="M13" s="19">
+        <f>M12/8</f>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
@@ -1801,6 +1838,13 @@
       <c r="J14" s="24" t="s">
         <v>24</v>
       </c>
+      <c r="L14" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="M14" s="30">
+        <f>M8*M13</f>
+        <v>2048</v>
+      </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B15" s="25"/>
@@ -1831,12 +1875,6 @@
       <c r="J15" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L15" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="N15" s="19" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B16" s="25"/>
@@ -1867,11 +1905,8 @@
       <c r="J16" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="L16" s="29" t="s">
-        <v>65</v>
-      </c>
-      <c r="M16" s="29">
-        <v>64</v>
+      <c r="L16" s="21" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
@@ -1903,11 +1938,11 @@
       <c r="J17" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L17" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="M17" s="19">
-        <v>16</v>
+      <c r="L17" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="M17" s="29">
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
@@ -1940,10 +1975,13 @@
         <v>22</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="M18" s="19">
         <v>16</v>
+      </c>
+      <c r="N18" s="19" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
@@ -1976,13 +2014,10 @@
         <v>30</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="M19" s="19">
-        <v>8</v>
-      </c>
-      <c r="N19" s="19" t="s">
-        <v>166</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
@@ -2000,7 +2035,7 @@
         <v>0x8821</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" ref="G20:H32" si="25">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
+        <f t="shared" ref="G20:H34" si="25">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
         <v>34816</v>
       </c>
       <c r="H20" s="24">
@@ -2015,11 +2050,11 @@
         <v>21</v>
       </c>
       <c r="L20" s="30" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="M20" s="30">
-        <f>M17*M18*M19</f>
-        <v>2048</v>
+        <f>M18*M19</f>
+        <v>512</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
@@ -2052,11 +2087,11 @@
         <v>30</v>
       </c>
       <c r="L21" s="19" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="M21" s="19">
         <f>M20/8</f>
-        <v>256</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
@@ -2089,11 +2124,11 @@
         <v>20</v>
       </c>
       <c r="L22" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M22" s="30">
-        <f>M16*M21</f>
-        <v>16384</v>
+        <f>M21*M17</f>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
@@ -2155,14 +2190,17 @@
         <v>90</v>
       </c>
       <c r="L24" s="21" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="N24" s="19" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="25"/>
-      <c r="C25" s="50"/>
+      <c r="C25" s="48"/>
       <c r="D25" s="24" t="str">
-        <f t="shared" ref="D25:D31" si="29">F24</f>
+        <f t="shared" ref="D25:D30" si="29">F24</f>
         <v>0x8A10</v>
       </c>
       <c r="E25" s="24" t="s">
@@ -2188,15 +2226,15 @@
         <v>88</v>
       </c>
       <c r="L25" s="29" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="M25" s="29">
-        <v>32</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="25"/>
-      <c r="C26" s="50"/>
+      <c r="C26" s="48"/>
       <c r="D26" s="24" t="str">
         <f t="shared" si="29"/>
         <v>0x8A20</v>
@@ -2223,16 +2261,16 @@
       <c r="J26" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="L26" s="32" t="s">
-        <v>79</v>
+      <c r="L26" s="19" t="s">
+        <v>66</v>
       </c>
       <c r="M26" s="19">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="25"/>
-      <c r="C27" s="49"/>
+      <c r="C27" s="46"/>
       <c r="D27" s="24" t="str">
         <f>F26</f>
         <v>0x8A30</v>
@@ -2257,13 +2295,13 @@
         <v>35377</v>
       </c>
       <c r="J27" s="24" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>164</v>
+        <v>67</v>
       </c>
       <c r="M27" s="19">
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
@@ -2274,7 +2312,7 @@
         <v>0x8A31</v>
       </c>
       <c r="E28" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F28" s="28" t="str">
         <f t="shared" ref="F28" si="34">_xlfn.CONCAT("0x",DEC2HEX(I28))</f>
@@ -2296,15 +2334,18 @@
         <v>30</v>
       </c>
       <c r="L28" s="19" t="s">
-        <v>167</v>
+        <v>68</v>
       </c>
       <c r="M28" s="19">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="N28" s="19" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="25"/>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="49" t="s">
         <v>156</v>
       </c>
       <c r="D29" s="24" t="str">
@@ -2331,18 +2372,19 @@
         <v>35600</v>
       </c>
       <c r="J29" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="L29" s="48" t="s">
-        <v>165</v>
-      </c>
-      <c r="M29" s="48">
-        <v>0</v>
+        <v>171</v>
+      </c>
+      <c r="L29" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="M29" s="30">
+        <f>M26*M27*M28</f>
+        <v>2048</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="25"/>
-      <c r="C30" s="31"/>
+      <c r="C30" s="48"/>
       <c r="D30" s="24" t="str">
         <f t="shared" si="29"/>
         <v>0x8B10</v>
@@ -2367,308 +2409,293 @@
         <v>35616</v>
       </c>
       <c r="J30" s="24" t="s">
-        <v>174</v>
-      </c>
-      <c r="L30" s="32" t="s">
-        <v>72</v>
+        <v>172</v>
+      </c>
+      <c r="L30" s="19" t="s">
+        <v>70</v>
       </c>
       <c r="M30" s="19">
-        <v>12</v>
-      </c>
-      <c r="N30" s="19" t="s">
-        <v>168</v>
+        <f>M29/8</f>
+        <v>256</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" s="25"/>
-      <c r="C31" s="33"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="28" t="str">
-        <f t="shared" si="29"/>
+        <f>F30</f>
         <v>0x8B20</v>
       </c>
       <c r="E31" s="28" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="F31" s="28" t="str">
         <f t="shared" ref="F31" si="40">_xlfn.CONCAT("0x",DEC2HEX(I31))</f>
-        <v>0x9000</v>
+        <v>0x8C00</v>
       </c>
       <c r="G31" s="28">
-        <f t="shared" ref="G31" si="41">HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
+        <f t="shared" ref="G31:G33" si="41">HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
         <v>35616</v>
       </c>
       <c r="H31" s="28">
-        <f t="shared" ref="H31" si="42">HEX2DEC(MID(E31, 3, LEN(E31)-2))</f>
-        <v>1248</v>
+        <f t="shared" ref="H31:H33" si="42">HEX2DEC(MID(E31, 3, LEN(E31)-2))</f>
+        <v>224</v>
       </c>
       <c r="I31" s="28">
         <f t="shared" ref="I31" si="43">G31+H31</f>
-        <v>36864</v>
+        <v>35840</v>
       </c>
       <c r="J31" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L31" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="M31" s="19">
-        <v>6</v>
+      <c r="L31" s="30" t="s">
+        <v>146</v>
+      </c>
+      <c r="M31" s="30">
+        <f>M25*M30</f>
+        <v>16384</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B32" s="25"/>
-      <c r="C32" s="34" t="s">
-        <v>48</v>
+      <c r="C32" s="50" t="s">
+        <v>188</v>
       </c>
       <c r="D32" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v>0x9000</v>
+        <f>F30</f>
+        <v>0x8B20</v>
       </c>
       <c r="E32" s="24" t="s">
-        <v>8</v>
+        <v>187</v>
       </c>
       <c r="F32" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
-        <v>0x9800</v>
+        <v>0x8D20</v>
       </c>
       <c r="G32" s="24">
-        <f>HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
-        <v>36864</v>
+        <f t="shared" ref="G32" si="44">HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
+        <v>35616</v>
       </c>
       <c r="H32" s="24">
+        <v>512</v>
+      </c>
+      <c r="I32" s="24">
+        <f>G32+H32</f>
+        <v>36128</v>
+      </c>
+      <c r="J32" s="24"/>
+    </row>
+    <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="25"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="24" t="str">
+        <f>F32</f>
+        <v>0x8D20</v>
+      </c>
+      <c r="E33" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="F33" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
+        <v>0x9120</v>
+      </c>
+      <c r="G33" s="24">
+        <f t="shared" si="41"/>
+        <v>36128</v>
+      </c>
+      <c r="H33" s="24">
+        <f t="shared" si="42"/>
+        <v>1024</v>
+      </c>
+      <c r="I33" s="24">
+        <f>G33+H33</f>
+        <v>37152</v>
+      </c>
+      <c r="J33" s="24"/>
+      <c r="L33" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B34" s="25"/>
+      <c r="C34" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" s="24" t="str">
+        <f>F33</f>
+        <v>0x9120</v>
+      </c>
+      <c r="E34" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
+        <v>0x9920</v>
+      </c>
+      <c r="G34" s="24">
+        <f>HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
+        <v>37152</v>
+      </c>
+      <c r="H34" s="24">
         <f t="shared" si="25"/>
         <v>2048</v>
       </c>
-      <c r="I32" s="24">
-        <f>G32+H32</f>
-        <v>38912</v>
-      </c>
-      <c r="J32" s="24" t="s">
+      <c r="I34" s="24">
+        <f>G34+H34</f>
+        <v>39200</v>
+      </c>
+      <c r="J34" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="L32" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="M32" s="19">
-        <v>10</v>
-      </c>
-      <c r="N32" s="19" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="25"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v>0x9800</v>
-      </c>
-      <c r="E33" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
-        <v>0xA000</v>
-      </c>
-      <c r="G33" s="24">
-        <f>HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
-        <v>38912</v>
-      </c>
-      <c r="H33" s="24">
-        <f>HEX2DEC(MID(E33, 3, LEN(E33)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I33" s="24">
-        <f>G33+H33</f>
-        <v>40960</v>
-      </c>
-      <c r="J33" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="L33" s="30" t="s">
-        <v>4</v>
-      </c>
-      <c r="M33" s="30">
-        <f>SUM(M26:M32)</f>
+      <c r="L34" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="M34" s="29">
         <v>32</v>
-      </c>
-      <c r="N33" s="35"/>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B34" s="25"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v>0xA000</v>
-      </c>
-      <c r="E34" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="24" t="str">
-        <f t="shared" ref="F34" si="44">_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
-        <v>0xA800</v>
-      </c>
-      <c r="G34" s="24">
-        <f t="shared" ref="G34" si="45">HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
-        <v>40960</v>
-      </c>
-      <c r="H34" s="24">
-        <f t="shared" ref="H34" si="46">HEX2DEC(MID(E34, 3, LEN(E34)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I34" s="24">
-        <f t="shared" ref="I34" si="47">G34+H34</f>
-        <v>43008</v>
-      </c>
-      <c r="J34" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="L34" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="M34" s="19">
-        <f>M33/8</f>
-        <v>4</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B35" s="25"/>
-      <c r="C35" s="37"/>
+      <c r="C35" s="34"/>
       <c r="D35" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0xA800</v>
+        <v>0x9920</v>
       </c>
       <c r="E35" s="24" t="s">
         <v>8</v>
       </c>
       <c r="F35" s="24" t="str">
-        <f t="shared" ref="F35" si="48">_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
-        <v>0xB000</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
+        <v>0xA120</v>
       </c>
       <c r="G35" s="24">
-        <f t="shared" ref="G35" si="49">HEX2DEC(MID(D35, 3, LEN(D35)-2))</f>
-        <v>43008</v>
+        <f>HEX2DEC(MID(D35, 3, LEN(D35)-2))</f>
+        <v>39200</v>
       </c>
       <c r="H35" s="24">
-        <f t="shared" ref="H35" si="50">HEX2DEC(MID(E35, 3, LEN(E35)-2))</f>
+        <f>HEX2DEC(MID(E35, 3, LEN(E35)-2))</f>
         <v>2048</v>
       </c>
       <c r="I35" s="24">
-        <f t="shared" ref="I35" si="51">G35+H35</f>
-        <v>45056</v>
+        <f>G35+H35</f>
+        <v>41248</v>
       </c>
       <c r="J35" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="L35" s="30" t="s">
-        <v>139</v>
-      </c>
-      <c r="M35" s="30">
-        <f>M25*M34</f>
-        <v>128</v>
+        <v>46</v>
+      </c>
+      <c r="L35" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="M35" s="19">
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="25"/>
-      <c r="C36" s="38" t="s">
-        <v>56</v>
-      </c>
+      <c r="C36" s="34"/>
       <c r="D36" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0xB000</v>
-      </c>
-      <c r="E36" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M35))</f>
-        <v>0x80</v>
+        <v>0xA120</v>
+      </c>
+      <c r="E36" s="24" t="s">
+        <v>8</v>
       </c>
       <c r="F36" s="24" t="str">
-        <f t="shared" ref="F36:F37" si="52">_xlfn.CONCAT("0x",DEC2HEX(I36))</f>
-        <v>0xB080</v>
+        <f t="shared" ref="F36" si="45">_xlfn.CONCAT("0x",DEC2HEX(I36))</f>
+        <v>0xA920</v>
       </c>
       <c r="G36" s="24">
-        <f t="shared" ref="G36:G37" si="53">HEX2DEC(MID(D36, 3, LEN(D36)-2))</f>
-        <v>45056</v>
+        <f t="shared" ref="G36" si="46">HEX2DEC(MID(D36, 3, LEN(D36)-2))</f>
+        <v>41248</v>
       </c>
       <c r="H36" s="24">
-        <f t="shared" ref="H36:H37" si="54">HEX2DEC(MID(E36, 3, LEN(E36)-2))</f>
-        <v>128</v>
+        <f t="shared" ref="H36" si="47">HEX2DEC(MID(E36, 3, LEN(E36)-2))</f>
+        <v>2048</v>
       </c>
       <c r="I36" s="24">
-        <f t="shared" ref="I36:I37" si="55">G36+H36</f>
-        <v>45184</v>
+        <f t="shared" ref="I36" si="48">G36+H36</f>
+        <v>43296</v>
       </c>
       <c r="J36" s="24" t="s">
-        <v>57</v>
+        <v>45</v>
+      </c>
+      <c r="L36" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="M36" s="19">
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" s="25"/>
-      <c r="C37" s="39"/>
-      <c r="D37" s="28" t="str">
+      <c r="C37" s="35"/>
+      <c r="D37" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0xB080</v>
-      </c>
-      <c r="E37" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="F37" s="28" t="str">
-        <f t="shared" si="52"/>
-        <v>0xB400</v>
-      </c>
-      <c r="G37" s="28">
-        <f t="shared" si="53"/>
-        <v>45184</v>
-      </c>
-      <c r="H37" s="28">
-        <f t="shared" si="54"/>
-        <v>896</v>
-      </c>
-      <c r="I37" s="28">
-        <f t="shared" si="55"/>
-        <v>46080</v>
-      </c>
-      <c r="J37" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L37" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="M37" s="19" t="s">
-        <v>136</v>
+        <v>0xA920</v>
+      </c>
+      <c r="E37" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="24" t="str">
+        <f t="shared" ref="F37" si="49">_xlfn.CONCAT("0x",DEC2HEX(I37))</f>
+        <v>0xB120</v>
+      </c>
+      <c r="G37" s="24">
+        <f t="shared" ref="G37" si="50">HEX2DEC(MID(D37, 3, LEN(D37)-2))</f>
+        <v>43296</v>
+      </c>
+      <c r="H37" s="24">
+        <f t="shared" ref="H37" si="51">HEX2DEC(MID(E37, 3, LEN(E37)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I37" s="24">
+        <f t="shared" ref="I37" si="52">G37+H37</f>
+        <v>45344</v>
+      </c>
+      <c r="J37" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="L37" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="M37" s="19">
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B38" s="25"/>
-      <c r="C38" s="39"/>
+      <c r="C38" s="36" t="s">
+        <v>56</v>
+      </c>
       <c r="D38" s="24" t="str">
-        <f t="shared" ref="D38:D39" si="56">F37</f>
-        <v>0xB400</v>
+        <f t="shared" si="1"/>
+        <v>0xB120</v>
       </c>
       <c r="E38" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M48))</f>
-        <v>0x4</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M46))</f>
+        <v>0x80</v>
       </c>
       <c r="F38" s="24" t="str">
-        <f t="shared" ref="F38:F39" si="57">_xlfn.CONCAT("0x",DEC2HEX(I38))</f>
-        <v>0xB404</v>
+        <f t="shared" ref="F38:F39" si="53">_xlfn.CONCAT("0x",DEC2HEX(I38))</f>
+        <v>0xB1A0</v>
       </c>
       <c r="G38" s="24">
-        <f t="shared" ref="G38:G39" si="58">HEX2DEC(MID(D38, 3, LEN(D38)-2))</f>
-        <v>46080</v>
+        <f t="shared" ref="G38:G39" si="54">HEX2DEC(MID(D38, 3, LEN(D38)-2))</f>
+        <v>45344</v>
       </c>
       <c r="H38" s="24">
-        <f t="shared" ref="H38:H39" si="59">HEX2DEC(MID(E38, 3, LEN(E38)-2))</f>
-        <v>4</v>
+        <f t="shared" ref="H38:H39" si="55">HEX2DEC(MID(E38, 3, LEN(E38)-2))</f>
+        <v>128</v>
       </c>
       <c r="I38" s="24">
-        <f t="shared" ref="I38:I39" si="60">G38+H38</f>
-        <v>46084</v>
+        <f t="shared" ref="I38:I39" si="56">G38+H38</f>
+        <v>45472</v>
       </c>
       <c r="J38" s="24" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="L38" s="19" t="s">
-        <v>80</v>
+        <v>189</v>
       </c>
       <c r="M38" s="19">
         <v>2</v>
@@ -2676,387 +2703,514 @@
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" s="25"/>
-      <c r="C39" s="39"/>
+      <c r="C39" s="37"/>
       <c r="D39" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB1A0</v>
+      </c>
+      <c r="E39" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="F39" s="28" t="str">
+        <f t="shared" si="53"/>
+        <v>0xB520</v>
+      </c>
+      <c r="G39" s="28">
+        <f t="shared" si="54"/>
+        <v>45472</v>
+      </c>
+      <c r="H39" s="28">
+        <f t="shared" si="55"/>
+        <v>896</v>
+      </c>
+      <c r="I39" s="28">
         <f t="shared" si="56"/>
-        <v>0xB404</v>
-      </c>
-      <c r="E39" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="F39" s="28" t="str">
-        <f t="shared" si="57"/>
-        <v>0xB800</v>
-      </c>
-      <c r="G39" s="28">
-        <f t="shared" si="58"/>
-        <v>46084</v>
-      </c>
-      <c r="H39" s="28">
-        <f t="shared" si="59"/>
-        <v>1020</v>
-      </c>
-      <c r="I39" s="28">
-        <f t="shared" si="60"/>
-        <v>47104</v>
+        <v>46368</v>
       </c>
       <c r="J39" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="L39" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="M39" s="19">
-        <v>512</v>
+      <c r="L39" s="47" t="s">
+        <v>164</v>
+      </c>
+      <c r="M39" s="47">
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B40" s="25"/>
-      <c r="C40" s="40"/>
+      <c r="C40" s="37"/>
       <c r="D40" s="24" t="str">
-        <f>F39</f>
-        <v>0xB800</v>
+        <f t="shared" ref="D40:D41" si="57">F39</f>
+        <v>0xB520</v>
       </c>
       <c r="E40" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M42))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M59))</f>
+        <v>0x4</v>
+      </c>
+      <c r="F40" s="24" t="str">
+        <f t="shared" ref="F40:F41" si="58">_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
+        <v>0xB524</v>
+      </c>
+      <c r="G40" s="24">
+        <f t="shared" ref="G40:G41" si="59">HEX2DEC(MID(D40, 3, LEN(D40)-2))</f>
+        <v>46368</v>
+      </c>
+      <c r="H40" s="24">
+        <f t="shared" ref="H40:H41" si="60">HEX2DEC(MID(E40, 3, LEN(E40)-2))</f>
+        <v>4</v>
+      </c>
+      <c r="I40" s="24">
+        <f t="shared" ref="I40:I41" si="61">G40+H40</f>
+        <v>46372</v>
+      </c>
+      <c r="J40" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="L40" s="31" t="s">
+        <v>72</v>
+      </c>
+      <c r="M40" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B41" s="25"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="28" t="str">
+        <f t="shared" si="57"/>
+        <v>0xB524</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="F41" s="28" t="str">
+        <f t="shared" si="58"/>
+        <v>0xB920</v>
+      </c>
+      <c r="G41" s="28">
+        <f t="shared" si="59"/>
+        <v>46372</v>
+      </c>
+      <c r="H41" s="28">
+        <f t="shared" si="60"/>
+        <v>1020</v>
+      </c>
+      <c r="I41" s="28">
+        <f t="shared" si="61"/>
+        <v>47392</v>
+      </c>
+      <c r="J41" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="L41" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="M41" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B42" s="25"/>
+      <c r="C42" s="38"/>
+      <c r="D42" s="24" t="str">
+        <f>F41</f>
+        <v>0xB920</v>
+      </c>
+      <c r="E42" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M53))</f>
         <v>0x800</v>
-      </c>
-      <c r="F40" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
-        <v>0xC000</v>
-      </c>
-      <c r="G40" s="24">
-        <f t="shared" ref="G40:H42" si="61">HEX2DEC(MID(D40, 3, LEN(D40)-2))</f>
-        <v>47104</v>
-      </c>
-      <c r="H40" s="24">
-        <f t="shared" si="61"/>
-        <v>2048</v>
-      </c>
-      <c r="I40" s="24">
-        <f>G40+H40</f>
-        <v>49152</v>
-      </c>
-      <c r="J40" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="L40" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="M40" s="29">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B41" s="41"/>
-      <c r="C41" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="D41" s="24" t="str">
-        <f>F40</f>
-        <v>0xC000</v>
-      </c>
-      <c r="E41" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I41))</f>
-        <v>0x10000</v>
-      </c>
-      <c r="G41" s="24">
-        <f t="shared" si="61"/>
-        <v>49152</v>
-      </c>
-      <c r="H41" s="24">
-        <f t="shared" si="61"/>
-        <v>16384</v>
-      </c>
-      <c r="I41" s="24">
-        <f>G41+H41</f>
-        <v>65536</v>
-      </c>
-      <c r="J41" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="L41" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="M41" s="19">
-        <f>M38*M39*M40</f>
-        <v>16384</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B42" s="43" t="s">
-        <v>144</v>
-      </c>
-      <c r="C42" s="45" t="s">
-        <v>55</v>
-      </c>
-      <c r="D42" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v>0x10000</v>
-      </c>
-      <c r="E42" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M13))</f>
-        <v>0x100</v>
       </c>
       <c r="F42" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I42))</f>
-        <v>0x10100</v>
+        <v>0xC120</v>
       </c>
       <c r="G42" s="24">
-        <f t="shared" si="61"/>
-        <v>65536</v>
+        <f t="shared" ref="G42:H44" si="62">HEX2DEC(MID(D42, 3, LEN(D42)-2))</f>
+        <v>47392</v>
       </c>
       <c r="H42" s="24">
-        <f t="shared" si="61"/>
-        <v>256</v>
+        <f t="shared" si="62"/>
+        <v>2048</v>
       </c>
       <c r="I42" s="24">
         <f>G42+H42</f>
-        <v>65792</v>
+        <v>49440</v>
       </c>
       <c r="J42" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="L42" s="47" t="s">
+        <v>164</v>
+      </c>
+      <c r="M42" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B43" s="39"/>
+      <c r="C43" s="40" t="s">
+        <v>49</v>
+      </c>
+      <c r="D43" s="24" t="str">
+        <f>F42</f>
+        <v>0xC120</v>
+      </c>
+      <c r="E43" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I43))</f>
+        <v>0x10120</v>
+      </c>
+      <c r="G43" s="24">
+        <f t="shared" si="62"/>
+        <v>49440</v>
+      </c>
+      <c r="H43" s="24">
+        <f t="shared" si="62"/>
+        <v>16384</v>
+      </c>
+      <c r="I43" s="24">
+        <f>G43+H43</f>
+        <v>65824</v>
+      </c>
+      <c r="J43" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="L43" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="M43" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B44" s="41" t="s">
+        <v>144</v>
+      </c>
+      <c r="C44" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>0x10120</v>
+      </c>
+      <c r="E44" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
+        <v>0x100</v>
+      </c>
+      <c r="F44" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I44))</f>
+        <v>0x10220</v>
+      </c>
+      <c r="G44" s="24">
+        <f t="shared" si="62"/>
+        <v>65824</v>
+      </c>
+      <c r="H44" s="24">
+        <f t="shared" si="62"/>
+        <v>256</v>
+      </c>
+      <c r="I44" s="24">
+        <f>G44+H44</f>
+        <v>66080</v>
+      </c>
+      <c r="J44" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="L42" s="19" t="s">
+      <c r="L44" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="M44" s="30">
+        <f>SUM(M35:M43)</f>
+        <v>32</v>
+      </c>
+      <c r="N44" s="33"/>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B45" s="42" t="s">
+        <v>143</v>
+      </c>
+      <c r="L45" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="M45" s="19">
+        <f>M44/8</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="B46" s="42"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="L46" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="M46" s="30">
+        <f>M34*M45</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B47" s="42"/>
+      <c r="C47" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M31))</f>
+        <v>0x4000</v>
+      </c>
+      <c r="F47" s="24"/>
+      <c r="G47" s="24"/>
+      <c r="H47" s="24">
+        <f>HEX2DEC(MID(E47, 3, LEN(E47)-2))</f>
+        <v>16384</v>
+      </c>
+      <c r="I47" s="24"/>
+      <c r="J47" s="24" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B48" s="42"/>
+      <c r="C48" s="38"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M65))</f>
+        <v>0x800</v>
+      </c>
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="24">
+        <f>HEX2DEC(MID(E48, 3, LEN(E48)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I48" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="J48" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="L48" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="M48" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B49" s="42"/>
+      <c r="L49" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="M49" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B50" s="42"/>
+      <c r="L50" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="M50" s="19">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B51" s="42"/>
+      <c r="C51" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24">
+        <f t="shared" ref="H51" si="63">HEX2DEC(MID(E51, 3, LEN(E51)-2))</f>
+        <v>131072</v>
+      </c>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="L51" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="M51" s="29">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B52" s="42"/>
+      <c r="C52" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="F52" s="24"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="24">
+        <f t="shared" ref="H52" si="64">HEX2DEC(MID(E52, 3, LEN(E52)-2))</f>
+        <v>65536</v>
+      </c>
+      <c r="I52" s="24"/>
+      <c r="J52" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="L52" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="M52" s="19">
+        <f>M49*M50*M51</f>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B53" s="42"/>
+      <c r="L53" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="M42" s="19">
-        <f>M41/8</f>
+      <c r="M53" s="19">
+        <f>M52/8</f>
         <v>2048</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B43" s="44" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" ht="15" x14ac:dyDescent="0.25">
-      <c r="B44" s="44"/>
-      <c r="C44"/>
-      <c r="D44"/>
-      <c r="E44"/>
-      <c r="F44"/>
-      <c r="G44"/>
-      <c r="H44"/>
-      <c r="I44"/>
-      <c r="J44"/>
-      <c r="L44" s="21" t="s">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B54" s="42"/>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B55" s="42"/>
+      <c r="L55" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="M44" s="19" t="s">
+      <c r="M55" s="19" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B45" s="44"/>
-      <c r="C45" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
-        <v>0x4000</v>
-      </c>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24">
-        <f>HEX2DEC(MID(E45, 3, LEN(E45)-2))</f>
-        <v>16384</v>
-      </c>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="L45" s="19" t="s">
+      <c r="P55" s="19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B56" s="42"/>
+      <c r="L56" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="M45" s="19">
+      <c r="M56" s="19">
         <v>32</v>
       </c>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B46" s="44"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M54))</f>
-        <v>0x800</v>
-      </c>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24">
-        <f>HEX2DEC(MID(E46, 3, LEN(E46)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I46" s="24" t="s">
-        <v>159</v>
-      </c>
-      <c r="J46" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="L46" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="M46" s="29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B47" s="44"/>
-      <c r="L47" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="M47" s="19">
-        <f>M45*M46</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B48" s="44"/>
-      <c r="L48" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="M48" s="19">
-        <f>M47/8</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B49" s="44"/>
-      <c r="C49" s="45" t="s">
-        <v>155</v>
-      </c>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24" t="s">
-        <v>158</v>
-      </c>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24">
-        <f t="shared" ref="H49" si="62">HEX2DEC(MID(E49, 3, LEN(E49)-2))</f>
-        <v>131072</v>
-      </c>
-      <c r="I49" s="24"/>
-      <c r="J49" s="24" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B50" s="44"/>
-      <c r="C50" s="45" t="s">
-        <v>171</v>
-      </c>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24" t="s">
-        <v>172</v>
-      </c>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24">
-        <f t="shared" ref="H50" si="63">HEX2DEC(MID(E50, 3, LEN(E50)-2))</f>
-        <v>65536</v>
-      </c>
-      <c r="I50" s="24"/>
-      <c r="J50" s="24" t="s">
-        <v>171</v>
-      </c>
-      <c r="L50" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="M50" s="19" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B51" s="44"/>
-      <c r="L51" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="M51" s="19">
-        <v>512</v>
-      </c>
-      <c r="N51" s="19" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B52" s="44"/>
-      <c r="L52" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="M52" s="29">
-        <v>32</v>
-      </c>
-      <c r="N52" s="19" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B53" s="44"/>
-      <c r="L53" s="30" t="s">
-        <v>142</v>
-      </c>
-      <c r="M53" s="19">
-        <f>M51*M52</f>
-        <v>16384</v>
-      </c>
-      <c r="P53" s="19" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B54" s="44"/>
-      <c r="L54" s="19" t="s">
-        <v>141</v>
-      </c>
-      <c r="M54" s="19">
-        <f>M53/8</f>
-        <v>2048</v>
-      </c>
-      <c r="O54" s="19">
+      <c r="O56" s="19">
         <f>384*2</f>
         <v>768</v>
       </c>
     </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B55" s="44"/>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B56" s="44"/>
-    </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B57" s="44"/>
+      <c r="B57" s="42"/>
+      <c r="L57" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="M57" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B58" s="44"/>
+      <c r="B58" s="42"/>
+      <c r="L58" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="M58" s="19">
+        <f>M56*M57</f>
+        <v>32</v>
+      </c>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B59" s="44"/>
+      <c r="B59" s="42"/>
+      <c r="L59" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="M59" s="19">
+        <f>M58/8</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B60" s="44"/>
+      <c r="B60" s="42"/>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B61" s="44"/>
+      <c r="B61" s="42"/>
+      <c r="L61" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="M61" s="19" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B62" s="44"/>
+      <c r="B62" s="42"/>
+      <c r="L62" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="M62" s="19">
+        <v>512</v>
+      </c>
+      <c r="N62" s="19" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B63" s="44"/>
+      <c r="B63" s="42"/>
+      <c r="L63" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="M63" s="29">
+        <v>32</v>
+      </c>
+      <c r="N63" s="19" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B64" s="44"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B65" s="46"/>
+      <c r="B64" s="42"/>
+      <c r="L64" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="M64" s="19">
+        <f>M62*M63</f>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="65" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B65" s="42"/>
+      <c r="L65" s="19" t="s">
+        <v>141</v>
+      </c>
+      <c r="M65" s="19">
+        <f>M64/8</f>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B66" s="42"/>
+    </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B67" s="44"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C32:C33"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3068,8 +3222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A3B691-5BC9-488D-96B0-3685B8BF2439}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21:I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3263,22 +3417,22 @@
         <v>118</v>
       </c>
       <c r="I21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="45" t="s">
         <v>161</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I23" s="47" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -3303,13 +3457,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" t="s">
         <v>175</v>
-      </c>
-      <c r="B1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3326,6 +3480,55 @@
       <c r="D2">
         <f>C2/A2</f>
         <v>16000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3600A3-DD76-4F08-ACE5-C540E0302F0E}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>352</v>
+      </c>
+      <c r="B1">
+        <v>272</v>
+      </c>
+      <c r="D1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <f>A1/D2</f>
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <f>B1/E2</f>
+        <v>17</v>
+      </c>
+      <c r="C2">
+        <f>A2*B2</f>
+        <v>374</v>
+      </c>
+      <c r="D2">
+        <v>16</v>
+      </c>
+      <c r="E2">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
4 way tilemap scrolling
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E59D738-BA04-4E4F-8508-A7B97D9687BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4FB1F7-92F7-43EF-A083-F6B9CED3784A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="215">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -742,6 +742,9 @@
   </si>
   <si>
     <t>0x00F0</t>
+  </si>
+  <si>
+    <t>O</t>
   </si>
 </sst>
 </file>
@@ -1092,14 +1095,14 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1417,7 +1420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="B1:P90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
@@ -2270,7 +2273,7 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="25"/>
-      <c r="C25" s="49"/>
+      <c r="C25" s="50"/>
       <c r="D25" s="24" t="str">
         <f t="shared" ref="D25:D30" si="29">F24</f>
         <v>0x8A10</v>
@@ -2306,7 +2309,7 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="25"/>
-      <c r="C26" s="49"/>
+      <c r="C26" s="50"/>
       <c r="D26" s="24" t="str">
         <f t="shared" si="29"/>
         <v>0x8A20</v>
@@ -2417,7 +2420,7 @@
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="25"/>
-      <c r="C29" s="50" t="s">
+      <c r="C29" s="51" t="s">
         <v>156</v>
       </c>
       <c r="D29" s="24" t="str">
@@ -2456,7 +2459,7 @@
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="25"/>
-      <c r="C30" s="49"/>
+      <c r="C30" s="50"/>
       <c r="D30" s="24" t="str">
         <f t="shared" si="29"/>
         <v>0x8B10</v>
@@ -2563,7 +2566,7 @@
     </row>
     <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="25"/>
-      <c r="C33" s="51"/>
+      <c r="C33" s="49"/>
       <c r="D33" s="24" t="str">
         <f>F32</f>
         <v>0x8C10</v>
@@ -3780,15 +3783,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3600A3-DD76-4F08-ACE5-C540E0302F0E}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="9" max="16" width="3" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>352</v>
       </c>
@@ -3802,7 +3808,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <f>A1/D2</f>
         <v>22</v>
@@ -3821,8 +3827,22 @@
       <c r="E2">
         <v>16</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>214</v>
+      </c>
+      <c r="L2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>214</v>
+      </c>
+      <c r="N3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <f>A2*B2</f>
         <v>374</v>

</xml_diff>

<commit_message>
Add menu triggers, formal starfield class, pilot demo update
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D4FB1F7-92F7-43EF-A083-F6B9CED3784A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0CC7DB-FF2A-4FAD-9C7D-A6FE49DDE91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="3" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="216">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -606,9 +606,6 @@
     <t>System pause trigger</t>
   </si>
   <si>
-    <t>0x00CF</t>
-  </si>
-  <si>
     <t>Sound ROM</t>
   </si>
   <si>
@@ -745,6 +742,12 @@
   </si>
   <si>
     <t>O</t>
+  </si>
+  <si>
+    <t>0x00CE</t>
+  </si>
+  <si>
+    <t>System menu trigger</t>
   </si>
 </sst>
 </file>
@@ -983,7 +986,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1097,6 +1100,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1420,8 +1426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="B1:P90"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1531,7 +1537,7 @@
         <v>44</v>
       </c>
       <c r="D4" s="24" t="str">
-        <f t="shared" ref="D4:D45" si="1">F3</f>
+        <f t="shared" ref="D4:D46" si="1">F3</f>
         <v>0x8000</v>
       </c>
       <c r="E4" s="24" t="s">
@@ -1663,7 +1669,7 @@
         <v>30</v>
       </c>
       <c r="L7" s="21" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
@@ -1696,7 +1702,7 @@
         <v>27</v>
       </c>
       <c r="L8" s="29" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M8" s="29">
         <v>256</v>
@@ -1732,7 +1738,7 @@
         <v>30</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M9" s="19">
         <v>8</v>
@@ -1768,7 +1774,7 @@
         <v>26</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M10" s="19">
         <v>8</v>
@@ -1804,7 +1810,7 @@
         <v>30</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M11" s="19">
         <v>1</v>
@@ -1840,7 +1846,7 @@
         <v>25</v>
       </c>
       <c r="L12" s="30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M12" s="30">
         <f>M9*M10*M11</f>
@@ -1877,7 +1883,7 @@
         <v>30</v>
       </c>
       <c r="L13" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M13" s="19">
         <f>M12/8</f>
@@ -1914,7 +1920,7 @@
         <v>24</v>
       </c>
       <c r="L14" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="M14" s="30">
         <f>M8*M13</f>
@@ -2110,7 +2116,7 @@
         <v>0x8821</v>
       </c>
       <c r="G20" s="24">
-        <f t="shared" ref="G20:H35" si="25">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
+        <f t="shared" ref="G20:H36" si="25">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
         <v>34816</v>
       </c>
       <c r="H20" s="24">
@@ -2273,9 +2279,9 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="25"/>
-      <c r="C25" s="50"/>
+      <c r="C25" s="51"/>
       <c r="D25" s="24" t="str">
-        <f t="shared" ref="D25:D30" si="29">F24</f>
+        <f t="shared" ref="D25:D31" si="29">F24</f>
         <v>0x8A10</v>
       </c>
       <c r="E25" s="24" t="s">
@@ -2309,7 +2315,7 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="25"/>
-      <c r="C26" s="50"/>
+      <c r="C26" s="51"/>
       <c r="D26" s="24" t="str">
         <f t="shared" si="29"/>
         <v>0x8A20</v>
@@ -2345,7 +2351,7 @@
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="25"/>
-      <c r="C27" s="46"/>
+      <c r="C27" s="50"/>
       <c r="D27" s="24" t="str">
         <f>F26</f>
         <v>0x8A30</v>
@@ -2381,32 +2387,32 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="25"/>
-      <c r="C28" s="28"/>
-      <c r="D28" s="28" t="str">
+      <c r="C28" s="46"/>
+      <c r="D28" s="24" t="str">
         <f>F27</f>
         <v>0x8A31</v>
       </c>
-      <c r="E28" s="28" t="s">
-        <v>168</v>
-      </c>
-      <c r="F28" s="28" t="str">
+      <c r="E28" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="24" t="str">
         <f t="shared" ref="F28" si="34">_xlfn.CONCAT("0x",DEC2HEX(I28))</f>
-        <v>0x8B00</v>
-      </c>
-      <c r="G28" s="28">
+        <v>0x8A32</v>
+      </c>
+      <c r="G28" s="24">
         <f>HEX2DEC(MID(D28, 3, LEN(D28)-2))</f>
         <v>35377</v>
       </c>
-      <c r="H28" s="28">
+      <c r="H28" s="24">
         <f t="shared" ref="H28" si="35">HEX2DEC(MID(E28, 3, LEN(E28)-2))</f>
-        <v>207</v>
-      </c>
-      <c r="I28" s="28">
+        <v>1</v>
+      </c>
+      <c r="I28" s="24">
         <f t="shared" ref="I28" si="36">G28+H28</f>
-        <v>35584</v>
-      </c>
-      <c r="J28" s="28" t="s">
-        <v>30</v>
+        <v>35378</v>
+      </c>
+      <c r="J28" s="24" t="s">
+        <v>215</v>
       </c>
       <c r="L28" s="19" t="s">
         <v>68</v>
@@ -2420,34 +2426,32 @@
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="25"/>
-      <c r="C29" s="51" t="s">
-        <v>156</v>
-      </c>
-      <c r="D29" s="24" t="str">
+      <c r="C29" s="28"/>
+      <c r="D29" s="28" t="str">
         <f>F28</f>
+        <v>0x8A32</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="F29" s="28" t="str">
+        <f t="shared" ref="F29" si="37">_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
         <v>0x8B00</v>
       </c>
-      <c r="E29" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="F29" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
-        <v>0x8B10</v>
-      </c>
-      <c r="G29" s="24">
-        <f t="shared" ref="G29" si="37">HEX2DEC(MID(D29, 3, LEN(D29)-2))</f>
+      <c r="G29" s="28">
+        <f>HEX2DEC(MID(D29, 3, LEN(D29)-2))</f>
+        <v>35378</v>
+      </c>
+      <c r="H29" s="28">
+        <f t="shared" ref="H29" si="38">HEX2DEC(MID(E29, 3, LEN(E29)-2))</f>
+        <v>206</v>
+      </c>
+      <c r="I29" s="28">
+        <f t="shared" ref="I29" si="39">G29+H29</f>
         <v>35584</v>
       </c>
-      <c r="H29" s="24">
-        <f t="shared" si="25"/>
-        <v>16</v>
-      </c>
-      <c r="I29" s="24">
-        <f>G29+H29</f>
-        <v>35600</v>
-      </c>
-      <c r="J29" s="24" t="s">
-        <v>171</v>
+      <c r="J29" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L29" s="30" t="s">
         <v>69</v>
@@ -2459,32 +2463,34 @@
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="25"/>
-      <c r="C30" s="50"/>
+      <c r="C30" s="52" t="s">
+        <v>156</v>
+      </c>
       <c r="D30" s="24" t="str">
-        <f t="shared" si="29"/>
-        <v>0x8B10</v>
+        <f>F29</f>
+        <v>0x8B00</v>
       </c>
       <c r="E30" s="24" t="s">
         <v>87</v>
       </c>
       <c r="F30" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
-        <v>0x8B20</v>
+        <v>0x8B10</v>
       </c>
       <c r="G30" s="24">
-        <f t="shared" ref="G30" si="38">HEX2DEC(MID(D30, 3, LEN(D30)-2))</f>
-        <v>35600</v>
+        <f t="shared" ref="G30" si="40">HEX2DEC(MID(D30, 3, LEN(D30)-2))</f>
+        <v>35584</v>
       </c>
       <c r="H30" s="24">
-        <f t="shared" ref="H30" si="39">HEX2DEC(MID(E30, 3, LEN(E30)-2))</f>
+        <f t="shared" si="25"/>
         <v>16</v>
       </c>
       <c r="I30" s="24">
         <f>G30+H30</f>
-        <v>35616</v>
+        <v>35600</v>
       </c>
       <c r="J30" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L30" s="19" t="s">
         <v>70</v>
@@ -2496,32 +2502,32 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" s="25"/>
-      <c r="C31" s="28"/>
-      <c r="D31" s="28" t="str">
-        <f>F30</f>
+      <c r="C31" s="51"/>
+      <c r="D31" s="24" t="str">
+        <f t="shared" si="29"/>
+        <v>0x8B10</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="F31" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I31))</f>
         <v>0x8B20</v>
       </c>
-      <c r="E31" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="F31" s="28" t="str">
-        <f t="shared" ref="F31" si="40">_xlfn.CONCAT("0x",DEC2HEX(I31))</f>
-        <v>0x8C00</v>
-      </c>
-      <c r="G31" s="28">
-        <f t="shared" ref="G31:G33" si="41">HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
+      <c r="G31" s="24">
+        <f t="shared" ref="G31" si="41">HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
+        <v>35600</v>
+      </c>
+      <c r="H31" s="24">
+        <f t="shared" ref="H31" si="42">HEX2DEC(MID(E31, 3, LEN(E31)-2))</f>
+        <v>16</v>
+      </c>
+      <c r="I31" s="24">
+        <f>G31+H31</f>
         <v>35616</v>
       </c>
-      <c r="H31" s="28">
-        <f t="shared" ref="H31:H34" si="42">HEX2DEC(MID(E31, 3, LEN(E31)-2))</f>
-        <v>224</v>
-      </c>
-      <c r="I31" s="28">
-        <f t="shared" ref="I31" si="43">G31+H31</f>
-        <v>35840</v>
-      </c>
-      <c r="J31" s="28" t="s">
-        <v>30</v>
+      <c r="J31" s="24" t="s">
+        <v>171</v>
       </c>
       <c r="L31" s="30" t="s">
         <v>146</v>
@@ -2533,99 +2539,99 @@
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B32" s="25"/>
-      <c r="C32" s="48" t="s">
-        <v>187</v>
-      </c>
-      <c r="D32" s="24" t="str">
+      <c r="C32" s="28"/>
+      <c r="D32" s="28" t="str">
         <f>F31</f>
+        <v>0x8B20</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="F32" s="28" t="str">
+        <f t="shared" ref="F32" si="43">_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
         <v>0x8C00</v>
       </c>
-      <c r="E32" s="24" t="str">
+      <c r="G32" s="28">
+        <f t="shared" ref="G32:G34" si="44">HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
+        <v>35616</v>
+      </c>
+      <c r="H32" s="28">
+        <f t="shared" ref="H32:H35" si="45">HEX2DEC(MID(E32, 3, LEN(E32)-2))</f>
+        <v>224</v>
+      </c>
+      <c r="I32" s="28">
+        <f t="shared" ref="I32" si="46">G32+H32</f>
+        <v>35840</v>
+      </c>
+      <c r="J32" s="28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="25"/>
+      <c r="C33" s="48" t="s">
+        <v>186</v>
+      </c>
+      <c r="D33" s="24" t="str">
+        <f>F32</f>
+        <v>0x8C00</v>
+      </c>
+      <c r="E33" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M74))</f>
         <v>0x10</v>
       </c>
-      <c r="F32" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
+      <c r="F33" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
         <v>0x8C10</v>
       </c>
-      <c r="G32" s="24">
-        <f t="shared" ref="G32" si="44">HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
+      <c r="G33" s="24">
+        <f t="shared" ref="G33" si="47">HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
         <v>35840</v>
       </c>
-      <c r="H32" s="24">
-        <f t="shared" si="42"/>
+      <c r="H33" s="24">
+        <f t="shared" si="45"/>
         <v>16</v>
       </c>
-      <c r="I32" s="24">
-        <f>G32+H32</f>
+      <c r="I33" s="24">
+        <f>G33+H33</f>
         <v>35856</v>
       </c>
-      <c r="J32" s="24" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="25"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="24" t="str">
-        <f>F32</f>
+      <c r="J33" s="24" t="s">
+        <v>188</v>
+      </c>
+      <c r="L33" s="21" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B34" s="25"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="24" t="str">
+        <f>F33</f>
         <v>0x8C10</v>
       </c>
-      <c r="E33" s="24" t="str">
+      <c r="E34" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M81))</f>
         <v>0x300</v>
       </c>
-      <c r="F33" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
+      <c r="F34" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
         <v>0x8F10</v>
       </c>
-      <c r="G33" s="24">
-        <f t="shared" si="41"/>
+      <c r="G34" s="24">
+        <f t="shared" si="44"/>
         <v>35856</v>
       </c>
-      <c r="H33" s="24">
-        <f t="shared" si="42"/>
+      <c r="H34" s="24">
+        <f t="shared" si="45"/>
         <v>768</v>
       </c>
-      <c r="I33" s="24">
-        <f>G33+H33</f>
+      <c r="I34" s="24">
+        <f>G34+H34</f>
         <v>36624</v>
       </c>
-      <c r="J33" s="24" t="s">
-        <v>194</v>
-      </c>
-      <c r="L33" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B34" s="25"/>
-      <c r="C34" s="28"/>
-      <c r="D34" s="28" t="str">
-        <f>F33</f>
-        <v>0x8F10</v>
-      </c>
-      <c r="E34" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="F34" s="28" t="str">
-        <f t="shared" ref="F34" si="45">_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
-        <v>0x9000</v>
-      </c>
-      <c r="G34" s="28">
-        <f t="shared" ref="G34" si="46">HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
-        <v>36624</v>
-      </c>
-      <c r="H34" s="28">
-        <f t="shared" si="42"/>
-        <v>240</v>
-      </c>
-      <c r="I34" s="28">
-        <f t="shared" ref="I34" si="47">G34+H34</f>
-        <v>36864</v>
-      </c>
-      <c r="J34" s="28" t="s">
-        <v>30</v>
+      <c r="J34" s="24" t="s">
+        <v>193</v>
       </c>
       <c r="L34" s="29" t="s">
         <v>62</v>
@@ -2636,70 +2642,70 @@
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B35" s="25"/>
-      <c r="C35" s="32" t="s">
+      <c r="C35" s="28"/>
+      <c r="D35" s="28" t="str">
+        <f>F34</f>
+        <v>0x8F10</v>
+      </c>
+      <c r="E35" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="F35" s="28" t="str">
+        <f t="shared" ref="F35" si="48">_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
+        <v>0x9000</v>
+      </c>
+      <c r="G35" s="28">
+        <f t="shared" ref="G35" si="49">HEX2DEC(MID(D35, 3, LEN(D35)-2))</f>
+        <v>36624</v>
+      </c>
+      <c r="H35" s="28">
+        <f t="shared" si="45"/>
+        <v>240</v>
+      </c>
+      <c r="I35" s="28">
+        <f t="shared" ref="I35" si="50">G35+H35</f>
+        <v>36864</v>
+      </c>
+      <c r="J35" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="L35" s="31" t="s">
+        <v>79</v>
+      </c>
+      <c r="M35" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B36" s="25"/>
+      <c r="C36" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="24" t="str">
-        <f>F34</f>
+      <c r="D36" s="24" t="str">
+        <f>F35</f>
         <v>0x9000</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E36" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
+      <c r="F36" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I36))</f>
         <v>0x9800</v>
       </c>
-      <c r="G35" s="24">
-        <f>HEX2DEC(MID(D35, 3, LEN(D35)-2))</f>
+      <c r="G36" s="24">
+        <f>HEX2DEC(MID(D36, 3, LEN(D36)-2))</f>
         <v>36864</v>
       </c>
-      <c r="H35" s="24">
+      <c r="H36" s="24">
         <f t="shared" si="25"/>
         <v>2048</v>
       </c>
-      <c r="I35" s="24">
-        <f>G35+H35</f>
-        <v>38912</v>
-      </c>
-      <c r="J35" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="L35" s="31" t="s">
-        <v>79</v>
-      </c>
-      <c r="M35" s="19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B36" s="25"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v>0x9800</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I36))</f>
-        <v>0xA000</v>
-      </c>
-      <c r="G36" s="24">
-        <f>HEX2DEC(MID(D36, 3, LEN(D36)-2))</f>
-        <v>38912</v>
-      </c>
-      <c r="H36" s="24">
-        <f>HEX2DEC(MID(E36, 3, LEN(E36)-2))</f>
-        <v>2048</v>
-      </c>
       <c r="I36" s="24">
         <f>G36+H36</f>
-        <v>40960</v>
+        <v>38912</v>
       </c>
       <c r="J36" s="24" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="L36" s="19" t="s">
         <v>163</v>
@@ -2713,29 +2719,29 @@
       <c r="C37" s="34"/>
       <c r="D37" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0xA000</v>
+        <v>0x9800</v>
       </c>
       <c r="E37" s="24" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="24" t="str">
-        <f t="shared" ref="F37" si="48">_xlfn.CONCAT("0x",DEC2HEX(I37))</f>
-        <v>0xA800</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I37))</f>
+        <v>0xA000</v>
       </c>
       <c r="G37" s="24">
-        <f t="shared" ref="G37" si="49">HEX2DEC(MID(D37, 3, LEN(D37)-2))</f>
+        <f>HEX2DEC(MID(D37, 3, LEN(D37)-2))</f>
+        <v>38912</v>
+      </c>
+      <c r="H37" s="24">
+        <f>HEX2DEC(MID(E37, 3, LEN(E37)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I37" s="24">
+        <f>G37+H37</f>
         <v>40960</v>
       </c>
-      <c r="H37" s="24">
-        <f t="shared" ref="H37" si="50">HEX2DEC(MID(E37, 3, LEN(E37)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I37" s="24">
-        <f t="shared" ref="I37" si="51">G37+H37</f>
-        <v>43008</v>
-      </c>
       <c r="J37" s="24" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L37" s="19" t="s">
         <v>166</v>
@@ -2746,35 +2752,35 @@
     </row>
     <row r="38" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B38" s="25"/>
-      <c r="C38" s="35"/>
+      <c r="C38" s="34"/>
       <c r="D38" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0xA800</v>
+        <v>0xA000</v>
       </c>
       <c r="E38" s="24" t="s">
         <v>8</v>
       </c>
       <c r="F38" s="24" t="str">
-        <f t="shared" ref="F38" si="52">_xlfn.CONCAT("0x",DEC2HEX(I38))</f>
-        <v>0xB000</v>
+        <f t="shared" ref="F38" si="51">_xlfn.CONCAT("0x",DEC2HEX(I38))</f>
+        <v>0xA800</v>
       </c>
       <c r="G38" s="24">
-        <f t="shared" ref="G38" si="53">HEX2DEC(MID(D38, 3, LEN(D38)-2))</f>
+        <f t="shared" ref="G38" si="52">HEX2DEC(MID(D38, 3, LEN(D38)-2))</f>
+        <v>40960</v>
+      </c>
+      <c r="H38" s="24">
+        <f t="shared" ref="H38" si="53">HEX2DEC(MID(E38, 3, LEN(E38)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I38" s="24">
+        <f t="shared" ref="I38" si="54">G38+H38</f>
         <v>43008</v>
       </c>
-      <c r="H38" s="24">
-        <f t="shared" ref="H38" si="54">HEX2DEC(MID(E38, 3, LEN(E38)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I38" s="24">
-        <f t="shared" ref="I38" si="55">G38+H38</f>
-        <v>45056</v>
-      </c>
       <c r="J38" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L38" s="19" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M38" s="19">
         <v>2</v>
@@ -2782,71 +2788,71 @@
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" s="25"/>
-      <c r="C39" s="36" t="s">
-        <v>56</v>
-      </c>
+      <c r="C39" s="35"/>
       <c r="D39" s="24" t="str">
         <f t="shared" si="1"/>
+        <v>0xA800</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F39" s="24" t="str">
+        <f t="shared" ref="F39" si="55">_xlfn.CONCAT("0x",DEC2HEX(I39))</f>
         <v>0xB000</v>
       </c>
-      <c r="E39" s="24" t="str">
+      <c r="G39" s="24">
+        <f t="shared" ref="G39" si="56">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
+        <v>43008</v>
+      </c>
+      <c r="H39" s="24">
+        <f t="shared" ref="H39" si="57">HEX2DEC(MID(E39, 3, LEN(E39)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I39" s="24">
+        <f t="shared" ref="I39" si="58">G39+H39</f>
+        <v>45056</v>
+      </c>
+      <c r="J39" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="L39" s="47" t="s">
+        <v>164</v>
+      </c>
+      <c r="M39" s="47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B40" s="25"/>
+      <c r="C40" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB000</v>
+      </c>
+      <c r="E40" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M46))</f>
         <v>0x80</v>
       </c>
-      <c r="F39" s="24" t="str">
-        <f t="shared" ref="F39:F40" si="56">_xlfn.CONCAT("0x",DEC2HEX(I39))</f>
+      <c r="F40" s="24" t="str">
+        <f t="shared" ref="F40:F41" si="59">_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
         <v>0xB080</v>
       </c>
-      <c r="G39" s="24">
-        <f t="shared" ref="G39:G40" si="57">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
+      <c r="G40" s="24">
+        <f t="shared" ref="G40:G41" si="60">HEX2DEC(MID(D40, 3, LEN(D40)-2))</f>
         <v>45056</v>
       </c>
-      <c r="H39" s="24">
-        <f t="shared" ref="H39:H40" si="58">HEX2DEC(MID(E39, 3, LEN(E39)-2))</f>
+      <c r="H40" s="24">
+        <f t="shared" ref="H40:H41" si="61">HEX2DEC(MID(E40, 3, LEN(E40)-2))</f>
         <v>128</v>
       </c>
-      <c r="I39" s="24">
-        <f t="shared" ref="I39:I40" si="59">G39+H39</f>
+      <c r="I40" s="24">
+        <f t="shared" ref="I40:I41" si="62">G40+H40</f>
         <v>45184</v>
       </c>
-      <c r="J39" s="24" t="s">
+      <c r="J40" s="24" t="s">
         <v>57</v>
-      </c>
-      <c r="L39" s="47" t="s">
-        <v>164</v>
-      </c>
-      <c r="M39" s="47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B40" s="25"/>
-      <c r="C40" s="37"/>
-      <c r="D40" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v>0xB080</v>
-      </c>
-      <c r="E40" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="F40" s="28" t="str">
-        <f t="shared" si="56"/>
-        <v>0xB400</v>
-      </c>
-      <c r="G40" s="28">
-        <f t="shared" si="57"/>
-        <v>45184</v>
-      </c>
-      <c r="H40" s="28">
-        <f t="shared" si="58"/>
-        <v>896</v>
-      </c>
-      <c r="I40" s="28">
-        <f t="shared" si="59"/>
-        <v>46080</v>
-      </c>
-      <c r="J40" s="28" t="s">
-        <v>30</v>
       </c>
       <c r="L40" s="31" t="s">
         <v>72</v>
@@ -2858,32 +2864,31 @@
     <row r="41" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B41" s="25"/>
       <c r="C41" s="37"/>
-      <c r="D41" s="24" t="str">
-        <f t="shared" ref="D41:D42" si="60">F40</f>
+      <c r="D41" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB080</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="F41" s="28" t="str">
+        <f t="shared" si="59"/>
         <v>0xB400</v>
       </c>
-      <c r="E41" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M59))</f>
-        <v>0x4</v>
-      </c>
-      <c r="F41" s="24" t="str">
-        <f t="shared" ref="F41:F42" si="61">_xlfn.CONCAT("0x",DEC2HEX(I41))</f>
-        <v>0xB404</v>
-      </c>
-      <c r="G41" s="24">
-        <f t="shared" ref="G41:G42" si="62">HEX2DEC(MID(D41, 3, LEN(D41)-2))</f>
+      <c r="G41" s="28">
+        <f t="shared" si="60"/>
+        <v>45184</v>
+      </c>
+      <c r="H41" s="28">
+        <f t="shared" si="61"/>
+        <v>896</v>
+      </c>
+      <c r="I41" s="28">
+        <f t="shared" si="62"/>
         <v>46080</v>
       </c>
-      <c r="H41" s="24">
-        <f t="shared" ref="H41:H42" si="63">HEX2DEC(MID(E41, 3, LEN(E41)-2))</f>
-        <v>4</v>
-      </c>
-      <c r="I41" s="24">
-        <f t="shared" ref="I41:I42" si="64">G41+H41</f>
-        <v>46084</v>
-      </c>
-      <c r="J41" s="24" t="s">
-        <v>91</v>
+      <c r="J41" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L41" s="31" t="s">
         <v>81</v>
@@ -2895,31 +2900,32 @@
     <row r="42" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B42" s="25"/>
       <c r="C42" s="37"/>
-      <c r="D42" s="28" t="str">
-        <f t="shared" si="60"/>
+      <c r="D42" s="24" t="str">
+        <f t="shared" ref="D42:D43" si="63">F41</f>
+        <v>0xB400</v>
+      </c>
+      <c r="E42" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M59))</f>
+        <v>0x4</v>
+      </c>
+      <c r="F42" s="24" t="str">
+        <f t="shared" ref="F42:F43" si="64">_xlfn.CONCAT("0x",DEC2HEX(I42))</f>
         <v>0xB404</v>
       </c>
-      <c r="E42" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="F42" s="28" t="str">
-        <f t="shared" si="61"/>
-        <v>0xB800</v>
-      </c>
-      <c r="G42" s="28">
-        <f t="shared" si="62"/>
+      <c r="G42" s="24">
+        <f t="shared" ref="G42:G43" si="65">HEX2DEC(MID(D42, 3, LEN(D42)-2))</f>
+        <v>46080</v>
+      </c>
+      <c r="H42" s="24">
+        <f t="shared" ref="H42:H43" si="66">HEX2DEC(MID(E42, 3, LEN(E42)-2))</f>
+        <v>4</v>
+      </c>
+      <c r="I42" s="24">
+        <f t="shared" ref="I42:I43" si="67">G42+H42</f>
         <v>46084</v>
       </c>
-      <c r="H42" s="28">
-        <f t="shared" si="63"/>
-        <v>1020</v>
-      </c>
-      <c r="I42" s="28">
-        <f t="shared" si="64"/>
-        <v>47104</v>
-      </c>
-      <c r="J42" s="28" t="s">
-        <v>30</v>
+      <c r="J42" s="24" t="s">
+        <v>91</v>
       </c>
       <c r="L42" s="47" t="s">
         <v>164</v>
@@ -2930,71 +2936,69 @@
     </row>
     <row r="43" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B43" s="25"/>
-      <c r="C43" s="38"/>
-      <c r="D43" s="24" t="str">
-        <f>F42</f>
+      <c r="C43" s="37"/>
+      <c r="D43" s="28" t="str">
+        <f t="shared" si="63"/>
+        <v>0xB404</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="F43" s="28" t="str">
+        <f t="shared" si="64"/>
         <v>0xB800</v>
       </c>
-      <c r="E43" s="24" t="str">
+      <c r="G43" s="28">
+        <f t="shared" si="65"/>
+        <v>46084</v>
+      </c>
+      <c r="H43" s="28">
+        <f t="shared" si="66"/>
+        <v>1020</v>
+      </c>
+      <c r="I43" s="28">
+        <f t="shared" si="67"/>
+        <v>47104</v>
+      </c>
+      <c r="J43" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="L43" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="M43" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B44" s="39"/>
+      <c r="C44" s="38"/>
+      <c r="D44" s="24" t="str">
+        <f>F43</f>
+        <v>0xB800</v>
+      </c>
+      <c r="E44" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M53))</f>
         <v>0x800</v>
       </c>
-      <c r="F43" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I43))</f>
-        <v>0xC000</v>
-      </c>
-      <c r="G43" s="24">
-        <f t="shared" ref="G43:H45" si="65">HEX2DEC(MID(D43, 3, LEN(D43)-2))</f>
-        <v>47104</v>
-      </c>
-      <c r="H43" s="24">
-        <f t="shared" si="65"/>
-        <v>2048</v>
-      </c>
-      <c r="I43" s="24">
-        <f>G43+H43</f>
-        <v>49152</v>
-      </c>
-      <c r="J43" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="L43" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="M43" s="19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B44" s="39"/>
-      <c r="C44" s="40" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="24" t="str">
-        <f>F43</f>
-        <v>0xC000</v>
-      </c>
-      <c r="E44" s="24" t="s">
-        <v>6</v>
-      </c>
       <c r="F44" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I44))</f>
-        <v>0x10000</v>
+        <v>0xC000</v>
       </c>
       <c r="G44" s="24">
-        <f t="shared" si="65"/>
-        <v>49152</v>
+        <f t="shared" ref="G44:H46" si="68">HEX2DEC(MID(D44, 3, LEN(D44)-2))</f>
+        <v>47104</v>
       </c>
       <c r="H44" s="24">
-        <f t="shared" si="65"/>
-        <v>16384</v>
+        <f t="shared" si="68"/>
+        <v>2048</v>
       </c>
       <c r="I44" s="24">
         <f>G44+H44</f>
-        <v>65536</v>
+        <v>49152</v>
       </c>
       <c r="J44" s="24" t="s">
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="L44" s="30" t="s">
         <v>4</v>
@@ -3009,35 +3013,34 @@
       <c r="B45" s="41" t="s">
         <v>144</v>
       </c>
-      <c r="C45" s="43" t="s">
-        <v>55</v>
+      <c r="C45" s="40" t="s">
+        <v>49</v>
       </c>
       <c r="D45" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v>0x10000</v>
-      </c>
-      <c r="E45" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
-        <v>0x100</v>
+        <f>F44</f>
+        <v>0xC000</v>
+      </c>
+      <c r="E45" s="24" t="s">
+        <v>6</v>
       </c>
       <c r="F45" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I45))</f>
-        <v>0x10100</v>
+        <v>0x10000</v>
       </c>
       <c r="G45" s="24">
-        <f t="shared" si="65"/>
-        <v>65536</v>
+        <f t="shared" si="68"/>
+        <v>49152</v>
       </c>
       <c r="H45" s="24">
-        <f t="shared" si="65"/>
-        <v>256</v>
+        <f t="shared" si="68"/>
+        <v>16384</v>
       </c>
       <c r="I45" s="24">
         <f>G45+H45</f>
-        <v>65792</v>
+        <v>65536</v>
       </c>
       <c r="J45" s="24" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="L45" s="19" t="s">
         <v>3</v>
@@ -3051,6 +3054,36 @@
       <c r="B46" s="42" t="s">
         <v>143</v>
       </c>
+      <c r="C46" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="D46" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>0x10000</v>
+      </c>
+      <c r="E46" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
+        <v>0x100</v>
+      </c>
+      <c r="F46" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I46))</f>
+        <v>0x10100</v>
+      </c>
+      <c r="G46" s="24">
+        <f t="shared" si="68"/>
+        <v>65536</v>
+      </c>
+      <c r="H46" s="24">
+        <f t="shared" si="68"/>
+        <v>256</v>
+      </c>
+      <c r="I46" s="24">
+        <f>G46+H46</f>
+        <v>65792</v>
+      </c>
+      <c r="J46" s="24" t="s">
+        <v>54</v>
+      </c>
       <c r="L46" s="30" t="s">
         <v>139</v>
       </c>
@@ -3059,63 +3092,45 @@
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B47" s="42"/>
-      <c r="C47"/>
-      <c r="D47"/>
-      <c r="E47"/>
-      <c r="F47"/>
-      <c r="G47"/>
-      <c r="H47"/>
-      <c r="I47"/>
-      <c r="J47"/>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="2:14" ht="15" x14ac:dyDescent="0.25">
       <c r="B48" s="42"/>
-      <c r="C48" s="36" t="s">
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="L48" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="M48" s="19" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B49" s="42"/>
+      <c r="C49" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="D48" s="24"/>
-      <c r="E48" s="24" t="str">
+      <c r="D49" s="24"/>
+      <c r="E49" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M31))</f>
         <v>0x4000</v>
-      </c>
-      <c r="F48" s="24"/>
-      <c r="G48" s="24"/>
-      <c r="H48" s="24">
-        <f>HEX2DEC(MID(E48, 3, LEN(E48)-2))</f>
-        <v>16384</v>
-      </c>
-      <c r="I48" s="24"/>
-      <c r="J48" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="L48" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="M48" s="19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B49" s="42"/>
-      <c r="C49" s="38"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M65))</f>
-        <v>0x800</v>
       </c>
       <c r="F49" s="24"/>
       <c r="G49" s="24"/>
       <c r="H49" s="24">
         <f>HEX2DEC(MID(E49, 3, LEN(E49)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I49" s="24" t="s">
-        <v>158</v>
-      </c>
+        <v>16384</v>
+      </c>
+      <c r="I49" s="24"/>
       <c r="J49" s="24" t="s">
-        <v>134</v>
+        <v>51</v>
       </c>
       <c r="L49" s="19" t="s">
         <v>80</v>
@@ -3126,6 +3141,24 @@
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B50" s="42"/>
+      <c r="C50" s="38"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M65))</f>
+        <v>0x800</v>
+      </c>
+      <c r="F50" s="24"/>
+      <c r="G50" s="24"/>
+      <c r="H50" s="24">
+        <f>HEX2DEC(MID(E50, 3, LEN(E50)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I50" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="J50" s="24" t="s">
+        <v>134</v>
+      </c>
       <c r="L50" s="19" t="s">
         <v>74</v>
       </c>
@@ -3144,23 +3177,6 @@
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B52" s="42"/>
-      <c r="C52" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="D52" s="24"/>
-      <c r="E52" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="F52" s="24"/>
-      <c r="G52" s="24"/>
-      <c r="H52" s="24">
-        <f t="shared" ref="H52" si="66">HEX2DEC(MID(E52, 3, LEN(E52)-2))</f>
-        <v>131072</v>
-      </c>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24" t="s">
-        <v>155</v>
-      </c>
       <c r="L52" s="19" t="s">
         <v>148</v>
       </c>
@@ -3172,21 +3188,21 @@
     <row r="53" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B53" s="42"/>
       <c r="C53" s="43" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="D53" s="24"/>
       <c r="E53" s="24" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="F53" s="24"/>
       <c r="G53" s="24"/>
       <c r="H53" s="24">
-        <f t="shared" ref="H53" si="67">HEX2DEC(MID(E53, 3, LEN(E53)-2))</f>
-        <v>65536</v>
+        <f t="shared" ref="H53" si="69">HEX2DEC(MID(E53, 3, LEN(E53)-2))</f>
+        <v>131072</v>
       </c>
       <c r="I53" s="24"/>
       <c r="J53" s="24" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="L53" s="19" t="s">
         <v>147</v>
@@ -3198,6 +3214,23 @@
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B54" s="42"/>
+      <c r="C54" s="43" t="s">
+        <v>168</v>
+      </c>
+      <c r="D54" s="24"/>
+      <c r="E54" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="F54" s="24"/>
+      <c r="G54" s="24"/>
+      <c r="H54" s="24">
+        <f t="shared" ref="H54" si="70">HEX2DEC(MID(E54, 3, LEN(E54)-2))</f>
+        <v>65536</v>
+      </c>
+      <c r="I54" s="24"/>
+      <c r="J54" s="24" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B55" s="42"/>
@@ -3315,13 +3348,13 @@
     <row r="67" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B67" s="42"/>
       <c r="L67" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B68" s="44"/>
       <c r="L68" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M68" s="19">
         <v>8</v>
@@ -3329,7 +3362,7 @@
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L69" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M69" s="19">
         <v>8</v>
@@ -3337,7 +3370,7 @@
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L70" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M70" s="19">
         <v>8</v>
@@ -3345,7 +3378,7 @@
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L71" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="M71" s="19">
         <v>8</v>
@@ -3361,7 +3394,7 @@
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L73" s="30" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M73" s="30">
         <f>SUM(M68:M72)</f>
@@ -3370,7 +3403,7 @@
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L74" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M74" s="19">
         <f>M73/8</f>
@@ -3379,34 +3412,34 @@
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L76" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L77" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M77" s="19">
         <v>32</v>
       </c>
       <c r="N77" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="78" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L78" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M78" s="19">
         <v>24</v>
       </c>
       <c r="N78" s="19" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L79" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="M79" s="19">
         <v>8</v>
@@ -3414,7 +3447,7 @@
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L80" s="30" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M80" s="30">
         <f>M77*M78*M79</f>
@@ -3423,7 +3456,7 @@
     </row>
     <row r="81" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L81" s="33" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M81" s="33">
         <f>M80/8</f>
@@ -3436,12 +3469,12 @@
     </row>
     <row r="83" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L83" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="84" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L84" s="29" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M84" s="29">
         <v>64</v>
@@ -3449,7 +3482,7 @@
     </row>
     <row r="85" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L85" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M85" s="19">
         <v>16</v>
@@ -3457,7 +3490,7 @@
     </row>
     <row r="86" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L86" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M86" s="19">
         <v>16</v>
@@ -3465,7 +3498,7 @@
     </row>
     <row r="87" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L87" s="19" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M87" s="19">
         <v>16</v>
@@ -3476,7 +3509,7 @@
     </row>
     <row r="88" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L88" s="30" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M88" s="30">
         <f>M85*M86*M87</f>
@@ -3485,7 +3518,7 @@
     </row>
     <row r="89" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L89" s="19" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M89" s="19">
         <f>M88/8</f>
@@ -3494,7 +3527,7 @@
     </row>
     <row r="90" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L90" s="30" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="M90" s="30">
         <f>M84*M89</f>
@@ -3504,7 +3537,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C30:C31"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3751,13 +3784,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" t="s">
         <v>173</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>174</v>
-      </c>
-      <c r="C1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3785,7 +3818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC3600A3-DD76-4F08-ACE5-C540E0302F0E}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
@@ -3802,10 +3835,10 @@
         <v>272</v>
       </c>
       <c r="D1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" t="s">
         <v>176</v>
-      </c>
-      <c r="E1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3828,18 +3861,18 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Various tidying up and fixes
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF0CC7DB-FF2A-4FAD-9C7D-A6FE49DDE91C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E7A58F-2558-42E2-9DF6-1847DA328092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
+    <workbookView xWindow="2175" yWindow="1830" windowWidth="24165" windowHeight="15015" activeTab="1" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware" sheetId="1" r:id="rId1"/>
@@ -1426,7 +1426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="B1:P90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -3549,7 +3549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A3B691-5BC9-488D-96B0-3685B8BF2439}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix timer, add sprite layer priority control
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98E7A58F-2558-42E2-9DF6-1847DA328092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A630BB9-856B-4235-A864-9303534F58F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2175" yWindow="1830" windowWidth="24165" windowHeight="15015" activeTab="1" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
+    <workbookView xWindow="1470" yWindow="2910" windowWidth="24165" windowHeight="14085" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="217">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -166,9 +166,6 @@
   </si>
   <si>
     <t>0x00DF</t>
-  </si>
-  <si>
-    <t>0x00FF</t>
   </si>
   <si>
     <t>Area</t>
@@ -748,6 +745,12 @@
   </si>
   <si>
     <t>System menu trigger</t>
+  </si>
+  <si>
+    <t>0x00FE</t>
+  </si>
+  <si>
+    <t>System outputs (video options)</t>
   </si>
 </sst>
 </file>
@@ -986,7 +989,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -1100,6 +1103,9 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1426,8 +1432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="B1:P90"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1441,7 +1447,7 @@
     <col min="7" max="7" width="6.42578125" style="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="19" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="6" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.28515625" style="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="19" customWidth="1"/>
     <col min="11" max="11" width="5.5703125" style="19" customWidth="1"/>
     <col min="12" max="12" width="43.28515625" style="19" customWidth="1"/>
     <col min="13" max="13" width="9.140625" style="19"/>
@@ -1456,10 +1462,10 @@
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B2" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D2" s="20" t="s">
         <v>36</v>
@@ -1483,12 +1489,12 @@
         <v>28</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C3" s="23" t="s">
         <v>7</v>
@@ -1497,14 +1503,14 @@
         <v>5</v>
       </c>
       <c r="E3" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F3" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I3))</f>
         <v>0x8000</v>
       </c>
       <c r="G3" s="24">
-        <f t="shared" ref="G3:H6" si="0">HEX2DEC(MID(D3, 3, LEN(D3)-2))</f>
+        <f t="shared" ref="G3:H7" si="0">HEX2DEC(MID(D3, 3, LEN(D3)-2))</f>
         <v>0</v>
       </c>
       <c r="H3" s="24">
@@ -1531,13 +1537,13 @@
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" s="25" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="24" t="str">
-        <f t="shared" ref="D4:D46" si="1">F3</f>
+        <f t="shared" ref="D4:D47" si="1">F3</f>
         <v>0x8000</v>
       </c>
       <c r="E4" s="24" t="s">
@@ -1575,32 +1581,32 @@
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B5" s="25"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="28" t="str">
-        <f t="shared" si="1"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="24" t="str">
+        <f t="shared" ref="D5" si="2">F4</f>
         <v>0x8001</v>
       </c>
-      <c r="E5" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="28" t="str">
-        <f t="shared" ref="F5" si="2">_xlfn.CONCAT("0x",DEC2HEX(I5))</f>
-        <v>0x8100</v>
-      </c>
-      <c r="G5" s="28">
-        <f t="shared" si="0"/>
+      <c r="E5" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I5))</f>
+        <v>0x8002</v>
+      </c>
+      <c r="G5" s="24">
+        <f t="shared" ref="G5" si="3">HEX2DEC(MID(D5, 3, LEN(D5)-2))</f>
         <v>32769</v>
       </c>
-      <c r="H5" s="28">
-        <f t="shared" si="0"/>
-        <v>255</v>
-      </c>
-      <c r="I5" s="28">
+      <c r="H5" s="24">
+        <f t="shared" ref="H5" si="4">HEX2DEC(MID(E5, 3, LEN(E5)-2))</f>
+        <v>1</v>
+      </c>
+      <c r="I5" s="24">
         <f>G5+H5</f>
-        <v>33024</v>
-      </c>
-      <c r="J5" s="28" t="s">
-        <v>30</v>
+        <v>32770</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>216</v>
       </c>
       <c r="L5" s="19" t="s">
         <v>0</v>
@@ -1612,97 +1618,97 @@
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" s="25"/>
       <c r="C6" s="27"/>
-      <c r="D6" s="24" t="str">
-        <f t="shared" si="1"/>
+      <c r="D6" s="28" t="str">
+        <f>F5</f>
+        <v>0x8002</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="F6" s="28" t="str">
+        <f t="shared" ref="F6" si="5">_xlfn.CONCAT("0x",DEC2HEX(I6))</f>
         <v>0x8100</v>
       </c>
-      <c r="E6" s="24" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I6))</f>
-        <v>0x81C0</v>
-      </c>
-      <c r="G6" s="24">
+      <c r="G6" s="28">
         <f t="shared" si="0"/>
+        <v>32770</v>
+      </c>
+      <c r="H6" s="28">
+        <f t="shared" si="0"/>
+        <v>254</v>
+      </c>
+      <c r="I6" s="28">
+        <f>G6+H6</f>
         <v>33024</v>
       </c>
-      <c r="H6" s="24">
-        <f t="shared" si="0"/>
-        <v>192</v>
-      </c>
-      <c r="I6" s="24">
-        <f>G6+H6</f>
-        <v>33216</v>
-      </c>
-      <c r="J6" s="24" t="s">
-        <v>12</v>
+      <c r="J6" s="28" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="25"/>
       <c r="C7" s="27"/>
-      <c r="D7" s="28" t="str">
+      <c r="D7" s="24" t="str">
         <f t="shared" si="1"/>
+        <v>0x8100</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I7))</f>
         <v>0x81C0</v>
       </c>
-      <c r="E7" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="28" t="str">
-        <f t="shared" ref="F7" si="3">_xlfn.CONCAT("0x",DEC2HEX(I7))</f>
-        <v>0x8200</v>
-      </c>
-      <c r="G7" s="28">
-        <f t="shared" ref="G7" si="4">HEX2DEC(MID(D7, 3, LEN(D7)-2))</f>
+      <c r="G7" s="24">
+        <f t="shared" si="0"/>
+        <v>33024</v>
+      </c>
+      <c r="H7" s="24">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="I7" s="24">
+        <f>G7+H7</f>
         <v>33216</v>
       </c>
-      <c r="H7" s="28">
-        <f t="shared" ref="H7" si="5">HEX2DEC(MID(E7, 3, LEN(E7)-2))</f>
-        <v>64</v>
-      </c>
-      <c r="I7" s="28">
-        <f t="shared" ref="I7" si="6">G7+H7</f>
-        <v>33280</v>
-      </c>
-      <c r="J7" s="28" t="s">
-        <v>30</v>
+      <c r="J7" s="24" t="s">
+        <v>12</v>
       </c>
       <c r="L7" s="21" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" s="25"/>
       <c r="C8" s="27"/>
-      <c r="D8" s="24" t="str">
+      <c r="D8" s="28" t="str">
         <f t="shared" si="1"/>
+        <v>0x81C0</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="28" t="str">
+        <f t="shared" ref="F8" si="6">_xlfn.CONCAT("0x",DEC2HEX(I8))</f>
         <v>0x8200</v>
       </c>
-      <c r="E8" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I8))</f>
-        <v>0x8260</v>
-      </c>
-      <c r="G8" s="24">
-        <f t="shared" ref="G8:H10" si="7">HEX2DEC(MID(D8, 3, LEN(D8)-2))</f>
+      <c r="G8" s="28">
+        <f t="shared" ref="G8" si="7">HEX2DEC(MID(D8, 3, LEN(D8)-2))</f>
+        <v>33216</v>
+      </c>
+      <c r="H8" s="28">
+        <f t="shared" ref="H8" si="8">HEX2DEC(MID(E8, 3, LEN(E8)-2))</f>
+        <v>64</v>
+      </c>
+      <c r="I8" s="28">
+        <f t="shared" ref="I8" si="9">G8+H8</f>
         <v>33280</v>
       </c>
-      <c r="H8" s="24">
-        <f t="shared" si="7"/>
-        <v>96</v>
-      </c>
-      <c r="I8" s="24">
-        <f>G8+H8</f>
-        <v>33376</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>27</v>
+      <c r="J8" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L8" s="29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M8" s="29">
         <v>256</v>
@@ -1711,34 +1717,34 @@
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B9" s="25"/>
       <c r="C9" s="27"/>
-      <c r="D9" s="28" t="str">
+      <c r="D9" s="24" t="str">
         <f t="shared" si="1"/>
+        <v>0x8200</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I9))</f>
         <v>0x8260</v>
       </c>
-      <c r="E9" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="F9" s="28" t="str">
-        <f t="shared" ref="F9" si="8">_xlfn.CONCAT("0x",DEC2HEX(I9))</f>
-        <v>0x8300</v>
-      </c>
-      <c r="G9" s="28">
-        <f t="shared" si="7"/>
+      <c r="G9" s="24">
+        <f t="shared" ref="G9:H11" si="10">HEX2DEC(MID(D9, 3, LEN(D9)-2))</f>
+        <v>33280</v>
+      </c>
+      <c r="H9" s="24">
+        <f t="shared" si="10"/>
+        <v>96</v>
+      </c>
+      <c r="I9" s="24">
+        <f>G9+H9</f>
         <v>33376</v>
       </c>
-      <c r="H9" s="28">
-        <f t="shared" si="7"/>
-        <v>160</v>
-      </c>
-      <c r="I9" s="28">
-        <f>G9+H9</f>
-        <v>33536</v>
-      </c>
-      <c r="J9" s="28" t="s">
-        <v>30</v>
+      <c r="J9" s="24" t="s">
+        <v>27</v>
       </c>
       <c r="L9" s="19" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M9" s="19">
         <v>8</v>
@@ -1747,34 +1753,34 @@
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10" s="25"/>
       <c r="C10" s="27"/>
-      <c r="D10" s="24" t="str">
+      <c r="D10" s="28" t="str">
         <f t="shared" si="1"/>
+        <v>0x8260</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="28" t="str">
+        <f t="shared" ref="F10" si="11">_xlfn.CONCAT("0x",DEC2HEX(I10))</f>
         <v>0x8300</v>
       </c>
-      <c r="E10" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I10))</f>
-        <v>0x8360</v>
-      </c>
-      <c r="G10" s="24">
-        <f t="shared" si="7"/>
+      <c r="G10" s="28">
+        <f t="shared" si="10"/>
+        <v>33376</v>
+      </c>
+      <c r="H10" s="28">
+        <f t="shared" si="10"/>
+        <v>160</v>
+      </c>
+      <c r="I10" s="28">
+        <f>G10+H10</f>
         <v>33536</v>
       </c>
-      <c r="H10" s="24">
-        <f t="shared" si="7"/>
-        <v>96</v>
-      </c>
-      <c r="I10" s="24">
-        <f>G10+H10</f>
-        <v>33632</v>
-      </c>
-      <c r="J10" s="24" t="s">
-        <v>26</v>
+      <c r="J10" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L10" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="M10" s="19">
         <v>8</v>
@@ -1783,34 +1789,34 @@
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11" s="25"/>
       <c r="C11" s="27"/>
-      <c r="D11" s="28" t="str">
+      <c r="D11" s="24" t="str">
         <f t="shared" si="1"/>
+        <v>0x8300</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I11))</f>
         <v>0x8360</v>
       </c>
-      <c r="E11" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="28" t="str">
-        <f t="shared" ref="F11" si="9">_xlfn.CONCAT("0x",DEC2HEX(I11))</f>
-        <v>0x8400</v>
-      </c>
-      <c r="G11" s="28">
-        <f t="shared" ref="G11" si="10">HEX2DEC(MID(D11, 3, LEN(D11)-2))</f>
+      <c r="G11" s="24">
+        <f t="shared" si="10"/>
+        <v>33536</v>
+      </c>
+      <c r="H11" s="24">
+        <f t="shared" si="10"/>
+        <v>96</v>
+      </c>
+      <c r="I11" s="24">
+        <f>G11+H11</f>
         <v>33632</v>
       </c>
-      <c r="H11" s="28">
-        <f t="shared" ref="H11" si="11">HEX2DEC(MID(E11, 3, LEN(E11)-2))</f>
-        <v>160</v>
-      </c>
-      <c r="I11" s="28">
-        <f t="shared" ref="I11" si="12">G11+H11</f>
-        <v>33792</v>
-      </c>
-      <c r="J11" s="28" t="s">
-        <v>30</v>
+      <c r="J11" s="24" t="s">
+        <v>26</v>
       </c>
       <c r="L11" s="19" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M11" s="19">
         <v>1</v>
@@ -1819,34 +1825,34 @@
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12" s="25"/>
       <c r="C12" s="27"/>
-      <c r="D12" s="24" t="str">
+      <c r="D12" s="28" t="str">
         <f t="shared" si="1"/>
+        <v>0x8360</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="28" t="str">
+        <f t="shared" ref="F12" si="12">_xlfn.CONCAT("0x",DEC2HEX(I12))</f>
         <v>0x8400</v>
       </c>
-      <c r="E12" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I12))</f>
-        <v>0x8430</v>
-      </c>
-      <c r="G12" s="24">
-        <f t="shared" ref="G12:H14" si="13">HEX2DEC(MID(D12, 3, LEN(D12)-2))</f>
+      <c r="G12" s="28">
+        <f t="shared" ref="G12" si="13">HEX2DEC(MID(D12, 3, LEN(D12)-2))</f>
+        <v>33632</v>
+      </c>
+      <c r="H12" s="28">
+        <f t="shared" ref="H12" si="14">HEX2DEC(MID(E12, 3, LEN(E12)-2))</f>
+        <v>160</v>
+      </c>
+      <c r="I12" s="28">
+        <f t="shared" ref="I12" si="15">G12+H12</f>
         <v>33792</v>
       </c>
-      <c r="H12" s="24">
-        <f t="shared" si="13"/>
-        <v>48</v>
-      </c>
-      <c r="I12" s="24">
-        <f>G12+H12</f>
-        <v>33840</v>
-      </c>
-      <c r="J12" s="24" t="s">
-        <v>25</v>
+      <c r="J12" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L12" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="M12" s="30">
         <f>M9*M10*M11</f>
@@ -1856,34 +1862,34 @@
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" s="25"/>
       <c r="C13" s="27"/>
-      <c r="D13" s="28" t="str">
+      <c r="D13" s="24" t="str">
         <f t="shared" si="1"/>
+        <v>0x8400</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I13))</f>
         <v>0x8430</v>
       </c>
-      <c r="E13" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="28" t="str">
-        <f t="shared" ref="F13" si="14">_xlfn.CONCAT("0x",DEC2HEX(I13))</f>
-        <v>0x8500</v>
-      </c>
-      <c r="G13" s="28">
-        <f t="shared" si="13"/>
+      <c r="G13" s="24">
+        <f t="shared" ref="G13:H15" si="16">HEX2DEC(MID(D13, 3, LEN(D13)-2))</f>
+        <v>33792</v>
+      </c>
+      <c r="H13" s="24">
+        <f t="shared" si="16"/>
+        <v>48</v>
+      </c>
+      <c r="I13" s="24">
+        <f>G13+H13</f>
         <v>33840</v>
       </c>
-      <c r="H13" s="28">
-        <f t="shared" si="13"/>
-        <v>208</v>
-      </c>
-      <c r="I13" s="28">
-        <f>G13+H13</f>
-        <v>34048</v>
-      </c>
-      <c r="J13" s="28" t="s">
-        <v>30</v>
+      <c r="J13" s="24" t="s">
+        <v>25</v>
       </c>
       <c r="L13" s="19" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="M13" s="19">
         <f>M12/8</f>
@@ -1893,34 +1899,34 @@
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B14" s="25"/>
       <c r="C14" s="27"/>
-      <c r="D14" s="24" t="str">
+      <c r="D14" s="28" t="str">
         <f t="shared" si="1"/>
+        <v>0x8430</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="28" t="str">
+        <f t="shared" ref="F14" si="17">_xlfn.CONCAT("0x",DEC2HEX(I14))</f>
         <v>0x8500</v>
       </c>
-      <c r="E14" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I14))</f>
-        <v>0x8560</v>
-      </c>
-      <c r="G14" s="24">
-        <f t="shared" si="13"/>
+      <c r="G14" s="28">
+        <f t="shared" si="16"/>
+        <v>33840</v>
+      </c>
+      <c r="H14" s="28">
+        <f t="shared" si="16"/>
+        <v>208</v>
+      </c>
+      <c r="I14" s="28">
+        <f>G14+H14</f>
         <v>34048</v>
       </c>
-      <c r="H14" s="24">
-        <f t="shared" si="13"/>
-        <v>96</v>
-      </c>
-      <c r="I14" s="24">
-        <f>G14+H14</f>
-        <v>34144</v>
-      </c>
-      <c r="J14" s="24" t="s">
-        <v>24</v>
+      <c r="J14" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L14" s="30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="M14" s="30">
         <f>M8*M13</f>
@@ -1930,97 +1936,97 @@
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B15" s="25"/>
       <c r="C15" s="27"/>
-      <c r="D15" s="28" t="str">
+      <c r="D15" s="24" t="str">
         <f t="shared" si="1"/>
+        <v>0x8500</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I15))</f>
         <v>0x8560</v>
       </c>
-      <c r="E15" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="28" t="str">
-        <f t="shared" ref="F15" si="15">_xlfn.CONCAT("0x",DEC2HEX(I15))</f>
-        <v>0x8600</v>
-      </c>
-      <c r="G15" s="28">
-        <f t="shared" ref="G15" si="16">HEX2DEC(MID(D15, 3, LEN(D15)-2))</f>
+      <c r="G15" s="24">
+        <f t="shared" si="16"/>
+        <v>34048</v>
+      </c>
+      <c r="H15" s="24">
+        <f t="shared" si="16"/>
+        <v>96</v>
+      </c>
+      <c r="I15" s="24">
+        <f>G15+H15</f>
         <v>34144</v>
       </c>
-      <c r="H15" s="28">
-        <f t="shared" ref="H15" si="17">HEX2DEC(MID(E15, 3, LEN(E15)-2))</f>
-        <v>160</v>
-      </c>
-      <c r="I15" s="28">
-        <f t="shared" ref="I15" si="18">G15+H15</f>
-        <v>34304</v>
-      </c>
-      <c r="J15" s="28" t="s">
-        <v>30</v>
+      <c r="J15" s="24" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B16" s="25"/>
       <c r="C16" s="27"/>
-      <c r="D16" s="24" t="str">
+      <c r="D16" s="28" t="str">
         <f t="shared" si="1"/>
+        <v>0x8560</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="28" t="str">
+        <f t="shared" ref="F16" si="18">_xlfn.CONCAT("0x",DEC2HEX(I16))</f>
         <v>0x8600</v>
       </c>
-      <c r="E16" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I16))</f>
-        <v>0x860C</v>
-      </c>
-      <c r="G16" s="24">
-        <f t="shared" ref="G16:H18" si="19">HEX2DEC(MID(D16, 3, LEN(D16)-2))</f>
+      <c r="G16" s="28">
+        <f t="shared" ref="G16" si="19">HEX2DEC(MID(D16, 3, LEN(D16)-2))</f>
+        <v>34144</v>
+      </c>
+      <c r="H16" s="28">
+        <f t="shared" ref="H16" si="20">HEX2DEC(MID(E16, 3, LEN(E16)-2))</f>
+        <v>160</v>
+      </c>
+      <c r="I16" s="28">
+        <f t="shared" ref="I16" si="21">G16+H16</f>
         <v>34304</v>
       </c>
-      <c r="H16" s="24">
-        <f t="shared" si="19"/>
-        <v>12</v>
-      </c>
-      <c r="I16" s="24">
-        <f>G16+H16</f>
-        <v>34316</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>23</v>
+      <c r="J16" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L16" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="25"/>
       <c r="C17" s="27"/>
-      <c r="D17" s="28" t="str">
+      <c r="D17" s="24" t="str">
         <f t="shared" si="1"/>
+        <v>0x8600</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I17))</f>
         <v>0x860C</v>
       </c>
-      <c r="E17" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="28" t="str">
-        <f t="shared" ref="F17" si="20">_xlfn.CONCAT("0x",DEC2HEX(I17))</f>
-        <v>0x8700</v>
-      </c>
-      <c r="G17" s="28">
-        <f t="shared" si="19"/>
+      <c r="G17" s="24">
+        <f t="shared" ref="G17:H19" si="22">HEX2DEC(MID(D17, 3, LEN(D17)-2))</f>
+        <v>34304</v>
+      </c>
+      <c r="H17" s="24">
+        <f t="shared" si="22"/>
+        <v>12</v>
+      </c>
+      <c r="I17" s="24">
+        <f>G17+H17</f>
         <v>34316</v>
       </c>
-      <c r="H17" s="28">
-        <f t="shared" si="19"/>
-        <v>244</v>
-      </c>
-      <c r="I17" s="28">
-        <f>G17+H17</f>
-        <v>34560</v>
-      </c>
-      <c r="J17" s="28" t="s">
-        <v>30</v>
+      <c r="J17" s="24" t="s">
+        <v>23</v>
       </c>
       <c r="L17" s="29" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M17" s="29">
         <v>4</v>
@@ -2029,73 +2035,73 @@
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="25"/>
       <c r="C18" s="27"/>
-      <c r="D18" s="24" t="str">
+      <c r="D18" s="28" t="str">
         <f t="shared" si="1"/>
+        <v>0x860C</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>40</v>
+      </c>
+      <c r="F18" s="28" t="str">
+        <f t="shared" ref="F18" si="23">_xlfn.CONCAT("0x",DEC2HEX(I18))</f>
         <v>0x8700</v>
       </c>
-      <c r="E18" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I18))</f>
-        <v>0x8730</v>
-      </c>
-      <c r="G18" s="24">
-        <f t="shared" si="19"/>
+      <c r="G18" s="28">
+        <f t="shared" si="22"/>
+        <v>34316</v>
+      </c>
+      <c r="H18" s="28">
+        <f t="shared" si="22"/>
+        <v>244</v>
+      </c>
+      <c r="I18" s="28">
+        <f>G18+H18</f>
         <v>34560</v>
       </c>
-      <c r="H18" s="24">
-        <f t="shared" si="19"/>
-        <v>48</v>
-      </c>
-      <c r="I18" s="24">
-        <f>G18+H18</f>
-        <v>34608</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>22</v>
+      <c r="J18" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L18" s="19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="M18" s="19">
         <v>16</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="25"/>
       <c r="C19" s="27"/>
-      <c r="D19" s="28" t="str">
+      <c r="D19" s="24" t="str">
         <f t="shared" si="1"/>
+        <v>0x8700</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I19))</f>
         <v>0x8730</v>
       </c>
-      <c r="E19" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="28" t="str">
-        <f t="shared" ref="F19" si="21">_xlfn.CONCAT("0x",DEC2HEX(I19))</f>
-        <v>0x8800</v>
-      </c>
-      <c r="G19" s="28">
-        <f t="shared" ref="G19" si="22">HEX2DEC(MID(D19, 3, LEN(D19)-2))</f>
+      <c r="G19" s="24">
+        <f t="shared" si="22"/>
+        <v>34560</v>
+      </c>
+      <c r="H19" s="24">
+        <f t="shared" si="22"/>
+        <v>48</v>
+      </c>
+      <c r="I19" s="24">
+        <f>G19+H19</f>
         <v>34608</v>
       </c>
-      <c r="H19" s="28">
-        <f t="shared" ref="H19" si="23">HEX2DEC(MID(E19, 3, LEN(E19)-2))</f>
-        <v>208</v>
-      </c>
-      <c r="I19" s="28">
-        <f t="shared" ref="I19" si="24">G19+H19</f>
-        <v>34816</v>
-      </c>
-      <c r="J19" s="28" t="s">
-        <v>30</v>
+      <c r="J19" s="24" t="s">
+        <v>22</v>
       </c>
       <c r="L19" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="M19" s="19">
         <v>32</v>
@@ -2104,34 +2110,34 @@
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="25"/>
       <c r="C20" s="27"/>
-      <c r="D20" s="24" t="str">
+      <c r="D20" s="28" t="str">
         <f t="shared" si="1"/>
+        <v>0x8730</v>
+      </c>
+      <c r="E20" s="28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="28" t="str">
+        <f t="shared" ref="F20" si="24">_xlfn.CONCAT("0x",DEC2HEX(I20))</f>
         <v>0x8800</v>
       </c>
-      <c r="E20" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F20" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I20))</f>
-        <v>0x8821</v>
-      </c>
-      <c r="G20" s="24">
-        <f t="shared" ref="G20:H36" si="25">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
+      <c r="G20" s="28">
+        <f t="shared" ref="G20" si="25">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
+        <v>34608</v>
+      </c>
+      <c r="H20" s="28">
+        <f t="shared" ref="H20" si="26">HEX2DEC(MID(E20, 3, LEN(E20)-2))</f>
+        <v>208</v>
+      </c>
+      <c r="I20" s="28">
+        <f t="shared" ref="I20" si="27">G20+H20</f>
         <v>34816</v>
       </c>
-      <c r="H20" s="24">
-        <f t="shared" si="25"/>
-        <v>33</v>
-      </c>
-      <c r="I20" s="24">
-        <f>G20+H20</f>
-        <v>34849</v>
-      </c>
-      <c r="J20" s="24" t="s">
-        <v>21</v>
+      <c r="J20" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L20" s="30" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M20" s="30">
         <f>M18*M19</f>
@@ -2141,34 +2147,34 @@
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" s="25"/>
       <c r="C21" s="27"/>
-      <c r="D21" s="28" t="str">
+      <c r="D21" s="24" t="str">
         <f t="shared" si="1"/>
+        <v>0x8800</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I21))</f>
         <v>0x8821</v>
       </c>
-      <c r="E21" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="F21" s="28" t="str">
-        <f t="shared" ref="F21" si="26">_xlfn.CONCAT("0x",DEC2HEX(I21))</f>
-        <v>0x8900</v>
-      </c>
-      <c r="G21" s="28">
-        <f t="shared" si="25"/>
+      <c r="G21" s="24">
+        <f t="shared" ref="G21:H37" si="28">HEX2DEC(MID(D21, 3, LEN(D21)-2))</f>
+        <v>34816</v>
+      </c>
+      <c r="H21" s="24">
+        <f t="shared" si="28"/>
+        <v>33</v>
+      </c>
+      <c r="I21" s="24">
+        <f>G21+H21</f>
         <v>34849</v>
       </c>
-      <c r="H21" s="28">
-        <f t="shared" si="25"/>
-        <v>223</v>
-      </c>
-      <c r="I21" s="28">
-        <f>G21+H21</f>
-        <v>35072</v>
-      </c>
-      <c r="J21" s="28" t="s">
-        <v>30</v>
+      <c r="J21" s="24" t="s">
+        <v>21</v>
       </c>
       <c r="L21" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M21" s="19">
         <f>M20/8</f>
@@ -2178,34 +2184,34 @@
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="25"/>
       <c r="C22" s="27"/>
-      <c r="D22" s="24" t="str">
+      <c r="D22" s="28" t="str">
         <f t="shared" si="1"/>
+        <v>0x8821</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="28" t="str">
+        <f t="shared" ref="F22" si="29">_xlfn.CONCAT("0x",DEC2HEX(I22))</f>
         <v>0x8900</v>
       </c>
-      <c r="E22" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I22))</f>
-        <v>0x8911</v>
-      </c>
-      <c r="G22" s="24">
-        <f t="shared" si="25"/>
+      <c r="G22" s="28">
+        <f t="shared" si="28"/>
+        <v>34849</v>
+      </c>
+      <c r="H22" s="28">
+        <f t="shared" si="28"/>
+        <v>223</v>
+      </c>
+      <c r="I22" s="28">
+        <f>G22+H22</f>
         <v>35072</v>
       </c>
-      <c r="H22" s="24">
-        <f t="shared" si="25"/>
-        <v>17</v>
-      </c>
-      <c r="I22" s="24">
-        <f>G22+H22</f>
-        <v>35089</v>
-      </c>
-      <c r="J22" s="24" t="s">
-        <v>20</v>
+      <c r="J22" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L22" s="30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M22" s="30">
         <f>M21*M17</f>
@@ -2215,99 +2221,99 @@
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" s="25"/>
       <c r="C23" s="27"/>
-      <c r="D23" s="28" t="str">
-        <f>F22</f>
+      <c r="D23" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>0x8900</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I23))</f>
         <v>0x8911</v>
       </c>
-      <c r="E23" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="F23" s="28" t="str">
-        <f t="shared" ref="F23" si="27">_xlfn.CONCAT("0x",DEC2HEX(I23))</f>
-        <v>0x8A00</v>
-      </c>
-      <c r="G23" s="28">
-        <f t="shared" si="25"/>
+      <c r="G23" s="24">
+        <f t="shared" si="28"/>
+        <v>35072</v>
+      </c>
+      <c r="H23" s="24">
+        <f t="shared" si="28"/>
+        <v>17</v>
+      </c>
+      <c r="I23" s="24">
+        <f>G23+H23</f>
         <v>35089</v>
       </c>
-      <c r="H23" s="28">
-        <f t="shared" si="25"/>
-        <v>239</v>
-      </c>
-      <c r="I23" s="28">
-        <f t="shared" ref="I23" si="28">G23+H23</f>
-        <v>35328</v>
-      </c>
-      <c r="J23" s="28" t="s">
-        <v>30</v>
+      <c r="J23" s="24" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" s="25"/>
       <c r="C24" s="27"/>
-      <c r="D24" s="24" t="s">
+      <c r="D24" s="28" t="str">
+        <f>F23</f>
+        <v>0x8911</v>
+      </c>
+      <c r="E24" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="E24" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="F24" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I24))</f>
-        <v>0x8A10</v>
-      </c>
-      <c r="G24" s="24">
-        <f t="shared" si="25"/>
+      <c r="F24" s="28" t="str">
+        <f t="shared" ref="F24" si="30">_xlfn.CONCAT("0x",DEC2HEX(I24))</f>
+        <v>0x8A00</v>
+      </c>
+      <c r="G24" s="28">
+        <f t="shared" si="28"/>
+        <v>35089</v>
+      </c>
+      <c r="H24" s="28">
+        <f t="shared" si="28"/>
+        <v>239</v>
+      </c>
+      <c r="I24" s="28">
+        <f t="shared" ref="I24" si="31">G24+H24</f>
         <v>35328</v>
       </c>
-      <c r="H24" s="24">
-        <f t="shared" si="25"/>
-        <v>16</v>
-      </c>
-      <c r="I24" s="24">
-        <f>G24+H24</f>
-        <v>35344</v>
-      </c>
-      <c r="J24" s="24" t="s">
-        <v>90</v>
+      <c r="J24" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L24" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N24" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="25"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="24" t="str">
-        <f t="shared" ref="D25:D31" si="29">F24</f>
-        <v>0x8A10</v>
+      <c r="C25" s="27"/>
+      <c r="D25" s="24" t="s">
+        <v>84</v>
       </c>
       <c r="E25" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F25" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I25))</f>
-        <v>0x8A20</v>
+        <v>0x8A10</v>
       </c>
       <c r="G25" s="24">
-        <f t="shared" ref="G25:G26" si="30">HEX2DEC(MID(D25, 3, LEN(D25)-2))</f>
-        <v>35344</v>
+        <f t="shared" si="28"/>
+        <v>35328</v>
       </c>
       <c r="H25" s="24">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="I25" s="24">
         <f>G25+H25</f>
-        <v>35360</v>
+        <v>35344</v>
       </c>
       <c r="J25" s="24" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="L25" s="29" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M25" s="29">
         <v>64</v>
@@ -2315,35 +2321,35 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="25"/>
-      <c r="C26" s="51"/>
+      <c r="C26" s="52"/>
       <c r="D26" s="24" t="str">
-        <f t="shared" si="29"/>
-        <v>0x8A20</v>
+        <f t="shared" ref="D26:D32" si="32">F25</f>
+        <v>0x8A10</v>
       </c>
       <c r="E26" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F26" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I26))</f>
-        <v>0x8A30</v>
+        <v>0x8A20</v>
       </c>
       <c r="G26" s="24">
-        <f t="shared" si="30"/>
-        <v>35360</v>
+        <f t="shared" ref="G26:G27" si="33">HEX2DEC(MID(D26, 3, LEN(D26)-2))</f>
+        <v>35344</v>
       </c>
       <c r="H26" s="24">
-        <f t="shared" si="25"/>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="I26" s="24">
         <f>G26+H26</f>
-        <v>35376</v>
+        <v>35360</v>
       </c>
       <c r="J26" s="24" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="L26" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M26" s="19">
         <v>16</v>
@@ -2351,35 +2357,35 @@
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="25"/>
-      <c r="C27" s="50"/>
+      <c r="C27" s="52"/>
       <c r="D27" s="24" t="str">
-        <f>F26</f>
+        <f t="shared" si="32"/>
+        <v>0x8A20</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I27))</f>
         <v>0x8A30</v>
       </c>
-      <c r="E27" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="24" t="str">
-        <f t="shared" ref="F27" si="31">_xlfn.CONCAT("0x",DEC2HEX(I27))</f>
-        <v>0x8A31</v>
-      </c>
       <c r="G27" s="24">
-        <f>HEX2DEC(MID(D27, 3, LEN(D27)-2))</f>
+        <f t="shared" si="33"/>
+        <v>35360</v>
+      </c>
+      <c r="H27" s="24">
+        <f t="shared" si="28"/>
+        <v>16</v>
+      </c>
+      <c r="I27" s="24">
+        <f>G27+H27</f>
         <v>35376</v>
       </c>
-      <c r="H27" s="24">
-        <f t="shared" ref="H27" si="32">HEX2DEC(MID(E27, 3, LEN(E27)-2))</f>
-        <v>1</v>
-      </c>
-      <c r="I27" s="24">
-        <f t="shared" ref="I27" si="33">G27+H27</f>
-        <v>35377</v>
-      </c>
       <c r="J27" s="24" t="s">
-        <v>167</v>
+        <v>88</v>
       </c>
       <c r="L27" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="M27" s="19">
         <v>16</v>
@@ -2387,21 +2393,21 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="25"/>
-      <c r="C28" s="46"/>
+      <c r="C28" s="50"/>
       <c r="D28" s="24" t="str">
         <f>F27</f>
-        <v>0x8A31</v>
+        <v>0x8A30</v>
       </c>
       <c r="E28" s="24" t="s">
         <v>10</v>
       </c>
       <c r="F28" s="24" t="str">
         <f t="shared" ref="F28" si="34">_xlfn.CONCAT("0x",DEC2HEX(I28))</f>
-        <v>0x8A32</v>
+        <v>0x8A31</v>
       </c>
       <c r="G28" s="24">
         <f>HEX2DEC(MID(D28, 3, LEN(D28)-2))</f>
-        <v>35377</v>
+        <v>35376</v>
       </c>
       <c r="H28" s="24">
         <f t="shared" ref="H28" si="35">HEX2DEC(MID(E28, 3, LEN(E28)-2))</f>
@@ -2409,52 +2415,52 @@
       </c>
       <c r="I28" s="24">
         <f t="shared" ref="I28" si="36">G28+H28</f>
-        <v>35378</v>
+        <v>35377</v>
       </c>
       <c r="J28" s="24" t="s">
-        <v>215</v>
+        <v>166</v>
       </c>
       <c r="L28" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="M28" s="19">
         <v>8</v>
       </c>
       <c r="N28" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="25"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28" t="str">
+      <c r="C29" s="46"/>
+      <c r="D29" s="24" t="str">
         <f>F28</f>
+        <v>0x8A31</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="24" t="str">
+        <f t="shared" ref="F29" si="37">_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
         <v>0x8A32</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="G29" s="24">
+        <f>HEX2DEC(MID(D29, 3, LEN(D29)-2))</f>
+        <v>35377</v>
+      </c>
+      <c r="H29" s="24">
+        <f t="shared" ref="H29" si="38">HEX2DEC(MID(E29, 3, LEN(E29)-2))</f>
+        <v>1</v>
+      </c>
+      <c r="I29" s="24">
+        <f t="shared" ref="I29" si="39">G29+H29</f>
+        <v>35378</v>
+      </c>
+      <c r="J29" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="F29" s="28" t="str">
-        <f t="shared" ref="F29" si="37">_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
-        <v>0x8B00</v>
-      </c>
-      <c r="G29" s="28">
-        <f>HEX2DEC(MID(D29, 3, LEN(D29)-2))</f>
-        <v>35378</v>
-      </c>
-      <c r="H29" s="28">
-        <f t="shared" ref="H29" si="38">HEX2DEC(MID(E29, 3, LEN(E29)-2))</f>
-        <v>206</v>
-      </c>
-      <c r="I29" s="28">
-        <f t="shared" ref="I29" si="39">G29+H29</f>
-        <v>35584</v>
-      </c>
-      <c r="J29" s="28" t="s">
-        <v>30</v>
-      </c>
       <c r="L29" s="30" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M29" s="30">
         <f>M26*M27*M28</f>
@@ -2463,37 +2469,35 @@
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="25"/>
-      <c r="C30" s="52" t="s">
-        <v>156</v>
-      </c>
-      <c r="D30" s="24" t="str">
+      <c r="C30" s="28"/>
+      <c r="D30" s="28" t="str">
         <f>F29</f>
+        <v>0x8A32</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>213</v>
+      </c>
+      <c r="F30" s="28" t="str">
+        <f t="shared" ref="F30" si="40">_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
         <v>0x8B00</v>
       </c>
-      <c r="E30" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="F30" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
-        <v>0x8B10</v>
-      </c>
-      <c r="G30" s="24">
-        <f t="shared" ref="G30" si="40">HEX2DEC(MID(D30, 3, LEN(D30)-2))</f>
+      <c r="G30" s="28">
+        <f>HEX2DEC(MID(D30, 3, LEN(D30)-2))</f>
+        <v>35378</v>
+      </c>
+      <c r="H30" s="28">
+        <f t="shared" ref="H30" si="41">HEX2DEC(MID(E30, 3, LEN(E30)-2))</f>
+        <v>206</v>
+      </c>
+      <c r="I30" s="28">
+        <f t="shared" ref="I30" si="42">G30+H30</f>
         <v>35584</v>
       </c>
-      <c r="H30" s="24">
-        <f t="shared" si="25"/>
-        <v>16</v>
-      </c>
-      <c r="I30" s="24">
-        <f>G30+H30</f>
-        <v>35600</v>
-      </c>
-      <c r="J30" s="24" t="s">
-        <v>170</v>
+      <c r="J30" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L30" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="M30" s="19">
         <f>M29/8</f>
@@ -2502,35 +2506,37 @@
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" s="25"/>
-      <c r="C31" s="51"/>
+      <c r="C31" s="53" t="s">
+        <v>155</v>
+      </c>
       <c r="D31" s="24" t="str">
-        <f t="shared" si="29"/>
-        <v>0x8B10</v>
+        <f>F30</f>
+        <v>0x8B00</v>
       </c>
       <c r="E31" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F31" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I31))</f>
-        <v>0x8B20</v>
+        <v>0x8B10</v>
       </c>
       <c r="G31" s="24">
-        <f t="shared" ref="G31" si="41">HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
-        <v>35600</v>
+        <f t="shared" ref="G31" si="43">HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
+        <v>35584</v>
       </c>
       <c r="H31" s="24">
-        <f t="shared" ref="H31" si="42">HEX2DEC(MID(E31, 3, LEN(E31)-2))</f>
+        <f t="shared" si="28"/>
         <v>16</v>
       </c>
       <c r="I31" s="24">
         <f>G31+H31</f>
-        <v>35616</v>
+        <v>35600</v>
       </c>
       <c r="J31" s="24" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L31" s="30" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M31" s="30">
         <f>M25*M30</f>
@@ -2539,138 +2545,138 @@
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B32" s="25"/>
-      <c r="C32" s="28"/>
-      <c r="D32" s="28" t="str">
-        <f>F31</f>
+      <c r="C32" s="52"/>
+      <c r="D32" s="24" t="str">
+        <f t="shared" si="32"/>
+        <v>0x8B10</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="F32" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
         <v>0x8B20</v>
       </c>
-      <c r="E32" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="F32" s="28" t="str">
-        <f t="shared" ref="F32" si="43">_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
-        <v>0x8C00</v>
-      </c>
-      <c r="G32" s="28">
-        <f t="shared" ref="G32:G34" si="44">HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
+      <c r="G32" s="24">
+        <f t="shared" ref="G32" si="44">HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
+        <v>35600</v>
+      </c>
+      <c r="H32" s="24">
+        <f t="shared" ref="H32" si="45">HEX2DEC(MID(E32, 3, LEN(E32)-2))</f>
+        <v>16</v>
+      </c>
+      <c r="I32" s="24">
+        <f>G32+H32</f>
         <v>35616</v>
       </c>
-      <c r="H32" s="28">
-        <f t="shared" ref="H32:H35" si="45">HEX2DEC(MID(E32, 3, LEN(E32)-2))</f>
-        <v>224</v>
-      </c>
-      <c r="I32" s="28">
-        <f t="shared" ref="I32" si="46">G32+H32</f>
-        <v>35840</v>
-      </c>
-      <c r="J32" s="28" t="s">
-        <v>30</v>
+      <c r="J32" s="24" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="25"/>
-      <c r="C33" s="48" t="s">
-        <v>186</v>
-      </c>
-      <c r="D33" s="24" t="str">
+      <c r="C33" s="28"/>
+      <c r="D33" s="28" t="str">
         <f>F32</f>
+        <v>0x8B20</v>
+      </c>
+      <c r="E33" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="F33" s="28" t="str">
+        <f t="shared" ref="F33" si="46">_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
         <v>0x8C00</v>
       </c>
-      <c r="E33" s="24" t="str">
+      <c r="G33" s="28">
+        <f t="shared" ref="G33:G35" si="47">HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
+        <v>35616</v>
+      </c>
+      <c r="H33" s="28">
+        <f t="shared" ref="H33:H36" si="48">HEX2DEC(MID(E33, 3, LEN(E33)-2))</f>
+        <v>224</v>
+      </c>
+      <c r="I33" s="28">
+        <f t="shared" ref="I33" si="49">G33+H33</f>
+        <v>35840</v>
+      </c>
+      <c r="J33" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="L33" s="21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B34" s="25"/>
+      <c r="C34" s="48" t="s">
+        <v>185</v>
+      </c>
+      <c r="D34" s="24" t="str">
+        <f>F33</f>
+        <v>0x8C00</v>
+      </c>
+      <c r="E34" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M74))</f>
         <v>0x10</v>
       </c>
-      <c r="F33" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
+      <c r="F34" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
         <v>0x8C10</v>
       </c>
-      <c r="G33" s="24">
-        <f t="shared" ref="G33" si="47">HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
+      <c r="G34" s="24">
+        <f t="shared" ref="G34" si="50">HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
         <v>35840</v>
       </c>
-      <c r="H33" s="24">
-        <f t="shared" si="45"/>
+      <c r="H34" s="24">
+        <f t="shared" si="48"/>
         <v>16</v>
       </c>
-      <c r="I33" s="24">
-        <f>G33+H33</f>
+      <c r="I34" s="24">
+        <f>G34+H34</f>
         <v>35856</v>
       </c>
-      <c r="J33" s="24" t="s">
-        <v>188</v>
-      </c>
-      <c r="L33" s="21" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B34" s="25"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="24" t="str">
-        <f>F33</f>
+      <c r="J34" s="24" t="s">
+        <v>187</v>
+      </c>
+      <c r="L34" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="M34" s="29">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B35" s="25"/>
+      <c r="C35" s="49"/>
+      <c r="D35" s="24" t="str">
+        <f>F34</f>
         <v>0x8C10</v>
       </c>
-      <c r="E34" s="24" t="str">
+      <c r="E35" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M81))</f>
         <v>0x300</v>
       </c>
-      <c r="F34" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
+      <c r="F35" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
         <v>0x8F10</v>
       </c>
-      <c r="G34" s="24">
-        <f t="shared" si="44"/>
+      <c r="G35" s="24">
+        <f t="shared" si="47"/>
         <v>35856</v>
       </c>
-      <c r="H34" s="24">
-        <f t="shared" si="45"/>
+      <c r="H35" s="24">
+        <f t="shared" si="48"/>
         <v>768</v>
       </c>
-      <c r="I34" s="24">
-        <f>G34+H34</f>
+      <c r="I35" s="24">
+        <f>G35+H35</f>
         <v>36624</v>
       </c>
-      <c r="J34" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="L34" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="M34" s="29">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B35" s="25"/>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28" t="str">
-        <f>F34</f>
-        <v>0x8F10</v>
-      </c>
-      <c r="E35" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="F35" s="28" t="str">
-        <f t="shared" ref="F35" si="48">_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
-        <v>0x9000</v>
-      </c>
-      <c r="G35" s="28">
-        <f t="shared" ref="G35" si="49">HEX2DEC(MID(D35, 3, LEN(D35)-2))</f>
-        <v>36624</v>
-      </c>
-      <c r="H35" s="28">
-        <f t="shared" si="45"/>
-        <v>240</v>
-      </c>
-      <c r="I35" s="28">
-        <f t="shared" ref="I35" si="50">G35+H35</f>
-        <v>36864</v>
-      </c>
-      <c r="J35" s="28" t="s">
-        <v>30</v>
+      <c r="J35" s="24" t="s">
+        <v>192</v>
       </c>
       <c r="L35" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M35" s="19">
         <v>1</v>
@@ -2678,37 +2684,35 @@
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="25"/>
-      <c r="C36" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="D36" s="24" t="str">
+      <c r="C36" s="28"/>
+      <c r="D36" s="28" t="str">
         <f>F35</f>
+        <v>0x8F10</v>
+      </c>
+      <c r="E36" s="28" t="s">
+        <v>211</v>
+      </c>
+      <c r="F36" s="28" t="str">
+        <f t="shared" ref="F36" si="51">_xlfn.CONCAT("0x",DEC2HEX(I36))</f>
         <v>0x9000</v>
       </c>
-      <c r="E36" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I36))</f>
-        <v>0x9800</v>
-      </c>
-      <c r="G36" s="24">
-        <f>HEX2DEC(MID(D36, 3, LEN(D36)-2))</f>
+      <c r="G36" s="28">
+        <f t="shared" ref="G36" si="52">HEX2DEC(MID(D36, 3, LEN(D36)-2))</f>
+        <v>36624</v>
+      </c>
+      <c r="H36" s="28">
+        <f t="shared" si="48"/>
+        <v>240</v>
+      </c>
+      <c r="I36" s="28">
+        <f t="shared" ref="I36" si="53">G36+H36</f>
         <v>36864</v>
       </c>
-      <c r="H36" s="24">
-        <f t="shared" si="25"/>
-        <v>2048</v>
-      </c>
-      <c r="I36" s="24">
-        <f>G36+H36</f>
-        <v>38912</v>
-      </c>
-      <c r="J36" s="24" t="s">
-        <v>9</v>
+      <c r="J36" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L36" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="M36" s="19">
         <v>1</v>
@@ -2716,35 +2720,37 @@
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" s="25"/>
-      <c r="C37" s="34"/>
+      <c r="C37" s="32" t="s">
+        <v>47</v>
+      </c>
       <c r="D37" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v>0x9800</v>
+        <f>F36</f>
+        <v>0x9000</v>
       </c>
       <c r="E37" s="24" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I37))</f>
-        <v>0xA000</v>
+        <v>0x9800</v>
       </c>
       <c r="G37" s="24">
         <f>HEX2DEC(MID(D37, 3, LEN(D37)-2))</f>
-        <v>38912</v>
+        <v>36864</v>
       </c>
       <c r="H37" s="24">
-        <f>HEX2DEC(MID(E37, 3, LEN(E37)-2))</f>
+        <f t="shared" si="28"/>
         <v>2048</v>
       </c>
       <c r="I37" s="24">
         <f>G37+H37</f>
-        <v>40960</v>
+        <v>38912</v>
       </c>
       <c r="J37" s="24" t="s">
-        <v>46</v>
+        <v>9</v>
       </c>
       <c r="L37" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M37" s="19">
         <v>2</v>
@@ -2755,32 +2761,32 @@
       <c r="C38" s="34"/>
       <c r="D38" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0xA000</v>
+        <v>0x9800</v>
       </c>
       <c r="E38" s="24" t="s">
         <v>8</v>
       </c>
       <c r="F38" s="24" t="str">
-        <f t="shared" ref="F38" si="51">_xlfn.CONCAT("0x",DEC2HEX(I38))</f>
-        <v>0xA800</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I38))</f>
+        <v>0xA000</v>
       </c>
       <c r="G38" s="24">
-        <f t="shared" ref="G38" si="52">HEX2DEC(MID(D38, 3, LEN(D38)-2))</f>
+        <f>HEX2DEC(MID(D38, 3, LEN(D38)-2))</f>
+        <v>38912</v>
+      </c>
+      <c r="H38" s="24">
+        <f>HEX2DEC(MID(E38, 3, LEN(E38)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I38" s="24">
+        <f>G38+H38</f>
         <v>40960</v>
-      </c>
-      <c r="H38" s="24">
-        <f t="shared" ref="H38" si="53">HEX2DEC(MID(E38, 3, LEN(E38)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I38" s="24">
-        <f t="shared" ref="I38" si="54">G38+H38</f>
-        <v>43008</v>
       </c>
       <c r="J38" s="24" t="s">
         <v>45</v>
       </c>
       <c r="L38" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M38" s="19">
         <v>2</v>
@@ -2788,35 +2794,35 @@
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" s="25"/>
-      <c r="C39" s="35"/>
+      <c r="C39" s="34"/>
       <c r="D39" s="24" t="str">
         <f t="shared" si="1"/>
-        <v>0xA800</v>
+        <v>0xA000</v>
       </c>
       <c r="E39" s="24" t="s">
         <v>8</v>
       </c>
       <c r="F39" s="24" t="str">
-        <f t="shared" ref="F39" si="55">_xlfn.CONCAT("0x",DEC2HEX(I39))</f>
-        <v>0xB000</v>
+        <f t="shared" ref="F39" si="54">_xlfn.CONCAT("0x",DEC2HEX(I39))</f>
+        <v>0xA800</v>
       </c>
       <c r="G39" s="24">
-        <f t="shared" ref="G39" si="56">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
+        <f t="shared" ref="G39" si="55">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
+        <v>40960</v>
+      </c>
+      <c r="H39" s="24">
+        <f t="shared" ref="H39" si="56">HEX2DEC(MID(E39, 3, LEN(E39)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I39" s="24">
+        <f t="shared" ref="I39" si="57">G39+H39</f>
         <v>43008</v>
       </c>
-      <c r="H39" s="24">
-        <f t="shared" ref="H39" si="57">HEX2DEC(MID(E39, 3, LEN(E39)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I39" s="24">
-        <f t="shared" ref="I39" si="58">G39+H39</f>
-        <v>45056</v>
-      </c>
       <c r="J39" s="24" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="L39" s="47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M39" s="47">
         <v>1</v>
@@ -2824,74 +2830,74 @@
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B40" s="25"/>
-      <c r="C40" s="36" t="s">
-        <v>56</v>
-      </c>
+      <c r="C40" s="35"/>
       <c r="D40" s="24" t="str">
         <f t="shared" si="1"/>
+        <v>0xA800</v>
+      </c>
+      <c r="E40" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="24" t="str">
+        <f t="shared" ref="F40" si="58">_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
         <v>0xB000</v>
       </c>
-      <c r="E40" s="24" t="str">
+      <c r="G40" s="24">
+        <f t="shared" ref="G40" si="59">HEX2DEC(MID(D40, 3, LEN(D40)-2))</f>
+        <v>43008</v>
+      </c>
+      <c r="H40" s="24">
+        <f t="shared" ref="H40" si="60">HEX2DEC(MID(E40, 3, LEN(E40)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I40" s="24">
+        <f t="shared" ref="I40" si="61">G40+H40</f>
+        <v>45056</v>
+      </c>
+      <c r="J40" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="L40" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="M40" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B41" s="25"/>
+      <c r="C41" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB000</v>
+      </c>
+      <c r="E41" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M46))</f>
         <v>0x80</v>
       </c>
-      <c r="F40" s="24" t="str">
-        <f t="shared" ref="F40:F41" si="59">_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
+      <c r="F41" s="24" t="str">
+        <f t="shared" ref="F41:F42" si="62">_xlfn.CONCAT("0x",DEC2HEX(I41))</f>
         <v>0xB080</v>
       </c>
-      <c r="G40" s="24">
-        <f t="shared" ref="G40:G41" si="60">HEX2DEC(MID(D40, 3, LEN(D40)-2))</f>
+      <c r="G41" s="24">
+        <f t="shared" ref="G41:G42" si="63">HEX2DEC(MID(D41, 3, LEN(D41)-2))</f>
         <v>45056</v>
       </c>
-      <c r="H40" s="24">
-        <f t="shared" ref="H40:H41" si="61">HEX2DEC(MID(E40, 3, LEN(E40)-2))</f>
+      <c r="H41" s="24">
+        <f t="shared" ref="H41:H42" si="64">HEX2DEC(MID(E41, 3, LEN(E41)-2))</f>
         <v>128</v>
       </c>
-      <c r="I40" s="24">
-        <f t="shared" ref="I40:I41" si="62">G40+H40</f>
+      <c r="I41" s="24">
+        <f t="shared" ref="I41:I42" si="65">G41+H41</f>
         <v>45184</v>
       </c>
-      <c r="J40" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="L40" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="M40" s="19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B41" s="25"/>
-      <c r="C41" s="37"/>
-      <c r="D41" s="28" t="str">
-        <f t="shared" si="1"/>
-        <v>0xB080</v>
-      </c>
-      <c r="E41" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="F41" s="28" t="str">
-        <f t="shared" si="59"/>
-        <v>0xB400</v>
-      </c>
-      <c r="G41" s="28">
-        <f t="shared" si="60"/>
-        <v>45184</v>
-      </c>
-      <c r="H41" s="28">
-        <f t="shared" si="61"/>
-        <v>896</v>
-      </c>
-      <c r="I41" s="28">
-        <f t="shared" si="62"/>
-        <v>46080</v>
-      </c>
-      <c r="J41" s="28" t="s">
-        <v>30</v>
+      <c r="J41" s="24" t="s">
+        <v>56</v>
       </c>
       <c r="L41" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M41" s="19">
         <v>6</v>
@@ -2900,35 +2906,34 @@
     <row r="42" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B42" s="25"/>
       <c r="C42" s="37"/>
-      <c r="D42" s="24" t="str">
-        <f t="shared" ref="D42:D43" si="63">F41</f>
+      <c r="D42" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>0xB080</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" s="28" t="str">
+        <f t="shared" si="62"/>
         <v>0xB400</v>
       </c>
-      <c r="E42" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M59))</f>
-        <v>0x4</v>
-      </c>
-      <c r="F42" s="24" t="str">
-        <f t="shared" ref="F42:F43" si="64">_xlfn.CONCAT("0x",DEC2HEX(I42))</f>
-        <v>0xB404</v>
-      </c>
-      <c r="G42" s="24">
-        <f t="shared" ref="G42:G43" si="65">HEX2DEC(MID(D42, 3, LEN(D42)-2))</f>
+      <c r="G42" s="28">
+        <f t="shared" si="63"/>
+        <v>45184</v>
+      </c>
+      <c r="H42" s="28">
+        <f t="shared" si="64"/>
+        <v>896</v>
+      </c>
+      <c r="I42" s="28">
+        <f t="shared" si="65"/>
         <v>46080</v>
       </c>
-      <c r="H42" s="24">
-        <f t="shared" ref="H42:H43" si="66">HEX2DEC(MID(E42, 3, LEN(E42)-2))</f>
-        <v>4</v>
-      </c>
-      <c r="I42" s="24">
-        <f t="shared" ref="I42:I43" si="67">G42+H42</f>
-        <v>46084</v>
-      </c>
-      <c r="J42" s="24" t="s">
-        <v>91</v>
+      <c r="J42" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L42" s="47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M42" s="47">
         <v>1</v>
@@ -2937,34 +2942,35 @@
     <row r="43" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B43" s="25"/>
       <c r="C43" s="37"/>
-      <c r="D43" s="28" t="str">
-        <f t="shared" si="63"/>
+      <c r="D43" s="24" t="str">
+        <f t="shared" ref="D43:D44" si="66">F42</f>
+        <v>0xB400</v>
+      </c>
+      <c r="E43" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M59))</f>
+        <v>0x4</v>
+      </c>
+      <c r="F43" s="24" t="str">
+        <f t="shared" ref="F43:F44" si="67">_xlfn.CONCAT("0x",DEC2HEX(I43))</f>
         <v>0xB404</v>
       </c>
-      <c r="E43" s="28" t="s">
-        <v>132</v>
-      </c>
-      <c r="F43" s="28" t="str">
-        <f t="shared" si="64"/>
-        <v>0xB800</v>
-      </c>
-      <c r="G43" s="28">
-        <f t="shared" si="65"/>
+      <c r="G43" s="24">
+        <f t="shared" ref="G43:G44" si="68">HEX2DEC(MID(D43, 3, LEN(D43)-2))</f>
+        <v>46080</v>
+      </c>
+      <c r="H43" s="24">
+        <f t="shared" ref="H43:H44" si="69">HEX2DEC(MID(E43, 3, LEN(E43)-2))</f>
+        <v>4</v>
+      </c>
+      <c r="I43" s="24">
+        <f t="shared" ref="I43:I44" si="70">G43+H43</f>
         <v>46084</v>
       </c>
-      <c r="H43" s="28">
-        <f t="shared" si="66"/>
-        <v>1020</v>
-      </c>
-      <c r="I43" s="28">
-        <f t="shared" si="67"/>
-        <v>47104</v>
-      </c>
-      <c r="J43" s="28" t="s">
-        <v>30</v>
+      <c r="J43" s="24" t="s">
+        <v>90</v>
       </c>
       <c r="L43" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M43" s="19">
         <v>9</v>
@@ -2972,33 +2978,32 @@
     </row>
     <row r="44" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B44" s="39"/>
-      <c r="C44" s="38"/>
-      <c r="D44" s="24" t="str">
-        <f>F43</f>
+      <c r="C44" s="37"/>
+      <c r="D44" s="28" t="str">
+        <f t="shared" si="66"/>
+        <v>0xB404</v>
+      </c>
+      <c r="E44" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="F44" s="28" t="str">
+        <f t="shared" si="67"/>
         <v>0xB800</v>
       </c>
-      <c r="E44" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M53))</f>
-        <v>0x800</v>
-      </c>
-      <c r="F44" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I44))</f>
-        <v>0xC000</v>
-      </c>
-      <c r="G44" s="24">
-        <f t="shared" ref="G44:H46" si="68">HEX2DEC(MID(D44, 3, LEN(D44)-2))</f>
+      <c r="G44" s="28">
+        <f t="shared" si="68"/>
+        <v>46084</v>
+      </c>
+      <c r="H44" s="28">
+        <f t="shared" si="69"/>
+        <v>1020</v>
+      </c>
+      <c r="I44" s="28">
+        <f t="shared" si="70"/>
         <v>47104</v>
       </c>
-      <c r="H44" s="24">
-        <f t="shared" si="68"/>
-        <v>2048</v>
-      </c>
-      <c r="I44" s="24">
-        <f>G44+H44</f>
-        <v>49152</v>
-      </c>
-      <c r="J44" s="24" t="s">
-        <v>76</v>
+      <c r="J44" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="L44" s="30" t="s">
         <v>4</v>
@@ -3011,36 +3016,35 @@
     </row>
     <row r="45" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B45" s="41" t="s">
-        <v>144</v>
-      </c>
-      <c r="C45" s="40" t="s">
-        <v>49</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="C45" s="38"/>
       <c r="D45" s="24" t="str">
         <f>F44</f>
-        <v>0xC000</v>
-      </c>
-      <c r="E45" s="24" t="s">
-        <v>6</v>
+        <v>0xB800</v>
+      </c>
+      <c r="E45" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M53))</f>
+        <v>0x800</v>
       </c>
       <c r="F45" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I45))</f>
-        <v>0x10000</v>
+        <v>0xC000</v>
       </c>
       <c r="G45" s="24">
-        <f t="shared" si="68"/>
-        <v>49152</v>
+        <f t="shared" ref="G45:H47" si="71">HEX2DEC(MID(D45, 3, LEN(D45)-2))</f>
+        <v>47104</v>
       </c>
       <c r="H45" s="24">
-        <f t="shared" si="68"/>
-        <v>16384</v>
+        <f t="shared" si="71"/>
+        <v>2048</v>
       </c>
       <c r="I45" s="24">
         <f>G45+H45</f>
-        <v>65536</v>
+        <v>49152</v>
       </c>
       <c r="J45" s="24" t="s">
-        <v>19</v>
+        <v>75</v>
       </c>
       <c r="L45" s="19" t="s">
         <v>3</v>
@@ -3052,40 +3056,39 @@
     </row>
     <row r="46" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B46" s="42" t="s">
-        <v>143</v>
-      </c>
-      <c r="C46" s="43" t="s">
-        <v>55</v>
+        <v>142</v>
+      </c>
+      <c r="C46" s="40" t="s">
+        <v>48</v>
       </c>
       <c r="D46" s="24" t="str">
-        <f t="shared" si="1"/>
-        <v>0x10000</v>
-      </c>
-      <c r="E46" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
-        <v>0x100</v>
+        <f>F45</f>
+        <v>0xC000</v>
+      </c>
+      <c r="E46" s="24" t="s">
+        <v>6</v>
       </c>
       <c r="F46" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I46))</f>
-        <v>0x10100</v>
+        <v>0x10000</v>
       </c>
       <c r="G46" s="24">
-        <f t="shared" si="68"/>
-        <v>65536</v>
+        <f t="shared" si="71"/>
+        <v>49152</v>
       </c>
       <c r="H46" s="24">
-        <f t="shared" si="68"/>
-        <v>256</v>
+        <f t="shared" si="71"/>
+        <v>16384</v>
       </c>
       <c r="I46" s="24">
         <f>G46+H46</f>
-        <v>65792</v>
+        <v>65536</v>
       </c>
       <c r="J46" s="24" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="L46" s="30" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M46" s="30">
         <f>M34*M45</f>
@@ -3094,73 +3097,85 @@
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B47" s="42"/>
-    </row>
-    <row r="48" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="C47" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="D47" s="24" t="str">
+        <f t="shared" si="1"/>
+        <v>0x10000</v>
+      </c>
+      <c r="E47" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
+        <v>0x100</v>
+      </c>
+      <c r="F47" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I47))</f>
+        <v>0x10100</v>
+      </c>
+      <c r="G47" s="24">
+        <f t="shared" si="71"/>
+        <v>65536</v>
+      </c>
+      <c r="H47" s="24">
+        <f t="shared" si="71"/>
+        <v>256</v>
+      </c>
+      <c r="I47" s="24">
+        <f>G47+H47</f>
+        <v>65792</v>
+      </c>
+      <c r="J47" s="24" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B48" s="42"/>
-      <c r="C48"/>
-      <c r="D48"/>
-      <c r="E48"/>
-      <c r="F48"/>
-      <c r="G48"/>
-      <c r="H48"/>
-      <c r="I48"/>
-      <c r="J48"/>
       <c r="L48" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M48" s="19" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" ht="15" x14ac:dyDescent="0.25">
       <c r="B49" s="42"/>
-      <c r="C49" s="36" t="s">
-        <v>56</v>
-      </c>
-      <c r="D49" s="24"/>
-      <c r="E49" s="24" t="str">
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="L49" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="M49" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B50" s="42"/>
+      <c r="C50" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M31))</f>
         <v>0x4000</v>
-      </c>
-      <c r="F49" s="24"/>
-      <c r="G49" s="24"/>
-      <c r="H49" s="24">
-        <f>HEX2DEC(MID(E49, 3, LEN(E49)-2))</f>
-        <v>16384</v>
-      </c>
-      <c r="I49" s="24"/>
-      <c r="J49" s="24" t="s">
-        <v>51</v>
-      </c>
-      <c r="L49" s="19" t="s">
-        <v>80</v>
-      </c>
-      <c r="M49" s="19">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B50" s="42"/>
-      <c r="C50" s="38"/>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M65))</f>
-        <v>0x800</v>
       </c>
       <c r="F50" s="24"/>
       <c r="G50" s="24"/>
       <c r="H50" s="24">
         <f>HEX2DEC(MID(E50, 3, LEN(E50)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I50" s="24" t="s">
-        <v>158</v>
-      </c>
+        <v>16384</v>
+      </c>
+      <c r="I50" s="24"/>
       <c r="J50" s="24" t="s">
-        <v>134</v>
+        <v>50</v>
       </c>
       <c r="L50" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M50" s="19">
         <v>512</v>
@@ -3168,8 +3183,26 @@
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B51" s="42"/>
+      <c r="C51" s="38"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M65))</f>
+        <v>0x800</v>
+      </c>
+      <c r="F51" s="24"/>
+      <c r="G51" s="24"/>
+      <c r="H51" s="24">
+        <f>HEX2DEC(MID(E51, 3, LEN(E51)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I51" s="24" t="s">
+        <v>157</v>
+      </c>
+      <c r="J51" s="24" t="s">
+        <v>133</v>
+      </c>
       <c r="L51" s="29" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M51" s="29">
         <v>16</v>
@@ -3178,7 +3211,7 @@
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B52" s="42"/>
       <c r="L52" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M52" s="19">
         <f>M49*M50*M51</f>
@@ -3187,25 +3220,8 @@
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B53" s="42"/>
-      <c r="C53" s="43" t="s">
-        <v>155</v>
-      </c>
-      <c r="D53" s="24"/>
-      <c r="E53" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="F53" s="24"/>
-      <c r="G53" s="24"/>
-      <c r="H53" s="24">
-        <f t="shared" ref="H53" si="69">HEX2DEC(MID(E53, 3, LEN(E53)-2))</f>
-        <v>131072</v>
-      </c>
-      <c r="I53" s="24"/>
-      <c r="J53" s="24" t="s">
-        <v>155</v>
-      </c>
       <c r="L53" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M53" s="19">
         <f>M52/8</f>
@@ -3215,39 +3231,56 @@
     <row r="54" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B54" s="42"/>
       <c r="C54" s="43" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="D54" s="24"/>
       <c r="E54" s="24" t="s">
-        <v>169</v>
+        <v>156</v>
       </c>
       <c r="F54" s="24"/>
       <c r="G54" s="24"/>
       <c r="H54" s="24">
-        <f t="shared" ref="H54" si="70">HEX2DEC(MID(E54, 3, LEN(E54)-2))</f>
-        <v>65536</v>
+        <f t="shared" ref="H54" si="72">HEX2DEC(MID(E54, 3, LEN(E54)-2))</f>
+        <v>131072</v>
       </c>
       <c r="I54" s="24"/>
       <c r="J54" s="24" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B55" s="42"/>
+      <c r="C55" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="D55" s="24"/>
+      <c r="E55" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="F55" s="24"/>
+      <c r="G55" s="24"/>
+      <c r="H55" s="24">
+        <f t="shared" ref="H55" si="73">HEX2DEC(MID(E55, 3, LEN(E55)-2))</f>
+        <v>65536</v>
+      </c>
+      <c r="I55" s="24"/>
+      <c r="J55" s="24" t="s">
+        <v>167</v>
+      </c>
       <c r="L55" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="M55" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="P55" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B56" s="42"/>
       <c r="L56" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M56" s="19">
         <v>32</v>
@@ -3269,7 +3302,7 @@
     <row r="58" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B58" s="42"/>
       <c r="L58" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M58" s="19">
         <f>M56*M57</f>
@@ -3279,7 +3312,7 @@
     <row r="59" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B59" s="42"/>
       <c r="L59" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M59" s="19">
         <f>M58/8</f>
@@ -3292,40 +3325,40 @@
     <row r="61" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B61" s="42"/>
       <c r="L61" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M61" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B62" s="42"/>
       <c r="L62" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="M62" s="19">
         <v>512</v>
       </c>
       <c r="N62" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B63" s="42"/>
       <c r="L63" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M63" s="29">
         <v>32</v>
       </c>
       <c r="N63" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B64" s="42"/>
       <c r="L64" s="30" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M64" s="19">
         <f>M62*M63</f>
@@ -3335,7 +3368,7 @@
     <row r="65" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B65" s="42"/>
       <c r="L65" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M65" s="19">
         <f>M64/8</f>
@@ -3348,13 +3381,13 @@
     <row r="67" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B67" s="42"/>
       <c r="L67" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B68" s="44"/>
       <c r="L68" s="19" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="M68" s="19">
         <v>8</v>
@@ -3362,7 +3395,7 @@
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L69" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="M69" s="19">
         <v>8</v>
@@ -3370,7 +3403,7 @@
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L70" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="M70" s="19">
         <v>8</v>
@@ -3378,7 +3411,7 @@
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L71" s="19" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="M71" s="19">
         <v>8</v>
@@ -3386,7 +3419,7 @@
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L72" s="47" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M72" s="47">
         <v>96</v>
@@ -3394,7 +3427,7 @@
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L73" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="M73" s="30">
         <f>SUM(M68:M72)</f>
@@ -3403,7 +3436,7 @@
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L74" s="19" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="M74" s="19">
         <f>M73/8</f>
@@ -3412,34 +3445,34 @@
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L76" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L77" s="19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M77" s="19">
         <v>32</v>
       </c>
       <c r="N77" s="19" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L78" s="19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="M78" s="19">
         <v>24</v>
       </c>
       <c r="N78" s="19" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L79" s="19" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M79" s="19">
         <v>8</v>
@@ -3447,7 +3480,7 @@
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L80" s="30" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="M80" s="30">
         <f>M77*M78*M79</f>
@@ -3456,7 +3489,7 @@
     </row>
     <row r="81" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L81" s="33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M81" s="33">
         <f>M80/8</f>
@@ -3469,12 +3502,12 @@
     </row>
     <row r="83" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L83" s="21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="84" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L84" s="29" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="M84" s="29">
         <v>64</v>
@@ -3482,7 +3515,7 @@
     </row>
     <row r="85" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L85" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="M85" s="19">
         <v>16</v>
@@ -3490,7 +3523,7 @@
     </row>
     <row r="86" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L86" s="19" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="M86" s="19">
         <v>16</v>
@@ -3498,18 +3531,18 @@
     </row>
     <row r="87" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L87" s="19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="M87" s="19">
         <v>16</v>
       </c>
       <c r="N87" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="88" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L88" s="30" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="M88" s="30">
         <f>M85*M86*M87</f>
@@ -3518,7 +3551,7 @@
     </row>
     <row r="89" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L89" s="19" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M89" s="19">
         <f>M88/8</f>
@@ -3527,7 +3560,7 @@
     </row>
     <row r="90" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L90" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="M90" s="30">
         <f>M84*M89</f>
@@ -3536,8 +3569,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C25:C26"/>
-    <mergeCell ref="C30:C31"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="C31:C32"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3549,7 +3582,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82A3B691-5BC9-488D-96B0-3685B8BF2439}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
@@ -3565,10 +3598,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
@@ -3577,189 +3610,189 @@
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="16" t="s">
         <v>126</v>
-      </c>
-      <c r="F3" s="16" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="10" t="s">
-        <v>78</v>
-      </c>
       <c r="G4" s="8" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="17" t="s">
-        <v>96</v>
-      </c>
       <c r="F6" s="12" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" s="11"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>100</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>102</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>104</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>112</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="5" t="s">
         <v>114</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B18" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>120</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I23" s="45" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -3784,13 +3817,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" t="s">
         <v>172</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>173</v>
-      </c>
-      <c r="C1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3835,10 +3868,10 @@
         <v>272</v>
       </c>
       <c r="D1" t="s">
+        <v>174</v>
+      </c>
+      <c r="E1" t="s">
         <v>175</v>
-      </c>
-      <c r="E1" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3861,18 +3894,18 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="L2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add sprite mirroring support, raiders continues
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A630BB9-856B-4235-A864-9303534F58F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E6F1D6-B41F-4063-94BB-CD3AC8B4DBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="2910" windowWidth="24165" windowHeight="14085" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware" sheetId="1" r:id="rId1"/>
@@ -102,9 +102,6 @@
     <t>Work RAM</t>
   </si>
   <si>
-    <t>Timer</t>
-  </si>
-  <si>
     <t>Timestamp</t>
   </si>
   <si>
@@ -751,6 +748,9 @@
   </si>
   <si>
     <t>System outputs (video options)</t>
+  </si>
+  <si>
+    <t>Millisecond Timer</t>
   </si>
 </sst>
 </file>
@@ -989,21 +989,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1013,23 +1012,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1055,11 +1054,9 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1094,21 +1091,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1432,1713 +1420,1712 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
   <dimension ref="B1:P90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="19" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" style="19" customWidth="1"/>
-    <col min="3" max="3" width="22.85546875" style="19" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" style="19" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.42578125" style="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" style="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6" style="19" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.85546875" style="19" customWidth="1"/>
-    <col min="11" max="11" width="5.5703125" style="19" customWidth="1"/>
-    <col min="12" max="12" width="43.28515625" style="19" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" style="19"/>
-    <col min="14" max="14" width="27" style="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="3.140625" style="18" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6" style="18" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="18" customWidth="1"/>
+    <col min="11" max="11" width="5.5703125" style="18" customWidth="1"/>
+    <col min="12" max="12" width="43.28515625" style="18" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="18"/>
+    <col min="14" max="14" width="27" style="18" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B1" s="18" t="s">
-        <v>29</v>
+      <c r="B1" s="17" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B2" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C2" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" s="20" t="s">
+      <c r="B2" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="F2" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="21" t="s">
-        <v>60</v>
+      <c r="J2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="L2" s="20" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="C3" s="23" t="s">
+      <c r="B3" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="24" t="s">
+      <c r="D3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="24" t="str">
+      <c r="E3" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I3))</f>
         <v>0x8000</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="23">
         <f t="shared" ref="G3:H7" si="0">HEX2DEC(MID(D3, 3, LEN(D3)-2))</f>
         <v>0</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="23">
         <f t="shared" si="0"/>
         <v>32768</v>
       </c>
-      <c r="I3" s="24">
+      <c r="I3" s="23">
         <f>G3+H3</f>
         <v>32768</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="L3" s="19" t="s">
+      <c r="L3" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="M3" s="19">
+      <c r="M3" s="18">
         <v>32</v>
       </c>
-      <c r="N3" s="19">
+      <c r="N3" s="18">
         <f>M4+SCREEN_BORDER_WIDTH</f>
         <v>352</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B4" s="25" t="s">
-        <v>152</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="24" t="str">
+      <c r="B4" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="C4" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="23" t="str">
         <f t="shared" ref="D4:D47" si="1">F3</f>
         <v>0x8000</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="24" t="str">
+      <c r="F4" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I4))</f>
         <v>0x8001</v>
       </c>
-      <c r="G4" s="24">
+      <c r="G4" s="23">
         <f t="shared" si="0"/>
         <v>32768</v>
       </c>
-      <c r="H4" s="24">
+      <c r="H4" s="23">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I4" s="24">
+      <c r="I4" s="23">
         <f>G4+H4</f>
         <v>32769</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="M4" s="19">
+      <c r="M4" s="18">
         <v>320</v>
       </c>
-      <c r="N4" s="19">
+      <c r="N4" s="18">
         <f>M5+SCREEN_BORDER_WIDTH</f>
         <v>272</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B5" s="25"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="24" t="str">
+      <c r="B5" s="24"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="23" t="str">
         <f t="shared" ref="D5" si="2">F4</f>
         <v>0x8001</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="24" t="str">
+      <c r="F5" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I5))</f>
         <v>0x8002</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5" s="23">
         <f t="shared" ref="G5" si="3">HEX2DEC(MID(D5, 3, LEN(D5)-2))</f>
         <v>32769</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5" s="23">
         <f t="shared" ref="H5" si="4">HEX2DEC(MID(E5, 3, LEN(E5)-2))</f>
         <v>1</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5" s="23">
         <f>G5+H5</f>
         <v>32770</v>
       </c>
-      <c r="J5" s="24" t="s">
-        <v>216</v>
-      </c>
-      <c r="L5" s="19" t="s">
+      <c r="J5" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="L5" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="18">
         <v>240</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B6" s="25"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="28" t="str">
+      <c r="B6" s="24"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="27" t="str">
         <f>F5</f>
         <v>0x8002</v>
       </c>
-      <c r="E6" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="F6" s="28" t="str">
+      <c r="E6" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="F6" s="27" t="str">
         <f t="shared" ref="F6" si="5">_xlfn.CONCAT("0x",DEC2HEX(I6))</f>
         <v>0x8100</v>
       </c>
-      <c r="G6" s="28">
+      <c r="G6" s="27">
         <f t="shared" si="0"/>
         <v>32770</v>
       </c>
-      <c r="H6" s="28">
+      <c r="H6" s="27">
         <f t="shared" si="0"/>
         <v>254</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I6" s="27">
         <f>G6+H6</f>
         <v>33024</v>
       </c>
-      <c r="J6" s="28" t="s">
-        <v>30</v>
+      <c r="J6" s="27" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B7" s="25"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="24" t="str">
+      <c r="B7" s="24"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0x8100</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="24" t="str">
+      <c r="F7" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I7))</f>
         <v>0x81C0</v>
       </c>
-      <c r="G7" s="24">
+      <c r="G7" s="23">
         <f t="shared" si="0"/>
         <v>33024</v>
       </c>
-      <c r="H7" s="24">
+      <c r="H7" s="23">
         <f t="shared" si="0"/>
         <v>192</v>
       </c>
-      <c r="I7" s="24">
+      <c r="I7" s="23">
         <f>G7+H7</f>
         <v>33216</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="J7" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="L7" s="21" t="s">
-        <v>176</v>
+      <c r="L7" s="20" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="25"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28" t="str">
+      <c r="B8" s="24"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27" t="str">
         <f t="shared" si="1"/>
         <v>0x81C0</v>
       </c>
-      <c r="E8" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="28" t="str">
+      <c r="E8" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" s="27" t="str">
         <f t="shared" ref="F8" si="6">_xlfn.CONCAT("0x",DEC2HEX(I8))</f>
         <v>0x8200</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="27">
         <f t="shared" ref="G8" si="7">HEX2DEC(MID(D8, 3, LEN(D8)-2))</f>
         <v>33216</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="27">
         <f t="shared" ref="H8" si="8">HEX2DEC(MID(E8, 3, LEN(E8)-2))</f>
         <v>64</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="27">
         <f t="shared" ref="I8" si="9">G8+H8</f>
         <v>33280</v>
       </c>
-      <c r="J8" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" s="29" t="s">
-        <v>177</v>
-      </c>
-      <c r="M8" s="29">
+      <c r="J8" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L8" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="M8" s="28">
         <v>256</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="25"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="24" t="str">
+      <c r="B9" s="24"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0x8200</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="24" t="str">
+      <c r="F9" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I9))</f>
         <v>0x8260</v>
       </c>
-      <c r="G9" s="24">
+      <c r="G9" s="23">
         <f t="shared" ref="G9:H11" si="10">HEX2DEC(MID(D9, 3, LEN(D9)-2))</f>
         <v>33280</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="23">
         <f t="shared" si="10"/>
         <v>96</v>
       </c>
-      <c r="I9" s="24">
+      <c r="I9" s="23">
         <f>G9+H9</f>
         <v>33376</v>
       </c>
-      <c r="J9" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="L9" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="M9" s="19">
+      <c r="J9" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="M9" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B10" s="25"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="28" t="str">
+      <c r="B10" s="24"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27" t="str">
         <f t="shared" si="1"/>
         <v>0x8260</v>
       </c>
-      <c r="E10" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="28" t="str">
+      <c r="E10" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="27" t="str">
         <f t="shared" ref="F10" si="11">_xlfn.CONCAT("0x",DEC2HEX(I10))</f>
         <v>0x8300</v>
       </c>
-      <c r="G10" s="28">
+      <c r="G10" s="27">
         <f t="shared" si="10"/>
         <v>33376</v>
       </c>
-      <c r="H10" s="28">
+      <c r="H10" s="27">
         <f t="shared" si="10"/>
         <v>160</v>
       </c>
-      <c r="I10" s="28">
+      <c r="I10" s="27">
         <f>G10+H10</f>
         <v>33536</v>
       </c>
-      <c r="J10" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="M10" s="19">
+      <c r="J10" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="M10" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="25"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="24" t="str">
+      <c r="B11" s="24"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0x8300</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="24" t="str">
+      <c r="F11" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I11))</f>
         <v>0x8360</v>
       </c>
-      <c r="G11" s="24">
+      <c r="G11" s="23">
         <f t="shared" si="10"/>
         <v>33536</v>
       </c>
-      <c r="H11" s="24">
+      <c r="H11" s="23">
         <f t="shared" si="10"/>
         <v>96</v>
       </c>
-      <c r="I11" s="24">
+      <c r="I11" s="23">
         <f>G11+H11</f>
         <v>33632</v>
       </c>
-      <c r="J11" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="L11" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="M11" s="19">
+      <c r="J11" s="23" t="s">
+        <v>25</v>
+      </c>
+      <c r="L11" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="M11" s="18">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B12" s="25"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="28" t="str">
+      <c r="B12" s="24"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="27" t="str">
         <f t="shared" si="1"/>
         <v>0x8360</v>
       </c>
-      <c r="E12" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="28" t="str">
+      <c r="E12" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="27" t="str">
         <f t="shared" ref="F12" si="12">_xlfn.CONCAT("0x",DEC2HEX(I12))</f>
         <v>0x8400</v>
       </c>
-      <c r="G12" s="28">
+      <c r="G12" s="27">
         <f t="shared" ref="G12" si="13">HEX2DEC(MID(D12, 3, LEN(D12)-2))</f>
         <v>33632</v>
       </c>
-      <c r="H12" s="28">
+      <c r="H12" s="27">
         <f t="shared" ref="H12" si="14">HEX2DEC(MID(E12, 3, LEN(E12)-2))</f>
         <v>160</v>
       </c>
-      <c r="I12" s="28">
+      <c r="I12" s="27">
         <f t="shared" ref="I12" si="15">G12+H12</f>
         <v>33792</v>
       </c>
-      <c r="J12" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="30" t="s">
-        <v>181</v>
-      </c>
-      <c r="M12" s="30">
+      <c r="J12" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L12" s="29" t="s">
+        <v>180</v>
+      </c>
+      <c r="M12" s="29">
         <f>M9*M10*M11</f>
         <v>64</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B13" s="25"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="24" t="str">
+      <c r="B13" s="24"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0x8400</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="24" t="str">
+      <c r="F13" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I13))</f>
         <v>0x8430</v>
       </c>
-      <c r="G13" s="24">
+      <c r="G13" s="23">
         <f t="shared" ref="G13:H15" si="16">HEX2DEC(MID(D13, 3, LEN(D13)-2))</f>
         <v>33792</v>
       </c>
-      <c r="H13" s="24">
+      <c r="H13" s="23">
         <f t="shared" si="16"/>
         <v>48</v>
       </c>
-      <c r="I13" s="24">
+      <c r="I13" s="23">
         <f>G13+H13</f>
         <v>33840</v>
       </c>
-      <c r="J13" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="L13" s="19" t="s">
-        <v>182</v>
-      </c>
-      <c r="M13" s="19">
+      <c r="J13" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="M13" s="18">
         <f>M12/8</f>
         <v>8</v>
       </c>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B14" s="25"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="28" t="str">
+      <c r="B14" s="24"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27" t="str">
         <f t="shared" si="1"/>
         <v>0x8430</v>
       </c>
-      <c r="E14" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="28" t="str">
+      <c r="E14" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="27" t="str">
         <f t="shared" ref="F14" si="17">_xlfn.CONCAT("0x",DEC2HEX(I14))</f>
         <v>0x8500</v>
       </c>
-      <c r="G14" s="28">
+      <c r="G14" s="27">
         <f t="shared" si="16"/>
         <v>33840</v>
       </c>
-      <c r="H14" s="28">
+      <c r="H14" s="27">
         <f t="shared" si="16"/>
         <v>208</v>
       </c>
-      <c r="I14" s="28">
+      <c r="I14" s="27">
         <f>G14+H14</f>
         <v>34048</v>
       </c>
-      <c r="J14" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L14" s="30" t="s">
-        <v>183</v>
-      </c>
-      <c r="M14" s="30">
+      <c r="J14" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L14" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="M14" s="29">
         <f>M8*M13</f>
         <v>2048</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="25"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="24" t="str">
+      <c r="B15" s="24"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0x8500</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="F15" s="24" t="str">
+      <c r="F15" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I15))</f>
         <v>0x8560</v>
       </c>
-      <c r="G15" s="24">
+      <c r="G15" s="23">
         <f t="shared" si="16"/>
         <v>34048</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15" s="23">
         <f t="shared" si="16"/>
         <v>96</v>
       </c>
-      <c r="I15" s="24">
+      <c r="I15" s="23">
         <f>G15+H15</f>
         <v>34144</v>
       </c>
-      <c r="J15" s="24" t="s">
-        <v>24</v>
+      <c r="J15" s="23" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B16" s="25"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="28" t="str">
+      <c r="B16" s="24"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="27" t="str">
         <f t="shared" si="1"/>
         <v>0x8560</v>
       </c>
-      <c r="E16" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="28" t="str">
+      <c r="E16" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="27" t="str">
         <f t="shared" ref="F16" si="18">_xlfn.CONCAT("0x",DEC2HEX(I16))</f>
         <v>0x8600</v>
       </c>
-      <c r="G16" s="28">
+      <c r="G16" s="27">
         <f t="shared" ref="G16" si="19">HEX2DEC(MID(D16, 3, LEN(D16)-2))</f>
         <v>34144</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="27">
         <f t="shared" ref="H16" si="20">HEX2DEC(MID(E16, 3, LEN(E16)-2))</f>
         <v>160</v>
       </c>
-      <c r="I16" s="28">
+      <c r="I16" s="27">
         <f t="shared" ref="I16" si="21">G16+H16</f>
         <v>34304</v>
       </c>
-      <c r="J16" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L16" s="21" t="s">
-        <v>54</v>
+      <c r="J16" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16" s="20" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B17" s="25"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="24" t="str">
+      <c r="B17" s="24"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0x8600</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="24" t="str">
+      <c r="F17" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I17))</f>
         <v>0x860C</v>
       </c>
-      <c r="G17" s="24">
+      <c r="G17" s="23">
         <f t="shared" ref="G17:H19" si="22">HEX2DEC(MID(D17, 3, LEN(D17)-2))</f>
         <v>34304</v>
       </c>
-      <c r="H17" s="24">
+      <c r="H17" s="23">
         <f t="shared" si="22"/>
         <v>12</v>
       </c>
-      <c r="I17" s="24">
+      <c r="I17" s="23">
         <f>G17+H17</f>
         <v>34316</v>
       </c>
-      <c r="J17" s="24" t="s">
-        <v>23</v>
-      </c>
-      <c r="L17" s="29" t="s">
-        <v>57</v>
-      </c>
-      <c r="M17" s="29">
+      <c r="J17" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="L17" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="M17" s="28">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B18" s="25"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="28" t="str">
+      <c r="B18" s="24"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="27" t="str">
         <f t="shared" si="1"/>
         <v>0x860C</v>
       </c>
-      <c r="E18" s="28" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="28" t="str">
+      <c r="E18" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" s="27" t="str">
         <f t="shared" ref="F18" si="23">_xlfn.CONCAT("0x",DEC2HEX(I18))</f>
         <v>0x8700</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="27">
         <f t="shared" si="22"/>
         <v>34316</v>
       </c>
-      <c r="H18" s="28">
+      <c r="H18" s="27">
         <f t="shared" si="22"/>
         <v>244</v>
       </c>
-      <c r="I18" s="28">
+      <c r="I18" s="27">
         <f>G18+H18</f>
         <v>34560</v>
       </c>
-      <c r="J18" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L18" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="M18" s="19">
+      <c r="J18" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L18" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="M18" s="18">
         <v>16</v>
       </c>
-      <c r="N18" s="19" t="s">
-        <v>81</v>
+      <c r="N18" s="18" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B19" s="25"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="24" t="str">
+      <c r="B19" s="24"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0x8700</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="24" t="str">
+      <c r="F19" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I19))</f>
         <v>0x8730</v>
       </c>
-      <c r="G19" s="24">
+      <c r="G19" s="23">
         <f t="shared" si="22"/>
         <v>34560</v>
       </c>
-      <c r="H19" s="24">
+      <c r="H19" s="23">
         <f t="shared" si="22"/>
         <v>48</v>
       </c>
-      <c r="I19" s="24">
+      <c r="I19" s="23">
         <f>G19+H19</f>
         <v>34608</v>
       </c>
-      <c r="J19" s="24" t="s">
-        <v>22</v>
-      </c>
-      <c r="L19" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="M19" s="19">
+      <c r="J19" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="L19" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="M19" s="18">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B20" s="25"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="28" t="str">
+      <c r="B20" s="24"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="27" t="str">
         <f t="shared" si="1"/>
         <v>0x8730</v>
       </c>
-      <c r="E20" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="28" t="str">
+      <c r="E20" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" s="27" t="str">
         <f t="shared" ref="F20" si="24">_xlfn.CONCAT("0x",DEC2HEX(I20))</f>
         <v>0x8800</v>
       </c>
-      <c r="G20" s="28">
+      <c r="G20" s="27">
         <f t="shared" ref="G20" si="25">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
         <v>34608</v>
       </c>
-      <c r="H20" s="28">
+      <c r="H20" s="27">
         <f t="shared" ref="H20" si="26">HEX2DEC(MID(E20, 3, LEN(E20)-2))</f>
         <v>208</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I20" s="27">
         <f t="shared" ref="I20" si="27">G20+H20</f>
         <v>34816</v>
       </c>
-      <c r="J20" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L20" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="M20" s="30">
+      <c r="J20" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L20" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="M20" s="29">
         <f>M18*M19</f>
         <v>512</v>
       </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B21" s="25"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="24" t="str">
+      <c r="B21" s="24"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0x8800</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="24" t="str">
+      <c r="F21" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I21))</f>
         <v>0x8821</v>
       </c>
-      <c r="G21" s="24">
+      <c r="G21" s="23">
         <f t="shared" ref="G21:H37" si="28">HEX2DEC(MID(D21, 3, LEN(D21)-2))</f>
         <v>34816</v>
       </c>
-      <c r="H21" s="24">
+      <c r="H21" s="23">
         <f t="shared" si="28"/>
         <v>33</v>
       </c>
-      <c r="I21" s="24">
+      <c r="I21" s="23">
         <f>G21+H21</f>
         <v>34849</v>
       </c>
-      <c r="J21" s="24" t="s">
-        <v>21</v>
-      </c>
-      <c r="L21" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="M21" s="19">
+      <c r="J21" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="L21" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="M21" s="18">
         <f>M20/8</f>
         <v>64</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B22" s="25"/>
-      <c r="C22" s="27"/>
-      <c r="D22" s="28" t="str">
+      <c r="B22" s="24"/>
+      <c r="C22" s="26"/>
+      <c r="D22" s="27" t="str">
         <f t="shared" si="1"/>
         <v>0x8821</v>
       </c>
-      <c r="E22" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="F22" s="28" t="str">
+      <c r="E22" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="27" t="str">
         <f t="shared" ref="F22" si="29">_xlfn.CONCAT("0x",DEC2HEX(I22))</f>
         <v>0x8900</v>
       </c>
-      <c r="G22" s="28">
+      <c r="G22" s="27">
         <f t="shared" si="28"/>
         <v>34849</v>
       </c>
-      <c r="H22" s="28">
+      <c r="H22" s="27">
         <f t="shared" si="28"/>
         <v>223</v>
       </c>
-      <c r="I22" s="28">
+      <c r="I22" s="27">
         <f>G22+H22</f>
         <v>35072</v>
       </c>
-      <c r="J22" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L22" s="30" t="s">
-        <v>144</v>
-      </c>
-      <c r="M22" s="30">
+      <c r="J22" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22" s="29" t="s">
+        <v>143</v>
+      </c>
+      <c r="M22" s="29">
         <f>M21*M17</f>
         <v>256</v>
       </c>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B23" s="25"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="24" t="str">
+      <c r="B23" s="24"/>
+      <c r="C23" s="26"/>
+      <c r="D23" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0x8900</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="F23" s="24" t="str">
+      <c r="F23" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I23))</f>
         <v>0x8911</v>
       </c>
-      <c r="G23" s="24">
+      <c r="G23" s="23">
         <f t="shared" si="28"/>
         <v>35072</v>
       </c>
-      <c r="H23" s="24">
+      <c r="H23" s="23">
         <f t="shared" si="28"/>
         <v>17</v>
       </c>
-      <c r="I23" s="24">
+      <c r="I23" s="23">
         <f>G23+H23</f>
         <v>35089</v>
       </c>
-      <c r="J23" s="24" t="s">
-        <v>20</v>
+      <c r="J23" s="23" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B24" s="25"/>
-      <c r="C24" s="27"/>
-      <c r="D24" s="28" t="str">
+      <c r="B24" s="24"/>
+      <c r="C24" s="26"/>
+      <c r="D24" s="27" t="str">
         <f>F23</f>
         <v>0x8911</v>
       </c>
-      <c r="E24" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="F24" s="28" t="str">
+      <c r="E24" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="27" t="str">
         <f t="shared" ref="F24" si="30">_xlfn.CONCAT("0x",DEC2HEX(I24))</f>
         <v>0x8A00</v>
       </c>
-      <c r="G24" s="28">
+      <c r="G24" s="27">
         <f t="shared" si="28"/>
         <v>35089</v>
       </c>
-      <c r="H24" s="28">
+      <c r="H24" s="27">
         <f t="shared" si="28"/>
         <v>239</v>
       </c>
-      <c r="I24" s="28">
+      <c r="I24" s="27">
         <f t="shared" ref="I24" si="31">G24+H24</f>
         <v>35328</v>
       </c>
-      <c r="J24" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L24" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="N24" s="19" t="s">
-        <v>153</v>
+      <c r="J24" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="N24" s="18" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B25" s="25"/>
-      <c r="C25" s="27"/>
-      <c r="D25" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F25" s="24" t="str">
+      <c r="B25" s="24"/>
+      <c r="C25" s="26"/>
+      <c r="D25" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F25" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I25))</f>
         <v>0x8A10</v>
       </c>
-      <c r="G25" s="24">
+      <c r="G25" s="23">
         <f t="shared" si="28"/>
         <v>35328</v>
       </c>
-      <c r="H25" s="24">
+      <c r="H25" s="23">
         <f t="shared" si="28"/>
         <v>16</v>
       </c>
-      <c r="I25" s="24">
+      <c r="I25" s="23">
         <f>G25+H25</f>
         <v>35344</v>
       </c>
-      <c r="J25" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="L25" s="29" t="s">
+      <c r="J25" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="L25" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="M25" s="28">
         <v>64</v>
       </c>
-      <c r="M25" s="29">
-        <v>64</v>
-      </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B26" s="25"/>
-      <c r="C26" s="52"/>
-      <c r="D26" s="24" t="str">
+      <c r="B26" s="24"/>
+      <c r="C26" s="46"/>
+      <c r="D26" s="23" t="str">
         <f t="shared" ref="D26:D32" si="32">F25</f>
         <v>0x8A10</v>
       </c>
-      <c r="E26" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F26" s="24" t="str">
+      <c r="E26" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I26))</f>
         <v>0x8A20</v>
       </c>
-      <c r="G26" s="24">
+      <c r="G26" s="23">
         <f t="shared" ref="G26:G27" si="33">HEX2DEC(MID(D26, 3, LEN(D26)-2))</f>
         <v>35344</v>
       </c>
-      <c r="H26" s="24">
+      <c r="H26" s="23">
         <f t="shared" si="28"/>
         <v>16</v>
       </c>
-      <c r="I26" s="24">
+      <c r="I26" s="23">
         <f>G26+H26</f>
         <v>35360</v>
       </c>
-      <c r="J26" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="L26" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="M26" s="19">
+      <c r="J26" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="L26" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="M26" s="18">
         <v>16</v>
       </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B27" s="25"/>
-      <c r="C27" s="52"/>
-      <c r="D27" s="24" t="str">
+      <c r="B27" s="24"/>
+      <c r="C27" s="46"/>
+      <c r="D27" s="23" t="str">
         <f t="shared" si="32"/>
         <v>0x8A20</v>
       </c>
-      <c r="E27" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F27" s="24" t="str">
+      <c r="E27" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I27))</f>
         <v>0x8A30</v>
       </c>
-      <c r="G27" s="24">
+      <c r="G27" s="23">
         <f t="shared" si="33"/>
         <v>35360</v>
       </c>
-      <c r="H27" s="24">
+      <c r="H27" s="23">
         <f t="shared" si="28"/>
         <v>16</v>
       </c>
-      <c r="I27" s="24">
+      <c r="I27" s="23">
         <f>G27+H27</f>
         <v>35376</v>
       </c>
-      <c r="J27" s="24" t="s">
-        <v>88</v>
-      </c>
-      <c r="L27" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="M27" s="19">
+      <c r="J27" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="L27" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="M27" s="18">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B28" s="25"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="24" t="str">
+      <c r="B28" s="24"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="23" t="str">
         <f>F27</f>
         <v>0x8A30</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E28" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="24" t="str">
+      <c r="F28" s="23" t="str">
         <f t="shared" ref="F28" si="34">_xlfn.CONCAT("0x",DEC2HEX(I28))</f>
         <v>0x8A31</v>
       </c>
-      <c r="G28" s="24">
+      <c r="G28" s="23">
         <f>HEX2DEC(MID(D28, 3, LEN(D28)-2))</f>
         <v>35376</v>
       </c>
-      <c r="H28" s="24">
+      <c r="H28" s="23">
         <f t="shared" ref="H28" si="35">HEX2DEC(MID(E28, 3, LEN(E28)-2))</f>
         <v>1</v>
       </c>
-      <c r="I28" s="24">
+      <c r="I28" s="23">
         <f t="shared" ref="I28" si="36">G28+H28</f>
         <v>35377</v>
       </c>
-      <c r="J28" s="24" t="s">
-        <v>166</v>
-      </c>
-      <c r="L28" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="M28" s="19">
+      <c r="J28" s="23" t="s">
+        <v>165</v>
+      </c>
+      <c r="L28" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M28" s="18">
         <v>8</v>
       </c>
-      <c r="N28" s="19" t="s">
-        <v>164</v>
+      <c r="N28" s="18" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B29" s="25"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="24" t="str">
+      <c r="B29" s="24"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="23" t="str">
         <f>F28</f>
         <v>0x8A31</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="24" t="str">
+      <c r="F29" s="23" t="str">
         <f t="shared" ref="F29" si="37">_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
         <v>0x8A32</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="23">
         <f>HEX2DEC(MID(D29, 3, LEN(D29)-2))</f>
         <v>35377</v>
       </c>
-      <c r="H29" s="24">
+      <c r="H29" s="23">
         <f t="shared" ref="H29" si="38">HEX2DEC(MID(E29, 3, LEN(E29)-2))</f>
         <v>1</v>
       </c>
-      <c r="I29" s="24">
+      <c r="I29" s="23">
         <f t="shared" ref="I29" si="39">G29+H29</f>
         <v>35378</v>
       </c>
-      <c r="J29" s="24" t="s">
-        <v>214</v>
-      </c>
-      <c r="L29" s="30" t="s">
-        <v>68</v>
-      </c>
-      <c r="M29" s="30">
+      <c r="J29" s="23" t="s">
+        <v>213</v>
+      </c>
+      <c r="L29" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="M29" s="29">
         <f>M26*M27*M28</f>
         <v>2048</v>
       </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B30" s="25"/>
-      <c r="C30" s="28"/>
-      <c r="D30" s="28" t="str">
+      <c r="B30" s="24"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="27" t="str">
         <f>F29</f>
         <v>0x8A32</v>
       </c>
-      <c r="E30" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="F30" s="28" t="str">
+      <c r="E30" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="F30" s="27" t="str">
         <f t="shared" ref="F30" si="40">_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
         <v>0x8B00</v>
       </c>
-      <c r="G30" s="28">
+      <c r="G30" s="27">
         <f>HEX2DEC(MID(D30, 3, LEN(D30)-2))</f>
         <v>35378</v>
       </c>
-      <c r="H30" s="28">
+      <c r="H30" s="27">
         <f t="shared" ref="H30" si="41">HEX2DEC(MID(E30, 3, LEN(E30)-2))</f>
         <v>206</v>
       </c>
-      <c r="I30" s="28">
+      <c r="I30" s="27">
         <f t="shared" ref="I30" si="42">G30+H30</f>
         <v>35584</v>
       </c>
-      <c r="J30" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L30" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="M30" s="19">
+      <c r="J30" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L30" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="M30" s="18">
         <f>M29/8</f>
         <v>256</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B31" s="25"/>
-      <c r="C31" s="53" t="s">
-        <v>155</v>
-      </c>
-      <c r="D31" s="24" t="str">
+      <c r="B31" s="24"/>
+      <c r="C31" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="D31" s="23" t="str">
         <f>F30</f>
         <v>0x8B00</v>
       </c>
-      <c r="E31" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F31" s="24" t="str">
+      <c r="E31" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I31))</f>
         <v>0x8B10</v>
       </c>
-      <c r="G31" s="24">
+      <c r="G31" s="23">
         <f t="shared" ref="G31" si="43">HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
         <v>35584</v>
       </c>
-      <c r="H31" s="24">
+      <c r="H31" s="23">
         <f t="shared" si="28"/>
         <v>16</v>
       </c>
-      <c r="I31" s="24">
+      <c r="I31" s="23">
         <f>G31+H31</f>
         <v>35600</v>
       </c>
-      <c r="J31" s="24" t="s">
-        <v>169</v>
-      </c>
-      <c r="L31" s="30" t="s">
-        <v>145</v>
-      </c>
-      <c r="M31" s="30">
+      <c r="J31" s="23" t="s">
+        <v>168</v>
+      </c>
+      <c r="L31" s="29" t="s">
+        <v>144</v>
+      </c>
+      <c r="M31" s="29">
         <f>M25*M30</f>
         <v>16384</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B32" s="25"/>
-      <c r="C32" s="52"/>
-      <c r="D32" s="24" t="str">
+      <c r="B32" s="24"/>
+      <c r="C32" s="46"/>
+      <c r="D32" s="23" t="str">
         <f t="shared" si="32"/>
         <v>0x8B10</v>
       </c>
-      <c r="E32" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="F32" s="24" t="str">
+      <c r="E32" s="23" t="s">
+        <v>85</v>
+      </c>
+      <c r="F32" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
         <v>0x8B20</v>
       </c>
-      <c r="G32" s="24">
+      <c r="G32" s="23">
         <f t="shared" ref="G32" si="44">HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
         <v>35600</v>
       </c>
-      <c r="H32" s="24">
+      <c r="H32" s="23">
         <f t="shared" ref="H32" si="45">HEX2DEC(MID(E32, 3, LEN(E32)-2))</f>
         <v>16</v>
       </c>
-      <c r="I32" s="24">
+      <c r="I32" s="23">
         <f>G32+H32</f>
         <v>35616</v>
       </c>
-      <c r="J32" s="24" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="25"/>
-      <c r="C33" s="28"/>
-      <c r="D33" s="28" t="str">
+      <c r="J32" s="23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="24"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="27" t="str">
         <f>F32</f>
         <v>0x8B20</v>
       </c>
-      <c r="E33" s="28" t="s">
-        <v>184</v>
-      </c>
-      <c r="F33" s="28" t="str">
+      <c r="E33" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="F33" s="27" t="str">
         <f t="shared" ref="F33" si="46">_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
         <v>0x8C00</v>
       </c>
-      <c r="G33" s="28">
+      <c r="G33" s="27">
         <f t="shared" ref="G33:G35" si="47">HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
         <v>35616</v>
       </c>
-      <c r="H33" s="28">
+      <c r="H33" s="27">
         <f t="shared" ref="H33:H36" si="48">HEX2DEC(MID(E33, 3, LEN(E33)-2))</f>
         <v>224</v>
       </c>
-      <c r="I33" s="28">
+      <c r="I33" s="27">
         <f t="shared" ref="I33" si="49">G33+H33</f>
         <v>35840</v>
       </c>
-      <c r="J33" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L33" s="21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B34" s="25"/>
-      <c r="C34" s="48" t="s">
-        <v>185</v>
-      </c>
-      <c r="D34" s="24" t="str">
+      <c r="J33" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L33" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B34" s="24"/>
+      <c r="C34" s="44" t="s">
+        <v>184</v>
+      </c>
+      <c r="D34" s="23" t="str">
         <f>F33</f>
         <v>0x8C00</v>
       </c>
-      <c r="E34" s="24" t="str">
+      <c r="E34" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M74))</f>
         <v>0x10</v>
       </c>
-      <c r="F34" s="24" t="str">
+      <c r="F34" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
         <v>0x8C10</v>
       </c>
-      <c r="G34" s="24">
+      <c r="G34" s="23">
         <f t="shared" ref="G34" si="50">HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
         <v>35840</v>
       </c>
-      <c r="H34" s="24">
+      <c r="H34" s="23">
         <f t="shared" si="48"/>
         <v>16</v>
       </c>
-      <c r="I34" s="24">
+      <c r="I34" s="23">
         <f>G34+H34</f>
         <v>35856</v>
       </c>
-      <c r="J34" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="L34" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="M34" s="29">
+      <c r="J34" s="23" t="s">
+        <v>186</v>
+      </c>
+      <c r="L34" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="M34" s="28">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B35" s="25"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="24" t="str">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B35" s="24"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="23" t="str">
         <f>F34</f>
         <v>0x8C10</v>
       </c>
-      <c r="E35" s="24" t="str">
+      <c r="E35" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M81))</f>
         <v>0x300</v>
       </c>
-      <c r="F35" s="24" t="str">
+      <c r="F35" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
         <v>0x8F10</v>
       </c>
-      <c r="G35" s="24">
+      <c r="G35" s="23">
         <f t="shared" si="47"/>
         <v>35856</v>
       </c>
-      <c r="H35" s="24">
+      <c r="H35" s="23">
         <f t="shared" si="48"/>
         <v>768</v>
       </c>
-      <c r="I35" s="24">
+      <c r="I35" s="23">
         <f>G35+H35</f>
         <v>36624</v>
       </c>
-      <c r="J35" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="L35" s="31" t="s">
-        <v>78</v>
-      </c>
-      <c r="M35" s="19">
+      <c r="J35" s="23" t="s">
+        <v>191</v>
+      </c>
+      <c r="L35" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="M35" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B36" s="25"/>
-      <c r="C36" s="28"/>
-      <c r="D36" s="28" t="str">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B36" s="24"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27" t="str">
         <f>F35</f>
         <v>0x8F10</v>
       </c>
-      <c r="E36" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="F36" s="28" t="str">
+      <c r="E36" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="F36" s="27" t="str">
         <f t="shared" ref="F36" si="51">_xlfn.CONCAT("0x",DEC2HEX(I36))</f>
         <v>0x9000</v>
       </c>
-      <c r="G36" s="28">
+      <c r="G36" s="27">
         <f t="shared" ref="G36" si="52">HEX2DEC(MID(D36, 3, LEN(D36)-2))</f>
         <v>36624</v>
       </c>
-      <c r="H36" s="28">
+      <c r="H36" s="27">
         <f t="shared" si="48"/>
         <v>240</v>
       </c>
-      <c r="I36" s="28">
+      <c r="I36" s="27">
         <f t="shared" ref="I36" si="53">G36+H36</f>
         <v>36864</v>
       </c>
-      <c r="J36" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L36" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="M36" s="19">
+      <c r="J36" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L36" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="M36" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B37" s="25"/>
-      <c r="C37" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" s="24" t="str">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B37" s="24"/>
+      <c r="C37" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="23" t="str">
         <f>F36</f>
         <v>0x9000</v>
       </c>
-      <c r="E37" s="24" t="s">
+      <c r="E37" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="24" t="str">
+      <c r="F37" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I37))</f>
         <v>0x9800</v>
       </c>
-      <c r="G37" s="24">
+      <c r="G37" s="23">
         <f>HEX2DEC(MID(D37, 3, LEN(D37)-2))</f>
         <v>36864</v>
       </c>
-      <c r="H37" s="24">
+      <c r="H37" s="23">
         <f t="shared" si="28"/>
         <v>2048</v>
       </c>
-      <c r="I37" s="24">
+      <c r="I37" s="23">
         <f>G37+H37</f>
         <v>38912</v>
       </c>
-      <c r="J37" s="24" t="s">
+      <c r="J37" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="L37" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="M37" s="19">
+      <c r="L37" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="M37" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B38" s="25"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="24" t="str">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B38" s="24"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0x9800</v>
       </c>
-      <c r="E38" s="24" t="s">
+      <c r="E38" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="24" t="str">
+      <c r="F38" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I38))</f>
         <v>0xA000</v>
       </c>
-      <c r="G38" s="24">
+      <c r="G38" s="23">
         <f>HEX2DEC(MID(D38, 3, LEN(D38)-2))</f>
         <v>38912</v>
       </c>
-      <c r="H38" s="24">
+      <c r="H38" s="23">
         <f>HEX2DEC(MID(E38, 3, LEN(E38)-2))</f>
         <v>2048</v>
       </c>
-      <c r="I38" s="24">
+      <c r="I38" s="23">
         <f>G38+H38</f>
         <v>40960</v>
       </c>
-      <c r="J38" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="L38" s="19" t="s">
-        <v>186</v>
-      </c>
-      <c r="M38" s="19">
+      <c r="J38" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="L38" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="M38" s="18">
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B39" s="25"/>
-      <c r="C39" s="34"/>
-      <c r="D39" s="24" t="str">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B39" s="24"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0xA000</v>
       </c>
-      <c r="E39" s="24" t="s">
+      <c r="E39" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F39" s="24" t="str">
+      <c r="F39" s="23" t="str">
         <f t="shared" ref="F39" si="54">_xlfn.CONCAT("0x",DEC2HEX(I39))</f>
         <v>0xA800</v>
       </c>
-      <c r="G39" s="24">
+      <c r="G39" s="23">
         <f t="shared" ref="G39" si="55">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
         <v>40960</v>
       </c>
-      <c r="H39" s="24">
+      <c r="H39" s="23">
         <f t="shared" ref="H39" si="56">HEX2DEC(MID(E39, 3, LEN(E39)-2))</f>
         <v>2048</v>
       </c>
-      <c r="I39" s="24">
+      <c r="I39" s="23">
         <f t="shared" ref="I39" si="57">G39+H39</f>
         <v>43008</v>
       </c>
-      <c r="J39" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="L39" s="47" t="s">
-        <v>163</v>
-      </c>
-      <c r="M39" s="47">
+      <c r="J39" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="L39" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="M39" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B40" s="25"/>
-      <c r="C40" s="35"/>
-      <c r="D40" s="24" t="str">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B40" s="24"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0xA800</v>
       </c>
-      <c r="E40" s="24" t="s">
+      <c r="E40" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="F40" s="24" t="str">
+      <c r="F40" s="23" t="str">
         <f t="shared" ref="F40" si="58">_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
         <v>0xB000</v>
       </c>
-      <c r="G40" s="24">
+      <c r="G40" s="23">
         <f t="shared" ref="G40" si="59">HEX2DEC(MID(D40, 3, LEN(D40)-2))</f>
         <v>43008</v>
       </c>
-      <c r="H40" s="24">
+      <c r="H40" s="23">
         <f t="shared" ref="H40" si="60">HEX2DEC(MID(E40, 3, LEN(E40)-2))</f>
         <v>2048</v>
       </c>
-      <c r="I40" s="24">
+      <c r="I40" s="23">
         <f t="shared" ref="I40" si="61">G40+H40</f>
         <v>45056</v>
       </c>
-      <c r="J40" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="L40" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="M40" s="19">
+      <c r="J40" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="L40" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="M40" s="18">
         <v>9</v>
       </c>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B41" s="25"/>
-      <c r="C41" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="D41" s="24" t="str">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B41" s="24"/>
+      <c r="C41" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0xB000</v>
       </c>
-      <c r="E41" s="24" t="str">
+      <c r="E41" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M46))</f>
         <v>0x80</v>
       </c>
-      <c r="F41" s="24" t="str">
+      <c r="F41" s="23" t="str">
         <f t="shared" ref="F41:F42" si="62">_xlfn.CONCAT("0x",DEC2HEX(I41))</f>
         <v>0xB080</v>
       </c>
-      <c r="G41" s="24">
+      <c r="G41" s="23">
         <f t="shared" ref="G41:G42" si="63">HEX2DEC(MID(D41, 3, LEN(D41)-2))</f>
         <v>45056</v>
       </c>
-      <c r="H41" s="24">
+      <c r="H41" s="23">
         <f t="shared" ref="H41:H42" si="64">HEX2DEC(MID(E41, 3, LEN(E41)-2))</f>
         <v>128</v>
       </c>
-      <c r="I41" s="24">
+      <c r="I41" s="23">
         <f t="shared" ref="I41:I42" si="65">G41+H41</f>
         <v>45184</v>
       </c>
-      <c r="J41" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="L41" s="31" t="s">
-        <v>80</v>
-      </c>
-      <c r="M41" s="19">
+      <c r="J41" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="L41" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="M41" s="18">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B42" s="25"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="28" t="str">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B42" s="24"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="27" t="str">
         <f t="shared" si="1"/>
         <v>0xB080</v>
       </c>
-      <c r="E42" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="F42" s="28" t="str">
+      <c r="E42" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="F42" s="27" t="str">
         <f t="shared" si="62"/>
         <v>0xB400</v>
       </c>
-      <c r="G42" s="28">
+      <c r="G42" s="27">
         <f t="shared" si="63"/>
         <v>45184</v>
       </c>
-      <c r="H42" s="28">
+      <c r="H42" s="27">
         <f t="shared" si="64"/>
         <v>896</v>
       </c>
-      <c r="I42" s="28">
+      <c r="I42" s="27">
         <f t="shared" si="65"/>
         <v>46080</v>
       </c>
-      <c r="J42" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L42" s="47" t="s">
-        <v>163</v>
-      </c>
-      <c r="M42" s="47">
+      <c r="J42" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L42" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="M42" s="43">
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B43" s="25"/>
-      <c r="C43" s="37"/>
-      <c r="D43" s="24" t="str">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B43" s="24"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="23" t="str">
         <f t="shared" ref="D43:D44" si="66">F42</f>
         <v>0xB400</v>
       </c>
-      <c r="E43" s="24" t="str">
+      <c r="E43" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M59))</f>
         <v>0x4</v>
       </c>
-      <c r="F43" s="24" t="str">
+      <c r="F43" s="23" t="str">
         <f t="shared" ref="F43:F44" si="67">_xlfn.CONCAT("0x",DEC2HEX(I43))</f>
         <v>0xB404</v>
       </c>
-      <c r="G43" s="24">
+      <c r="G43" s="23">
         <f t="shared" ref="G43:G44" si="68">HEX2DEC(MID(D43, 3, LEN(D43)-2))</f>
         <v>46080</v>
       </c>
-      <c r="H43" s="24">
+      <c r="H43" s="23">
         <f t="shared" ref="H43:H44" si="69">HEX2DEC(MID(E43, 3, LEN(E43)-2))</f>
         <v>4</v>
       </c>
-      <c r="I43" s="24">
+      <c r="I43" s="23">
         <f t="shared" ref="I43:I44" si="70">G43+H43</f>
         <v>46084</v>
       </c>
-      <c r="J43" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="L43" s="31" t="s">
-        <v>70</v>
-      </c>
-      <c r="M43" s="19">
+      <c r="J43" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="L43" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="M43" s="18">
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B44" s="39"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="28" t="str">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B44" s="36"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="27" t="str">
         <f t="shared" si="66"/>
         <v>0xB404</v>
       </c>
-      <c r="E44" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="F44" s="28" t="str">
+      <c r="E44" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="F44" s="27" t="str">
         <f t="shared" si="67"/>
         <v>0xB800</v>
       </c>
-      <c r="G44" s="28">
+      <c r="G44" s="27">
         <f t="shared" si="68"/>
         <v>46084</v>
       </c>
-      <c r="H44" s="28">
+      <c r="H44" s="27">
         <f t="shared" si="69"/>
         <v>1020</v>
       </c>
-      <c r="I44" s="28">
+      <c r="I44" s="27">
         <f t="shared" si="70"/>
         <v>47104</v>
       </c>
-      <c r="J44" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="L44" s="30" t="s">
+      <c r="J44" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="L44" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="M44" s="30">
+      <c r="M44" s="29">
         <f>SUM(M35:M43)</f>
         <v>32</v>
       </c>
-      <c r="N44" s="33"/>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B45" s="41" t="s">
-        <v>143</v>
-      </c>
-      <c r="C45" s="38"/>
-      <c r="D45" s="24" t="str">
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B45" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="C45" s="35"/>
+      <c r="D45" s="23" t="str">
         <f>F44</f>
         <v>0xB800</v>
       </c>
-      <c r="E45" s="24" t="str">
+      <c r="E45" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M53))</f>
         <v>0x800</v>
       </c>
-      <c r="F45" s="24" t="str">
+      <c r="F45" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I45))</f>
         <v>0xC000</v>
       </c>
-      <c r="G45" s="24">
+      <c r="G45" s="23">
         <f t="shared" ref="G45:H47" si="71">HEX2DEC(MID(D45, 3, LEN(D45)-2))</f>
         <v>47104</v>
       </c>
-      <c r="H45" s="24">
+      <c r="H45" s="23">
         <f t="shared" si="71"/>
         <v>2048</v>
       </c>
-      <c r="I45" s="24">
+      <c r="I45" s="23">
         <f>G45+H45</f>
         <v>49152</v>
       </c>
-      <c r="J45" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="L45" s="19" t="s">
+      <c r="J45" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="L45" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="M45" s="19">
+      <c r="M45" s="18">
         <f>M44/8</f>
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B46" s="42" t="s">
-        <v>142</v>
-      </c>
-      <c r="C46" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="D46" s="24" t="str">
+    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B46" s="39" t="s">
+        <v>141</v>
+      </c>
+      <c r="C46" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" s="23" t="str">
         <f>F45</f>
         <v>0xC000</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="E46" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="F46" s="24" t="str">
+      <c r="F46" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I46))</f>
         <v>0x10000</v>
       </c>
-      <c r="G46" s="24">
+      <c r="G46" s="23">
         <f t="shared" si="71"/>
         <v>49152</v>
       </c>
-      <c r="H46" s="24">
+      <c r="H46" s="23">
         <f t="shared" si="71"/>
         <v>16384</v>
       </c>
-      <c r="I46" s="24">
+      <c r="I46" s="23">
         <f>G46+H46</f>
         <v>65536</v>
       </c>
-      <c r="J46" s="24" t="s">
+      <c r="J46" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="L46" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="M46" s="30">
+      <c r="L46" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="M46" s="29">
         <f>M34*M45</f>
         <v>128</v>
       </c>
     </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B47" s="42"/>
-      <c r="C47" s="43" t="s">
-        <v>54</v>
-      </c>
-      <c r="D47" s="24" t="str">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B47" s="39"/>
+      <c r="C47" s="40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0x10000</v>
       </c>
-      <c r="E47" s="24" t="str">
+      <c r="E47" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
         <v>0x100</v>
       </c>
-      <c r="F47" s="24" t="str">
+      <c r="F47" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I47))</f>
         <v>0x10100</v>
       </c>
-      <c r="G47" s="24">
+      <c r="G47" s="23">
         <f t="shared" si="71"/>
         <v>65536</v>
       </c>
-      <c r="H47" s="24">
+      <c r="H47" s="23">
         <f t="shared" si="71"/>
         <v>256</v>
       </c>
-      <c r="I47" s="24">
+      <c r="I47" s="23">
         <f>G47+H47</f>
         <v>65792</v>
       </c>
-      <c r="J47" s="24" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B48" s="42"/>
-      <c r="L48" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="M48" s="19" t="s">
-        <v>135</v>
+      <c r="J47" s="23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B48" s="39"/>
+      <c r="L48" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="M48" s="18" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="2:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="B49" s="42"/>
+      <c r="B49" s="39"/>
       <c r="C49"/>
       <c r="D49"/>
       <c r="E49"/>
@@ -3147,422 +3134,418 @@
       <c r="H49"/>
       <c r="I49"/>
       <c r="J49"/>
-      <c r="L49" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="M49" s="19">
+      <c r="L49" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="M49" s="18">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B50" s="42"/>
-      <c r="C50" s="36" t="s">
-        <v>55</v>
-      </c>
-      <c r="D50" s="24"/>
-      <c r="E50" s="24" t="str">
+      <c r="B50" s="39"/>
+      <c r="C50" s="33" t="s">
+        <v>54</v>
+      </c>
+      <c r="D50" s="23"/>
+      <c r="E50" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M31))</f>
         <v>0x4000</v>
       </c>
-      <c r="F50" s="24"/>
-      <c r="G50" s="24"/>
-      <c r="H50" s="24">
+      <c r="F50" s="23"/>
+      <c r="G50" s="23"/>
+      <c r="H50" s="23">
         <f>HEX2DEC(MID(E50, 3, LEN(E50)-2))</f>
         <v>16384</v>
       </c>
-      <c r="I50" s="24"/>
-      <c r="J50" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="L50" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="M50" s="19">
+      <c r="I50" s="23"/>
+      <c r="J50" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="L50" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="M50" s="18">
         <v>512</v>
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B51" s="42"/>
-      <c r="C51" s="38"/>
-      <c r="D51" s="24"/>
-      <c r="E51" s="24" t="str">
+      <c r="B51" s="39"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="23"/>
+      <c r="E51" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(M65))</f>
         <v>0x800</v>
       </c>
-      <c r="F51" s="24"/>
-      <c r="G51" s="24"/>
-      <c r="H51" s="24">
+      <c r="F51" s="23"/>
+      <c r="G51" s="23"/>
+      <c r="H51" s="23">
         <f>HEX2DEC(MID(E51, 3, LEN(E51)-2))</f>
         <v>2048</v>
       </c>
-      <c r="I51" s="24" t="s">
-        <v>157</v>
-      </c>
-      <c r="J51" s="24" t="s">
-        <v>133</v>
-      </c>
-      <c r="L51" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="M51" s="29">
+      <c r="I51" s="23" t="s">
+        <v>156</v>
+      </c>
+      <c r="J51" s="23" t="s">
+        <v>132</v>
+      </c>
+      <c r="L51" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="M51" s="28">
         <v>16</v>
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B52" s="42"/>
-      <c r="L52" s="19" t="s">
-        <v>147</v>
-      </c>
-      <c r="M52" s="19">
+      <c r="B52" s="39"/>
+      <c r="L52" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="M52" s="18">
         <f>M49*M50*M51</f>
         <v>16384</v>
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B53" s="42"/>
-      <c r="L53" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="M53" s="19">
+      <c r="B53" s="39"/>
+      <c r="L53" s="18" t="s">
+        <v>145</v>
+      </c>
+      <c r="M53" s="18">
         <f>M52/8</f>
         <v>2048</v>
       </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B54" s="42"/>
-      <c r="C54" s="43" t="s">
-        <v>154</v>
-      </c>
-      <c r="D54" s="24"/>
-      <c r="E54" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="F54" s="24"/>
-      <c r="G54" s="24"/>
-      <c r="H54" s="24">
+      <c r="B54" s="39"/>
+      <c r="C54" s="40" t="s">
+        <v>153</v>
+      </c>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="23">
         <f t="shared" ref="H54" si="72">HEX2DEC(MID(E54, 3, LEN(E54)-2))</f>
         <v>131072</v>
       </c>
-      <c r="I54" s="24"/>
-      <c r="J54" s="24" t="s">
-        <v>154</v>
+      <c r="I54" s="23"/>
+      <c r="J54" s="23" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B55" s="42"/>
-      <c r="C55" s="43" t="s">
+      <c r="B55" s="39"/>
+      <c r="C55" s="40" t="s">
+        <v>166</v>
+      </c>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="D55" s="24"/>
-      <c r="E55" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="F55" s="24"/>
-      <c r="G55" s="24"/>
-      <c r="H55" s="24">
+      <c r="F55" s="23"/>
+      <c r="G55" s="23"/>
+      <c r="H55" s="23">
         <f t="shared" ref="H55" si="73">HEX2DEC(MID(E55, 3, LEN(E55)-2))</f>
         <v>65536</v>
       </c>
-      <c r="I55" s="24"/>
-      <c r="J55" s="24" t="s">
-        <v>167</v>
-      </c>
-      <c r="L55" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="M55" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="P55" s="19" t="s">
-        <v>150</v>
+      <c r="I55" s="23"/>
+      <c r="J55" s="23" t="s">
+        <v>166</v>
+      </c>
+      <c r="L55" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="M55" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="P55" s="18" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B56" s="42"/>
-      <c r="L56" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="M56" s="19">
+      <c r="B56" s="39"/>
+      <c r="L56" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="M56" s="18">
         <v>32</v>
       </c>
-      <c r="O56" s="19">
+      <c r="O56" s="18">
         <f>384*2</f>
         <v>768</v>
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B57" s="42"/>
-      <c r="L57" s="29" t="s">
+      <c r="B57" s="39"/>
+      <c r="L57" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="M57" s="29">
+      <c r="M57" s="28">
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B58" s="42"/>
-      <c r="L58" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="M58" s="19">
+      <c r="B58" s="39"/>
+      <c r="L58" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="M58" s="18">
         <f>M56*M57</f>
         <v>32</v>
       </c>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B59" s="42"/>
-      <c r="L59" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="M59" s="19">
+      <c r="B59" s="39"/>
+      <c r="L59" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="M59" s="18">
         <f>M58/8</f>
         <v>4</v>
       </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B60" s="42"/>
+      <c r="B60" s="39"/>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B61" s="42"/>
-      <c r="L61" s="21" t="s">
+      <c r="B61" s="39"/>
+      <c r="L61" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="M61" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B62" s="39"/>
+      <c r="L62" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="M61" s="19" t="s">
+      <c r="M62" s="18">
+        <v>512</v>
+      </c>
+      <c r="N62" s="18" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B63" s="39"/>
+      <c r="L63" s="18" t="s">
+        <v>147</v>
+      </c>
+      <c r="M63" s="28">
+        <v>32</v>
+      </c>
+      <c r="N63" s="18" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B62" s="42"/>
-      <c r="L62" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="M62" s="19">
-        <v>512</v>
-      </c>
-      <c r="N62" s="19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B63" s="42"/>
-      <c r="L63" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="M63" s="29">
-        <v>32</v>
-      </c>
-      <c r="N63" s="19" t="s">
-        <v>137</v>
-      </c>
-    </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B64" s="42"/>
-      <c r="L64" s="30" t="s">
-        <v>141</v>
-      </c>
-      <c r="M64" s="19">
+      <c r="B64" s="39"/>
+      <c r="L64" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="M64" s="18">
         <f>M62*M63</f>
         <v>16384</v>
       </c>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B65" s="42"/>
-      <c r="L65" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="M65" s="19">
+      <c r="B65" s="39"/>
+      <c r="L65" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="M65" s="18">
         <f>M64/8</f>
         <v>2048</v>
       </c>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B66" s="42"/>
+      <c r="B66" s="39"/>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B67" s="42"/>
-      <c r="L67" s="21" t="s">
-        <v>208</v>
+      <c r="B67" s="39"/>
+      <c r="L67" s="20" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B68" s="44"/>
-      <c r="L68" s="19" t="s">
+      <c r="B68" s="41"/>
+      <c r="L68" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="M68" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L69" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="M68" s="19">
+      <c r="M69" s="18">
         <v>8</v>
       </c>
     </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L69" s="19" t="s">
+    <row r="70" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L70" s="18" t="s">
         <v>189</v>
       </c>
-      <c r="M69" s="19">
+      <c r="M70" s="18">
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L70" s="19" t="s">
+    <row r="71" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L71" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="M70" s="19">
+      <c r="M71" s="18">
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L71" s="19" t="s">
-        <v>191</v>
-      </c>
-      <c r="M71" s="19">
-        <v>8</v>
-      </c>
-    </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L72" s="47" t="s">
-        <v>163</v>
-      </c>
-      <c r="M72" s="47">
+      <c r="L72" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="M72" s="43">
         <v>96</v>
       </c>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L73" s="30" t="s">
-        <v>194</v>
-      </c>
-      <c r="M73" s="30">
+      <c r="L73" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="M73" s="29">
         <f>SUM(M68:M72)</f>
         <v>128</v>
       </c>
     </row>
     <row r="74" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L74" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="M74" s="19">
+      <c r="L74" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="M74" s="18">
         <f>M73/8</f>
         <v>16</v>
       </c>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L76" s="21" t="s">
-        <v>192</v>
+      <c r="L76" s="20" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L77" s="19" t="s">
+      <c r="L77" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="M77" s="18">
+        <v>32</v>
+      </c>
+      <c r="N77" s="18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="78" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L78" s="18" t="s">
         <v>195</v>
       </c>
-      <c r="M77" s="19">
-        <v>32</v>
-      </c>
-      <c r="N77" s="19" t="s">
+      <c r="M78" s="18">
+        <v>24</v>
+      </c>
+      <c r="N78" s="18" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L78" s="19" t="s">
+    <row r="79" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L79" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="M79" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="80" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L80" s="29" t="s">
         <v>196</v>
       </c>
-      <c r="M78" s="19">
-        <v>24</v>
-      </c>
-      <c r="N78" s="19" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L79" s="19" t="s">
-        <v>199</v>
-      </c>
-      <c r="M79" s="19">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L80" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="M80" s="30">
+      <c r="M80" s="29">
         <f>M77*M78*M79</f>
         <v>6144</v>
       </c>
     </row>
     <row r="81" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L81" s="33" t="s">
-        <v>198</v>
-      </c>
-      <c r="M81" s="33">
+      <c r="L81" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="M81" s="18">
         <f>M80/8</f>
         <v>768</v>
       </c>
     </row>
-    <row r="82" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L82" s="33"/>
-      <c r="M82" s="33"/>
-    </row>
     <row r="83" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L83" s="21" t="s">
+      <c r="L83" s="20" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="84" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L84" s="28" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="84" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L84" s="29" t="s">
+      <c r="M84" s="28">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="85" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L85" s="18" t="s">
         <v>201</v>
       </c>
-      <c r="M84" s="29">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="85" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L85" s="19" t="s">
+      <c r="M85" s="18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L86" s="18" t="s">
         <v>202</v>
       </c>
-      <c r="M85" s="19">
+      <c r="M86" s="18">
         <v>16</v>
       </c>
     </row>
-    <row r="86" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L86" s="19" t="s">
+    <row r="87" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L87" s="18" t="s">
         <v>203</v>
       </c>
-      <c r="M86" s="19">
+      <c r="M87" s="18">
         <v>16</v>
       </c>
-    </row>
-    <row r="87" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L87" s="19" t="s">
+      <c r="N87" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="88" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L88" s="29" t="s">
         <v>204</v>
       </c>
-      <c r="M87" s="19">
-        <v>16</v>
-      </c>
-      <c r="N87" s="19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="88" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L88" s="30" t="s">
-        <v>205</v>
-      </c>
-      <c r="M88" s="30">
+      <c r="M88" s="29">
         <f>M85*M86*M87</f>
         <v>4096</v>
       </c>
     </row>
     <row r="89" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L89" s="19" t="s">
-        <v>206</v>
-      </c>
-      <c r="M89" s="19">
+      <c r="L89" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="M89" s="18">
         <f>M88/8</f>
         <v>512</v>
       </c>
     </row>
     <row r="90" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L90" s="30" t="s">
-        <v>207</v>
-      </c>
-      <c r="M90" s="30">
+      <c r="L90" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="M90" s="29">
         <f>M84*M89</f>
         <v>32768</v>
       </c>
@@ -3588,7 +3571,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="43.5703125" customWidth="1"/>
     <col min="4" max="4" width="3.5703125" customWidth="1"/>
     <col min="5" max="5" width="9.7109375" customWidth="1"/>
@@ -3597,202 +3580,202 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A2" s="13"/>
+      <c r="B2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-    </row>
-    <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="16" t="s">
+      <c r="F3" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="F3" s="16" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="G5" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="G5" s="7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="12" t="s">
+      <c r="G6" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="17" t="s">
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F7" s="10"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="F6" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="G6" s="17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F7" s="11"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="B8" s="5" t="s">
+    </row>
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="B9" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="B9" s="6" t="s">
+    </row>
+    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="B10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B10" s="5" t="s">
+    </row>
+    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="B11" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="7" t="s">
+    </row>
+    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="11" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="12" t="s">
+      <c r="B12" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
+      <c r="B15" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B15" s="5" t="s">
+    </row>
+    <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
+      <c r="B16" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B16" s="5" t="s">
+    </row>
+    <row r="17" spans="1:9" ht="180" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="180" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
+      <c r="B17" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B17" s="4" t="s">
+    </row>
+    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
+      <c r="B18" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B18" s="4" t="s">
+    </row>
+    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="10" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
+      <c r="B19" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="B19" s="7" t="s">
+    </row>
+    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+      <c r="B20" s="6" t="s">
         <v>121</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I23" s="42" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="I23" s="45" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -3817,13 +3800,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" t="s">
         <v>171</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>172</v>
-      </c>
-      <c r="C1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3868,10 +3851,10 @@
         <v>272</v>
       </c>
       <c r="D1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E1" t="s">
         <v>174</v>
-      </c>
-      <c r="E1" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3894,18 +3877,18 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="L2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Extend max frame index to 128
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69E6F1D6-B41F-4063-94BB-CD3AC8B4DBB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7700E7E-5CF6-4CEE-848C-38E15C5285D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="218">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -751,6 +751,9 @@
   </si>
   <si>
     <t>Millisecond Timer</t>
+  </si>
+  <si>
+    <t>SPRITE_MIRROR</t>
   </si>
 </sst>
 </file>
@@ -1418,10 +1421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
-  <dimension ref="B1:P90"/>
+  <dimension ref="B1:P89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M39" sqref="M39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2604,7 +2607,7 @@
         <v>0x8C00</v>
       </c>
       <c r="E34" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M74))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M73))</f>
         <v>0x10</v>
       </c>
       <c r="F34" s="23" t="str">
@@ -2641,7 +2644,7 @@
         <v>0x8C10</v>
       </c>
       <c r="E35" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M81))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M80))</f>
         <v>0x300</v>
       </c>
       <c r="F35" s="23" t="str">
@@ -2809,10 +2812,10 @@
       <c r="J39" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="L39" s="43" t="s">
-        <v>162</v>
-      </c>
-      <c r="M39" s="43">
+      <c r="L39" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="M39" s="18">
         <v>1</v>
       </c>
     </row>
@@ -2862,7 +2865,7 @@
         <v>0xB000</v>
       </c>
       <c r="E41" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M46))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M45))</f>
         <v>0x80</v>
       </c>
       <c r="F41" s="23" t="str">
@@ -2888,7 +2891,7 @@
         <v>79</v>
       </c>
       <c r="M41" s="18">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.2">
@@ -2920,11 +2923,11 @@
       <c r="J42" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="L42" s="43" t="s">
-        <v>162</v>
-      </c>
-      <c r="M42" s="43">
-        <v>1</v>
+      <c r="L42" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="M42" s="18">
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.2">
@@ -2935,7 +2938,7 @@
         <v>0xB400</v>
       </c>
       <c r="E43" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M59))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M58))</f>
         <v>0x4</v>
       </c>
       <c r="F43" s="23" t="str">
@@ -2957,11 +2960,12 @@
       <c r="J43" s="23" t="s">
         <v>89</v>
       </c>
-      <c r="L43" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="M43" s="18">
-        <v>9</v>
+      <c r="L43" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="M43" s="29">
+        <f>SUM(M35:M42)</f>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="2:13" x14ac:dyDescent="0.2">
@@ -2993,12 +2997,12 @@
       <c r="J44" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="L44" s="29" t="s">
+      <c r="L44" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M44" s="18">
+        <f>M43/8</f>
         <v>4</v>
-      </c>
-      <c r="M44" s="29">
-        <f>SUM(M35:M43)</f>
-        <v>32</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.2">
@@ -3011,7 +3015,7 @@
         <v>0xB800</v>
       </c>
       <c r="E45" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M53))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M52))</f>
         <v>0x800</v>
       </c>
       <c r="F45" s="23" t="str">
@@ -3033,12 +3037,12 @@
       <c r="J45" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="L45" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="M45" s="18">
-        <f>M44/8</f>
-        <v>4</v>
+      <c r="L45" s="29" t="s">
+        <v>137</v>
+      </c>
+      <c r="M45" s="29">
+        <f>M34*M44</f>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.2">
@@ -3073,13 +3077,6 @@
       </c>
       <c r="J46" s="23" t="s">
         <v>19</v>
-      </c>
-      <c r="L46" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="M46" s="29">
-        <f>M34*M45</f>
-        <v>128</v>
       </c>
     </row>
     <row r="47" spans="2:13" x14ac:dyDescent="0.2">
@@ -3114,14 +3111,20 @@
       <c r="J47" s="23" t="s">
         <v>52</v>
       </c>
+      <c r="L47" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="M47" s="18" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B48" s="39"/>
-      <c r="L48" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="M48" s="18" t="s">
-        <v>134</v>
+      <c r="L48" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="M48" s="18">
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="2:16" ht="15" x14ac:dyDescent="0.25">
@@ -3135,10 +3138,10 @@
       <c r="I49"/>
       <c r="J49"/>
       <c r="L49" s="18" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="M49" s="18">
-        <v>2</v>
+        <v>512</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.2">
@@ -3161,11 +3164,11 @@
       <c r="J50" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="L50" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="M50" s="18">
-        <v>512</v>
+      <c r="L50" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="M50" s="28">
+        <v>16</v>
       </c>
     </row>
     <row r="51" spans="2:16" x14ac:dyDescent="0.2">
@@ -3173,7 +3176,7 @@
       <c r="C51" s="35"/>
       <c r="D51" s="23"/>
       <c r="E51" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M65))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M64))</f>
         <v>0x800</v>
       </c>
       <c r="F51" s="23"/>
@@ -3188,32 +3191,26 @@
       <c r="J51" s="23" t="s">
         <v>132</v>
       </c>
-      <c r="L51" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="M51" s="28">
-        <v>16</v>
+      <c r="L51" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="M51" s="18">
+        <f>M48*M49*M50</f>
+        <v>16384</v>
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B52" s="39"/>
       <c r="L52" s="18" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M52" s="18">
-        <f>M49*M50*M51</f>
-        <v>16384</v>
+        <f>M51/8</f>
+        <v>2048</v>
       </c>
     </row>
     <row r="53" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B53" s="39"/>
-      <c r="L53" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="M53" s="18">
-        <f>M52/8</f>
-        <v>2048</v>
-      </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B54" s="39"/>
@@ -3234,6 +3231,15 @@
       <c r="J54" s="23" t="s">
         <v>153</v>
       </c>
+      <c r="L54" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="M54" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="P54" s="18" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="55" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B55" s="39"/>
@@ -3254,127 +3260,124 @@
       <c r="J55" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="L55" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="M55" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="P55" s="18" t="s">
-        <v>149</v>
+      <c r="L55" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="M55" s="18">
+        <v>32</v>
+      </c>
+      <c r="O55" s="18">
+        <f>384*2</f>
+        <v>768</v>
       </c>
     </row>
     <row r="56" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B56" s="39"/>
-      <c r="L56" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="M56" s="18">
-        <v>32</v>
-      </c>
-      <c r="O56" s="18">
-        <f>384*2</f>
-        <v>768</v>
+      <c r="L56" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="M56" s="28">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B57" s="39"/>
-      <c r="L57" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="M57" s="28">
-        <v>1</v>
+      <c r="L57" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="M57" s="18">
+        <f>M55*M56</f>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B58" s="39"/>
       <c r="L58" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="M58" s="18">
-        <f>M56*M57</f>
-        <v>32</v>
+        <f>M57/8</f>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B59" s="39"/>
-      <c r="L59" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="M59" s="18">
-        <f>M58/8</f>
-        <v>4</v>
-      </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B60" s="39"/>
+      <c r="L60" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="M60" s="18" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B61" s="39"/>
-      <c r="L61" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="M61" s="18" t="s">
-        <v>135</v>
+      <c r="L61" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="M61" s="18">
+        <v>512</v>
+      </c>
+      <c r="N61" s="18" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B62" s="39"/>
       <c r="L62" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="M62" s="18">
-        <v>512</v>
+        <v>147</v>
+      </c>
+      <c r="M62" s="28">
+        <v>32</v>
       </c>
       <c r="N62" s="18" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B63" s="39"/>
-      <c r="L63" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="M63" s="28">
-        <v>32</v>
-      </c>
-      <c r="N63" s="18" t="s">
-        <v>136</v>
+      <c r="L63" s="29" t="s">
+        <v>140</v>
+      </c>
+      <c r="M63" s="18">
+        <f>M61*M62</f>
+        <v>16384</v>
       </c>
     </row>
     <row r="64" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B64" s="39"/>
-      <c r="L64" s="29" t="s">
-        <v>140</v>
+      <c r="L64" s="18" t="s">
+        <v>139</v>
       </c>
       <c r="M64" s="18">
-        <f>M62*M63</f>
-        <v>16384</v>
+        <f>M63/8</f>
+        <v>2048</v>
       </c>
     </row>
     <row r="65" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B65" s="39"/>
-      <c r="L65" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="M65" s="18">
-        <f>M64/8</f>
-        <v>2048</v>
-      </c>
     </row>
     <row r="66" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B66" s="39"/>
+      <c r="L66" s="20" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="67" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B67" s="39"/>
-      <c r="L67" s="20" t="s">
-        <v>207</v>
+      <c r="L67" s="18" t="s">
+        <v>187</v>
+      </c>
+      <c r="M67" s="18">
+        <v>8</v>
       </c>
     </row>
     <row r="68" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B68" s="41"/>
       <c r="L68" s="18" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="M68" s="18">
         <v>8</v>
@@ -3382,7 +3385,7 @@
     </row>
     <row r="69" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L69" s="18" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="M69" s="18">
         <v>8</v>
@@ -3390,115 +3393,115 @@
     </row>
     <row r="70" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L70" s="18" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="M70" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="71" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L71" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="M71" s="18">
-        <v>8</v>
+      <c r="L71" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="M71" s="43">
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L72" s="43" t="s">
-        <v>162</v>
-      </c>
-      <c r="M72" s="43">
-        <v>96</v>
+      <c r="L72" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="M72" s="29">
+        <f>SUM(M67:M71)</f>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L73" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="M73" s="29">
-        <f>SUM(M68:M72)</f>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L74" s="18" t="s">
+      <c r="L73" s="18" t="s">
         <v>192</v>
       </c>
-      <c r="M74" s="18">
-        <f>M73/8</f>
+      <c r="M73" s="18">
+        <f>M72/8</f>
         <v>16</v>
       </c>
     </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L75" s="20" t="s">
+        <v>191</v>
+      </c>
+    </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L76" s="20" t="s">
-        <v>191</v>
+      <c r="L76" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="M76" s="18">
+        <v>32</v>
+      </c>
+      <c r="N76" s="18" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="77" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L77" s="18" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="M77" s="18">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="N77" s="18" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="2:14" x14ac:dyDescent="0.2">
       <c r="L78" s="18" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="M78" s="18">
-        <v>24</v>
-      </c>
-      <c r="N78" s="18" t="s">
-        <v>209</v>
+        <v>8</v>
       </c>
     </row>
     <row r="79" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L79" s="18" t="s">
-        <v>198</v>
-      </c>
-      <c r="M79" s="18">
-        <v>8</v>
+      <c r="L79" s="29" t="s">
+        <v>196</v>
+      </c>
+      <c r="M79" s="29">
+        <f>M76*M77*M78</f>
+        <v>6144</v>
       </c>
     </row>
     <row r="80" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L80" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="M80" s="29">
-        <f>M77*M78*M79</f>
-        <v>6144</v>
-      </c>
-    </row>
-    <row r="81" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L81" s="18" t="s">
+      <c r="L80" s="18" t="s">
         <v>197</v>
       </c>
-      <c r="M81" s="18">
-        <f>M80/8</f>
+      <c r="M80" s="18">
+        <f>M79/8</f>
         <v>768</v>
       </c>
     </row>
+    <row r="82" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L82" s="20" t="s">
+        <v>199</v>
+      </c>
+    </row>
     <row r="83" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L83" s="20" t="s">
-        <v>199</v>
+      <c r="L83" s="28" t="s">
+        <v>200</v>
+      </c>
+      <c r="M83" s="28">
+        <v>64</v>
       </c>
     </row>
     <row r="84" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L84" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="M84" s="28">
-        <v>64</v>
+      <c r="L84" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="M84" s="18">
+        <v>16</v>
       </c>
     </row>
     <row r="85" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L85" s="18" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="M85" s="18">
         <v>16</v>
@@ -3506,47 +3509,39 @@
     </row>
     <row r="86" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L86" s="18" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="M86" s="18">
         <v>16</v>
       </c>
+      <c r="N86" s="18" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="87" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L87" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="M87" s="18">
-        <v>16</v>
-      </c>
-      <c r="N87" s="18" t="s">
-        <v>80</v>
+      <c r="L87" s="29" t="s">
+        <v>204</v>
+      </c>
+      <c r="M87" s="29">
+        <f>M84*M85*M86</f>
+        <v>4096</v>
       </c>
     </row>
     <row r="88" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L88" s="29" t="s">
-        <v>204</v>
-      </c>
-      <c r="M88" s="29">
-        <f>M85*M86*M87</f>
-        <v>4096</v>
+      <c r="L88" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="M88" s="18">
+        <f>M87/8</f>
+        <v>512</v>
       </c>
     </row>
     <row r="89" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L89" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="M89" s="18">
-        <f>M88/8</f>
-        <v>512</v>
-      </c>
-    </row>
-    <row r="90" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L90" s="29" t="s">
+      <c r="L89" s="29" t="s">
         <v>206</v>
       </c>
-      <c r="M90" s="29">
-        <f>M84*M89</f>
+      <c r="M89" s="29">
+        <f>M83*M88</f>
         <v>32768</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Start HFCR, memory map reshuffle
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7700E7E-5CF6-4CEE-848C-38E15C5285D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFEF2A89-B4EE-4476-A13D-93403991A1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hardware" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="215">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -93,12 +93,6 @@
     <t>0x000C</t>
   </si>
   <si>
-    <t>0x0021</t>
-  </si>
-  <si>
-    <t>0x0011</t>
-  </si>
-  <si>
     <t>Work RAM</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>0x0040</t>
   </si>
   <si>
-    <t>0x00A0</t>
-  </si>
-  <si>
     <t>Length D</t>
   </si>
   <si>
@@ -156,15 +147,6 @@
     <t>End H</t>
   </si>
   <si>
-    <t>0x00D0</t>
-  </si>
-  <si>
-    <t>0x00F4</t>
-  </si>
-  <si>
-    <t>0x00DF</t>
-  </si>
-  <si>
     <t>Area</t>
   </si>
   <si>
@@ -289,12 +271,6 @@
   </si>
   <si>
     <t>0x8000</t>
-  </si>
-  <si>
-    <t>0x8A00</t>
-  </si>
-  <si>
-    <t>0x00EF</t>
   </si>
   <si>
     <t>0x0010</t>
@@ -651,9 +627,6 @@
     <t>CHAR_ROM_BYTES_TOTAL</t>
   </si>
   <si>
-    <t>0x00E0</t>
-  </si>
-  <si>
     <t>(Tile map)</t>
   </si>
   <si>
@@ -738,15 +711,9 @@
     <t>O</t>
   </si>
   <si>
-    <t>0x00CE</t>
-  </si>
-  <si>
     <t>System menu trigger</t>
   </si>
   <si>
-    <t>0x00FE</t>
-  </si>
-  <si>
     <t>System outputs (video options)</t>
   </si>
   <si>
@@ -754,6 +721,30 @@
   </si>
   <si>
     <t>SPRITE_MIRROR</t>
+  </si>
+  <si>
+    <t>0x0020</t>
+  </si>
+  <si>
+    <t>0x0050</t>
+  </si>
+  <si>
+    <t>0x0074</t>
+  </si>
+  <si>
+    <t>0x007E</t>
+  </si>
+  <si>
+    <t>0x004E</t>
+  </si>
+  <si>
+    <t>0x0004</t>
+  </si>
+  <si>
+    <t>0x006C</t>
+  </si>
+  <si>
+    <t>0x0600</t>
   </si>
 </sst>
 </file>
@@ -992,7 +983,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1107,6 +1098,7 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1421,10 +1413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
-  <dimension ref="B1:P89"/>
+  <dimension ref="B1:P104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M39" sqref="M39"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1446,46 +1438,46 @@
     <col min="15" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B1" s="17" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B2" s="19" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F2" s="19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I2" s="19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="J2" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L2" s="20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="3" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="21" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C3" s="22" t="s">
         <v>7</v>
@@ -1494,14 +1486,14 @@
         <v>5</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="F3" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I3))</f>
         <v>0x8000</v>
       </c>
       <c r="G3" s="23">
-        <f t="shared" ref="G3:H7" si="0">HEX2DEC(MID(D3, 3, LEN(D3)-2))</f>
+        <f t="shared" ref="G3:H11" si="0">HEX2DEC(MID(D3, 3, LEN(D3)-2))</f>
         <v>0</v>
       </c>
       <c r="H3" s="23">
@@ -1526,15 +1518,15 @@
         <v>352</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B4" s="24" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D4" s="23" t="str">
-        <f t="shared" ref="D4:D47" si="1">F3</f>
+        <f t="shared" ref="D4:D48" si="1">F3</f>
         <v>0x8000</v>
       </c>
       <c r="E4" s="23" t="s">
@@ -1569,8 +1561,12 @@
         <f>M5+SCREEN_BORDER_WIDTH</f>
         <v>272</v>
       </c>
-    </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O4" s="18">
+        <f>M4/8</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B5" s="24"/>
       <c r="C5" s="26"/>
       <c r="D5" s="23" t="str">
@@ -1597,7 +1593,7 @@
         <v>32770</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="L5" s="18" t="s">
         <v>0</v>
@@ -1605,8 +1601,12 @@
       <c r="M5" s="18">
         <v>240</v>
       </c>
-    </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="O5" s="18">
+        <f>M5/8</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B6" s="24"/>
       <c r="C6" s="26"/>
       <c r="D6" s="27" t="str">
@@ -1614,11 +1614,11 @@
         <v>0x8002</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="F6" s="27" t="str">
         <f t="shared" ref="F6" si="5">_xlfn.CONCAT("0x",DEC2HEX(I6))</f>
-        <v>0x8100</v>
+        <v>0x8080</v>
       </c>
       <c r="G6" s="27">
         <f t="shared" si="0"/>
@@ -1626,401 +1626,406 @@
       </c>
       <c r="H6" s="27">
         <f t="shared" si="0"/>
-        <v>254</v>
+        <v>126</v>
       </c>
       <c r="I6" s="27">
         <f>G6+H6</f>
-        <v>33024</v>
+        <v>32896</v>
       </c>
       <c r="J6" s="27" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B7" s="24"/>
       <c r="C7" s="26"/>
       <c r="D7" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>0x8100</v>
+        <f t="shared" ref="D7" si="6">F6</f>
+        <v>0x8080</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>13</v>
+        <v>207</v>
       </c>
       <c r="F7" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I7))</f>
-        <v>0x81C0</v>
+        <v>0x80A0</v>
       </c>
       <c r="G7" s="23">
         <f t="shared" si="0"/>
-        <v>33024</v>
+        <v>32896</v>
       </c>
       <c r="H7" s="23">
         <f t="shared" si="0"/>
-        <v>192</v>
+        <v>32</v>
       </c>
       <c r="I7" s="23">
         <f>G7+H7</f>
-        <v>33216</v>
+        <v>32928</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+      <c r="O7" s="18">
+        <f>O4*O5</f>
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B8" s="24"/>
       <c r="C8" s="26"/>
       <c r="D8" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>0x81C0</v>
+        <f>F7</f>
+        <v>0x80A0</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>30</v>
+        <v>207</v>
       </c>
       <c r="F8" s="27" t="str">
-        <f t="shared" ref="F8" si="6">_xlfn.CONCAT("0x",DEC2HEX(I8))</f>
-        <v>0x8200</v>
+        <f t="shared" ref="F8" si="7">_xlfn.CONCAT("0x",DEC2HEX(I8))</f>
+        <v>0x80C0</v>
       </c>
       <c r="G8" s="27">
-        <f t="shared" ref="G8" si="7">HEX2DEC(MID(D8, 3, LEN(D8)-2))</f>
-        <v>33216</v>
+        <f t="shared" ref="G8:G10" si="8">HEX2DEC(MID(D8, 3, LEN(D8)-2))</f>
+        <v>32928</v>
       </c>
       <c r="H8" s="27">
-        <f t="shared" ref="H8" si="8">HEX2DEC(MID(E8, 3, LEN(E8)-2))</f>
-        <v>64</v>
+        <f t="shared" ref="H8:H10" si="9">HEX2DEC(MID(E8, 3, LEN(E8)-2))</f>
+        <v>32</v>
       </c>
       <c r="I8" s="27">
-        <f t="shared" ref="I8" si="9">G8+H8</f>
-        <v>33280</v>
+        <f>G8+H8</f>
+        <v>32960</v>
       </c>
       <c r="J8" s="27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L8" s="28" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="M8" s="28">
         <v>256</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B9" s="24"/>
       <c r="C9" s="26"/>
       <c r="D9" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>0x8200</v>
+        <f t="shared" ref="D9" si="10">F8</f>
+        <v>0x80C0</v>
       </c>
       <c r="E9" s="23" t="s">
-        <v>14</v>
+        <v>77</v>
       </c>
       <c r="F9" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I9))</f>
-        <v>0x8260</v>
+        <v>0x80D0</v>
       </c>
       <c r="G9" s="23">
-        <f t="shared" ref="G9:H11" si="10">HEX2DEC(MID(D9, 3, LEN(D9)-2))</f>
-        <v>33280</v>
+        <f t="shared" si="8"/>
+        <v>32960</v>
       </c>
       <c r="H9" s="23">
-        <f t="shared" si="10"/>
-        <v>96</v>
+        <f t="shared" si="9"/>
+        <v>16</v>
       </c>
       <c r="I9" s="23">
         <f>G9+H9</f>
-        <v>33376</v>
+        <v>32976</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>26</v>
+        <v>205</v>
       </c>
       <c r="L9" s="18" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="M9" s="18">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B10" s="24"/>
       <c r="C10" s="26"/>
       <c r="D10" s="27" t="str">
-        <f t="shared" si="1"/>
-        <v>0x8260</v>
+        <f>F9</f>
+        <v>0x80D0</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="F10" s="27" t="str">
         <f t="shared" ref="F10" si="11">_xlfn.CONCAT("0x",DEC2HEX(I10))</f>
-        <v>0x8300</v>
+        <v>0x8100</v>
       </c>
       <c r="G10" s="27">
-        <f t="shared" si="10"/>
-        <v>33376</v>
+        <f t="shared" si="8"/>
+        <v>32976</v>
       </c>
       <c r="H10" s="27">
-        <f t="shared" si="10"/>
-        <v>160</v>
+        <f t="shared" si="9"/>
+        <v>48</v>
       </c>
       <c r="I10" s="27">
-        <f>G10+H10</f>
-        <v>33536</v>
+        <f t="shared" ref="I10" si="12">G10+H10</f>
+        <v>33024</v>
       </c>
       <c r="J10" s="27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L10" s="18" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="M10" s="18">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B11" s="24"/>
       <c r="C11" s="26"/>
       <c r="D11" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>0x8300</v>
+        <f>F10</f>
+        <v>0x8100</v>
       </c>
       <c r="E11" s="23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F11" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I11))</f>
-        <v>0x8360</v>
+        <v>0x81C0</v>
       </c>
       <c r="G11" s="23">
-        <f t="shared" si="10"/>
-        <v>33536</v>
+        <f t="shared" si="0"/>
+        <v>33024</v>
       </c>
       <c r="H11" s="23">
-        <f t="shared" si="10"/>
-        <v>96</v>
+        <f t="shared" si="0"/>
+        <v>192</v>
       </c>
       <c r="I11" s="23">
         <f>G11+H11</f>
-        <v>33632</v>
+        <v>33216</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="M11" s="18">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B12" s="24"/>
       <c r="C12" s="26"/>
       <c r="D12" s="27" t="str">
         <f t="shared" si="1"/>
-        <v>0x8360</v>
+        <v>0x81C0</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F12" s="27" t="str">
-        <f t="shared" ref="F12" si="12">_xlfn.CONCAT("0x",DEC2HEX(I12))</f>
-        <v>0x8400</v>
+        <f t="shared" ref="F12" si="13">_xlfn.CONCAT("0x",DEC2HEX(I12))</f>
+        <v>0x8200</v>
       </c>
       <c r="G12" s="27">
-        <f t="shared" ref="G12" si="13">HEX2DEC(MID(D12, 3, LEN(D12)-2))</f>
-        <v>33632</v>
+        <f t="shared" ref="G12" si="14">HEX2DEC(MID(D12, 3, LEN(D12)-2))</f>
+        <v>33216</v>
       </c>
       <c r="H12" s="27">
-        <f t="shared" ref="H12" si="14">HEX2DEC(MID(E12, 3, LEN(E12)-2))</f>
-        <v>160</v>
+        <f t="shared" ref="H12" si="15">HEX2DEC(MID(E12, 3, LEN(E12)-2))</f>
+        <v>64</v>
       </c>
       <c r="I12" s="27">
-        <f t="shared" ref="I12" si="15">G12+H12</f>
-        <v>33792</v>
+        <f t="shared" ref="I12" si="16">G12+H12</f>
+        <v>33280</v>
       </c>
       <c r="J12" s="27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L12" s="29" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="M12" s="29">
         <f>M9*M10*M11</f>
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B13" s="24"/>
       <c r="C13" s="26"/>
       <c r="D13" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0x8400</v>
+        <v>0x8200</v>
       </c>
       <c r="E13" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F13" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I13))</f>
-        <v>0x8430</v>
+        <v>0x8260</v>
       </c>
       <c r="G13" s="23">
-        <f t="shared" ref="G13:H15" si="16">HEX2DEC(MID(D13, 3, LEN(D13)-2))</f>
-        <v>33792</v>
+        <f t="shared" ref="G13:H15" si="17">HEX2DEC(MID(D13, 3, LEN(D13)-2))</f>
+        <v>33280</v>
       </c>
       <c r="H13" s="23">
-        <f t="shared" si="16"/>
-        <v>48</v>
+        <f t="shared" si="17"/>
+        <v>96</v>
       </c>
       <c r="I13" s="23">
         <f>G13+H13</f>
-        <v>33840</v>
+        <v>33376</v>
       </c>
       <c r="J13" s="23" t="s">
         <v>24</v>
       </c>
       <c r="L13" s="18" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="M13" s="18">
         <f>M12/8</f>
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B14" s="24"/>
       <c r="C14" s="26"/>
       <c r="D14" s="27" t="str">
         <f t="shared" si="1"/>
-        <v>0x8430</v>
+        <v>0x8260</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>38</v>
+        <v>207</v>
       </c>
       <c r="F14" s="27" t="str">
-        <f t="shared" ref="F14" si="17">_xlfn.CONCAT("0x",DEC2HEX(I14))</f>
-        <v>0x8500</v>
+        <f t="shared" ref="F14" si="18">_xlfn.CONCAT("0x",DEC2HEX(I14))</f>
+        <v>0x8280</v>
       </c>
       <c r="G14" s="27">
-        <f t="shared" si="16"/>
-        <v>33840</v>
+        <f t="shared" si="17"/>
+        <v>33376</v>
       </c>
       <c r="H14" s="27">
-        <f t="shared" si="16"/>
-        <v>208</v>
+        <f t="shared" si="17"/>
+        <v>32</v>
       </c>
       <c r="I14" s="27">
         <f>G14+H14</f>
-        <v>34048</v>
+        <v>33408</v>
       </c>
       <c r="J14" s="27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L14" s="29" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="M14" s="29">
         <f>M8*M13</f>
         <v>2048</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B15" s="24"/>
       <c r="C15" s="26"/>
       <c r="D15" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>0x8500</v>
+        <f>F14</f>
+        <v>0x8280</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F15" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I15))</f>
-        <v>0x8560</v>
+        <v>0x82E0</v>
       </c>
       <c r="G15" s="23">
-        <f t="shared" si="16"/>
-        <v>34048</v>
+        <f t="shared" si="17"/>
+        <v>33408</v>
       </c>
       <c r="H15" s="23">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>96</v>
       </c>
       <c r="I15" s="23">
         <f>G15+H15</f>
-        <v>34144</v>
+        <v>33504</v>
       </c>
       <c r="J15" s="23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L15" s="48"/>
+      <c r="M15" s="48"/>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B16" s="24"/>
       <c r="C16" s="26"/>
       <c r="D16" s="27" t="str">
         <f t="shared" si="1"/>
-        <v>0x8560</v>
+        <v>0x82E0</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>31</v>
+        <v>207</v>
       </c>
       <c r="F16" s="27" t="str">
-        <f t="shared" ref="F16" si="18">_xlfn.CONCAT("0x",DEC2HEX(I16))</f>
-        <v>0x8600</v>
+        <f t="shared" ref="F16" si="19">_xlfn.CONCAT("0x",DEC2HEX(I16))</f>
+        <v>0x8300</v>
       </c>
       <c r="G16" s="27">
-        <f t="shared" ref="G16" si="19">HEX2DEC(MID(D16, 3, LEN(D16)-2))</f>
-        <v>34144</v>
+        <f t="shared" ref="G16" si="20">HEX2DEC(MID(D16, 3, LEN(D16)-2))</f>
+        <v>33504</v>
       </c>
       <c r="H16" s="27">
-        <f t="shared" ref="H16" si="20">HEX2DEC(MID(E16, 3, LEN(E16)-2))</f>
-        <v>160</v>
+        <f t="shared" ref="H16" si="21">HEX2DEC(MID(E16, 3, LEN(E16)-2))</f>
+        <v>32</v>
       </c>
       <c r="I16" s="27">
-        <f t="shared" ref="I16" si="21">G16+H16</f>
-        <v>34304</v>
+        <f t="shared" ref="I16" si="22">G16+H16</f>
+        <v>33536</v>
       </c>
       <c r="J16" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L16" s="20" t="s">
-        <v>53</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L16" s="48"/>
+      <c r="M16" s="48"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="24"/>
       <c r="C17" s="26"/>
       <c r="D17" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0x8600</v>
+        <v>0x8300</v>
       </c>
       <c r="E17" s="23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F17" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I17))</f>
-        <v>0x860C</v>
+        <v>0x8330</v>
       </c>
       <c r="G17" s="23">
-        <f t="shared" ref="G17:H19" si="22">HEX2DEC(MID(D17, 3, LEN(D17)-2))</f>
-        <v>34304</v>
+        <f t="shared" ref="G17:H19" si="23">HEX2DEC(MID(D17, 3, LEN(D17)-2))</f>
+        <v>33536</v>
       </c>
       <c r="H17" s="23">
-        <f t="shared" si="22"/>
-        <v>12</v>
+        <f t="shared" si="23"/>
+        <v>48</v>
       </c>
       <c r="I17" s="23">
         <f>G17+H17</f>
-        <v>34316</v>
+        <v>33584</v>
       </c>
       <c r="J17" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="L17" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="M17" s="28">
-        <v>4</v>
+      <c r="L17" s="48"/>
+      <c r="M17" s="48"/>
+      <c r="N17" s="18">
+        <f>256*3</f>
+        <v>768</v>
       </c>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.2">
@@ -2028,742 +2033,695 @@
       <c r="C18" s="26"/>
       <c r="D18" s="27" t="str">
         <f t="shared" si="1"/>
-        <v>0x860C</v>
+        <v>0x8330</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>39</v>
+        <v>208</v>
       </c>
       <c r="F18" s="27" t="str">
-        <f t="shared" ref="F18" si="23">_xlfn.CONCAT("0x",DEC2HEX(I18))</f>
-        <v>0x8700</v>
+        <f t="shared" ref="F18" si="24">_xlfn.CONCAT("0x",DEC2HEX(I18))</f>
+        <v>0x8380</v>
       </c>
       <c r="G18" s="27">
-        <f t="shared" si="22"/>
-        <v>34316</v>
+        <f t="shared" si="23"/>
+        <v>33584</v>
       </c>
       <c r="H18" s="27">
-        <f t="shared" si="22"/>
-        <v>244</v>
+        <f t="shared" si="23"/>
+        <v>80</v>
       </c>
       <c r="I18" s="27">
         <f>G18+H18</f>
-        <v>34560</v>
+        <v>33664</v>
       </c>
       <c r="J18" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="M18" s="18">
-        <v>16</v>
-      </c>
-      <c r="N18" s="18" t="s">
-        <v>80</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L18" s="48"/>
+      <c r="M18" s="48"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="24"/>
       <c r="C19" s="26"/>
       <c r="D19" s="23" t="str">
-        <f t="shared" si="1"/>
-        <v>0x8700</v>
+        <f>F18</f>
+        <v>0x8380</v>
       </c>
       <c r="E19" s="23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I19))</f>
-        <v>0x8730</v>
+        <v>0x83E0</v>
       </c>
       <c r="G19" s="23">
-        <f t="shared" si="22"/>
-        <v>34560</v>
+        <f t="shared" si="23"/>
+        <v>33664</v>
       </c>
       <c r="H19" s="23">
-        <f t="shared" si="22"/>
-        <v>48</v>
+        <f t="shared" si="23"/>
+        <v>96</v>
       </c>
       <c r="I19" s="23">
         <f>G19+H19</f>
-        <v>34608</v>
+        <v>33760</v>
       </c>
       <c r="J19" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="L19" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="M19" s="18">
-        <v>32</v>
-      </c>
+      <c r="L19" s="48"/>
+      <c r="M19" s="48"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="24"/>
       <c r="C20" s="26"/>
       <c r="D20" s="27" t="str">
         <f t="shared" si="1"/>
-        <v>0x8730</v>
+        <v>0x83E0</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>38</v>
+        <v>207</v>
       </c>
       <c r="F20" s="27" t="str">
-        <f t="shared" ref="F20" si="24">_xlfn.CONCAT("0x",DEC2HEX(I20))</f>
-        <v>0x8800</v>
+        <f t="shared" ref="F20" si="25">_xlfn.CONCAT("0x",DEC2HEX(I20))</f>
+        <v>0x8400</v>
       </c>
       <c r="G20" s="27">
-        <f t="shared" ref="G20" si="25">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
-        <v>34608</v>
+        <f t="shared" ref="G20" si="26">HEX2DEC(MID(D20, 3, LEN(D20)-2))</f>
+        <v>33760</v>
       </c>
       <c r="H20" s="27">
-        <f t="shared" ref="H20" si="26">HEX2DEC(MID(E20, 3, LEN(E20)-2))</f>
-        <v>208</v>
+        <f t="shared" ref="H20" si="27">HEX2DEC(MID(E20, 3, LEN(E20)-2))</f>
+        <v>32</v>
       </c>
       <c r="I20" s="27">
-        <f t="shared" ref="I20" si="27">G20+H20</f>
-        <v>34816</v>
+        <f t="shared" ref="I20" si="28">G20+H20</f>
+        <v>33792</v>
       </c>
       <c r="J20" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L20" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="M20" s="29">
-        <f>M18*M19</f>
-        <v>512</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L20" s="48"/>
+      <c r="M20" s="48"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" s="24"/>
       <c r="C21" s="26"/>
       <c r="D21" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0x8800</v>
+        <v>0x8400</v>
       </c>
       <c r="E21" s="23" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F21" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I21))</f>
-        <v>0x8821</v>
+        <v>0x840C</v>
       </c>
       <c r="G21" s="23">
-        <f t="shared" ref="G21:H37" si="28">HEX2DEC(MID(D21, 3, LEN(D21)-2))</f>
-        <v>34816</v>
+        <f t="shared" ref="G21:H23" si="29">HEX2DEC(MID(D21, 3, LEN(D21)-2))</f>
+        <v>33792</v>
       </c>
       <c r="H21" s="23">
-        <f t="shared" si="28"/>
-        <v>33</v>
+        <f t="shared" si="29"/>
+        <v>12</v>
       </c>
       <c r="I21" s="23">
         <f>G21+H21</f>
-        <v>34849</v>
+        <v>33804</v>
       </c>
       <c r="J21" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="L21" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="M21" s="18">
-        <f>M20/8</f>
-        <v>64</v>
-      </c>
+      <c r="L21" s="48"/>
+      <c r="M21" s="48"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="24"/>
       <c r="C22" s="26"/>
       <c r="D22" s="27" t="str">
         <f t="shared" si="1"/>
-        <v>0x8821</v>
+        <v>0x840C</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>40</v>
+        <v>209</v>
       </c>
       <c r="F22" s="27" t="str">
-        <f t="shared" ref="F22" si="29">_xlfn.CONCAT("0x",DEC2HEX(I22))</f>
-        <v>0x8900</v>
+        <f t="shared" ref="F22" si="30">_xlfn.CONCAT("0x",DEC2HEX(I22))</f>
+        <v>0x8480</v>
       </c>
       <c r="G22" s="27">
-        <f t="shared" si="28"/>
-        <v>34849</v>
+        <f t="shared" si="29"/>
+        <v>33804</v>
       </c>
       <c r="H22" s="27">
-        <f t="shared" si="28"/>
-        <v>223</v>
+        <f t="shared" si="29"/>
+        <v>116</v>
       </c>
       <c r="I22" s="27">
         <f>G22+H22</f>
-        <v>35072</v>
+        <v>33920</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L22" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="M22" s="29">
-        <f>M21*M17</f>
-        <v>256</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L22" s="48"/>
+      <c r="M22" s="48"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" s="24"/>
       <c r="C23" s="26"/>
       <c r="D23" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0x8900</v>
+        <v>0x8480</v>
       </c>
       <c r="E23" s="23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F23" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I23))</f>
-        <v>0x8911</v>
+        <v>0x84B0</v>
       </c>
       <c r="G23" s="23">
-        <f t="shared" si="28"/>
-        <v>35072</v>
+        <f t="shared" si="29"/>
+        <v>33920</v>
       </c>
       <c r="H23" s="23">
-        <f t="shared" si="28"/>
-        <v>17</v>
+        <f t="shared" si="29"/>
+        <v>48</v>
       </c>
       <c r="I23" s="23">
         <f>G23+H23</f>
-        <v>35089</v>
+        <v>33968</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>216</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="L23" s="48"/>
+      <c r="M23" s="48"/>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" s="24"/>
       <c r="C24" s="26"/>
       <c r="D24" s="27" t="str">
         <f>F23</f>
-        <v>0x8911</v>
+        <v>0x84B0</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>84</v>
+        <v>208</v>
       </c>
       <c r="F24" s="27" t="str">
-        <f t="shared" ref="F24" si="30">_xlfn.CONCAT("0x",DEC2HEX(I24))</f>
-        <v>0x8A00</v>
+        <f t="shared" ref="F24" si="31">_xlfn.CONCAT("0x",DEC2HEX(I24))</f>
+        <v>0x8500</v>
       </c>
       <c r="G24" s="27">
-        <f t="shared" si="28"/>
-        <v>35089</v>
+        <f t="shared" ref="G24:H37" si="32">HEX2DEC(MID(D24, 3, LEN(D24)-2))</f>
+        <v>33968</v>
       </c>
       <c r="H24" s="27">
-        <f t="shared" si="28"/>
-        <v>239</v>
+        <f t="shared" si="32"/>
+        <v>80</v>
       </c>
       <c r="I24" s="27">
-        <f t="shared" ref="I24" si="31">G24+H24</f>
-        <v>35328</v>
+        <f>G24+H24</f>
+        <v>34048</v>
       </c>
       <c r="J24" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L24" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="N24" s="18" t="s">
-        <v>152</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="L24" s="48"/>
+      <c r="M24" s="48"/>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B25" s="24"/>
       <c r="C25" s="26"/>
-      <c r="D25" s="23" t="s">
-        <v>83</v>
+      <c r="D25" s="23" t="str">
+        <f>F24</f>
+        <v>0x8500</v>
       </c>
       <c r="E25" s="23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F25" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I25))</f>
-        <v>0x8A10</v>
+        <v>0x8510</v>
       </c>
       <c r="G25" s="23">
-        <f t="shared" si="28"/>
-        <v>35328</v>
+        <f t="shared" si="32"/>
+        <v>34048</v>
       </c>
       <c r="H25" s="23">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>16</v>
       </c>
       <c r="I25" s="23">
         <f>G25+H25</f>
-        <v>35344</v>
+        <v>34064</v>
       </c>
       <c r="J25" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="L25" s="28" t="s">
-        <v>63</v>
-      </c>
-      <c r="M25" s="28">
-        <v>64</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="L25" s="48"/>
+      <c r="M25" s="48"/>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="24"/>
       <c r="C26" s="46"/>
       <c r="D26" s="23" t="str">
-        <f t="shared" ref="D26:D32" si="32">F25</f>
-        <v>0x8A10</v>
+        <f t="shared" ref="D26:D32" si="33">F25</f>
+        <v>0x8510</v>
       </c>
       <c r="E26" s="23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F26" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I26))</f>
-        <v>0x8A20</v>
+        <v>0x8520</v>
       </c>
       <c r="G26" s="23">
-        <f t="shared" ref="G26:G27" si="33">HEX2DEC(MID(D26, 3, LEN(D26)-2))</f>
-        <v>35344</v>
+        <f t="shared" ref="G26:G27" si="34">HEX2DEC(MID(D26, 3, LEN(D26)-2))</f>
+        <v>34064</v>
       </c>
       <c r="H26" s="23">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>16</v>
       </c>
       <c r="I26" s="23">
         <f>G26+H26</f>
-        <v>35360</v>
+        <v>34080</v>
       </c>
       <c r="J26" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="L26" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="M26" s="18">
-        <v>16</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="L26" s="48"/>
+      <c r="M26" s="48"/>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="24"/>
       <c r="C27" s="46"/>
       <c r="D27" s="23" t="str">
-        <f t="shared" si="32"/>
-        <v>0x8A20</v>
+        <f t="shared" si="33"/>
+        <v>0x8520</v>
       </c>
       <c r="E27" s="23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F27" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I27))</f>
-        <v>0x8A30</v>
+        <v>0x8530</v>
       </c>
       <c r="G27" s="23">
-        <f t="shared" si="33"/>
-        <v>35360</v>
+        <f t="shared" si="34"/>
+        <v>34080</v>
       </c>
       <c r="H27" s="23">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>16</v>
       </c>
       <c r="I27" s="23">
         <f>G27+H27</f>
-        <v>35376</v>
+        <v>34096</v>
       </c>
       <c r="J27" s="23" t="s">
-        <v>87</v>
-      </c>
-      <c r="L27" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="M27" s="18">
-        <v>16</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="L27" s="48"/>
+      <c r="M27" s="48"/>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="24"/>
       <c r="C28" s="26"/>
       <c r="D28" s="23" t="str">
         <f>F27</f>
-        <v>0x8A30</v>
+        <v>0x8530</v>
       </c>
       <c r="E28" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F28" s="23" t="str">
-        <f t="shared" ref="F28" si="34">_xlfn.CONCAT("0x",DEC2HEX(I28))</f>
-        <v>0x8A31</v>
+        <f t="shared" ref="F28" si="35">_xlfn.CONCAT("0x",DEC2HEX(I28))</f>
+        <v>0x8531</v>
       </c>
       <c r="G28" s="23">
         <f>HEX2DEC(MID(D28, 3, LEN(D28)-2))</f>
-        <v>35376</v>
+        <v>34096</v>
       </c>
       <c r="H28" s="23">
-        <f t="shared" ref="H28" si="35">HEX2DEC(MID(E28, 3, LEN(E28)-2))</f>
+        <f t="shared" ref="H28" si="36">HEX2DEC(MID(E28, 3, LEN(E28)-2))</f>
         <v>1</v>
       </c>
       <c r="I28" s="23">
-        <f t="shared" ref="I28" si="36">G28+H28</f>
-        <v>35377</v>
+        <f t="shared" ref="I28" si="37">G28+H28</f>
+        <v>34097</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>165</v>
-      </c>
-      <c r="L28" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="M28" s="18">
-        <v>8</v>
-      </c>
-      <c r="N28" s="18" t="s">
-        <v>163</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="L28" s="48"/>
+      <c r="M28" s="48"/>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="24"/>
       <c r="C29" s="26"/>
       <c r="D29" s="23" t="str">
         <f>F28</f>
-        <v>0x8A31</v>
+        <v>0x8531</v>
       </c>
       <c r="E29" s="23" t="s">
         <v>10</v>
       </c>
       <c r="F29" s="23" t="str">
-        <f t="shared" ref="F29" si="37">_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
-        <v>0x8A32</v>
+        <f t="shared" ref="F29" si="38">_xlfn.CONCAT("0x",DEC2HEX(I29))</f>
+        <v>0x8532</v>
       </c>
       <c r="G29" s="23">
         <f>HEX2DEC(MID(D29, 3, LEN(D29)-2))</f>
-        <v>35377</v>
+        <v>34097</v>
       </c>
       <c r="H29" s="23">
-        <f t="shared" ref="H29" si="38">HEX2DEC(MID(E29, 3, LEN(E29)-2))</f>
+        <f t="shared" ref="H29" si="39">HEX2DEC(MID(E29, 3, LEN(E29)-2))</f>
         <v>1</v>
       </c>
       <c r="I29" s="23">
-        <f t="shared" ref="I29" si="39">G29+H29</f>
-        <v>35378</v>
+        <f t="shared" ref="I29" si="40">G29+H29</f>
+        <v>34098</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>213</v>
-      </c>
-      <c r="L29" s="29" t="s">
-        <v>67</v>
-      </c>
-      <c r="M29" s="29">
-        <f>M26*M27*M28</f>
-        <v>2048</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="L29" s="48"/>
+      <c r="M29" s="48"/>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="24"/>
       <c r="C30" s="27"/>
       <c r="D30" s="27" t="str">
         <f>F29</f>
-        <v>0x8A32</v>
+        <v>0x8532</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F30" s="27" t="str">
-        <f t="shared" ref="F30" si="40">_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
-        <v>0x8B00</v>
+        <f t="shared" ref="F30" si="41">_xlfn.CONCAT("0x",DEC2HEX(I30))</f>
+        <v>0x8580</v>
       </c>
       <c r="G30" s="27">
         <f>HEX2DEC(MID(D30, 3, LEN(D30)-2))</f>
-        <v>35378</v>
+        <v>34098</v>
       </c>
       <c r="H30" s="27">
-        <f t="shared" ref="H30" si="41">HEX2DEC(MID(E30, 3, LEN(E30)-2))</f>
-        <v>206</v>
+        <f t="shared" ref="H30" si="42">HEX2DEC(MID(E30, 3, LEN(E30)-2))</f>
+        <v>78</v>
       </c>
       <c r="I30" s="27">
-        <f t="shared" ref="I30" si="42">G30+H30</f>
-        <v>35584</v>
+        <f t="shared" ref="I30" si="43">G30+H30</f>
+        <v>34176</v>
       </c>
       <c r="J30" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L30" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="M30" s="18">
-        <f>M29/8</f>
-        <v>256</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B31" s="24"/>
       <c r="C31" s="47" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D31" s="23" t="str">
         <f>F30</f>
-        <v>0x8B00</v>
+        <v>0x8580</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="F31" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I31))</f>
-        <v>0x8B10</v>
+        <v>0x8590</v>
       </c>
       <c r="G31" s="23">
-        <f t="shared" ref="G31" si="43">HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
-        <v>35584</v>
+        <f t="shared" ref="G31" si="44">HEX2DEC(MID(D31, 3, LEN(D31)-2))</f>
+        <v>34176</v>
       </c>
       <c r="H31" s="23">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>16</v>
       </c>
       <c r="I31" s="23">
         <f>G31+H31</f>
-        <v>35600</v>
+        <v>34192</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>168</v>
-      </c>
-      <c r="L31" s="29" t="s">
-        <v>144</v>
-      </c>
-      <c r="M31" s="29">
-        <f>M25*M30</f>
-        <v>16384</v>
+        <v>160</v>
+      </c>
+      <c r="L31" s="20" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B32" s="24"/>
       <c r="C32" s="46"/>
       <c r="D32" s="23" t="str">
-        <f t="shared" si="32"/>
-        <v>0x8B10</v>
+        <f t="shared" si="33"/>
+        <v>0x8590</v>
       </c>
       <c r="E32" s="23" t="s">
-        <v>85</v>
+        <v>212</v>
       </c>
       <c r="F32" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I32))</f>
-        <v>0x8B20</v>
+        <v>0x8594</v>
       </c>
       <c r="G32" s="23">
-        <f t="shared" ref="G32" si="44">HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
-        <v>35600</v>
+        <f t="shared" ref="G32" si="45">HEX2DEC(MID(D32, 3, LEN(D32)-2))</f>
+        <v>34192</v>
       </c>
       <c r="H32" s="23">
-        <f t="shared" ref="H32" si="45">HEX2DEC(MID(E32, 3, LEN(E32)-2))</f>
-        <v>16</v>
+        <f t="shared" ref="H32" si="46">HEX2DEC(MID(E32, 3, LEN(E32)-2))</f>
+        <v>4</v>
       </c>
       <c r="I32" s="23">
         <f>G32+H32</f>
-        <v>35616</v>
+        <v>34196</v>
       </c>
       <c r="J32" s="23" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="33" spans="2:13" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="L32" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="M32" s="28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="24"/>
       <c r="C33" s="27"/>
       <c r="D33" s="27" t="str">
         <f>F32</f>
-        <v>0x8B20</v>
+        <v>0x8594</v>
       </c>
       <c r="E33" s="27" t="s">
-        <v>183</v>
+        <v>213</v>
       </c>
       <c r="F33" s="27" t="str">
-        <f t="shared" ref="F33" si="46">_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
-        <v>0x8C00</v>
+        <f t="shared" ref="F33" si="47">_xlfn.CONCAT("0x",DEC2HEX(I33))</f>
+        <v>0x8600</v>
       </c>
       <c r="G33" s="27">
-        <f t="shared" ref="G33:G35" si="47">HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
-        <v>35616</v>
+        <f t="shared" ref="G33:G35" si="48">HEX2DEC(MID(D33, 3, LEN(D33)-2))</f>
+        <v>34196</v>
       </c>
       <c r="H33" s="27">
-        <f t="shared" ref="H33:H36" si="48">HEX2DEC(MID(E33, 3, LEN(E33)-2))</f>
-        <v>224</v>
+        <f t="shared" ref="H33:H36" si="49">HEX2DEC(MID(E33, 3, LEN(E33)-2))</f>
+        <v>108</v>
       </c>
       <c r="I33" s="27">
-        <f t="shared" ref="I33" si="49">G33+H33</f>
-        <v>35840</v>
+        <f t="shared" ref="I33" si="50">G33+H33</f>
+        <v>34304</v>
       </c>
       <c r="J33" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L33" s="20" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="L33" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="M33" s="18">
+        <v>16</v>
+      </c>
+      <c r="N33" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B34" s="24"/>
       <c r="C34" s="44" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="D34" s="23" t="str">
         <f>F33</f>
-        <v>0x8C00</v>
+        <v>0x8600</v>
       </c>
       <c r="E34" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M73))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M88))</f>
         <v>0x10</v>
       </c>
       <c r="F34" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I34))</f>
-        <v>0x8C10</v>
+        <v>0x8610</v>
       </c>
       <c r="G34" s="23">
-        <f t="shared" ref="G34" si="50">HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
-        <v>35840</v>
+        <f t="shared" ref="G34" si="51">HEX2DEC(MID(D34, 3, LEN(D34)-2))</f>
+        <v>34304</v>
       </c>
       <c r="H34" s="23">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>16</v>
       </c>
       <c r="I34" s="23">
         <f>G34+H34</f>
-        <v>35856</v>
+        <v>34320</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>186</v>
-      </c>
-      <c r="L34" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="M34" s="28">
+        <v>177</v>
+      </c>
+      <c r="L34" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="M34" s="18">
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B35" s="24"/>
       <c r="C35" s="45"/>
       <c r="D35" s="23" t="str">
         <f>F34</f>
-        <v>0x8C10</v>
+        <v>0x8610</v>
       </c>
       <c r="E35" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M80))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M95))</f>
         <v>0x300</v>
       </c>
       <c r="F35" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I35))</f>
-        <v>0x8F10</v>
+        <v>0x8910</v>
       </c>
       <c r="G35" s="23">
-        <f t="shared" si="47"/>
-        <v>35856</v>
+        <f t="shared" si="48"/>
+        <v>34320</v>
       </c>
       <c r="H35" s="23">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>768</v>
       </c>
       <c r="I35" s="23">
         <f>G35+H35</f>
-        <v>36624</v>
+        <v>35088</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="L35" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="M35" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+      <c r="L35" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="M35" s="29">
+        <f>M33*M34</f>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B36" s="24"/>
       <c r="C36" s="27"/>
       <c r="D36" s="27" t="str">
         <f>F35</f>
-        <v>0x8F10</v>
+        <v>0x8910</v>
       </c>
       <c r="E36" s="27" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="F36" s="27" t="str">
-        <f t="shared" ref="F36" si="51">_xlfn.CONCAT("0x",DEC2HEX(I36))</f>
-        <v>0x9000</v>
+        <f t="shared" ref="F36" si="52">_xlfn.CONCAT("0x",DEC2HEX(I36))</f>
+        <v>0x8A00</v>
       </c>
       <c r="G36" s="27">
-        <f t="shared" ref="G36" si="52">HEX2DEC(MID(D36, 3, LEN(D36)-2))</f>
-        <v>36624</v>
+        <f t="shared" ref="G36" si="53">HEX2DEC(MID(D36, 3, LEN(D36)-2))</f>
+        <v>35088</v>
       </c>
       <c r="H36" s="27">
-        <f t="shared" si="48"/>
+        <f t="shared" si="49"/>
         <v>240</v>
       </c>
       <c r="I36" s="27">
-        <f t="shared" ref="I36" si="53">G36+H36</f>
-        <v>36864</v>
+        <f t="shared" ref="I36" si="54">G36+H36</f>
+        <v>35328</v>
       </c>
       <c r="J36" s="27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L36" s="18" t="s">
-        <v>161</v>
+        <v>56</v>
       </c>
       <c r="M36" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.2">
+        <f>M35/8</f>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B37" s="24"/>
       <c r="C37" s="30" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="D37" s="23" t="str">
         <f>F36</f>
-        <v>0x9000</v>
+        <v>0x8A00</v>
       </c>
       <c r="E37" s="23" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I37))</f>
-        <v>0x9800</v>
+        <v>0x9200</v>
       </c>
       <c r="G37" s="23">
         <f>HEX2DEC(MID(D37, 3, LEN(D37)-2))</f>
-        <v>36864</v>
+        <v>35328</v>
       </c>
       <c r="H37" s="23">
-        <f t="shared" si="28"/>
+        <f t="shared" si="32"/>
         <v>2048</v>
       </c>
       <c r="I37" s="23">
         <f>G37+H37</f>
-        <v>38912</v>
+        <v>37376</v>
       </c>
       <c r="J37" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="L37" s="18" t="s">
-        <v>164</v>
-      </c>
-      <c r="M37" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L37" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="M37" s="29">
+        <f>M36*M32</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B38" s="24"/>
       <c r="C38" s="31"/>
       <c r="D38" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0x9800</v>
+        <v>0x9200</v>
       </c>
       <c r="E38" s="23" t="s">
         <v>8</v>
       </c>
       <c r="F38" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I38))</f>
-        <v>0xA000</v>
+        <v>0x9A00</v>
       </c>
       <c r="G38" s="23">
         <f>HEX2DEC(MID(D38, 3, LEN(D38)-2))</f>
-        <v>38912</v>
+        <v>37376</v>
       </c>
       <c r="H38" s="23">
         <f>HEX2DEC(MID(E38, 3, LEN(E38)-2))</f>
@@ -2771,777 +2729,912 @@
       </c>
       <c r="I38" s="23">
         <f>G38+H38</f>
-        <v>40960</v>
+        <v>39424</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="L38" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="M38" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" s="24"/>
       <c r="C39" s="31"/>
       <c r="D39" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0xA000</v>
+        <v>0x9A00</v>
       </c>
       <c r="E39" s="23" t="s">
         <v>8</v>
       </c>
       <c r="F39" s="23" t="str">
-        <f t="shared" ref="F39" si="54">_xlfn.CONCAT("0x",DEC2HEX(I39))</f>
-        <v>0xA800</v>
+        <f t="shared" ref="F39" si="55">_xlfn.CONCAT("0x",DEC2HEX(I39))</f>
+        <v>0xA200</v>
       </c>
       <c r="G39" s="23">
-        <f t="shared" ref="G39" si="55">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
-        <v>40960</v>
+        <f t="shared" ref="G39" si="56">HEX2DEC(MID(D39, 3, LEN(D39)-2))</f>
+        <v>39424</v>
       </c>
       <c r="H39" s="23">
-        <f t="shared" ref="H39" si="56">HEX2DEC(MID(E39, 3, LEN(E39)-2))</f>
+        <f t="shared" ref="H39" si="57">HEX2DEC(MID(E39, 3, LEN(E39)-2))</f>
         <v>2048</v>
       </c>
       <c r="I39" s="23">
-        <f t="shared" ref="I39" si="57">G39+H39</f>
-        <v>43008</v>
+        <f t="shared" ref="I39" si="58">G39+H39</f>
+        <v>41472</v>
       </c>
       <c r="J39" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="L39" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="M39" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+      <c r="L39" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="N39" s="18" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B40" s="24"/>
       <c r="C40" s="32"/>
       <c r="D40" s="23" t="str">
         <f t="shared" si="1"/>
-        <v>0xA800</v>
+        <v>0xA200</v>
       </c>
       <c r="E40" s="23" t="s">
         <v>8</v>
       </c>
       <c r="F40" s="23" t="str">
-        <f t="shared" ref="F40" si="58">_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
+        <f t="shared" ref="F40:F41" si="59">_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
+        <v>0xAA00</v>
+      </c>
+      <c r="G40" s="23">
+        <f t="shared" ref="G40:G41" si="60">HEX2DEC(MID(D40, 3, LEN(D40)-2))</f>
+        <v>41472</v>
+      </c>
+      <c r="H40" s="23">
+        <f t="shared" ref="H40:H41" si="61">HEX2DEC(MID(E40, 3, LEN(E40)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I40" s="23">
+        <f t="shared" ref="I40:I41" si="62">G40+H40</f>
+        <v>43520</v>
+      </c>
+      <c r="J40" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="L40" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="M40" s="28">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B41" s="24"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="27" t="str">
+        <f>F40</f>
+        <v>0xAA00</v>
+      </c>
+      <c r="E41" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="F41" s="27" t="str">
+        <f t="shared" si="59"/>
         <v>0xB000</v>
       </c>
-      <c r="G40" s="23">
-        <f t="shared" ref="G40" si="59">HEX2DEC(MID(D40, 3, LEN(D40)-2))</f>
-        <v>43008</v>
-      </c>
-      <c r="H40" s="23">
-        <f t="shared" ref="H40" si="60">HEX2DEC(MID(E40, 3, LEN(E40)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I40" s="23">
-        <f t="shared" ref="I40" si="61">G40+H40</f>
+      <c r="G41" s="27">
+        <f t="shared" si="60"/>
+        <v>43520</v>
+      </c>
+      <c r="H41" s="27">
+        <f t="shared" si="61"/>
+        <v>1536</v>
+      </c>
+      <c r="I41" s="27">
+        <f t="shared" si="62"/>
         <v>45056</v>
       </c>
-      <c r="J40" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="L40" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="M40" s="18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B41" s="24"/>
-      <c r="C41" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D41" s="23" t="str">
-        <f t="shared" si="1"/>
+      <c r="J41" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="L41" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="M41" s="18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B42" s="24"/>
+      <c r="C42" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="23" t="str">
+        <f>F41</f>
         <v>0xB000</v>
       </c>
-      <c r="E41" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M45))</f>
+      <c r="E42" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M60))</f>
         <v>0x80</v>
       </c>
-      <c r="F41" s="23" t="str">
-        <f t="shared" ref="F41:F42" si="62">_xlfn.CONCAT("0x",DEC2HEX(I41))</f>
+      <c r="F42" s="23" t="str">
+        <f t="shared" ref="F42:F43" si="63">_xlfn.CONCAT("0x",DEC2HEX(I42))</f>
         <v>0xB080</v>
       </c>
-      <c r="G41" s="23">
-        <f t="shared" ref="G41:G42" si="63">HEX2DEC(MID(D41, 3, LEN(D41)-2))</f>
+      <c r="G42" s="23">
+        <f t="shared" ref="G42:G43" si="64">HEX2DEC(MID(D42, 3, LEN(D42)-2))</f>
         <v>45056</v>
       </c>
-      <c r="H41" s="23">
-        <f t="shared" ref="H41:H42" si="64">HEX2DEC(MID(E41, 3, LEN(E41)-2))</f>
+      <c r="H42" s="23">
+        <f t="shared" ref="H42:H43" si="65">HEX2DEC(MID(E42, 3, LEN(E42)-2))</f>
         <v>128</v>
       </c>
-      <c r="I41" s="23">
-        <f t="shared" ref="I41:I42" si="65">G41+H41</f>
+      <c r="I42" s="23">
+        <f t="shared" ref="I42:I43" si="66">G42+H42</f>
         <v>45184</v>
       </c>
-      <c r="J41" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="L41" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="M41" s="18">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B42" s="24"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="27" t="str">
+      <c r="J42" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="L42" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="M42" s="18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B43" s="24"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="27" t="str">
         <f t="shared" si="1"/>
         <v>0xB080</v>
       </c>
-      <c r="E42" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="F42" s="27" t="str">
-        <f t="shared" si="62"/>
+      <c r="E43" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="F43" s="27" t="str">
+        <f t="shared" si="63"/>
         <v>0xB400</v>
       </c>
-      <c r="G42" s="27">
-        <f t="shared" si="63"/>
+      <c r="G43" s="27">
+        <f t="shared" si="64"/>
         <v>45184</v>
       </c>
-      <c r="H42" s="27">
-        <f t="shared" si="64"/>
+      <c r="H43" s="27">
+        <f t="shared" si="65"/>
         <v>896</v>
       </c>
-      <c r="I42" s="27">
-        <f t="shared" si="65"/>
+      <c r="I43" s="27">
+        <f t="shared" si="66"/>
         <v>46080</v>
       </c>
-      <c r="J42" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L42" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="M42" s="18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B43" s="24"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="23" t="str">
-        <f t="shared" ref="D43:D44" si="66">F42</f>
+      <c r="J43" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="L43" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="M43" s="18">
+        <v>8</v>
+      </c>
+      <c r="N43" s="18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B44" s="24"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="23" t="str">
+        <f t="shared" ref="D44:D45" si="67">F43</f>
         <v>0xB400</v>
       </c>
-      <c r="E43" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M58))</f>
+      <c r="E44" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M73))</f>
         <v>0x4</v>
       </c>
-      <c r="F43" s="23" t="str">
-        <f t="shared" ref="F43:F44" si="67">_xlfn.CONCAT("0x",DEC2HEX(I43))</f>
+      <c r="F44" s="23" t="str">
+        <f t="shared" ref="F44:F45" si="68">_xlfn.CONCAT("0x",DEC2HEX(I44))</f>
         <v>0xB404</v>
       </c>
-      <c r="G43" s="23">
-        <f t="shared" ref="G43:G44" si="68">HEX2DEC(MID(D43, 3, LEN(D43)-2))</f>
+      <c r="G44" s="23">
+        <f t="shared" ref="G44:G45" si="69">HEX2DEC(MID(D44, 3, LEN(D44)-2))</f>
         <v>46080</v>
       </c>
-      <c r="H43" s="23">
-        <f t="shared" ref="H43:H44" si="69">HEX2DEC(MID(E43, 3, LEN(E43)-2))</f>
+      <c r="H44" s="23">
+        <f t="shared" ref="H44:H45" si="70">HEX2DEC(MID(E44, 3, LEN(E44)-2))</f>
         <v>4</v>
       </c>
-      <c r="I43" s="23">
-        <f t="shared" ref="I43:I44" si="70">G43+H43</f>
+      <c r="I44" s="23">
+        <f t="shared" ref="I44:I45" si="71">G44+H44</f>
         <v>46084</v>
       </c>
-      <c r="J43" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="L43" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="M43" s="29">
-        <f>SUM(M35:M42)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B44" s="36"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="27" t="str">
-        <f t="shared" si="66"/>
+      <c r="J44" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="L44" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="M44" s="29">
+        <f>M41*M42*M43</f>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B45" s="36"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="27" t="str">
+        <f t="shared" si="67"/>
         <v>0xB404</v>
       </c>
-      <c r="E44" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="F44" s="27" t="str">
-        <f t="shared" si="67"/>
+      <c r="E45" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="F45" s="27" t="str">
+        <f t="shared" si="68"/>
         <v>0xB800</v>
       </c>
-      <c r="G44" s="27">
-        <f t="shared" si="68"/>
+      <c r="G45" s="27">
+        <f t="shared" si="69"/>
         <v>46084</v>
       </c>
-      <c r="H44" s="27">
-        <f t="shared" si="69"/>
+      <c r="H45" s="27">
+        <f t="shared" si="70"/>
         <v>1020</v>
       </c>
-      <c r="I44" s="27">
-        <f t="shared" si="70"/>
+      <c r="I45" s="27">
+        <f t="shared" si="71"/>
         <v>47104</v>
       </c>
-      <c r="J44" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="L44" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="M44" s="18">
-        <f>M43/8</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B45" s="38" t="s">
-        <v>142</v>
-      </c>
-      <c r="C45" s="35"/>
-      <c r="D45" s="23" t="str">
-        <f>F44</f>
-        <v>0xB800</v>
-      </c>
-      <c r="E45" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M52))</f>
-        <v>0x800</v>
-      </c>
-      <c r="F45" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I45))</f>
-        <v>0xC000</v>
-      </c>
-      <c r="G45" s="23">
-        <f t="shared" ref="G45:H47" si="71">HEX2DEC(MID(D45, 3, LEN(D45)-2))</f>
-        <v>47104</v>
-      </c>
-      <c r="H45" s="23">
-        <f t="shared" si="71"/>
-        <v>2048</v>
-      </c>
-      <c r="I45" s="23">
-        <f>G45+H45</f>
-        <v>49152</v>
-      </c>
-      <c r="J45" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="L45" s="29" t="s">
-        <v>137</v>
-      </c>
-      <c r="M45" s="29">
-        <f>M34*M44</f>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B46" s="39" t="s">
-        <v>141</v>
-      </c>
-      <c r="C46" s="37" t="s">
-        <v>47</v>
-      </c>
+      <c r="J45" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="L45" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="M45" s="18">
+        <f>M44/8</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B46" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="C46" s="35"/>
       <c r="D46" s="23" t="str">
         <f>F45</f>
-        <v>0xC000</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>6</v>
+        <v>0xB800</v>
+      </c>
+      <c r="E46" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M67))</f>
+        <v>0x800</v>
       </c>
       <c r="F46" s="23" t="str">
         <f>_xlfn.CONCAT("0x",DEC2HEX(I46))</f>
-        <v>0x10000</v>
+        <v>0xC000</v>
       </c>
       <c r="G46" s="23">
-        <f t="shared" si="71"/>
-        <v>49152</v>
+        <f t="shared" ref="G46:H48" si="72">HEX2DEC(MID(D46, 3, LEN(D46)-2))</f>
+        <v>47104</v>
       </c>
       <c r="H46" s="23">
-        <f t="shared" si="71"/>
-        <v>16384</v>
+        <f t="shared" si="72"/>
+        <v>2048</v>
       </c>
       <c r="I46" s="23">
         <f>G46+H46</f>
+        <v>49152</v>
+      </c>
+      <c r="J46" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="L46" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="M46" s="29">
+        <f>M40*M45</f>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B47" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="C47" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D47" s="23" t="str">
+        <f>F46</f>
+        <v>0xC000</v>
+      </c>
+      <c r="E47" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F47" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I47))</f>
+        <v>0x10000</v>
+      </c>
+      <c r="G47" s="23">
+        <f t="shared" si="72"/>
+        <v>49152</v>
+      </c>
+      <c r="H47" s="23">
+        <f t="shared" si="72"/>
+        <v>16384</v>
+      </c>
+      <c r="I47" s="23">
+        <f>G47+H47</f>
         <v>65536</v>
       </c>
-      <c r="J46" s="23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B47" s="39"/>
-      <c r="C47" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="D47" s="23" t="str">
+      <c r="J47" s="23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B48" s="39"/>
+      <c r="C48" s="40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" s="23" t="str">
         <f t="shared" si="1"/>
         <v>0x10000</v>
       </c>
-      <c r="E47" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M22))</f>
+      <c r="E48" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M37))</f>
         <v>0x100</v>
       </c>
-      <c r="F47" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I47))</f>
+      <c r="F48" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I48))</f>
         <v>0x10100</v>
       </c>
-      <c r="G47" s="23">
-        <f t="shared" si="71"/>
+      <c r="G48" s="23">
+        <f t="shared" si="72"/>
         <v>65536</v>
       </c>
-      <c r="H47" s="23">
-        <f t="shared" si="71"/>
+      <c r="H48" s="23">
+        <f t="shared" si="72"/>
         <v>256</v>
       </c>
-      <c r="I47" s="23">
-        <f>G47+H47</f>
+      <c r="I48" s="23">
+        <f>G48+H48</f>
         <v>65792</v>
       </c>
-      <c r="J47" s="23" t="s">
+      <c r="J48" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="L48" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="L47" s="20" t="s">
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B49" s="39"/>
+      <c r="L49" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="M49" s="28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="B50" s="39"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="L50" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="M47" s="18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B48" s="39"/>
-      <c r="L48" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="M48" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="49" spans="2:16" ht="15" x14ac:dyDescent="0.25">
-      <c r="B49" s="39"/>
-      <c r="C49"/>
-      <c r="D49"/>
-      <c r="E49"/>
-      <c r="F49"/>
-      <c r="G49"/>
-      <c r="H49"/>
-      <c r="I49"/>
-      <c r="J49"/>
-      <c r="L49" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="M49" s="18">
-        <v>512</v>
-      </c>
-    </row>
-    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B50" s="39"/>
-      <c r="C50" s="33" t="s">
-        <v>54</v>
-      </c>
-      <c r="D50" s="23"/>
-      <c r="E50" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M31))</f>
-        <v>0x4000</v>
-      </c>
-      <c r="F50" s="23"/>
-      <c r="G50" s="23"/>
-      <c r="H50" s="23">
-        <f>HEX2DEC(MID(E50, 3, LEN(E50)-2))</f>
-        <v>16384</v>
-      </c>
-      <c r="I50" s="23"/>
-      <c r="J50" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="L50" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="M50" s="28">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="51" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="M50" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B51" s="39"/>
-      <c r="C51" s="35"/>
+      <c r="C51" s="33" t="s">
+        <v>48</v>
+      </c>
       <c r="D51" s="23"/>
       <c r="E51" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M64))</f>
-        <v>0x800</v>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M46))</f>
+        <v>0x4000</v>
       </c>
       <c r="F51" s="23"/>
       <c r="G51" s="23"/>
       <c r="H51" s="23">
         <f>HEX2DEC(MID(E51, 3, LEN(E51)-2))</f>
+        <v>16384</v>
+      </c>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="L51" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="M51" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B52" s="39"/>
+      <c r="C52" s="35"/>
+      <c r="D52" s="23"/>
+      <c r="E52" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M79))</f>
+        <v>0x800</v>
+      </c>
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="23">
+        <f>HEX2DEC(MID(E52, 3, LEN(E52)-2))</f>
         <v>2048</v>
       </c>
-      <c r="I51" s="23" t="s">
+      <c r="I52" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="J52" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="L52" s="18" t="s">
         <v>156</v>
       </c>
-      <c r="J51" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="L51" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="M51" s="18">
-        <f>M48*M49*M50</f>
-        <v>16384</v>
-      </c>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B52" s="39"/>
-      <c r="L52" s="18" t="s">
-        <v>145</v>
-      </c>
       <c r="M52" s="18">
-        <f>M51/8</f>
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B53" s="39"/>
-    </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="L53" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="M53" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B54" s="39"/>
-      <c r="C54" s="40" t="s">
-        <v>153</v>
-      </c>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="F54" s="23"/>
-      <c r="G54" s="23"/>
-      <c r="H54" s="23">
-        <f t="shared" ref="H54" si="72">HEX2DEC(MID(E54, 3, LEN(E54)-2))</f>
-        <v>131072</v>
-      </c>
-      <c r="I54" s="23"/>
-      <c r="J54" s="23" t="s">
-        <v>153</v>
-      </c>
-      <c r="L54" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="M54" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="P54" s="18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="L54" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="M54" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B55" s="39"/>
       <c r="C55" s="40" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="D55" s="23"/>
       <c r="E55" s="23" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="F55" s="23"/>
       <c r="G55" s="23"/>
       <c r="H55" s="23">
         <f t="shared" ref="H55" si="73">HEX2DEC(MID(E55, 3, LEN(E55)-2))</f>
-        <v>65536</v>
+        <v>131072</v>
       </c>
       <c r="I55" s="23"/>
       <c r="J55" s="23" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="L55" s="18" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="M55" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B56" s="39"/>
+      <c r="C56" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="F56" s="23"/>
+      <c r="G56" s="23"/>
+      <c r="H56" s="23">
+        <f t="shared" ref="H56" si="74">HEX2DEC(MID(E56, 3, LEN(E56)-2))</f>
+        <v>65536</v>
+      </c>
+      <c r="I56" s="23"/>
+      <c r="J56" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="L56" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="M56" s="18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B57" s="39"/>
+      <c r="L57" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="M57" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B58" s="39"/>
+      <c r="L58" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="M58" s="29">
+        <f>SUM(M50:M57)</f>
         <v>32</v>
       </c>
-      <c r="O55" s="18">
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B59" s="39"/>
+      <c r="L59" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M59" s="18">
+        <f>M58/8</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B60" s="39"/>
+      <c r="L60" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="M60" s="29">
+        <f>M49*M59</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="61" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B61" s="39"/>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B62" s="39"/>
+      <c r="L62" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="M62" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B63" s="39"/>
+      <c r="L63" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="M63" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B64" s="39"/>
+      <c r="L64" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M64" s="18">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B65" s="39"/>
+      <c r="L65" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="M65" s="28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="66" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B66" s="39"/>
+      <c r="L66" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="M66" s="18">
+        <f>M63*M64*M65</f>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="67" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B67" s="39"/>
+      <c r="L67" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="M67" s="18">
+        <f>M66/8</f>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B68" s="39"/>
+    </row>
+    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B69" s="41"/>
+      <c r="L69" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="M69" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="P69" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="L70" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="M70" s="18">
+        <v>32</v>
+      </c>
+      <c r="O70" s="18">
         <f>384*2</f>
         <v>768</v>
       </c>
     </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B56" s="39"/>
-      <c r="L56" s="28" t="s">
+    <row r="71" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="L71" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="M56" s="28">
+      <c r="M71" s="28">
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B57" s="39"/>
-      <c r="L57" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="M57" s="18">
-        <f>M55*M56</f>
+    <row r="72" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="L72" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="M72" s="18">
+        <f>M70*M71</f>
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B58" s="39"/>
-      <c r="L58" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="M58" s="18">
-        <f>M57/8</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B59" s="39"/>
-    </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B60" s="39"/>
-      <c r="L60" s="20" t="s">
-        <v>132</v>
-      </c>
-      <c r="M60" s="18" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B61" s="39"/>
-      <c r="L61" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="M61" s="18">
-        <v>512</v>
-      </c>
-      <c r="N61" s="18" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="62" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B62" s="39"/>
-      <c r="L62" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="M62" s="28">
-        <v>32</v>
-      </c>
-      <c r="N62" s="18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B63" s="39"/>
-      <c r="L63" s="29" t="s">
-        <v>140</v>
-      </c>
-      <c r="M63" s="18">
-        <f>M61*M62</f>
-        <v>16384</v>
-      </c>
-    </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B64" s="39"/>
-      <c r="L64" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="M64" s="18">
-        <f>M63/8</f>
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="65" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B65" s="39"/>
-    </row>
-    <row r="66" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B66" s="39"/>
-      <c r="L66" s="20" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="67" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B67" s="39"/>
-      <c r="L67" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="M67" s="18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B68" s="41"/>
-      <c r="L68" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="M68" s="18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="69" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L69" s="18" t="s">
-        <v>189</v>
-      </c>
-      <c r="M69" s="18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="70" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L70" s="18" t="s">
-        <v>190</v>
-      </c>
-      <c r="M70" s="18">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L71" s="43" t="s">
-        <v>162</v>
-      </c>
-      <c r="M71" s="43">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="72" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L72" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="M72" s="29">
-        <f>SUM(M67:M71)</f>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="73" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.2">
       <c r="L73" s="18" t="s">
-        <v>192</v>
+        <v>129</v>
       </c>
       <c r="M73" s="18">
         <f>M72/8</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="2:16" x14ac:dyDescent="0.2">
       <c r="L75" s="20" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="76" spans="2:14" x14ac:dyDescent="0.2">
+        <v>124</v>
+      </c>
+      <c r="M75" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="76" spans="2:16" x14ac:dyDescent="0.2">
       <c r="L76" s="18" t="s">
-        <v>194</v>
+        <v>125</v>
       </c>
       <c r="M76" s="18">
+        <v>512</v>
+      </c>
+      <c r="N76" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="77" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="L77" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="M77" s="28">
         <v>32</v>
       </c>
-      <c r="N76" s="18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="77" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L77" s="18" t="s">
-        <v>195</v>
-      </c>
-      <c r="M77" s="18">
-        <v>24</v>
-      </c>
       <c r="N77" s="18" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="78" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L78" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="78" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="L78" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="M78" s="18">
+        <f>M76*M77</f>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="79" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="L79" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="M79" s="18">
+        <f>M78/8</f>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="81" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L81" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="M78" s="18">
+    </row>
+    <row r="82" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L82" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="M82" s="18">
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L79" s="29" t="s">
-        <v>196</v>
-      </c>
-      <c r="M79" s="29">
-        <f>M76*M77*M78</f>
-        <v>6144</v>
-      </c>
-    </row>
-    <row r="80" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="L80" s="18" t="s">
-        <v>197</v>
-      </c>
-      <c r="M80" s="18">
-        <f>M79/8</f>
-        <v>768</v>
-      </c>
-    </row>
-    <row r="82" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L82" s="20" t="s">
-        <v>199</v>
-      </c>
-    </row>
     <row r="83" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L83" s="28" t="s">
-        <v>200</v>
-      </c>
-      <c r="M83" s="28">
-        <v>64</v>
+      <c r="L83" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="M83" s="18">
+        <v>8</v>
       </c>
     </row>
     <row r="84" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L84" s="18" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="M84" s="18">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L85" s="18" t="s">
-        <v>202</v>
+        <v>181</v>
       </c>
       <c r="M85" s="18">
-        <v>16</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L86" s="18" t="s">
-        <v>203</v>
-      </c>
-      <c r="M86" s="18">
-        <v>16</v>
-      </c>
-      <c r="N86" s="18" t="s">
-        <v>80</v>
+      <c r="L86" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="M86" s="43">
+        <v>96</v>
       </c>
     </row>
     <row r="87" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L87" s="29" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="M87" s="29">
-        <f>M84*M85*M86</f>
-        <v>4096</v>
+        <f>SUM(M82:M86)</f>
+        <v>128</v>
       </c>
     </row>
     <row r="88" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L88" s="18" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="M88" s="18">
         <f>M87/8</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L90" s="20" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="91" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L91" s="18" t="s">
+        <v>185</v>
+      </c>
+      <c r="M91" s="18">
+        <v>32</v>
+      </c>
+      <c r="N91" s="18" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="92" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L92" s="18" t="s">
+        <v>186</v>
+      </c>
+      <c r="M92" s="18">
+        <v>24</v>
+      </c>
+      <c r="N92" s="18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="93" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L93" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="M93" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L94" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="M94" s="29">
+        <f>M91*M92*M93</f>
+        <v>6144</v>
+      </c>
+    </row>
+    <row r="95" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L95" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="M95" s="18">
+        <f>M94/8</f>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="97" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L97" s="20" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="98" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L98" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="M98" s="28">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="99" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L99" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="M99" s="18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="100" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L100" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="M100" s="18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="101" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L101" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="M101" s="18">
+        <v>16</v>
+      </c>
+      <c r="N101" s="18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="102" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L102" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="M102" s="29">
+        <f>M99*M100*M101</f>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="103" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L103" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="M103" s="18">
+        <f>M102/8</f>
         <v>512</v>
       </c>
     </row>
-    <row r="89" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L89" s="29" t="s">
-        <v>206</v>
-      </c>
-      <c r="M89" s="29">
-        <f>M83*M88</f>
+    <row r="104" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L104" s="29" t="s">
+        <v>197</v>
+      </c>
+      <c r="M104" s="29">
+        <f>M98*M103</f>
         <v>32768</v>
       </c>
     </row>
@@ -3576,10 +3669,10 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="8" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">
@@ -3588,189 +3681,189 @@
     </row>
     <row r="3" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="G6" s="16" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F7" s="10"/>
       <c r="G7" s="3"/>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="180" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="I21" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I22" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I23" s="42" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="I24" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -3795,13 +3888,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="B1" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C1" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3846,10 +3939,10 @@
         <v>272</v>
       </c>
       <c r="D1" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="E1" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -3872,18 +3965,18 @@
         <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="L2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M3" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="N3" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add 24-bit palettes for char map
</commit_message>
<xml_diff>
--- a/docs/Hardware.xlsx
+++ b/docs/Hardware.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\Aznable\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC9DA5C-766D-44F5-805C-73D40426A77C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FBFE3B-C280-4EE8-81E3-50FAD27BE6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{8387191E-7D8B-4623-897E-A5E3E75A545C}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="225">
   <si>
     <t>HEIGHT</t>
   </si>
@@ -744,7 +744,37 @@
     <t>0x006C</t>
   </si>
   <si>
-    <t>0x0600</t>
+    <t>Char Palette RAM</t>
+  </si>
+  <si>
+    <t>CHAR_PALETTE_RAM_COUNT</t>
+  </si>
+  <si>
+    <t>CHAR_PALETTE_RAM_COLOUR_DEPTH</t>
+  </si>
+  <si>
+    <t>CHAR_PALETTE_RAM_BITS_PER</t>
+  </si>
+  <si>
+    <t>CHAR_PALETTE_RAM_BYTES_PER</t>
+  </si>
+  <si>
+    <t>CHAR_PALETTE_RAM_BYTES_TOTAL</t>
+  </si>
+  <si>
+    <t>0x100</t>
+  </si>
+  <si>
+    <t>0x0300</t>
+  </si>
+  <si>
+    <t>Char Palette RAM R</t>
+  </si>
+  <si>
+    <t>Char Palette RAM G</t>
+  </si>
+  <si>
+    <t>Char Palette RAM B</t>
   </si>
 </sst>
 </file>
@@ -1412,10 +1442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C319FCBA-55CF-4FE5-A99F-6174DD3BEDA9}">
-  <dimension ref="B1:P104"/>
+  <dimension ref="B1:P96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B14" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L25" sqref="L25"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J44" sqref="J44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1525,7 +1555,7 @@
         <v>36</v>
       </c>
       <c r="D4" s="23" t="str">
-        <f t="shared" ref="D4:D48" si="2">F3</f>
+        <f t="shared" ref="D4:D51" si="2">F3</f>
         <v>0x8000</v>
       </c>
       <c r="E4" s="23" t="s">
@@ -1986,6 +2016,9 @@
       <c r="J16" s="27" t="s">
         <v>27</v>
       </c>
+      <c r="L16" s="20" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" s="24"/>
@@ -2016,6 +2049,12 @@
       <c r="J17" s="23" t="s">
         <v>22</v>
       </c>
+      <c r="L17" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="M17" s="28">
+        <v>256</v>
+      </c>
       <c r="N17" s="18">
         <f>256*3</f>
         <v>768</v>
@@ -2050,6 +2089,12 @@
       <c r="J18" s="27" t="s">
         <v>27</v>
       </c>
+      <c r="L18" s="18" t="s">
+        <v>216</v>
+      </c>
+      <c r="M18" s="18">
+        <v>32</v>
+      </c>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B19" s="24"/>
@@ -2080,6 +2125,13 @@
       <c r="J19" s="23" t="s">
         <v>21</v>
       </c>
+      <c r="L19" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="M19" s="29">
+        <f>M18</f>
+        <v>32</v>
+      </c>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B20" s="24"/>
@@ -2110,6 +2162,13 @@
       <c r="J20" s="27" t="s">
         <v>27</v>
       </c>
+      <c r="L20" s="18" t="s">
+        <v>218</v>
+      </c>
+      <c r="M20" s="18">
+        <f>M19/8</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B21" s="24"/>
@@ -2140,6 +2199,13 @@
       <c r="J21" s="23" t="s">
         <v>20</v>
       </c>
+      <c r="L21" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="M21" s="29">
+        <f>M17*M20</f>
+        <v>1024</v>
+      </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B22" s="24"/>
@@ -2200,6 +2266,9 @@
       <c r="J23" s="23" t="s">
         <v>19</v>
       </c>
+      <c r="L23" s="20" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B24" s="24"/>
@@ -2230,9 +2299,11 @@
       <c r="J24" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L24" s="18">
-        <f>64*30</f>
-        <v>1920</v>
+      <c r="L24" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="M24" s="28">
+        <v>4</v>
       </c>
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.2">
@@ -2264,6 +2335,15 @@
       <c r="J25" s="23" t="s">
         <v>80</v>
       </c>
+      <c r="L25" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="M25" s="18">
+        <v>16</v>
+      </c>
+      <c r="N25" s="18" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B26" s="24"/>
@@ -2294,6 +2374,12 @@
       <c r="J26" s="23" t="s">
         <v>78</v>
       </c>
+      <c r="L26" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="M26" s="18">
+        <v>32</v>
+      </c>
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B27" s="24"/>
@@ -2324,6 +2410,13 @@
       <c r="J27" s="23" t="s">
         <v>79</v>
       </c>
+      <c r="L27" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="M27" s="29">
+        <f>M25*M26</f>
+        <v>512</v>
+      </c>
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B28" s="24"/>
@@ -2354,6 +2447,13 @@
       <c r="J28" s="23" t="s">
         <v>157</v>
       </c>
+      <c r="L28" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="M28" s="18">
+        <f>M27/8</f>
+        <v>64</v>
+      </c>
     </row>
     <row r="29" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B29" s="24"/>
@@ -2384,6 +2484,13 @@
       <c r="J29" s="23" t="s">
         <v>203</v>
       </c>
+      <c r="L29" s="29" t="s">
+        <v>135</v>
+      </c>
+      <c r="M29" s="29">
+        <f>M28*M24</f>
+        <v>256</v>
+      </c>
     </row>
     <row r="30" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B30" s="24"/>
@@ -2447,7 +2554,10 @@
         <v>160</v>
       </c>
       <c r="L31" s="20" t="s">
-        <v>47</v>
+        <v>51</v>
+      </c>
+      <c r="N31" s="18" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="2:14" x14ac:dyDescent="0.2">
@@ -2480,10 +2590,10 @@
         <v>161</v>
       </c>
       <c r="L32" s="28" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="M32" s="28">
-        <v>4</v>
+        <v>64</v>
       </c>
     </row>
     <row r="33" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2516,13 +2626,10 @@
         <v>27</v>
       </c>
       <c r="L33" s="18" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="M33" s="18">
         <v>16</v>
-      </c>
-      <c r="N33" s="18" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="34" spans="2:14" x14ac:dyDescent="0.2">
@@ -2535,7 +2642,7 @@
         <v>0x8600</v>
       </c>
       <c r="E34" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M88))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M80))</f>
         <v>0x10</v>
       </c>
       <c r="F34" s="23" t="str">
@@ -2558,10 +2665,10 @@
         <v>177</v>
       </c>
       <c r="L34" s="18" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
       <c r="M34" s="18">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" spans="2:14" x14ac:dyDescent="0.2">
@@ -2572,7 +2679,7 @@
         <v>0x8610</v>
       </c>
       <c r="E35" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M95))</f>
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M87))</f>
         <v>0x300</v>
       </c>
       <c r="F35" s="23" t="str">
@@ -2594,12 +2701,14 @@
       <c r="J35" s="23" t="s">
         <v>182</v>
       </c>
-      <c r="L35" s="29" t="s">
-        <v>55</v>
-      </c>
-      <c r="M35" s="29">
-        <f>M33*M34</f>
-        <v>512</v>
+      <c r="L35" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="M35" s="18">
+        <v>8</v>
+      </c>
+      <c r="N35" s="18" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="36" spans="2:14" x14ac:dyDescent="0.2">
@@ -2631,12 +2740,12 @@
       <c r="J36" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L36" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="M36" s="18">
-        <f>M35/8</f>
-        <v>64</v>
+      <c r="L36" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="M36" s="29">
+        <f>M33*M34*M35</f>
+        <v>2048</v>
       </c>
     </row>
     <row r="37" spans="2:14" x14ac:dyDescent="0.2">
@@ -2670,11 +2779,11 @@
       <c r="J37" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="L37" s="29" t="s">
-        <v>135</v>
-      </c>
-      <c r="M37" s="29">
-        <f>M36*M32</f>
+      <c r="L37" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="M37" s="18">
+        <f>M36/8</f>
         <v>256</v>
       </c>
     </row>
@@ -2707,6 +2816,13 @@
       <c r="J38" s="23" t="s">
         <v>38</v>
       </c>
+      <c r="L38" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="M38" s="29">
+        <f>M32*M37</f>
+        <v>16384</v>
+      </c>
     </row>
     <row r="39" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B39" s="24"/>
@@ -2737,16 +2853,10 @@
       <c r="J39" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="L39" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="N39" s="18" t="s">
-        <v>144</v>
-      </c>
     </row>
     <row r="40" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B40" s="24"/>
-      <c r="C40" s="32"/>
+      <c r="C40" s="31"/>
       <c r="D40" s="23" t="str">
         <f t="shared" si="2"/>
         <v>0xA200</v>
@@ -2755,859 +2865,885 @@
         <v>8</v>
       </c>
       <c r="F40" s="23" t="str">
-        <f t="shared" ref="F40:F41" si="61">_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
+        <f t="shared" ref="F40:F44" si="61">_xlfn.CONCAT("0x",DEC2HEX(I40))</f>
         <v>0xAA00</v>
       </c>
       <c r="G40" s="23">
-        <f t="shared" ref="G40:G41" si="62">HEX2DEC(MID(D40, 3, LEN(D40)-2))</f>
+        <f t="shared" ref="G40:G44" si="62">HEX2DEC(MID(D40, 3, LEN(D40)-2))</f>
         <v>41472</v>
       </c>
       <c r="H40" s="23">
-        <f t="shared" ref="H40:H41" si="63">HEX2DEC(MID(E40, 3, LEN(E40)-2))</f>
+        <f t="shared" ref="H40:H44" si="63">HEX2DEC(MID(E40, 3, LEN(E40)-2))</f>
         <v>2048</v>
       </c>
       <c r="I40" s="23">
-        <f t="shared" ref="I40:I41" si="64">G40+H40</f>
+        <f t="shared" ref="I40:I44" si="64">G40+H40</f>
         <v>43520</v>
       </c>
       <c r="J40" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="L40" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="M40" s="28">
-        <v>64</v>
+      <c r="L40" s="20" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="41" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B41" s="24"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27" t="str">
+      <c r="C41" s="31"/>
+      <c r="D41" s="23" t="str">
         <f>F40</f>
         <v>0xAA00</v>
       </c>
-      <c r="E41" s="27" t="s">
-        <v>214</v>
-      </c>
-      <c r="F41" s="27" t="str">
+      <c r="E41" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="F41" s="23" t="str">
+        <f t="shared" ref="F41" si="65">_xlfn.CONCAT("0x",DEC2HEX(I41))</f>
+        <v>0xAB00</v>
+      </c>
+      <c r="G41" s="23">
+        <f t="shared" ref="G41" si="66">HEX2DEC(MID(D41, 3, LEN(D41)-2))</f>
+        <v>43520</v>
+      </c>
+      <c r="H41" s="23">
+        <f t="shared" ref="H41" si="67">HEX2DEC(MID(E41, 3, LEN(E41)-2))</f>
+        <v>256</v>
+      </c>
+      <c r="I41" s="23">
+        <f t="shared" ref="I41" si="68">G41+H41</f>
+        <v>43776</v>
+      </c>
+      <c r="J41" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="L41" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="M41" s="28">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B42" s="24"/>
+      <c r="C42" s="31"/>
+      <c r="D42" s="23" t="str">
+        <f>F41</f>
+        <v>0xAB00</v>
+      </c>
+      <c r="E42" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="F42" s="23" t="str">
+        <f t="shared" si="61"/>
+        <v>0xAC00</v>
+      </c>
+      <c r="G42" s="23">
+        <f t="shared" si="62"/>
+        <v>43776</v>
+      </c>
+      <c r="H42" s="23">
+        <f t="shared" si="63"/>
+        <v>256</v>
+      </c>
+      <c r="I42" s="23">
+        <f t="shared" si="64"/>
+        <v>44032</v>
+      </c>
+      <c r="J42" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="L42" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="M42" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B43" s="24"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="23" t="str">
+        <f>F42</f>
+        <v>0xAC00</v>
+      </c>
+      <c r="E43" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="F43" s="23" t="str">
+        <f t="shared" ref="F43" si="69">_xlfn.CONCAT("0x",DEC2HEX(I43))</f>
+        <v>0xAD00</v>
+      </c>
+      <c r="G43" s="23">
+        <f t="shared" ref="G43" si="70">HEX2DEC(MID(D43, 3, LEN(D43)-2))</f>
+        <v>44032</v>
+      </c>
+      <c r="H43" s="23">
+        <f t="shared" ref="H43" si="71">HEX2DEC(MID(E43, 3, LEN(E43)-2))</f>
+        <v>256</v>
+      </c>
+      <c r="I43" s="23">
+        <f t="shared" ref="I43" si="72">G43+H43</f>
+        <v>44288</v>
+      </c>
+      <c r="J43" s="23" t="s">
+        <v>224</v>
+      </c>
+      <c r="L43" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="M43" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B44" s="24"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="27" t="str">
+        <f>F43</f>
+        <v>0xAD00</v>
+      </c>
+      <c r="E44" s="27" t="s">
+        <v>221</v>
+      </c>
+      <c r="F44" s="27" t="str">
         <f t="shared" si="61"/>
         <v>0xB000</v>
       </c>
-      <c r="G41" s="27">
+      <c r="G44" s="27">
         <f t="shared" si="62"/>
-        <v>43520</v>
-      </c>
-      <c r="H41" s="27">
+        <v>44288</v>
+      </c>
+      <c r="H44" s="27">
         <f t="shared" si="63"/>
-        <v>1536</v>
-      </c>
-      <c r="I41" s="27">
+        <v>768</v>
+      </c>
+      <c r="I44" s="27">
         <f t="shared" si="64"/>
         <v>45056</v>
       </c>
-      <c r="J41" s="27" t="s">
+      <c r="J44" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L41" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="M41" s="18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B42" s="24"/>
-      <c r="C42" s="33" t="s">
+      <c r="L44" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="M44" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B45" s="24"/>
+      <c r="C45" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D42" s="23" t="str">
-        <f>F41</f>
+      <c r="D45" s="23" t="str">
+        <f>F44</f>
         <v>0xB000</v>
       </c>
-      <c r="E42" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M60))</f>
+      <c r="E45" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M52))</f>
         <v>0x80</v>
       </c>
-      <c r="F42" s="23" t="str">
-        <f t="shared" ref="F42:F43" si="65">_xlfn.CONCAT("0x",DEC2HEX(I42))</f>
+      <c r="F45" s="23" t="str">
+        <f t="shared" ref="F45:F46" si="73">_xlfn.CONCAT("0x",DEC2HEX(I45))</f>
         <v>0xB080</v>
       </c>
-      <c r="G42" s="23">
-        <f t="shared" ref="G42:G43" si="66">HEX2DEC(MID(D42, 3, LEN(D42)-2))</f>
+      <c r="G45" s="23">
+        <f t="shared" ref="G45:G46" si="74">HEX2DEC(MID(D45, 3, LEN(D45)-2))</f>
         <v>45056</v>
       </c>
-      <c r="H42" s="23">
-        <f t="shared" ref="H42:H43" si="67">HEX2DEC(MID(E42, 3, LEN(E42)-2))</f>
+      <c r="H45" s="23">
+        <f t="shared" ref="H45:H46" si="75">HEX2DEC(MID(E45, 3, LEN(E45)-2))</f>
         <v>128</v>
       </c>
-      <c r="I42" s="23">
-        <f t="shared" ref="I42:I43" si="68">G42+H42</f>
+      <c r="I45" s="23">
+        <f t="shared" ref="I45:I46" si="76">G45+H45</f>
         <v>45184</v>
       </c>
-      <c r="J42" s="23" t="s">
+      <c r="J45" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="L42" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="M42" s="18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B43" s="24"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="27" t="str">
+      <c r="L45" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="M45" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B46" s="24"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="27" t="str">
         <f t="shared" si="2"/>
         <v>0xB080</v>
       </c>
-      <c r="E43" s="27" t="s">
+      <c r="E46" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="F43" s="27" t="str">
-        <f t="shared" si="65"/>
+      <c r="F46" s="27" t="str">
+        <f t="shared" si="73"/>
         <v>0xB400</v>
       </c>
-      <c r="G43" s="27">
-        <f t="shared" si="66"/>
+      <c r="G46" s="27">
+        <f t="shared" si="74"/>
         <v>45184</v>
       </c>
-      <c r="H43" s="27">
-        <f t="shared" si="67"/>
+      <c r="H46" s="27">
+        <f t="shared" si="75"/>
         <v>896</v>
       </c>
-      <c r="I43" s="27">
-        <f t="shared" si="68"/>
+      <c r="I46" s="27">
+        <f t="shared" si="76"/>
         <v>46080</v>
       </c>
-      <c r="J43" s="27" t="s">
+      <c r="J46" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="L43" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="M43" s="18">
-        <v>8</v>
-      </c>
-      <c r="N43" s="18" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B44" s="24"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="23" t="str">
-        <f t="shared" ref="D44:D45" si="69">F43</f>
+      <c r="L46" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="M46" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B47" s="24"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="23" t="str">
+        <f t="shared" ref="D47:D48" si="77">F46</f>
         <v>0xB400</v>
       </c>
-      <c r="E44" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M73))</f>
+      <c r="E47" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M65))</f>
         <v>0x4</v>
       </c>
-      <c r="F44" s="23" t="str">
-        <f t="shared" ref="F44:F45" si="70">_xlfn.CONCAT("0x",DEC2HEX(I44))</f>
+      <c r="F47" s="23" t="str">
+        <f t="shared" ref="F47:F48" si="78">_xlfn.CONCAT("0x",DEC2HEX(I47))</f>
         <v>0xB404</v>
       </c>
-      <c r="G44" s="23">
-        <f t="shared" ref="G44:G45" si="71">HEX2DEC(MID(D44, 3, LEN(D44)-2))</f>
+      <c r="G47" s="23">
+        <f t="shared" ref="G47:G48" si="79">HEX2DEC(MID(D47, 3, LEN(D47)-2))</f>
         <v>46080</v>
       </c>
-      <c r="H44" s="23">
-        <f t="shared" ref="H44:H45" si="72">HEX2DEC(MID(E44, 3, LEN(E44)-2))</f>
+      <c r="H47" s="23">
+        <f t="shared" ref="H47:H48" si="80">HEX2DEC(MID(E47, 3, LEN(E47)-2))</f>
         <v>4</v>
       </c>
-      <c r="I44" s="23">
-        <f t="shared" ref="I44:I45" si="73">G44+H44</f>
+      <c r="I47" s="23">
+        <f t="shared" ref="I47:I48" si="81">G47+H47</f>
         <v>46084</v>
       </c>
-      <c r="J44" s="23" t="s">
+      <c r="J47" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="L44" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="M44" s="29">
-        <f>M41*M42*M43</f>
+      <c r="L47" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="M47" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B48" s="24"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="27" t="str">
+        <f t="shared" si="77"/>
+        <v>0xB404</v>
+      </c>
+      <c r="E48" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="F48" s="27" t="str">
+        <f t="shared" si="78"/>
+        <v>0xB800</v>
+      </c>
+      <c r="G48" s="27">
+        <f t="shared" si="79"/>
+        <v>46084</v>
+      </c>
+      <c r="H48" s="27">
+        <f t="shared" si="80"/>
+        <v>1020</v>
+      </c>
+      <c r="I48" s="27">
+        <f t="shared" si="81"/>
+        <v>47104</v>
+      </c>
+      <c r="J48" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="L48" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="M48" s="18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B49" s="24"/>
+      <c r="C49" s="35"/>
+      <c r="D49" s="23" t="str">
+        <f>F48</f>
+        <v>0xB800</v>
+      </c>
+      <c r="E49" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M59))</f>
+        <v>0x800</v>
+      </c>
+      <c r="F49" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I49))</f>
+        <v>0xC000</v>
+      </c>
+      <c r="G49" s="23">
+        <f t="shared" ref="G49:H51" si="82">HEX2DEC(MID(D49, 3, LEN(D49)-2))</f>
+        <v>47104</v>
+      </c>
+      <c r="H49" s="23">
+        <f t="shared" si="82"/>
         <v>2048</v>
       </c>
-    </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B45" s="36"/>
-      <c r="C45" s="34"/>
-      <c r="D45" s="27" t="str">
-        <f t="shared" si="69"/>
-        <v>0xB404</v>
-      </c>
-      <c r="E45" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="F45" s="27" t="str">
-        <f t="shared" si="70"/>
-        <v>0xB800</v>
-      </c>
-      <c r="G45" s="27">
-        <f t="shared" si="71"/>
-        <v>46084</v>
-      </c>
-      <c r="H45" s="27">
-        <f t="shared" si="72"/>
-        <v>1020</v>
-      </c>
-      <c r="I45" s="27">
-        <f t="shared" si="73"/>
-        <v>47104</v>
-      </c>
-      <c r="J45" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="L45" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="M45" s="18">
-        <f>M44/8</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B46" s="38" t="s">
+      <c r="I49" s="23">
+        <f>G49+H49</f>
+        <v>49152</v>
+      </c>
+      <c r="J49" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="L49" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="M49" s="18">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B50" s="36"/>
+      <c r="C50" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="D50" s="23" t="str">
+        <f>F49</f>
+        <v>0xC000</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F50" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I50))</f>
+        <v>0x10000</v>
+      </c>
+      <c r="G50" s="23">
+        <f t="shared" si="82"/>
+        <v>49152</v>
+      </c>
+      <c r="H50" s="23">
+        <f t="shared" si="82"/>
+        <v>16384</v>
+      </c>
+      <c r="I50" s="23">
+        <f>G50+H50</f>
+        <v>65536</v>
+      </c>
+      <c r="J50" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="L50" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="M50" s="29">
+        <f>SUM(M42:M49)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B51" s="38" t="s">
         <v>134</v>
       </c>
-      <c r="C46" s="35"/>
-      <c r="D46" s="23" t="str">
-        <f>F45</f>
-        <v>0xB800</v>
-      </c>
-      <c r="E46" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M67))</f>
-        <v>0x800</v>
-      </c>
-      <c r="F46" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I46))</f>
-        <v>0xC000</v>
-      </c>
-      <c r="G46" s="23">
-        <f t="shared" ref="G46:H48" si="74">HEX2DEC(MID(D46, 3, LEN(D46)-2))</f>
-        <v>47104</v>
-      </c>
-      <c r="H46" s="23">
-        <f t="shared" si="74"/>
-        <v>2048</v>
-      </c>
-      <c r="I46" s="23">
-        <f>G46+H46</f>
-        <v>49152</v>
-      </c>
-      <c r="J46" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="L46" s="29" t="s">
-        <v>136</v>
-      </c>
-      <c r="M46" s="29">
-        <f>M40*M45</f>
-        <v>16384</v>
-      </c>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B47" s="39" t="s">
-        <v>133</v>
-      </c>
-      <c r="C47" s="37" t="s">
-        <v>41</v>
-      </c>
-      <c r="D47" s="23" t="str">
-        <f>F46</f>
-        <v>0xC000</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>6</v>
-      </c>
-      <c r="F47" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I47))</f>
-        <v>0x10000</v>
-      </c>
-      <c r="G47" s="23">
-        <f t="shared" si="74"/>
-        <v>49152</v>
-      </c>
-      <c r="H47" s="23">
-        <f t="shared" si="74"/>
-        <v>16384</v>
-      </c>
-      <c r="I47" s="23">
-        <f>G47+H47</f>
-        <v>65536</v>
-      </c>
-      <c r="J47" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B48" s="39"/>
-      <c r="C48" s="40" t="s">
+      <c r="C51" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="D48" s="23" t="str">
+      <c r="D51" s="23" t="str">
         <f t="shared" si="2"/>
         <v>0x10000</v>
       </c>
-      <c r="E48" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M37))</f>
+      <c r="E51" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M29))</f>
         <v>0x100</v>
       </c>
-      <c r="F48" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(I48))</f>
+      <c r="F51" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(I51))</f>
         <v>0x10100</v>
       </c>
-      <c r="G48" s="23">
-        <f t="shared" si="74"/>
+      <c r="G51" s="23">
+        <f t="shared" si="82"/>
         <v>65536</v>
       </c>
-      <c r="H48" s="23">
-        <f t="shared" si="74"/>
+      <c r="H51" s="23">
+        <f t="shared" si="82"/>
         <v>256</v>
       </c>
-      <c r="I48" s="23">
-        <f>G48+H48</f>
+      <c r="I51" s="23">
+        <f>G51+H51</f>
         <v>65792</v>
       </c>
-      <c r="J48" s="23" t="s">
+      <c r="J51" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="L48" s="20" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B49" s="39"/>
-      <c r="L49" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="M49" s="28">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="50" spans="2:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="B50" s="39"/>
-      <c r="C50"/>
-      <c r="D50"/>
-      <c r="E50"/>
-      <c r="F50"/>
-      <c r="G50"/>
-      <c r="H50"/>
-      <c r="I50"/>
-      <c r="J50"/>
-      <c r="L50" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="M50" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B51" s="39"/>
-      <c r="C51" s="33" t="s">
+      <c r="L51" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="M51" s="18">
+        <f>M50/8</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B52" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="L52" s="29" t="s">
+        <v>129</v>
+      </c>
+      <c r="M52" s="29">
+        <f>M41*M51</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" ht="15" x14ac:dyDescent="0.25">
+      <c r="B53" s="39"/>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53"/>
+    </row>
+    <row r="54" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B54" s="39"/>
+      <c r="C54" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="D51" s="23"/>
-      <c r="E51" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M46))</f>
+      <c r="D54" s="23"/>
+      <c r="E54" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M38))</f>
         <v>0x4000</v>
       </c>
-      <c r="F51" s="23"/>
-      <c r="G51" s="23"/>
-      <c r="H51" s="23">
-        <f>HEX2DEC(MID(E51, 3, LEN(E51)-2))</f>
+      <c r="F54" s="23"/>
+      <c r="G54" s="23"/>
+      <c r="H54" s="23">
+        <f>HEX2DEC(MID(E54, 3, LEN(E54)-2))</f>
         <v>16384</v>
       </c>
-      <c r="I51" s="23"/>
-      <c r="J51" s="23" t="s">
+      <c r="I54" s="23"/>
+      <c r="J54" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="L51" s="18" t="s">
-        <v>153</v>
-      </c>
-      <c r="M51" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B52" s="39"/>
-      <c r="C52" s="35"/>
-      <c r="D52" s="23"/>
-      <c r="E52" s="23" t="str">
-        <f>_xlfn.CONCAT("0x",DEC2HEX(M79))</f>
+      <c r="L54" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="M54" s="18" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B55" s="39"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23" t="str">
+        <f>_xlfn.CONCAT("0x",DEC2HEX(M71))</f>
         <v>0x800</v>
-      </c>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23"/>
-      <c r="H52" s="23">
-        <f>HEX2DEC(MID(E52, 3, LEN(E52)-2))</f>
-        <v>2048</v>
-      </c>
-      <c r="I52" s="23" t="s">
-        <v>148</v>
-      </c>
-      <c r="J52" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="L52" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="M52" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B53" s="39"/>
-      <c r="L53" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="M53" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B54" s="39"/>
-      <c r="L54" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="M54" s="18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B55" s="39"/>
-      <c r="C55" s="40" t="s">
-        <v>145</v>
-      </c>
-      <c r="D55" s="23"/>
-      <c r="E55" s="23" t="s">
-        <v>147</v>
       </c>
       <c r="F55" s="23"/>
       <c r="G55" s="23"/>
       <c r="H55" s="23">
-        <f t="shared" ref="H55" si="75">HEX2DEC(MID(E55, 3, LEN(E55)-2))</f>
+        <f>HEX2DEC(MID(E55, 3, LEN(E55)-2))</f>
+        <v>2048</v>
+      </c>
+      <c r="I55" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="J55" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="L55" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="M55" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B56" s="39"/>
+      <c r="L56" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="M56" s="18">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B57" s="39"/>
+      <c r="L57" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="M57" s="28">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="58" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B58" s="39"/>
+      <c r="C58" s="40" t="s">
+        <v>145</v>
+      </c>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23" t="s">
+        <v>147</v>
+      </c>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23">
+        <f t="shared" ref="H58" si="83">HEX2DEC(MID(E58, 3, LEN(E58)-2))</f>
         <v>131072</v>
       </c>
-      <c r="I55" s="23"/>
-      <c r="J55" s="23" t="s">
+      <c r="I58" s="23"/>
+      <c r="J58" s="23" t="s">
         <v>145</v>
       </c>
-      <c r="L55" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="M55" s="18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B56" s="39"/>
-      <c r="C56" s="40" t="s">
+      <c r="L58" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="M58" s="18">
+        <f>M55*M56*M57</f>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="59" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B59" s="39"/>
+      <c r="C59" s="40" t="s">
         <v>158</v>
       </c>
-      <c r="D56" s="23"/>
-      <c r="E56" s="23" t="s">
+      <c r="D59" s="23"/>
+      <c r="E59" s="23" t="s">
         <v>159</v>
       </c>
-      <c r="F56" s="23"/>
-      <c r="G56" s="23"/>
-      <c r="H56" s="23">
-        <f t="shared" ref="H56" si="76">HEX2DEC(MID(E56, 3, LEN(E56)-2))</f>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="23">
+        <f t="shared" ref="H59" si="84">HEX2DEC(MID(E59, 3, LEN(E59)-2))</f>
         <v>65536</v>
       </c>
-      <c r="I56" s="23"/>
-      <c r="J56" s="23" t="s">
+      <c r="I59" s="23"/>
+      <c r="J59" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="L56" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="M56" s="18">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B57" s="39"/>
-      <c r="L57" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="M57" s="18">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B58" s="39"/>
-      <c r="L58" s="29" t="s">
-        <v>4</v>
-      </c>
-      <c r="M58" s="29">
-        <f>SUM(M50:M57)</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B59" s="39"/>
       <c r="L59" s="18" t="s">
-        <v>3</v>
+        <v>137</v>
       </c>
       <c r="M59" s="18">
         <f>M58/8</f>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="60" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B60" s="39"/>
+    </row>
+    <row r="61" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B61" s="39"/>
+      <c r="L61" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="M61" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="P61" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="62" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B62" s="39"/>
+      <c r="L62" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="M62" s="18">
+        <v>32</v>
+      </c>
+      <c r="O62" s="18">
+        <f>384*2</f>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="63" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B63" s="39"/>
+      <c r="L63" s="28" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B60" s="39"/>
-      <c r="L60" s="29" t="s">
-        <v>129</v>
-      </c>
-      <c r="M60" s="29">
-        <f>M49*M59</f>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="61" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B61" s="39"/>
-    </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B62" s="39"/>
-      <c r="L62" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="M62" s="18" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B63" s="39"/>
-      <c r="L63" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="M63" s="18">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M63" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B64" s="39"/>
       <c r="L64" s="18" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="M64" s="18">
+        <f>M62*M63</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B65" s="39"/>
+      <c r="L65" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="M65" s="18">
+        <f>M64/8</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B66" s="39"/>
+    </row>
+    <row r="67" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B67" s="39"/>
+      <c r="L67" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="M67" s="18" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="68" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B68" s="39"/>
+      <c r="L68" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="M68" s="18">
         <v>512</v>
       </c>
-    </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B65" s="39"/>
-      <c r="L65" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="M65" s="28">
+      <c r="N68" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="69" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B69" s="39"/>
+      <c r="L69" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="M69" s="28">
+        <v>32</v>
+      </c>
+      <c r="N69" s="18" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="70" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B70" s="39"/>
+      <c r="L70" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="M70" s="18">
+        <f>M68*M69</f>
+        <v>16384</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B71" s="39"/>
+      <c r="L71" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="M71" s="18">
+        <f>M70/8</f>
+        <v>2048</v>
+      </c>
+    </row>
+    <row r="72" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B72" s="39"/>
+    </row>
+    <row r="73" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B73" s="39"/>
+      <c r="L73" s="20" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B74" s="41"/>
+      <c r="L74" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="M74" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="75" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L75" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="M75" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L76" s="18" t="s">
+        <v>180</v>
+      </c>
+      <c r="M76" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L77" s="18" t="s">
+        <v>181</v>
+      </c>
+      <c r="M77" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L78" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="M78" s="43">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="79" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L79" s="29" t="s">
+        <v>184</v>
+      </c>
+      <c r="M79" s="29">
+        <f>SUM(M74:M78)</f>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="80" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="L80" s="18" t="s">
+        <v>183</v>
+      </c>
+      <c r="M80" s="18">
+        <f>M79/8</f>
         <v>16</v>
       </c>
     </row>
-    <row r="66" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B66" s="39"/>
-      <c r="L66" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="M66" s="18">
-        <f>M63*M64*M65</f>
-        <v>16384</v>
-      </c>
-    </row>
-    <row r="67" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B67" s="39"/>
-      <c r="L67" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="M67" s="18">
-        <f>M66/8</f>
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B68" s="39"/>
-    </row>
-    <row r="69" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B69" s="41"/>
-      <c r="L69" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="M69" s="18" t="s">
-        <v>123</v>
-      </c>
-      <c r="P69" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="L70" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="M70" s="18">
-        <v>32</v>
-      </c>
-      <c r="O70" s="18">
-        <f>384*2</f>
-        <v>768</v>
-      </c>
-    </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="L71" s="28" t="s">
-        <v>4</v>
-      </c>
-      <c r="M71" s="28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="L72" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="M72" s="18">
-        <f>M70*M71</f>
-        <v>32</v>
-      </c>
-    </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="L73" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="M73" s="18">
-        <f>M72/8</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="L75" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="M75" s="18" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="76" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="L76" s="18" t="s">
-        <v>125</v>
-      </c>
-      <c r="M76" s="18">
-        <v>512</v>
-      </c>
-      <c r="N76" s="18" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="77" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="L77" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="M77" s="28">
-        <v>32</v>
-      </c>
-      <c r="N77" s="18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="78" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="L78" s="29" t="s">
-        <v>132</v>
-      </c>
-      <c r="M78" s="18">
-        <f>M76*M77</f>
-        <v>16384</v>
-      </c>
-    </row>
-    <row r="79" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="L79" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="M79" s="18">
-        <f>M78/8</f>
-        <v>2048</v>
-      </c>
-    </row>
-    <row r="81" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L81" s="20" t="s">
-        <v>198</v>
-      </c>
-    </row>
     <row r="82" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L82" s="18" t="s">
-        <v>178</v>
-      </c>
-      <c r="M82" s="18">
-        <v>8</v>
+      <c r="L82" s="20" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="83" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L83" s="18" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="M83" s="18">
-        <v>8</v>
+        <v>32</v>
+      </c>
+      <c r="N83" s="18" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="84" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L84" s="18" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="M84" s="18">
-        <v>8</v>
+        <v>24</v>
+      </c>
+      <c r="N84" s="18" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="85" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L85" s="18" t="s">
-        <v>181</v>
+        <v>189</v>
       </c>
       <c r="M85" s="18">
         <v>8</v>
       </c>
     </row>
     <row r="86" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L86" s="43" t="s">
-        <v>154</v>
-      </c>
-      <c r="M86" s="43">
-        <v>96</v>
+      <c r="L86" s="29" t="s">
+        <v>187</v>
+      </c>
+      <c r="M86" s="29">
+        <f>M83*M84*M85</f>
+        <v>6144</v>
       </c>
     </row>
     <row r="87" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L87" s="29" t="s">
-        <v>184</v>
-      </c>
-      <c r="M87" s="29">
-        <f>SUM(M82:M86)</f>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="88" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L88" s="18" t="s">
-        <v>183</v>
-      </c>
-      <c r="M88" s="18">
-        <f>M87/8</f>
-        <v>16</v>
+      <c r="L87" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="M87" s="18">
+        <f>M86/8</f>
+        <v>768</v>
+      </c>
+    </row>
+    <row r="89" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L89" s="20" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="90" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L90" s="20" t="s">
-        <v>182</v>
+      <c r="L90" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="M90" s="28">
+        <v>64</v>
       </c>
     </row>
     <row r="91" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L91" s="18" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="M91" s="18">
-        <v>32</v>
-      </c>
-      <c r="N91" s="18" t="s">
-        <v>199</v>
+        <v>16</v>
       </c>
     </row>
     <row r="92" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L92" s="18" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="M92" s="18">
-        <v>24</v>
-      </c>
-      <c r="N92" s="18" t="s">
-        <v>200</v>
+        <v>16</v>
       </c>
     </row>
     <row r="93" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L93" s="18" t="s">
-        <v>189</v>
+        <v>194</v>
       </c>
       <c r="M93" s="18">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="N93" s="18" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="94" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L94" s="29" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="M94" s="29">
         <f>M91*M92*M93</f>
-        <v>6144</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="95" spans="12:14" x14ac:dyDescent="0.2">
       <c r="L95" s="18" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="M95" s="18">
         <f>M94/8</f>
-        <v>768</v>
-      </c>
-    </row>
-    <row r="97" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L97" s="20" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="98" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L98" s="28" t="s">
-        <v>191</v>
-      </c>
-      <c r="M98" s="28">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="99" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L99" s="18" t="s">
-        <v>192</v>
-      </c>
-      <c r="M99" s="18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="100" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L100" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="M100" s="18">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="101" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L101" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="M101" s="18">
-        <v>16</v>
-      </c>
-      <c r="N101" s="18" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="102" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L102" s="29" t="s">
-        <v>195</v>
-      </c>
-      <c r="M102" s="29">
-        <f>M99*M100*M101</f>
-        <v>4096</v>
-      </c>
-    </row>
-    <row r="103" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L103" s="18" t="s">
-        <v>196</v>
-      </c>
-      <c r="M103" s="18">
-        <f>M102/8</f>
         <v>512</v>
       </c>
     </row>
-    <row r="104" spans="12:14" x14ac:dyDescent="0.2">
-      <c r="L104" s="29" t="s">
+    <row r="96" spans="12:14" x14ac:dyDescent="0.2">
+      <c r="L96" s="29" t="s">
         <v>197</v>
       </c>
-      <c r="M104" s="29">
-        <f>M98*M103</f>
+      <c r="M96" s="29">
+        <f>M90*M95</f>
         <v>32768</v>
       </c>
     </row>

</xml_diff>